<commit_message>
2017.03.31 stress and strain
</commit_message>
<xml_diff>
--- a/quiz_calc.xlsx
+++ b/quiz_calc.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17766"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17830"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="64">
   <si>
     <t>Ix</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -203,6 +203,82 @@
   </si>
   <si>
     <t>M</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>L</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>delta_L</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>d</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>delta_d</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>P</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>sigma</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>epsilon</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>E</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>nu</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>G</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Area</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>beta</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>강봉</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>L</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>d</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>A</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>P</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>delta_L</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>E</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -210,12 +286,14 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="5">
+  <numFmts count="7">
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="176" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="177" formatCode="_-* #,##0.00000_-;\-* #,##0.00000_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="179" formatCode="_-* #,##0.000_-;\-* #,##0.000_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="180" formatCode="_-* #,##0.0000_-;\-* #,##0.0000_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="178" formatCode="_-* #,##0.000_-;\-* #,##0.000_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="179" formatCode="_-* #,##0.0000_-;\-* #,##0.0000_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="180" formatCode="_-* #,##0.000000_-;\-* #,##0.000000_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="181" formatCode="_-* #,##0.00000000_-;\-* #,##0.00000000_-;_-* &quot;-&quot;_-;_-@_-"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -267,7 +345,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -280,10 +358,16 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="179" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="180" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="181" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -601,10 +685,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P49"/>
+  <dimension ref="A1:P85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="L49" sqref="L49"/>
+    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="G84" sqref="G84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -615,7 +699,8 @@
     <col min="7" max="7" width="13.5" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="17.25" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="13.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="17.25" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.25" style="1" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="15.625" style="1" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="17.25" style="1" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="13.5" style="1" bestFit="1" customWidth="1"/>
@@ -1582,6 +1667,12 @@
         <v>112500</v>
       </c>
     </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="C27" s="2">
+        <f>7530000/300/500</f>
+        <v>50.2</v>
+      </c>
+    </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B30" s="1" t="s">
         <v>28</v>
@@ -1631,7 +1722,7 @@
         <v>25</v>
       </c>
       <c r="E31" s="1">
-        <f>C31/2-D31</f>
+        <f t="shared" ref="E31:E39" si="10">C31/2-D31</f>
         <v>100</v>
       </c>
       <c r="F31" s="1">
@@ -1643,7 +1734,7 @@
         <v>351562.5</v>
       </c>
       <c r="H31" s="1">
-        <f>B31*C31^3/12</f>
+        <f t="shared" ref="H31:H39" si="11">B31*C31^3/12</f>
         <v>162760416.66666666</v>
       </c>
       <c r="I31" s="2">
@@ -1676,7 +1767,7 @@
         <v>125</v>
       </c>
       <c r="E32" s="1">
-        <f>C32/2-D32</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="F32" s="1">
@@ -1688,7 +1779,7 @@
         <v>976562.5</v>
       </c>
       <c r="H32" s="1">
-        <f>B32*C32^3/12</f>
+        <f t="shared" si="11"/>
         <v>162760416.66666666</v>
       </c>
       <c r="I32" s="2">
@@ -1696,15 +1787,15 @@
         <v>57.6</v>
       </c>
       <c r="J32" s="1">
-        <f t="shared" ref="J32:J33" si="10">250000000</f>
+        <f t="shared" ref="J32:J33" si="12">250000000</f>
         <v>250000000</v>
       </c>
       <c r="K32" s="1">
-        <f t="shared" ref="K32:K33" si="11">J32/H32*E32</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
+        <f t="shared" ref="K32:K33" si="13">J32/H32*E32</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A33" s="3">
         <v>3</v>
       </c>
@@ -1720,7 +1811,7 @@
         <v>0</v>
       </c>
       <c r="E33" s="1">
-        <f>C33/2-D33</f>
+        <f t="shared" si="10"/>
         <v>125</v>
       </c>
       <c r="F33" s="1">
@@ -1732,7 +1823,7 @@
         <v>0</v>
       </c>
       <c r="H33" s="1">
-        <f>B33*C33^3/12</f>
+        <f t="shared" si="11"/>
         <v>162760416.66666666</v>
       </c>
       <c r="I33" s="2">
@@ -1740,15 +1831,15 @@
         <v>0</v>
       </c>
       <c r="J33" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>250000000</v>
       </c>
       <c r="K33" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>192</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A34" s="3">
         <v>4</v>
       </c>
@@ -1763,7 +1854,7 @@
         <v>60</v>
       </c>
       <c r="E34" s="1">
-        <f>C34/2-D34</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="F34" s="1">
@@ -1775,7 +1866,7 @@
         <v>90000</v>
       </c>
       <c r="H34" s="1">
-        <f>B34*C34^3/12</f>
+        <f t="shared" si="11"/>
         <v>7200000</v>
       </c>
       <c r="I34" s="2">
@@ -1783,7 +1874,7 @@
         <v>18.75</v>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A35" s="3">
         <v>5</v>
       </c>
@@ -1797,7 +1888,7 @@
         <v>300</v>
       </c>
       <c r="E35" s="1">
-        <f>C35/2-D35</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="F35" s="1">
@@ -1808,15 +1899,16 @@
         <v>18000000</v>
       </c>
       <c r="H35" s="1">
-        <f>B35*C35^3/12</f>
+        <f t="shared" si="11"/>
         <v>7200000000</v>
       </c>
       <c r="I35" s="2">
         <f>F35*G35/H35/B35</f>
         <v>3.125</v>
       </c>
-    </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M35" s="6"/>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A36" s="3">
         <v>5</v>
       </c>
@@ -1830,11 +1922,11 @@
         <v>0</v>
       </c>
       <c r="E36" s="1">
-        <f>C36/2-D36</f>
+        <f t="shared" si="10"/>
         <v>300</v>
       </c>
       <c r="H36" s="1">
-        <f>B36*C36^3/12</f>
+        <f t="shared" si="11"/>
         <v>7200000000</v>
       </c>
       <c r="I36" s="2"/>
@@ -1843,11 +1935,12 @@
         <v>750000000</v>
       </c>
       <c r="K36" s="4">
-        <f t="shared" ref="K36" si="12">J36/H36*E36</f>
+        <f t="shared" ref="K36" si="14">J36/H36*E36</f>
         <v>31.25</v>
       </c>
-    </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M36" s="2"/>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A37" s="3">
         <v>6</v>
       </c>
@@ -1861,7 +1954,7 @@
         <v>250</v>
       </c>
       <c r="E37" s="1">
-        <f>C37/2-D37</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="F37" s="1">
@@ -1872,15 +1965,16 @@
         <v>9375000</v>
       </c>
       <c r="H37" s="1">
-        <f>B37*C37^3/12</f>
+        <f t="shared" si="11"/>
         <v>3125000000</v>
       </c>
       <c r="I37" s="2">
         <f>F37*G37/H37/B37</f>
         <v>20</v>
       </c>
-    </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M37" s="5"/>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A38" s="3">
         <v>6</v>
       </c>
@@ -1894,11 +1988,11 @@
         <v>0</v>
       </c>
       <c r="E38" s="1">
-        <f>C38/2-D38</f>
+        <f t="shared" si="10"/>
         <v>250</v>
       </c>
       <c r="H38" s="1">
-        <f>B38*C38^3/12</f>
+        <f t="shared" si="11"/>
         <v>3125000000</v>
       </c>
       <c r="I38" s="2"/>
@@ -1907,11 +2001,12 @@
         <v>6000000000</v>
       </c>
       <c r="K38" s="4">
-        <f t="shared" ref="K38:K39" si="13">J38/H38*E38</f>
+        <f t="shared" ref="K38:K39" si="15">J38/H38*E38</f>
         <v>480</v>
       </c>
-    </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M38" s="6"/>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A39" s="3">
         <v>7</v>
       </c>
@@ -1926,7 +2021,7 @@
         <v>140</v>
       </c>
       <c r="E39" s="1">
-        <f>C39/2-D39</f>
+        <f t="shared" si="10"/>
         <v>40</v>
       </c>
       <c r="F39" s="1">
@@ -1938,385 +2033,1475 @@
         <v>3696000</v>
       </c>
       <c r="H39" s="1">
-        <f>B39*C39^3/12</f>
+        <f t="shared" si="11"/>
         <v>933120000</v>
       </c>
       <c r="I39" s="5">
-        <f>F39*G39/H39/B39</f>
+        <f t="shared" ref="I39:I48" si="16">F39*G39/H39/B39</f>
         <v>3.9609053497942388</v>
       </c>
       <c r="J39" s="1">
         <v>720000000</v>
       </c>
       <c r="K39" s="5">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>30.864197530864196</v>
       </c>
-    </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="I40" s="2"/>
-    </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B42" s="1" t="s">
+      <c r="M39" s="6"/>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A40" s="3">
+        <v>8</v>
+      </c>
+      <c r="B40" s="1">
+        <v>300</v>
+      </c>
+      <c r="C40" s="1">
+        <v>500</v>
+      </c>
+      <c r="D40" s="1">
+        <v>250</v>
+      </c>
+      <c r="E40" s="1">
+        <f t="shared" ref="E40" si="17">C40/2-D40</f>
+        <v>0</v>
+      </c>
+      <c r="F40" s="1">
+        <v>753000</v>
+      </c>
+      <c r="G40" s="1">
+        <f>B40*D40*(E40+D40/2)</f>
+        <v>9375000</v>
+      </c>
+      <c r="H40" s="1">
+        <f t="shared" ref="H40" si="18">B40*C40^3/12</f>
+        <v>3125000000</v>
+      </c>
+      <c r="I40" s="5">
+        <f t="shared" si="16"/>
+        <v>7.53</v>
+      </c>
+      <c r="K40" s="5"/>
+      <c r="M40" s="2"/>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A41" s="3">
+        <v>9</v>
+      </c>
+      <c r="B41" s="1">
+        <v>10</v>
+      </c>
+      <c r="F41" s="1">
+        <v>9265</v>
+      </c>
+      <c r="G41" s="1">
+        <f>100*20*70+10*60*30</f>
+        <v>158000</v>
+      </c>
+      <c r="H41" s="1">
+        <f>100*160^3/12-90*120^3/12</f>
+        <v>21173333.333333336</v>
+      </c>
+      <c r="I41" s="6">
+        <f t="shared" si="16"/>
+        <v>6.9137437027707804</v>
+      </c>
+      <c r="K41" s="5"/>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A42" s="3">
+        <v>10</v>
+      </c>
+      <c r="B42" s="1">
+        <v>10</v>
+      </c>
+      <c r="F42" s="1">
+        <v>9265</v>
+      </c>
+      <c r="G42" s="1">
+        <f>100*20*70+10*30*45</f>
+        <v>153500</v>
+      </c>
+      <c r="H42" s="1">
+        <f>100*160^3/12-90*120^3/12</f>
+        <v>21173333.333333336</v>
+      </c>
+      <c r="I42" s="5">
+        <f t="shared" si="16"/>
+        <v>6.7168332808564228</v>
+      </c>
+      <c r="K42" s="7"/>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A43" s="3">
+        <v>11</v>
+      </c>
+      <c r="B43" s="1">
+        <v>200</v>
+      </c>
+      <c r="C43" s="1">
+        <v>360</v>
+      </c>
+      <c r="D43" s="1">
+        <v>0</v>
+      </c>
+      <c r="E43" s="1">
+        <f t="shared" ref="E43" si="19">C43/2-D43</f>
+        <v>180</v>
+      </c>
+      <c r="G43" s="1">
+        <f t="shared" ref="G43:G48" si="20">B43*D43*(E43+D43/2)</f>
+        <v>0</v>
+      </c>
+      <c r="H43" s="1">
+        <f t="shared" ref="H43" si="21">B43*C43^3/12</f>
+        <v>777600000</v>
+      </c>
+      <c r="I43" s="5">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="J43" s="1">
+        <f>350*1000000</f>
+        <v>350000000</v>
+      </c>
+      <c r="K43" s="5">
+        <f t="shared" ref="K43" si="22">J43/H43*E43</f>
+        <v>81.018518518518519</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A44" s="3">
+        <v>11</v>
+      </c>
+      <c r="B44" s="1">
+        <v>200</v>
+      </c>
+      <c r="C44" s="1">
+        <v>360</v>
+      </c>
+      <c r="D44" s="1">
+        <f>C44/2</f>
+        <v>180</v>
+      </c>
+      <c r="E44" s="1">
+        <f t="shared" ref="E44:E45" si="23">C44/2-D44</f>
+        <v>0</v>
+      </c>
+      <c r="G44" s="1">
+        <f t="shared" si="20"/>
+        <v>3240000</v>
+      </c>
+      <c r="H44" s="1">
+        <f t="shared" ref="H44:H45" si="24">B44*C44^3/12</f>
+        <v>777600000</v>
+      </c>
+      <c r="I44" s="5">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="J44" s="1">
+        <f>350*1000000</f>
+        <v>350000000</v>
+      </c>
+      <c r="K44" s="5">
+        <f t="shared" ref="K44:K45" si="25">J44/H44*E44</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A45" s="3">
+        <v>12</v>
+      </c>
+      <c r="B45" s="1">
+        <v>100</v>
+      </c>
+      <c r="C45" s="1">
+        <v>220</v>
+      </c>
+      <c r="D45" s="1">
+        <v>0</v>
+      </c>
+      <c r="E45" s="1">
+        <f t="shared" si="23"/>
+        <v>110</v>
+      </c>
+      <c r="G45" s="1">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="H45" s="1">
+        <f t="shared" si="24"/>
+        <v>88733333.333333328</v>
+      </c>
+      <c r="I45" s="5">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="J45" s="1">
+        <f>76.3*1000000</f>
+        <v>76300000</v>
+      </c>
+      <c r="K45" s="5">
+        <f t="shared" si="25"/>
+        <v>94.586776859504141</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A46" s="3">
+        <v>12</v>
+      </c>
+      <c r="B46" s="1">
+        <v>100</v>
+      </c>
+      <c r="C46" s="1">
+        <v>220</v>
+      </c>
+      <c r="D46" s="1">
+        <v>35</v>
+      </c>
+      <c r="E46" s="1">
+        <f t="shared" ref="E46:E47" si="26">C46/2-D46</f>
+        <v>75</v>
+      </c>
+      <c r="G46" s="1">
+        <f t="shared" si="20"/>
+        <v>323750</v>
+      </c>
+      <c r="H46" s="1">
+        <f t="shared" ref="H46:H47" si="27">B46*C46^3/12</f>
+        <v>88733333.333333328</v>
+      </c>
+      <c r="I46" s="5">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="J46" s="1">
+        <f t="shared" ref="J46:J48" si="28">76.3*1000000</f>
+        <v>76300000</v>
+      </c>
+      <c r="K46" s="5">
+        <f t="shared" ref="K46:K47" si="29">J46/H46*E46</f>
+        <v>64.490984222389187</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A47" s="3">
+        <v>12</v>
+      </c>
+      <c r="B47" s="1">
+        <v>100</v>
+      </c>
+      <c r="C47" s="1">
+        <v>220</v>
+      </c>
+      <c r="D47" s="1">
+        <v>60</v>
+      </c>
+      <c r="E47" s="1">
+        <f t="shared" si="26"/>
+        <v>50</v>
+      </c>
+      <c r="G47" s="1">
+        <f t="shared" si="20"/>
+        <v>480000</v>
+      </c>
+      <c r="H47" s="1">
+        <f t="shared" si="27"/>
+        <v>88733333.333333328</v>
+      </c>
+      <c r="I47" s="5">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="J47" s="1">
+        <f t="shared" si="28"/>
+        <v>76300000</v>
+      </c>
+      <c r="K47" s="5">
+        <f t="shared" si="29"/>
+        <v>42.993989481592791</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A48" s="3">
+        <v>12</v>
+      </c>
+      <c r="B48" s="1">
+        <v>100</v>
+      </c>
+      <c r="C48" s="1">
+        <v>220</v>
+      </c>
+      <c r="D48" s="1">
+        <v>85</v>
+      </c>
+      <c r="E48" s="1">
+        <f t="shared" ref="E48" si="30">C48/2-D48</f>
+        <v>25</v>
+      </c>
+      <c r="G48" s="1">
+        <f t="shared" si="20"/>
+        <v>573750</v>
+      </c>
+      <c r="H48" s="1">
+        <f t="shared" ref="H48" si="31">B48*C48^3/12</f>
+        <v>88733333.333333328</v>
+      </c>
+      <c r="I48" s="5">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="J48" s="1">
+        <f t="shared" si="28"/>
+        <v>76300000</v>
+      </c>
+      <c r="K48" s="5">
+        <f t="shared" ref="K48" si="32">J48/H48*E48</f>
+        <v>21.496994740796396</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A49" s="3">
+        <v>13</v>
+      </c>
+      <c r="B49" s="1">
+        <v>10</v>
+      </c>
+      <c r="E49" s="1">
+        <v>0</v>
+      </c>
+      <c r="H49" s="1">
+        <f>100*160^3/12-90*120^3/12</f>
+        <v>21173333.333333336</v>
+      </c>
+      <c r="I49" s="6"/>
+      <c r="J49" s="1">
+        <f>73*1000000</f>
+        <v>73000000</v>
+      </c>
+      <c r="K49" s="5">
+        <f t="shared" ref="K49:K50" si="33">J49/H49*E49</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A50" s="3">
+        <v>13</v>
+      </c>
+      <c r="B50" s="1">
+        <v>10</v>
+      </c>
+      <c r="E50" s="1">
+        <v>30</v>
+      </c>
+      <c r="H50" s="1">
+        <f>100*160^3/12-90*120^3/12</f>
+        <v>21173333.333333336</v>
+      </c>
+      <c r="I50" s="5"/>
+      <c r="J50" s="1">
+        <f>73*1000000</f>
+        <v>73000000</v>
+      </c>
+      <c r="K50" s="5">
+        <f t="shared" si="33"/>
+        <v>103.43198992443322</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A51" s="3">
+        <v>13</v>
+      </c>
+      <c r="B51" s="1">
+        <v>10</v>
+      </c>
+      <c r="E51" s="1">
+        <v>60</v>
+      </c>
+      <c r="H51" s="1">
+        <f>100*160^3/12-90*120^3/12</f>
+        <v>21173333.333333336</v>
+      </c>
+      <c r="I51" s="6"/>
+      <c r="J51" s="1">
+        <f>73*1000000</f>
+        <v>73000000</v>
+      </c>
+      <c r="K51" s="5">
+        <f t="shared" ref="K51:K55" si="34">J51/H51*E51</f>
+        <v>206.86397984886645</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A52" s="3">
+        <v>13</v>
+      </c>
+      <c r="B52" s="1">
+        <v>10</v>
+      </c>
+      <c r="E52" s="1">
+        <v>80</v>
+      </c>
+      <c r="H52" s="1">
+        <f>100*160^3/12-90*120^3/12</f>
+        <v>21173333.333333336</v>
+      </c>
+      <c r="I52" s="5"/>
+      <c r="J52" s="1">
+        <f>73*1000000</f>
+        <v>73000000</v>
+      </c>
+      <c r="K52" s="5">
+        <f t="shared" si="34"/>
+        <v>275.81863979848862</v>
+      </c>
+    </row>
+    <row r="53" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A53" s="3">
+        <v>14</v>
+      </c>
+      <c r="B53" s="1">
+        <v>200</v>
+      </c>
+      <c r="C53" s="1">
+        <v>360</v>
+      </c>
+      <c r="D53" s="1">
+        <v>0</v>
+      </c>
+      <c r="E53" s="1">
+        <f t="shared" ref="E53:E54" si="35">C53/2-D53</f>
+        <v>180</v>
+      </c>
+      <c r="F53" s="1">
+        <f>80*4/2*1000</f>
+        <v>160000</v>
+      </c>
+      <c r="G53" s="1">
+        <f>B53*D53*(E53+D53/2)</f>
+        <v>0</v>
+      </c>
+      <c r="H53" s="1">
+        <f t="shared" ref="H53" si="36">B53*C53^3/12</f>
+        <v>777600000</v>
+      </c>
+      <c r="I53" s="5">
+        <f>F53*G53/H53/B53</f>
+        <v>0</v>
+      </c>
+      <c r="J53" s="1">
+        <f>80*4^2/8*1000000</f>
+        <v>160000000</v>
+      </c>
+      <c r="K53" s="5">
+        <f t="shared" ref="K53" si="37">J53/H53*E53</f>
+        <v>37.037037037037038</v>
+      </c>
+    </row>
+    <row r="54" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A54" s="3">
+        <v>14</v>
+      </c>
+      <c r="B54" s="1">
+        <v>200</v>
+      </c>
+      <c r="C54" s="1">
+        <v>360</v>
+      </c>
+      <c r="D54" s="1">
+        <f>C54/2</f>
+        <v>180</v>
+      </c>
+      <c r="E54" s="1">
+        <f t="shared" si="35"/>
+        <v>0</v>
+      </c>
+      <c r="F54" s="1">
+        <f>80*4/2*1000</f>
+        <v>160000</v>
+      </c>
+      <c r="G54" s="1">
+        <f>B54*D54*(E54+D54/2)</f>
+        <v>3240000</v>
+      </c>
+      <c r="H54" s="1">
+        <f t="shared" ref="H54:H55" si="38">B54*C54^3/12</f>
+        <v>777600000</v>
+      </c>
+      <c r="I54" s="5">
+        <f>F54*G54/H54/B54</f>
+        <v>3.333333333333333</v>
+      </c>
+      <c r="J54" s="1">
+        <f>80*4^2/8*1000000</f>
+        <v>160000000</v>
+      </c>
+      <c r="K54" s="5">
+        <f t="shared" si="34"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A55" s="3">
+        <v>15</v>
+      </c>
+      <c r="B55" s="1">
+        <v>360</v>
+      </c>
+      <c r="C55" s="1">
+        <v>600</v>
+      </c>
+      <c r="D55" s="1">
+        <f>C55/2-50</f>
+        <v>250</v>
+      </c>
+      <c r="E55" s="1">
+        <f t="shared" ref="E55" si="39">C55/2-D55</f>
+        <v>50</v>
+      </c>
+      <c r="F55" s="1">
+        <f>350*6*1000</f>
+        <v>2100000</v>
+      </c>
+      <c r="G55" s="1">
+        <f>B55*D55*(E55+D55/2)</f>
+        <v>15750000</v>
+      </c>
+      <c r="H55" s="1">
+        <f t="shared" si="38"/>
+        <v>6480000000</v>
+      </c>
+      <c r="I55" s="5">
+        <f>F55*G55/H55/B55</f>
+        <v>14.178240740740742</v>
+      </c>
+      <c r="J55" s="1">
+        <f>350*6*3*1000000</f>
+        <v>6300000000</v>
+      </c>
+      <c r="K55" s="5">
+        <f t="shared" si="34"/>
+        <v>48.611111111111107</v>
+      </c>
+    </row>
+    <row r="56" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="I56" s="5"/>
+      <c r="K56" s="5"/>
+    </row>
+    <row r="57" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="I57" s="5"/>
+      <c r="K57" s="7"/>
+    </row>
+    <row r="58" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K58" s="7"/>
+    </row>
+    <row r="59" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B59" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C42" s="1" t="s">
+      <c r="C59" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="D42" s="1" t="s">
+      <c r="D59" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="E42" s="1" t="s">
+      <c r="E59" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F42" s="1" t="s">
+      <c r="F59" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="G42" s="1" t="s">
+      <c r="G59" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="H42" s="1" t="s">
+      <c r="H59" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="I42" s="1" t="s">
+      <c r="I59" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="J42" s="1" t="s">
+      <c r="J59" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="K42" s="1" t="s">
+      <c r="K59" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="L42" s="1" t="s">
+      <c r="L59" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A43" s="3">
+    <row r="60" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A60" s="3">
         <v>1</v>
       </c>
-      <c r="B43" s="1">
+      <c r="B60" s="1">
         <v>1000</v>
       </c>
-      <c r="C43" s="1">
+      <c r="C60" s="1">
         <v>500</v>
       </c>
-      <c r="D43" s="1">
+      <c r="D60" s="1">
         <v>-50</v>
       </c>
-      <c r="E43" s="1">
-        <f>ATAN(-2*D43/(B43-C43))/2</f>
+      <c r="E60" s="1">
+        <f t="shared" ref="E60:E66" si="40">ATAN(-2*D60/(B60-C60))/2</f>
         <v>9.8697779924940388E-2</v>
       </c>
-      <c r="F43" s="1">
-        <f>E43*180/PI()</f>
+      <c r="F60" s="1">
+        <f t="shared" ref="F60:F66" si="41">E60*180/PI()</f>
         <v>5.6549662370101066</v>
       </c>
-      <c r="G43" s="1">
-        <f>(B43+C43)/2</f>
+      <c r="G60" s="1">
+        <f t="shared" ref="G60:G66" si="42">(B60+C60)/2</f>
         <v>750</v>
       </c>
-      <c r="H43" s="1">
-        <f>SQRT((B43-C43)^2/4+D43^2)</f>
+      <c r="H60" s="1">
+        <f t="shared" ref="H60:H66" si="43">SQRT((B60-C60)^2/4+D60^2)</f>
         <v>254.95097567963924</v>
       </c>
-      <c r="I43" s="1">
-        <f>G43+H43</f>
+      <c r="I60" s="1">
+        <f t="shared" ref="I60:I66" si="44">G60+H60</f>
         <v>1004.9509756796392</v>
       </c>
-      <c r="J43" s="1">
-        <f>G43-H43</f>
+      <c r="J60" s="1">
+        <f t="shared" ref="J60:J66" si="45">G60-H60</f>
         <v>495.04902432036079</v>
       </c>
-      <c r="K43" s="1">
-        <f t="shared" ref="K43:K47" si="14">F43+45</f>
+      <c r="K60" s="1">
+        <f t="shared" ref="K60:K64" si="46">F60+45</f>
         <v>50.654966237010107</v>
       </c>
-      <c r="L43" s="1">
-        <f t="shared" ref="L43:L47" si="15">K43-90</f>
+      <c r="L60" s="1">
+        <f t="shared" ref="L60:L64" si="47">K60-90</f>
         <v>-39.345033762989893</v>
       </c>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A44" s="3">
+    <row r="61" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A61" s="3">
         <v>2</v>
       </c>
-      <c r="B44" s="1">
+      <c r="B61" s="1">
         <v>5333333.3333333302</v>
       </c>
-      <c r="C44" s="1">
+      <c r="C61" s="1">
         <v>3333333.3333333302</v>
       </c>
-      <c r="D44" s="1">
+      <c r="D61" s="1">
         <v>-2400000</v>
       </c>
-      <c r="E44" s="1">
-        <f>ATAN(-2*D44/(B44-C44))/2</f>
+      <c r="E61" s="1">
+        <f t="shared" si="40"/>
         <v>0.5880026035475675</v>
       </c>
-      <c r="F44" s="1">
-        <f>E44*180/PI()</f>
+      <c r="F61" s="1">
+        <f t="shared" si="41"/>
         <v>33.690067525979785</v>
       </c>
-      <c r="G44" s="1">
-        <f>(B44+C44)/2</f>
+      <c r="G61" s="1">
+        <f t="shared" si="42"/>
         <v>4333333.3333333302</v>
       </c>
-      <c r="H44" s="1">
-        <f>SQRT((B44-C44)^2/4+D44^2)</f>
+      <c r="H61" s="1">
+        <f t="shared" si="43"/>
         <v>2600000</v>
       </c>
-      <c r="I44" s="1">
-        <f>G44+H44</f>
+      <c r="I61" s="1">
+        <f t="shared" si="44"/>
         <v>6933333.3333333302</v>
       </c>
-      <c r="J44" s="1">
-        <f>G44-H44</f>
+      <c r="J61" s="1">
+        <f t="shared" si="45"/>
         <v>1733333.3333333302</v>
       </c>
-      <c r="K44" s="1">
-        <f t="shared" si="14"/>
+      <c r="K61" s="1">
+        <f t="shared" si="46"/>
         <v>78.690067525979785</v>
       </c>
-      <c r="L44" s="1">
-        <f t="shared" si="15"/>
+      <c r="L61" s="1">
+        <f t="shared" si="47"/>
         <v>-11.309932474020215</v>
       </c>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A45" s="3">
+    <row r="62" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A62" s="3">
         <v>3</v>
       </c>
-      <c r="B45" s="1">
+      <c r="B62" s="1">
         <v>532</v>
       </c>
-      <c r="C45" s="1">
+      <c r="C62" s="1">
         <v>740</v>
       </c>
-      <c r="D45" s="1">
+      <c r="D62" s="1">
         <v>345</v>
       </c>
-      <c r="E45" s="1">
-        <f>ATAN(-2*D45/(B45-C45))/2</f>
+      <c r="E62" s="1">
+        <f t="shared" si="40"/>
         <v>0.6390052264115833</v>
       </c>
-      <c r="F45" s="1">
-        <f>E45*180/PI()</f>
+      <c r="F62" s="1">
+        <f t="shared" si="41"/>
         <v>36.612302560185327</v>
       </c>
-      <c r="G45" s="1">
-        <f>(B45+C45)/2</f>
+      <c r="G62" s="1">
+        <f t="shared" si="42"/>
         <v>636</v>
       </c>
-      <c r="H45" s="1">
-        <f>SQRT((B45-C45)^2/4+D45^2)</f>
+      <c r="H62" s="1">
+        <f t="shared" si="43"/>
         <v>360.33456675706259</v>
       </c>
-      <c r="I45" s="1">
-        <f>G45+H45</f>
+      <c r="I62" s="1">
+        <f t="shared" si="44"/>
         <v>996.33456675706259</v>
       </c>
-      <c r="J45" s="1">
-        <f>G45-H45</f>
+      <c r="J62" s="1">
+        <f t="shared" si="45"/>
         <v>275.66543324293741</v>
       </c>
-      <c r="K45" s="1">
-        <f t="shared" si="14"/>
+      <c r="K62" s="1">
+        <f t="shared" si="46"/>
         <v>81.612302560185327</v>
       </c>
-      <c r="L45" s="1">
-        <f t="shared" si="15"/>
+      <c r="L62" s="1">
+        <f t="shared" si="47"/>
         <v>-8.3876974398146729</v>
       </c>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A46" s="3">
+    <row r="63" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A63" s="3">
         <v>4</v>
       </c>
-      <c r="B46" s="1">
+      <c r="B63" s="1">
         <v>300</v>
       </c>
-      <c r="C46" s="1">
+      <c r="C63" s="1">
         <v>150</v>
       </c>
-      <c r="D46" s="1">
+      <c r="D63" s="1">
         <v>200</v>
       </c>
-      <c r="E46" s="1">
-        <f>ATAN(-2*D46/(B46-C46))/2</f>
+      <c r="E63" s="1">
+        <f t="shared" si="40"/>
         <v>-0.60601282826216218</v>
       </c>
-      <c r="F46" s="1">
-        <f>E46*180/PI()</f>
+      <c r="F63" s="1">
+        <f t="shared" si="41"/>
         <v>-34.721977390208266</v>
       </c>
-      <c r="G46" s="1">
-        <f>(B46+C46)/2</f>
+      <c r="G63" s="1">
+        <f t="shared" si="42"/>
         <v>225</v>
       </c>
-      <c r="H46" s="1">
-        <f>SQRT((B46-C46)^2/4+D46^2)</f>
+      <c r="H63" s="1">
+        <f t="shared" si="43"/>
         <v>213.60009363293827</v>
       </c>
-      <c r="I46" s="1">
-        <f>G46+H46</f>
+      <c r="I63" s="1">
+        <f t="shared" si="44"/>
         <v>438.6000936329383</v>
       </c>
-      <c r="J46" s="1">
-        <f>G46-H46</f>
+      <c r="J63" s="1">
+        <f t="shared" si="45"/>
         <v>11.399906367061732</v>
       </c>
-      <c r="K46" s="1">
-        <f t="shared" si="14"/>
+      <c r="K63" s="1">
+        <f t="shared" si="46"/>
         <v>10.278022609791734</v>
       </c>
-      <c r="L46" s="1">
-        <f t="shared" si="15"/>
+      <c r="L63" s="1">
+        <f t="shared" si="47"/>
         <v>-79.721977390208266</v>
       </c>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A47" s="3">
+    <row r="64" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A64" s="3">
         <v>5</v>
       </c>
-      <c r="B47" s="1">
+      <c r="B64" s="1">
         <v>50</v>
       </c>
-      <c r="C47" s="1">
+      <c r="C64" s="1">
         <v>-10</v>
       </c>
-      <c r="D47" s="1">
+      <c r="D64" s="1">
         <v>40</v>
       </c>
-      <c r="E47" s="1">
-        <f>ATAN(-2*D47/(B47-C47))/2</f>
+      <c r="E64" s="1">
+        <f t="shared" si="40"/>
         <v>-0.46364760900080609</v>
       </c>
-      <c r="F47" s="1">
-        <f>E47*180/PI()</f>
+      <c r="F64" s="1">
+        <f t="shared" si="41"/>
         <v>-26.56505117707799</v>
       </c>
-      <c r="G47" s="1">
-        <f>(B47+C47)/2</f>
+      <c r="G64" s="1">
+        <f t="shared" si="42"/>
         <v>20</v>
       </c>
-      <c r="H47" s="1">
-        <f>SQRT((B47-C47)^2/4+D47^2)</f>
+      <c r="H64" s="1">
+        <f t="shared" si="43"/>
         <v>50</v>
       </c>
-      <c r="I47" s="1">
-        <f>G47+H47</f>
+      <c r="I64" s="1">
+        <f t="shared" si="44"/>
         <v>70</v>
       </c>
-      <c r="J47" s="1">
-        <f>G47-H47</f>
+      <c r="J64" s="1">
+        <f t="shared" si="45"/>
         <v>-30</v>
       </c>
-      <c r="K47" s="1">
-        <f t="shared" si="14"/>
+      <c r="K64" s="1">
+        <f t="shared" si="46"/>
         <v>18.43494882292201</v>
       </c>
-      <c r="L47" s="1">
-        <f t="shared" si="15"/>
+      <c r="L64" s="1">
+        <f t="shared" si="47"/>
         <v>-71.56505117707799</v>
       </c>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A48" s="3">
+    <row r="65" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A65" s="3">
         <v>6</v>
       </c>
-      <c r="B48" s="1">
+      <c r="B65" s="1">
         <v>800</v>
       </c>
-      <c r="C48" s="1">
+      <c r="C65" s="1">
         <v>400</v>
       </c>
-      <c r="D48" s="1">
+      <c r="D65" s="1">
         <v>-550</v>
       </c>
-      <c r="E48" s="1">
-        <f>ATAN(-2*D48/(B48-C48))/2</f>
+      <c r="E65" s="1">
+        <f t="shared" si="40"/>
         <v>0.61101266160549483</v>
       </c>
-      <c r="F48" s="1">
-        <f>E48*180/PI()</f>
+      <c r="F65" s="1">
+        <f t="shared" si="41"/>
         <v>35.008446739050015</v>
       </c>
-      <c r="G48" s="1">
-        <f>(B48+C48)/2</f>
+      <c r="G65" s="1">
+        <f t="shared" si="42"/>
         <v>600</v>
       </c>
-      <c r="H48" s="1">
-        <f>SQRT((B48-C48)^2/4+D48^2)</f>
+      <c r="H65" s="1">
+        <f t="shared" si="43"/>
         <v>585.23499553598128</v>
       </c>
-      <c r="I48" s="1">
-        <f>G48+H48</f>
+      <c r="I65" s="1">
+        <f t="shared" si="44"/>
         <v>1185.2349955359814</v>
       </c>
-      <c r="J48" s="1">
-        <f>G48-H48</f>
+      <c r="J65" s="1">
+        <f t="shared" si="45"/>
         <v>14.765004464018716</v>
       </c>
-      <c r="K48" s="1">
-        <f>F48+45</f>
+      <c r="K65" s="1">
+        <f t="shared" ref="K65:K72" si="48">F65+45</f>
         <v>80.008446739050015</v>
       </c>
-      <c r="L48" s="1">
-        <f>K48-90</f>
+      <c r="L65" s="1">
+        <f t="shared" ref="L65:L72" si="49">K65-90</f>
         <v>-9.9915532609499849</v>
       </c>
     </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A49" s="3">
+    <row r="66" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A66" s="3">
         <v>7</v>
       </c>
-      <c r="B49" s="5">
+      <c r="B66" s="5">
         <f>K39</f>
         <v>30.864197530864196</v>
       </c>
-      <c r="C49" s="1">
-        <v>0</v>
-      </c>
-      <c r="D49" s="5">
+      <c r="C66" s="1">
+        <v>0</v>
+      </c>
+      <c r="D66" s="5">
         <f>I39</f>
         <v>3.9609053497942388</v>
       </c>
-      <c r="E49" s="5">
-        <f>ATAN(-2*D49/(B49-C49))/2</f>
+      <c r="E66" s="5">
+        <f t="shared" si="40"/>
         <v>-0.12562163201205953</v>
       </c>
-      <c r="F49" s="5">
-        <f>E49*180/PI()</f>
+      <c r="F66" s="5">
+        <f t="shared" si="41"/>
         <v>-7.1975893298365268</v>
       </c>
-      <c r="G49" s="5">
-        <f>(B49+C49)/2</f>
+      <c r="G66" s="5">
+        <f t="shared" si="42"/>
         <v>15.432098765432098</v>
       </c>
-      <c r="H49" s="5">
-        <f>SQRT((B49-C49)^2/4+D49^2)</f>
+      <c r="H66" s="5">
+        <f t="shared" si="43"/>
         <v>15.932308165990248</v>
       </c>
-      <c r="I49" s="5">
-        <f>G49+H49</f>
+      <c r="I66" s="5">
+        <f t="shared" si="44"/>
         <v>31.364406931422344</v>
       </c>
-      <c r="J49" s="5">
-        <f>G49-H49</f>
+      <c r="J66" s="5">
+        <f t="shared" si="45"/>
         <v>-0.50020940055815011</v>
       </c>
-      <c r="K49" s="5">
-        <f>F49+45</f>
+      <c r="K66" s="5">
+        <f t="shared" si="48"/>
         <v>37.802410670163475</v>
       </c>
-      <c r="L49" s="5">
-        <f>K49-90</f>
+      <c r="L66" s="5">
+        <f t="shared" si="49"/>
         <v>-52.197589329836525</v>
       </c>
-      <c r="M49" s="5">
-        <f>L49*2</f>
+      <c r="M66" s="5">
+        <f>L66*2</f>
         <v>-104.39517865967305</v>
+      </c>
+    </row>
+    <row r="67" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A67" s="3">
+        <v>8</v>
+      </c>
+      <c r="B67" s="1">
+        <v>-150</v>
+      </c>
+      <c r="C67" s="1">
+        <v>352</v>
+      </c>
+      <c r="D67" s="1">
+        <v>-24</v>
+      </c>
+      <c r="E67" s="5">
+        <f t="shared" ref="E67:E71" si="50">ATAN(-2*D67/(B67-C67))/2</f>
+        <v>-4.7663858426665248E-2</v>
+      </c>
+      <c r="F67" s="5">
+        <f t="shared" ref="F67:F71" si="51">E67*180/PI()</f>
+        <v>-2.7309379231569828</v>
+      </c>
+      <c r="G67" s="5">
+        <f t="shared" ref="G67:G71" si="52">(B67+C67)/2</f>
+        <v>101</v>
+      </c>
+      <c r="H67" s="5">
+        <f t="shared" ref="H67:H71" si="53">SQRT((B67-C67)^2/4+D67^2)</f>
+        <v>252.14479966876175</v>
+      </c>
+      <c r="I67" s="5">
+        <f t="shared" ref="I67:I71" si="54">G67+H67</f>
+        <v>353.14479966876172</v>
+      </c>
+      <c r="J67" s="5">
+        <f t="shared" ref="J67:J71" si="55">G67-H67</f>
+        <v>-151.14479966876175</v>
+      </c>
+      <c r="K67" s="5">
+        <f t="shared" si="48"/>
+        <v>42.269062076843014</v>
+      </c>
+      <c r="L67" s="5">
+        <f t="shared" si="49"/>
+        <v>-47.730937923156986</v>
+      </c>
+      <c r="M67" s="5">
+        <f>L67*2</f>
+        <v>-95.461875846313973</v>
+      </c>
+    </row>
+    <row r="68" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A68" s="3">
+        <v>9</v>
+      </c>
+      <c r="B68" s="1">
+        <v>-400</v>
+      </c>
+      <c r="C68" s="1">
+        <v>-300</v>
+      </c>
+      <c r="D68" s="1">
+        <v>120</v>
+      </c>
+      <c r="E68" s="1">
+        <f t="shared" si="50"/>
+        <v>0.5880026035475675</v>
+      </c>
+      <c r="F68" s="5">
+        <f t="shared" si="51"/>
+        <v>33.690067525979785</v>
+      </c>
+      <c r="G68" s="1">
+        <f t="shared" si="52"/>
+        <v>-350</v>
+      </c>
+      <c r="H68" s="1">
+        <f t="shared" si="53"/>
+        <v>130</v>
+      </c>
+      <c r="I68" s="1">
+        <f t="shared" si="54"/>
+        <v>-220</v>
+      </c>
+      <c r="J68" s="1">
+        <f t="shared" si="55"/>
+        <v>-480</v>
+      </c>
+      <c r="K68" s="5">
+        <f t="shared" si="48"/>
+        <v>78.690067525979785</v>
+      </c>
+      <c r="L68" s="1">
+        <f t="shared" si="49"/>
+        <v>-11.309932474020215</v>
+      </c>
+    </row>
+    <row r="69" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A69" s="3">
+        <v>10</v>
+      </c>
+      <c r="B69" s="1">
+        <v>-150</v>
+      </c>
+      <c r="C69" s="1">
+        <v>120</v>
+      </c>
+      <c r="D69" s="1">
+        <v>80</v>
+      </c>
+      <c r="E69" s="1">
+        <f t="shared" si="50"/>
+        <v>0.26747753689304821</v>
+      </c>
+      <c r="F69" s="5">
+        <f t="shared" si="51"/>
+        <v>15.325333978526434</v>
+      </c>
+      <c r="G69" s="5">
+        <f t="shared" si="52"/>
+        <v>-15</v>
+      </c>
+      <c r="H69" s="5">
+        <f t="shared" si="53"/>
+        <v>156.92354826475216</v>
+      </c>
+      <c r="I69" s="5">
+        <f t="shared" si="54"/>
+        <v>141.92354826475216</v>
+      </c>
+      <c r="J69" s="5">
+        <f t="shared" si="55"/>
+        <v>-171.92354826475216</v>
+      </c>
+      <c r="K69" s="5">
+        <f t="shared" si="48"/>
+        <v>60.32533397852643</v>
+      </c>
+      <c r="L69" s="5">
+        <f t="shared" si="49"/>
+        <v>-29.67466602147357</v>
+      </c>
+    </row>
+    <row r="70" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A70" s="3">
+        <v>11</v>
+      </c>
+      <c r="B70" s="1">
+        <v>265</v>
+      </c>
+      <c r="C70" s="1">
+        <v>128</v>
+      </c>
+      <c r="D70" s="1">
+        <v>95</v>
+      </c>
+      <c r="E70" s="1">
+        <f t="shared" si="50"/>
+        <v>-0.47304018463635611</v>
+      </c>
+      <c r="F70" s="5">
+        <f t="shared" si="51"/>
+        <v>-27.103206119752414</v>
+      </c>
+      <c r="G70" s="5">
+        <f t="shared" si="52"/>
+        <v>196.5</v>
+      </c>
+      <c r="H70" s="5">
+        <f t="shared" si="53"/>
+        <v>117.1206642740725</v>
+      </c>
+      <c r="I70" s="5">
+        <f t="shared" si="54"/>
+        <v>313.62066427407251</v>
+      </c>
+      <c r="J70" s="5">
+        <f t="shared" si="55"/>
+        <v>79.379335725927504</v>
+      </c>
+      <c r="K70" s="5">
+        <f t="shared" si="48"/>
+        <v>17.896793880247586</v>
+      </c>
+      <c r="L70" s="5">
+        <f t="shared" si="49"/>
+        <v>-72.103206119752414</v>
+      </c>
+    </row>
+    <row r="71" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A71" s="3">
+        <v>12</v>
+      </c>
+      <c r="B71" s="1">
+        <v>132</v>
+      </c>
+      <c r="C71" s="1">
+        <v>-387</v>
+      </c>
+      <c r="D71" s="1">
+        <v>-765</v>
+      </c>
+      <c r="E71" s="1">
+        <f t="shared" si="50"/>
+        <v>0.62188051502639119</v>
+      </c>
+      <c r="F71" s="5">
+        <f t="shared" si="51"/>
+        <v>35.631128872434189</v>
+      </c>
+      <c r="G71" s="5">
+        <f t="shared" si="52"/>
+        <v>-127.5</v>
+      </c>
+      <c r="H71" s="5">
+        <f t="shared" si="53"/>
+        <v>807.81510879656116</v>
+      </c>
+      <c r="I71" s="5">
+        <f t="shared" si="54"/>
+        <v>680.31510879656116</v>
+      </c>
+      <c r="J71" s="5">
+        <f t="shared" si="55"/>
+        <v>-935.31510879656116</v>
+      </c>
+      <c r="K71" s="5">
+        <f t="shared" si="48"/>
+        <v>80.631128872434189</v>
+      </c>
+      <c r="L71" s="5">
+        <f t="shared" si="49"/>
+        <v>-9.3688711275658108</v>
+      </c>
+    </row>
+    <row r="72" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A72" s="3">
+        <v>13</v>
+      </c>
+      <c r="B72" s="1">
+        <f>K55</f>
+        <v>48.611111111111107</v>
+      </c>
+      <c r="C72" s="1">
+        <v>0</v>
+      </c>
+      <c r="D72" s="1">
+        <f>I55</f>
+        <v>14.178240740740742</v>
+      </c>
+      <c r="E72" s="1">
+        <f t="shared" ref="E72" si="56">ATAN(-2*D72/(B72-C72))/2</f>
+        <v>-0.26403722421317988</v>
+      </c>
+      <c r="F72" s="5">
+        <f t="shared" ref="F72" si="57">E72*180/PI()</f>
+        <v>-15.128218581764637</v>
+      </c>
+      <c r="G72" s="5">
+        <f t="shared" ref="G72" si="58">(B72+C72)/2</f>
+        <v>24.305555555555554</v>
+      </c>
+      <c r="H72" s="5">
+        <f t="shared" ref="H72" si="59">SQRT((B72-C72)^2/4+D72^2)</f>
+        <v>28.138630765668005</v>
+      </c>
+      <c r="I72" s="5">
+        <f t="shared" ref="I72" si="60">G72+H72</f>
+        <v>52.444186321223555</v>
+      </c>
+      <c r="J72" s="5">
+        <f t="shared" ref="J72" si="61">G72-H72</f>
+        <v>-3.833075210112451</v>
+      </c>
+      <c r="K72" s="5">
+        <f t="shared" si="48"/>
+        <v>29.871781418235365</v>
+      </c>
+      <c r="L72" s="5">
+        <f t="shared" si="49"/>
+        <v>-60.128218581764635</v>
+      </c>
+    </row>
+    <row r="75" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B75" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C75" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D75" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E75" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="F75" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="G75" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="H75" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="I75" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="J75" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="K75" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="L75" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="M75" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="76" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A76" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="B76" s="1">
+        <v>2000</v>
+      </c>
+      <c r="C76" s="1">
+        <v>50</v>
+      </c>
+      <c r="D76" s="1">
+        <v>30</v>
+      </c>
+      <c r="E76" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="F76" s="1">
+        <f>PI()*(D76/2)^2</f>
+        <v>706.85834705770344</v>
+      </c>
+      <c r="G76" s="1">
+        <f>3600*1000</f>
+        <v>3600000</v>
+      </c>
+      <c r="H76" s="5">
+        <f>G76/F76</f>
+        <v>5092.9581789406511</v>
+      </c>
+      <c r="I76" s="5">
+        <f>C76/B76</f>
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="J76" s="5">
+        <f>H76/I76</f>
+        <v>203718.32715762604</v>
+      </c>
+      <c r="K76" s="5">
+        <f>E76/D76</f>
+        <v>0.01</v>
+      </c>
+      <c r="L76" s="5">
+        <f>K76/I76</f>
+        <v>0.39999999999999997</v>
+      </c>
+      <c r="M76" s="1">
+        <f>J76/(2*(1+L76))</f>
+        <v>72756.545413437882</v>
+      </c>
+    </row>
+    <row r="77" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="H77" s="5"/>
+      <c r="I77" s="5"/>
+      <c r="J77" s="5"/>
+      <c r="K77" s="5"/>
+      <c r="L77" s="5"/>
+    </row>
+    <row r="78" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="H78" s="5"/>
+      <c r="I78" s="5"/>
+      <c r="J78" s="5"/>
+      <c r="K78" s="5"/>
+      <c r="L78" s="5"/>
+    </row>
+    <row r="79" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B79" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C79" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D79" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="E79" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="F79" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="G79" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="I79" s="5"/>
+      <c r="L79" s="5"/>
+    </row>
+    <row r="80" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A80" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="B80" s="1">
+        <v>50</v>
+      </c>
+      <c r="C80" s="5">
+        <f>PI()*(B80/2)^2</f>
+        <v>1963.4954084936207</v>
+      </c>
+      <c r="D80" s="5">
+        <v>205000</v>
+      </c>
+      <c r="E80" s="1">
+        <f>390*1000</f>
+        <v>390000</v>
+      </c>
+      <c r="F80" s="1">
+        <v>1300</v>
+      </c>
+      <c r="G80" s="5">
+        <f>E80*F80/C80/D80</f>
+        <v>1.2595755105965414</v>
+      </c>
+      <c r="I80" s="5"/>
+      <c r="L80" s="5"/>
+    </row>
+    <row r="81" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A81" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="C81" s="1">
+        <v>1000</v>
+      </c>
+      <c r="D81" s="5">
+        <v>200000</v>
+      </c>
+      <c r="E81" s="1">
+        <f>200*1000</f>
+        <v>200000</v>
+      </c>
+      <c r="F81" s="1">
+        <v>1000</v>
+      </c>
+      <c r="G81" s="5">
+        <f>E81*F81/C81/D81</f>
+        <v>1</v>
+      </c>
+      <c r="I81" s="5"/>
+      <c r="L81" s="5"/>
+    </row>
+    <row r="82" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="C82" s="1">
+        <v>2000</v>
+      </c>
+      <c r="D82" s="5">
+        <v>27000</v>
+      </c>
+      <c r="E82" s="1">
+        <f>250*1000</f>
+        <v>250000</v>
+      </c>
+      <c r="F82" s="1">
+        <v>2000</v>
+      </c>
+      <c r="G82" s="5">
+        <f>E82*F82/C82/D82</f>
+        <v>9.2592592592592595</v>
+      </c>
+    </row>
+    <row r="83" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B83" s="1">
+        <v>500</v>
+      </c>
+      <c r="C83" s="1">
+        <f>B83^2</f>
+        <v>250000</v>
+      </c>
+      <c r="D83" s="1">
+        <v>28500</v>
+      </c>
+      <c r="E83" s="1">
+        <f>7800*1000</f>
+        <v>7800000</v>
+      </c>
+      <c r="F83" s="1">
+        <v>2400</v>
+      </c>
+      <c r="G83" s="5">
+        <f>E83*F83/C83/D83</f>
+        <v>2.6273684210526316</v>
+      </c>
+    </row>
+    <row r="84" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B84" s="1">
+        <v>550</v>
+      </c>
+      <c r="C84" s="1">
+        <f>B84^2</f>
+        <v>302500</v>
+      </c>
+      <c r="D84" s="1">
+        <v>28500</v>
+      </c>
+      <c r="E84" s="1">
+        <f>7800*1000</f>
+        <v>7800000</v>
+      </c>
+      <c r="F84" s="1">
+        <v>2400</v>
+      </c>
+      <c r="G84" s="5">
+        <f>E84*F84/C84/D84</f>
+        <v>2.1713788603740758</v>
+      </c>
+    </row>
+    <row r="85" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B85" s="5">
+        <f>SQRT(C85)</f>
+        <v>452.0224821005304</v>
+      </c>
+      <c r="C85" s="1">
+        <f>E85*F85/D85/G85</f>
+        <v>204324.32432432432</v>
+      </c>
+      <c r="D85" s="1">
+        <v>37000</v>
+      </c>
+      <c r="E85" s="1">
+        <f>3600*1000</f>
+        <v>3600000</v>
+      </c>
+      <c r="F85" s="1">
+        <v>2100</v>
+      </c>
+      <c r="G85" s="5">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
2017.04.17 error of Part IV
</commit_message>
<xml_diff>
--- a/quiz_calc.xlsx
+++ b/quiz_calc.xlsx
@@ -288,11 +288,11 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="6">
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="182" formatCode="0_ ;[Red]\-0\ "/>
-    <numFmt numFmtId="185" formatCode="0.000_ ;[Red]\-0.000\ "/>
-    <numFmt numFmtId="186" formatCode="0.0000_ ;[Red]\-0.0000\ "/>
-    <numFmt numFmtId="187" formatCode="0.00000_ ;[Red]\-0.00000\ "/>
-    <numFmt numFmtId="188" formatCode="0.0000E+00"/>
+    <numFmt numFmtId="176" formatCode="0_ ;[Red]\-0\ "/>
+    <numFmt numFmtId="177" formatCode="0.000_ ;[Red]\-0.000\ "/>
+    <numFmt numFmtId="178" formatCode="0.0000_ ;[Red]\-0.0000\ "/>
+    <numFmt numFmtId="179" formatCode="0.00000_ ;[Red]\-0.00000\ "/>
+    <numFmt numFmtId="180" formatCode="0.0000E+00"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -348,19 +348,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="182" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="185" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1">
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="186" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1">
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="187" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1">
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="188" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1">
+    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -678,10 +678,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P85"/>
+  <dimension ref="A1:P92"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="A37" sqref="A37:XFD37"/>
+    <sheetView tabSelected="1" topLeftCell="A58" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="L79" sqref="L79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1189,10 +1189,6 @@
         <f>C10*B10^3/12+G10^2*D10</f>
         <v>1009114.5833333334</v>
       </c>
-      <c r="M10" s="2">
-        <f t="shared" ref="M10:M11" si="5">SUM(K10:L10)</f>
-        <v>5533854.166666666</v>
-      </c>
       <c r="N10" s="4">
         <f>D10*G10*H10</f>
         <v>-1464843.75</v>
@@ -1244,10 +1240,6 @@
         <f>C11*B11^3/12+G11^2*D11</f>
         <v>2962239.583333333</v>
       </c>
-      <c r="M11" s="2">
-        <f t="shared" si="5"/>
-        <v>5533854.166666666</v>
-      </c>
       <c r="N11" s="4">
         <f>D11*G11*H11</f>
         <v>-1464843.75</v>
@@ -1269,20 +1261,20 @@
         <f>SUM(D10:D11)</f>
         <v>5000</v>
       </c>
-      <c r="K12" s="2">
-        <f t="shared" ref="K12:N12" si="6">SUM(K10:K11)</f>
+      <c r="K12" s="3">
+        <f t="shared" ref="K12:N12" si="5">SUM(K10:K11)</f>
         <v>7096354.166666666</v>
       </c>
-      <c r="L12" s="2">
-        <f t="shared" si="6"/>
+      <c r="L12" s="3">
+        <f t="shared" si="5"/>
         <v>3971354.1666666665</v>
       </c>
-      <c r="M12" s="2">
+      <c r="M12" s="3">
         <f>SUM(K12:L12)</f>
         <v>11067708.333333332</v>
       </c>
       <c r="N12" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>-2929687.5</v>
       </c>
       <c r="O12" s="4">
@@ -1339,7 +1331,7 @@
         <v>112500</v>
       </c>
       <c r="M13" s="2">
-        <f t="shared" ref="M13" si="7">SUM(K13:L13)</f>
+        <f t="shared" ref="M13" si="6">SUM(K13:L13)</f>
         <v>425000</v>
       </c>
       <c r="N13" s="4">
@@ -1400,7 +1392,7 @@
         <v>651041666.66666663</v>
       </c>
       <c r="M14" s="2">
-        <f t="shared" ref="M14" si="8">SUM(K14:L14)</f>
+        <f t="shared" ref="M14" si="7">SUM(K14:L14)</f>
         <v>3255208333.333333</v>
       </c>
       <c r="N14" s="4">
@@ -1467,7 +1459,7 @@
         <v>3200000000</v>
       </c>
       <c r="M16" s="2">
-        <f t="shared" ref="M16" si="9">SUM(K16:L16)</f>
+        <f t="shared" ref="M16" si="8">SUM(K16:L16)</f>
         <v>10400000000</v>
       </c>
       <c r="N16" s="4">
@@ -1479,2000 +1471,2209 @@
         <v>115.47005383792515</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B21" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C21" s="2" t="s">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="B17" s="2">
+        <v>15</v>
+      </c>
+      <c r="C17" s="2">
         <v>20</v>
       </c>
-      <c r="D21" s="2" t="s">
+      <c r="D17" s="2">
+        <f>B17*C17</f>
+        <v>300</v>
+      </c>
+      <c r="E17" s="2">
+        <f>B17/2</f>
+        <v>7.5</v>
+      </c>
+      <c r="F17" s="2">
+        <f>C17/2</f>
+        <v>10</v>
+      </c>
+      <c r="G17" s="2">
+        <v>0</v>
+      </c>
+      <c r="H17" s="2">
+        <v>20</v>
+      </c>
+      <c r="I17" s="2">
+        <f>D17*G17/D17</f>
+        <v>0</v>
+      </c>
+      <c r="J17" s="2">
+        <f>D17*H17/D17</f>
+        <v>20</v>
+      </c>
+      <c r="K17" s="2">
+        <f>B17*C17^3/12+H17^2*D17</f>
+        <v>130000</v>
+      </c>
+      <c r="L17" s="2">
+        <f>C17*B17^3/12+G17^2*D17</f>
+        <v>5625</v>
+      </c>
+      <c r="M17" s="2">
+        <f t="shared" ref="M17" si="9">SUM(K17:L17)</f>
+        <v>135625</v>
+      </c>
+      <c r="N17" s="4">
+        <f>D17*G17*H17</f>
+        <v>0</v>
+      </c>
+      <c r="O17" s="4">
+        <f>SQRT(L17/D17)</f>
+        <v>4.3301270189221936</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="B18" s="2">
+        <v>100</v>
+      </c>
+      <c r="C18" s="2">
+        <v>20</v>
+      </c>
+      <c r="D18" s="2">
+        <f>B18*C18</f>
+        <v>2000</v>
+      </c>
+      <c r="E18" s="2">
+        <f>B18/2</f>
+        <v>50</v>
+      </c>
+      <c r="F18" s="2">
+        <f>C18/2</f>
+        <v>10</v>
+      </c>
+      <c r="G18" s="2">
+        <v>0</v>
+      </c>
+      <c r="H18" s="2">
+        <f>130-103.75</f>
+        <v>26.25</v>
+      </c>
+      <c r="I18" s="2">
+        <f>D18*G18/D18</f>
+        <v>0</v>
+      </c>
+      <c r="J18" s="2">
+        <f>D18*H18/D18</f>
+        <v>26.25</v>
+      </c>
+      <c r="K18" s="3">
+        <f>B18*C18^3/12+H18^2*D18</f>
+        <v>1444791.6666666667</v>
+      </c>
+      <c r="L18" s="2">
+        <f>C18*B18^3/12+G18^2*D18</f>
+        <v>1666666.6666666667</v>
+      </c>
+      <c r="M18" s="2">
+        <f t="shared" ref="M18" si="10">SUM(K18:L18)</f>
+        <v>3111458.3333333335</v>
+      </c>
+      <c r="N18" s="4">
+        <f>D18*G18*H18</f>
+        <v>0</v>
+      </c>
+      <c r="O18" s="4">
+        <f>SQRT(L18/D18)</f>
+        <v>28.867513459481287</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="B19" s="2">
+        <v>10</v>
+      </c>
+      <c r="C19" s="2">
+        <v>120</v>
+      </c>
+      <c r="D19" s="2">
+        <f>B19*C19</f>
+        <v>1200</v>
+      </c>
+      <c r="E19" s="2">
+        <f>B19/2</f>
+        <v>5</v>
+      </c>
+      <c r="F19" s="2">
+        <f>C19/2</f>
+        <v>60</v>
+      </c>
+      <c r="G19" s="2">
+        <v>0</v>
+      </c>
+      <c r="H19" s="2">
+        <f>103.75-60</f>
+        <v>43.75</v>
+      </c>
+      <c r="I19" s="2">
+        <f>D19*G19/D19</f>
+        <v>0</v>
+      </c>
+      <c r="J19" s="2">
+        <f>D19*H19/D19</f>
+        <v>43.75</v>
+      </c>
+      <c r="K19" s="3">
+        <f>B19*C19^3/12+H19^2*D19</f>
+        <v>3736875</v>
+      </c>
+      <c r="L19" s="2">
+        <f>C19*B19^3/12+G19^2*D19</f>
+        <v>10000</v>
+      </c>
+      <c r="M19" s="2">
+        <f t="shared" ref="M19:M20" si="11">SUM(K19:L19)</f>
+        <v>3746875</v>
+      </c>
+      <c r="N19" s="4">
+        <f>D19*G19*H19</f>
+        <v>0</v>
+      </c>
+      <c r="O19" s="4">
+        <f>SQRT(L19/D19)</f>
+        <v>2.8867513459481291</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="K20" s="3">
+        <f>SUM(K18:K19)</f>
+        <v>5181666.666666667</v>
+      </c>
+      <c r="L20" s="3">
+        <f>K20/103.75</f>
+        <v>49943.77510040161</v>
+      </c>
+      <c r="M20" s="3">
+        <f>K20/(140-103.75)</f>
+        <v>142942.52873563219</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="B21" s="3">
+        <f>700*(120^2+70^2)</f>
+        <v>13510000</v>
+      </c>
+      <c r="G21" s="3"/>
+      <c r="H21" s="3"/>
+      <c r="K21" s="3"/>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="K22" s="3"/>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="B25" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D25" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="E21" s="2" t="s">
+      <c r="E25" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="F21" s="2" t="s">
+      <c r="F25" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="G21" s="2" t="s">
+      <c r="G25" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="H21" s="2" t="s">
+      <c r="H25" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="I21" s="2" t="s">
+      <c r="I25" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="J21" s="2" t="s">
+      <c r="J25" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A22" s="1">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A26" s="1">
         <v>1</v>
       </c>
-      <c r="B22" s="2">
+      <c r="B26" s="2">
         <v>1000</v>
       </c>
-      <c r="C22" s="2">
+      <c r="C26" s="2">
         <v>500</v>
       </c>
-      <c r="D22" s="2">
+      <c r="D26" s="2">
         <v>-50</v>
       </c>
-      <c r="E22" s="2">
-        <f>ATAN(-2*D22/(B22-C22))/2</f>
+      <c r="E26" s="2">
+        <f>ATAN(-2*D26/(B26-C26))/2</f>
         <v>9.8697779924940388E-2</v>
       </c>
-      <c r="F22" s="2">
-        <f>E22*180/PI()</f>
+      <c r="F26" s="3">
+        <f>E26*180/PI()</f>
         <v>5.6549662370101066</v>
       </c>
-      <c r="G22" s="2">
-        <f>(B22+C22)/2</f>
+      <c r="G26" s="3">
+        <f>(B26+C26)/2</f>
         <v>750</v>
       </c>
-      <c r="H22" s="2">
-        <f>SQRT((B22-C22)^2/4+D22^2)</f>
+      <c r="H26" s="3">
+        <f>SQRT((B26-C26)^2/4+D26^2)</f>
         <v>254.95097567963924</v>
       </c>
-      <c r="I22" s="2">
-        <f>G22+H22</f>
+      <c r="I26" s="3">
+        <f>G26+H26</f>
         <v>1004.9509756796392</v>
       </c>
-      <c r="J22" s="2">
-        <f>G22-H22</f>
+      <c r="J26" s="3">
+        <f>G26-H26</f>
         <v>495.04902432036079</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A23" s="1">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A27" s="1">
         <v>2</v>
       </c>
-      <c r="B23" s="2">
+      <c r="B27" s="2">
         <v>5333333.3333333302</v>
       </c>
-      <c r="C23" s="2">
+      <c r="C27" s="2">
         <v>3333333.3333333302</v>
       </c>
-      <c r="D23" s="2">
+      <c r="D27" s="2">
         <v>-2400000</v>
       </c>
-      <c r="E23" s="2">
-        <f>ATAN(-2*D23/(B23-C23))/2</f>
+      <c r="E27" s="2">
+        <f>ATAN(-2*D27/(B27-C27))/2</f>
         <v>0.5880026035475675</v>
       </c>
-      <c r="F23" s="2">
-        <f>E23*180/PI()</f>
+      <c r="F27" s="3">
+        <f>E27*180/PI()</f>
         <v>33.690067525979785</v>
       </c>
-      <c r="G23" s="2">
-        <f>(B23+C23)/2</f>
+      <c r="G27" s="3">
+        <f>(B27+C27)/2</f>
         <v>4333333.3333333302</v>
       </c>
-      <c r="H23" s="2">
-        <f>SQRT((B23-C23)^2/4+D23^2)</f>
+      <c r="H27" s="3">
+        <f>SQRT((B27-C27)^2/4+D27^2)</f>
         <v>2600000</v>
       </c>
-      <c r="I23" s="2">
-        <f>G23+H23</f>
+      <c r="I27" s="3">
+        <f>G27+H27</f>
         <v>6933333.3333333302</v>
       </c>
-      <c r="J23" s="2">
-        <f>G23-H23</f>
+      <c r="J27" s="3">
+        <f>G27-H27</f>
         <v>1733333.3333333302</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A24" s="1">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A28" s="1">
         <v>3</v>
       </c>
-      <c r="B24" s="2">
+      <c r="B28" s="2">
         <v>532</v>
       </c>
-      <c r="C24" s="2">
+      <c r="C28" s="2">
         <v>740</v>
       </c>
-      <c r="D24" s="2">
+      <c r="D28" s="2">
         <v>345</v>
       </c>
-      <c r="E24" s="2">
-        <f>ATAN(-2*D24/(B24-C24))/2</f>
+      <c r="E28" s="2">
+        <f>ATAN(-2*D28/(B28-C28))/2</f>
         <v>0.6390052264115833</v>
       </c>
-      <c r="F24" s="2">
-        <f>E24*180/PI()</f>
+      <c r="F28" s="3">
+        <f>E28*180/PI()</f>
         <v>36.612302560185327</v>
       </c>
-      <c r="G24" s="2">
-        <f>(B24+C24)/2</f>
+      <c r="G28" s="3">
+        <f>(B28+C28)/2</f>
         <v>636</v>
       </c>
-      <c r="H24" s="2">
-        <f>SQRT((B24-C24)^2/4+D24^2)</f>
+      <c r="H28" s="3">
+        <f>SQRT((B28-C28)^2/4+D28^2)</f>
         <v>360.33456675706259</v>
       </c>
-      <c r="I24" s="2">
-        <f>G24+H24</f>
+      <c r="I28" s="3">
+        <f>G28+H28</f>
         <v>996.33456675706259</v>
       </c>
-      <c r="J24" s="2">
-        <f>G24-H24</f>
+      <c r="J28" s="3">
+        <f>G28-H28</f>
         <v>275.66543324293741</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A25" s="1">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A29" s="1">
         <v>4</v>
       </c>
-      <c r="B25" s="2">
+      <c r="B29" s="2">
         <f>K13</f>
         <v>312500</v>
       </c>
-      <c r="C25" s="2">
+      <c r="C29" s="2">
         <f>L13</f>
         <v>112500</v>
       </c>
-      <c r="D25" s="2">
+      <c r="D29" s="2">
         <f>N13</f>
         <v>0</v>
       </c>
-      <c r="E25" s="2">
-        <f>ATAN(-2*D25/(B25-C25))/2</f>
-        <v>0</v>
-      </c>
-      <c r="F25" s="2">
-        <f>E25*180/PI()</f>
-        <v>0</v>
-      </c>
-      <c r="G25" s="2">
-        <f>(B25+C25)/2</f>
+      <c r="E29" s="2">
+        <f>ATAN(-2*D29/(B29-C29))/2</f>
+        <v>0</v>
+      </c>
+      <c r="F29" s="3">
+        <f>E29*180/PI()</f>
+        <v>0</v>
+      </c>
+      <c r="G29" s="3">
+        <f>(B29+C29)/2</f>
         <v>212500</v>
       </c>
-      <c r="H25" s="2">
-        <f>SQRT((B25-C25)^2/4+D25^2)</f>
+      <c r="H29" s="3">
+        <f>SQRT((B29-C29)^2/4+D29^2)</f>
         <v>100000</v>
       </c>
-      <c r="I25" s="2">
-        <f>G25+H25</f>
+      <c r="I29" s="3">
+        <f>G29+H29</f>
         <v>312500</v>
       </c>
-      <c r="J25" s="2">
-        <f>G25-H25</f>
+      <c r="J29" s="3">
+        <f>G29-H29</f>
         <v>112500</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="C27" s="2">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="C31" s="2">
         <f>7530000/300/500</f>
         <v>50.2</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B30" s="2" t="s">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B34" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C30" s="2" t="s">
+      <c r="C34" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D30" s="2" t="s">
+      <c r="D34" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="E30" s="2" t="s">
+      <c r="E34" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="F30" s="2" t="s">
+      <c r="F34" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="G30" s="2" t="s">
+      <c r="G34" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="H30" s="2" t="s">
+      <c r="H34" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="I30" s="2" t="s">
+      <c r="I34" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="J30" s="2" t="s">
+      <c r="J34" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="K30" s="2" t="s">
+      <c r="K34" s="2" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A31" s="1">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A35" s="1">
         <v>1</v>
       </c>
-      <c r="B31" s="2">
+      <c r="B35" s="2">
         <f>250/2</f>
         <v>125</v>
       </c>
-      <c r="C31" s="2">
+      <c r="C35" s="2">
         <f>500/2</f>
         <v>250</v>
       </c>
-      <c r="D31" s="2">
+      <c r="D35" s="2">
         <f>50/2</f>
         <v>25</v>
       </c>
-      <c r="E31" s="2">
-        <f t="shared" ref="E31:E39" si="10">C31/2-D31</f>
+      <c r="E35" s="2">
+        <f t="shared" ref="E35:E43" si="12">C35/2-D35</f>
         <v>100</v>
       </c>
-      <c r="F31" s="2">
+      <c r="F35" s="2">
         <f>1200*1000</f>
         <v>1200000</v>
       </c>
-      <c r="G31" s="2">
-        <f>B31*D31*(E31+D31/2)</f>
+      <c r="G35" s="2">
+        <f>B35*D35*(E35+D35/2)</f>
         <v>351562.5</v>
       </c>
-      <c r="H31" s="2">
-        <f t="shared" ref="H31:H39" si="11">B31*C31^3/12</f>
+      <c r="H35" s="2">
+        <f t="shared" ref="H35:H43" si="13">B35*C35^3/12</f>
         <v>162760416.66666666</v>
       </c>
-      <c r="I31" s="2">
-        <f>F31*G31/H31/B31</f>
+      <c r="I35" s="2">
+        <f>F35*G35/H35/B35</f>
         <v>20.736000000000001</v>
       </c>
-      <c r="J31" s="5">
+      <c r="J35" s="5">
         <f>250000000</f>
         <v>250000000</v>
       </c>
-      <c r="K31" s="3">
-        <f>J31/H31*E31</f>
+      <c r="K35" s="3">
+        <f>J35/H35*E35</f>
         <v>153.6</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A32" s="1">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A36" s="1">
         <v>2</v>
       </c>
-      <c r="B32" s="2">
+      <c r="B36" s="2">
         <f>250/2</f>
         <v>125</v>
       </c>
-      <c r="C32" s="2">
+      <c r="C36" s="2">
         <f>500/2</f>
         <v>250</v>
       </c>
-      <c r="D32" s="2">
-        <f>C32/2</f>
+      <c r="D36" s="2">
+        <f>C36/2</f>
         <v>125</v>
       </c>
-      <c r="E32" s="2">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="F32" s="2">
+      <c r="E36" s="2">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="F36" s="2">
         <f>1200*1000</f>
         <v>1200000</v>
       </c>
-      <c r="G32" s="2">
-        <f>B32*D32*(E32+D32/2)</f>
+      <c r="G36" s="2">
+        <f>B36*D36*(E36+D36/2)</f>
         <v>976562.5</v>
       </c>
-      <c r="H32" s="2">
-        <f t="shared" si="11"/>
+      <c r="H36" s="2">
+        <f t="shared" si="13"/>
         <v>162760416.66666666</v>
       </c>
-      <c r="I32" s="2">
-        <f>F32*G32/H32/B32</f>
+      <c r="I36" s="2">
+        <f>F36*G36/H36/B36</f>
         <v>57.6</v>
       </c>
-      <c r="J32" s="5">
-        <f t="shared" ref="J32:J33" si="12">250000000</f>
+      <c r="J36" s="5">
+        <f t="shared" ref="J36:J37" si="14">250000000</f>
         <v>250000000</v>
       </c>
-      <c r="K32" s="3">
-        <f t="shared" ref="K32:K33" si="13">J32/H32*E32</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A33" s="1">
+      <c r="K36" s="3">
+        <f t="shared" ref="K36:K37" si="15">J36/H36*E36</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A37" s="1">
         <v>3</v>
       </c>
-      <c r="B33" s="2">
+      <c r="B37" s="2">
         <f>250/2</f>
         <v>125</v>
       </c>
-      <c r="C33" s="2">
+      <c r="C37" s="2">
         <f>500/2</f>
         <v>250</v>
       </c>
-      <c r="D33" s="2">
-        <v>0</v>
-      </c>
-      <c r="E33" s="2">
-        <f t="shared" si="10"/>
+      <c r="D37" s="2">
+        <v>0</v>
+      </c>
+      <c r="E37" s="2">
+        <f t="shared" si="12"/>
         <v>125</v>
       </c>
-      <c r="F33" s="2">
+      <c r="F37" s="2">
         <f>1200*1000</f>
         <v>1200000</v>
       </c>
-      <c r="G33" s="2">
-        <f>B33*D33*(E33+D33/2)</f>
-        <v>0</v>
-      </c>
-      <c r="H33" s="2">
-        <f t="shared" si="11"/>
+      <c r="G37" s="2">
+        <f>B37*D37*(E37+D37/2)</f>
+        <v>0</v>
+      </c>
+      <c r="H37" s="2">
+        <f t="shared" si="13"/>
         <v>162760416.66666666</v>
       </c>
-      <c r="I33" s="2">
-        <f>F33*G33/H33/B33</f>
-        <v>0</v>
-      </c>
-      <c r="J33" s="5">
+      <c r="I37" s="2">
+        <f>F37*G37/H37/B37</f>
+        <v>0</v>
+      </c>
+      <c r="J37" s="5">
+        <f t="shared" si="14"/>
+        <v>250000000</v>
+      </c>
+      <c r="K37" s="3">
+        <f t="shared" si="15"/>
+        <v>192</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A38" s="1">
+        <v>4</v>
+      </c>
+      <c r="B38" s="2">
+        <v>50</v>
+      </c>
+      <c r="C38" s="2">
+        <v>120</v>
+      </c>
+      <c r="D38" s="2">
+        <f>C38/2</f>
+        <v>60</v>
+      </c>
+      <c r="E38" s="2">
         <f t="shared" si="12"/>
-        <v>250000000</v>
-      </c>
-      <c r="K33" s="3">
-        <f t="shared" si="13"/>
-        <v>192</v>
-      </c>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A34" s="1">
-        <v>4</v>
-      </c>
-      <c r="B34" s="2">
-        <v>50</v>
-      </c>
-      <c r="C34" s="2">
-        <v>120</v>
-      </c>
-      <c r="D34" s="2">
-        <f>C34/2</f>
-        <v>60</v>
-      </c>
-      <c r="E34" s="2">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="F34" s="2">
+        <v>0</v>
+      </c>
+      <c r="F38" s="2">
         <f>75*1000</f>
         <v>75000</v>
       </c>
-      <c r="G34" s="2">
-        <f>B34*D34*(E34+D34/2)</f>
+      <c r="G38" s="2">
+        <f>B38*D38*(E38+D38/2)</f>
         <v>90000</v>
       </c>
-      <c r="H34" s="2">
-        <f t="shared" si="11"/>
+      <c r="H38" s="2">
+        <f t="shared" si="13"/>
         <v>7200000</v>
       </c>
-      <c r="I34" s="2">
-        <f>F34*G34/H34/B34</f>
+      <c r="I38" s="2">
+        <f>F38*G38/H38/B38</f>
         <v>18.75</v>
       </c>
-      <c r="J34" s="5"/>
-      <c r="K34" s="3"/>
-    </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A35" s="1">
+      <c r="J38" s="5"/>
+      <c r="K38" s="3"/>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A39" s="1">
         <v>5</v>
       </c>
-      <c r="B35" s="2">
+      <c r="B39" s="2">
         <v>400</v>
       </c>
-      <c r="C35" s="2">
+      <c r="C39" s="2">
         <v>600</v>
       </c>
-      <c r="D35" s="2">
+      <c r="D39" s="2">
         <v>300</v>
       </c>
-      <c r="E35" s="2">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="F35" s="2">
+      <c r="E39" s="2">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="F39" s="2">
         <v>500000</v>
       </c>
-      <c r="G35" s="2">
-        <f>B35*D35*(E35+D35/2)</f>
+      <c r="G39" s="2">
+        <f>B39*D39*(E39+D39/2)</f>
         <v>18000000</v>
       </c>
-      <c r="H35" s="2">
-        <f t="shared" si="11"/>
+      <c r="H39" s="2">
+        <f t="shared" si="13"/>
         <v>7200000000</v>
       </c>
-      <c r="I35" s="2">
-        <f>F35*G35/H35/B35</f>
+      <c r="I39" s="2">
+        <f>F39*G39/H39/B39</f>
         <v>3.125</v>
       </c>
-      <c r="J35" s="5"/>
-      <c r="K35" s="3"/>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A36" s="1">
+      <c r="J39" s="5"/>
+      <c r="K39" s="3"/>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A40" s="1">
         <v>5</v>
       </c>
-      <c r="B36" s="2">
+      <c r="B40" s="2">
         <v>400</v>
       </c>
-      <c r="C36" s="2">
+      <c r="C40" s="2">
         <v>600</v>
       </c>
-      <c r="D36" s="2">
-        <v>0</v>
-      </c>
-      <c r="E36" s="2">
-        <f t="shared" si="10"/>
+      <c r="D40" s="2">
+        <v>0</v>
+      </c>
+      <c r="E40" s="2">
+        <f t="shared" si="12"/>
         <v>300</v>
       </c>
-      <c r="H36" s="2">
-        <f t="shared" si="11"/>
+      <c r="H40" s="2">
+        <f t="shared" si="13"/>
         <v>7200000000</v>
       </c>
-      <c r="J36" s="5">
+      <c r="J40" s="5">
         <f>750000000</f>
         <v>750000000</v>
       </c>
-      <c r="K36" s="3">
-        <f t="shared" ref="K36" si="14">J36/H36*E36</f>
+      <c r="K40" s="3">
+        <f t="shared" ref="K40" si="16">J40/H40*E40</f>
         <v>31.25</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A37" s="1">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A41" s="1">
         <v>6</v>
       </c>
-      <c r="B37" s="2">
+      <c r="B41" s="2">
         <v>300</v>
       </c>
-      <c r="C37" s="2">
+      <c r="C41" s="2">
         <v>500</v>
       </c>
-      <c r="D37" s="2">
+      <c r="D41" s="2">
         <v>250</v>
       </c>
-      <c r="E37" s="2">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="F37" s="2">
+      <c r="E41" s="2">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="F41" s="2">
         <v>2000000</v>
       </c>
-      <c r="G37" s="2">
-        <f>B37*D37*(E37+D37/2)</f>
+      <c r="G41" s="2">
+        <f>B41*D41*(E41+D41/2)</f>
         <v>9375000</v>
       </c>
-      <c r="H37" s="2">
-        <f t="shared" si="11"/>
+      <c r="H41" s="2">
+        <f t="shared" si="13"/>
         <v>3125000000</v>
       </c>
-      <c r="I37" s="2">
-        <f>F37*G37/H37/B37</f>
+      <c r="I41" s="2">
+        <f>F41*G41/H41/B41</f>
         <v>20</v>
       </c>
-      <c r="J37" s="5"/>
-      <c r="K37" s="3"/>
-    </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A38" s="1">
+      <c r="J41" s="5"/>
+      <c r="K41" s="3"/>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A42" s="1">
         <v>6</v>
       </c>
-      <c r="B38" s="2">
+      <c r="B42" s="2">
         <v>300</v>
       </c>
-      <c r="C38" s="2">
+      <c r="C42" s="2">
         <v>500</v>
       </c>
-      <c r="D38" s="2">
-        <v>0</v>
-      </c>
-      <c r="E38" s="2">
-        <f t="shared" si="10"/>
+      <c r="D42" s="2">
+        <v>0</v>
+      </c>
+      <c r="E42" s="2">
+        <f t="shared" si="12"/>
         <v>250</v>
       </c>
-      <c r="H38" s="2">
-        <f t="shared" si="11"/>
+      <c r="H42" s="2">
+        <f t="shared" si="13"/>
         <v>3125000000</v>
       </c>
-      <c r="J38" s="5">
+      <c r="J42" s="5">
         <f>6000000000</f>
         <v>6000000000</v>
       </c>
-      <c r="K38" s="3">
-        <f t="shared" ref="K38:K39" si="15">J38/H38*E38</f>
+      <c r="K42" s="3">
+        <f t="shared" ref="K42:K43" si="17">J42/H42*E42</f>
         <v>480</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A39" s="1">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A43" s="1">
         <v>7</v>
       </c>
-      <c r="B39" s="2">
+      <c r="B43" s="2">
         <v>240</v>
       </c>
-      <c r="C39" s="2">
+      <c r="C43" s="2">
         <v>360</v>
       </c>
-      <c r="D39" s="2">
-        <f>C39/2-40</f>
+      <c r="D43" s="2">
+        <f>C43/2-40</f>
         <v>140</v>
       </c>
-      <c r="E39" s="2">
-        <f t="shared" si="10"/>
+      <c r="E43" s="2">
+        <f t="shared" si="12"/>
         <v>40</v>
       </c>
-      <c r="F39" s="2">
+      <c r="F43" s="2">
         <f>240*1000</f>
         <v>240000</v>
       </c>
-      <c r="G39" s="2">
-        <f>B39*D39*(E39+D39/2)</f>
+      <c r="G43" s="2">
+        <f>B43*D43*(E43+D43/2)</f>
         <v>3696000</v>
       </c>
-      <c r="H39" s="2">
-        <f t="shared" si="11"/>
+      <c r="H43" s="2">
+        <f t="shared" si="13"/>
         <v>933120000</v>
       </c>
-      <c r="I39" s="2">
-        <f t="shared" ref="I39:I48" si="16">F39*G39/H39/B39</f>
+      <c r="I43" s="2">
+        <f t="shared" ref="I43:I52" si="18">F43*G43/H43/B43</f>
         <v>3.9609053497942388</v>
       </c>
-      <c r="J39" s="5">
+      <c r="J43" s="5">
         <v>720000000</v>
       </c>
-      <c r="K39" s="3">
-        <f t="shared" si="15"/>
+      <c r="K43" s="3">
+        <f t="shared" si="17"/>
         <v>30.864197530864196</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A40" s="1">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A44" s="1">
         <v>8</v>
       </c>
-      <c r="B40" s="2">
+      <c r="B44" s="2">
         <v>300</v>
       </c>
-      <c r="C40" s="2">
+      <c r="C44" s="2">
         <v>500</v>
       </c>
-      <c r="D40" s="2">
+      <c r="D44" s="2">
         <v>250</v>
       </c>
-      <c r="E40" s="2">
-        <f t="shared" ref="E40" si="17">C40/2-D40</f>
-        <v>0</v>
-      </c>
-      <c r="F40" s="2">
+      <c r="E44" s="2">
+        <f t="shared" ref="E44" si="19">C44/2-D44</f>
+        <v>0</v>
+      </c>
+      <c r="F44" s="2">
         <v>753000</v>
       </c>
-      <c r="G40" s="2">
-        <f>B40*D40*(E40+D40/2)</f>
+      <c r="G44" s="2">
+        <f>B44*D44*(E44+D44/2)</f>
         <v>9375000</v>
       </c>
-      <c r="H40" s="2">
-        <f t="shared" ref="H40" si="18">B40*C40^3/12</f>
+      <c r="H44" s="2">
+        <f t="shared" ref="H44" si="20">B44*C44^3/12</f>
         <v>3125000000</v>
       </c>
-      <c r="I40" s="2">
-        <f t="shared" si="16"/>
+      <c r="I44" s="2">
+        <f t="shared" si="18"/>
         <v>7.53</v>
       </c>
-      <c r="J40" s="5"/>
-      <c r="K40" s="3"/>
-    </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A41" s="1">
+      <c r="J44" s="5"/>
+      <c r="K44" s="3"/>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A45" s="1">
         <v>9</v>
       </c>
-      <c r="B41" s="2">
+      <c r="B45" s="2">
         <v>10</v>
       </c>
-      <c r="F41" s="2">
+      <c r="F45" s="2">
         <v>9265</v>
       </c>
-      <c r="G41" s="2">
+      <c r="G45" s="2">
         <f>100*20*70+10*60*30</f>
         <v>158000</v>
       </c>
-      <c r="H41" s="2">
+      <c r="H45" s="2">
         <f>100*160^3/12-90*120^3/12</f>
         <v>21173333.333333336</v>
       </c>
-      <c r="I41" s="2">
-        <f t="shared" si="16"/>
+      <c r="I45" s="2">
+        <f t="shared" si="18"/>
         <v>6.9137437027707804</v>
       </c>
-      <c r="J41" s="5"/>
-      <c r="K41" s="3"/>
-    </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A42" s="1">
+      <c r="J45" s="5"/>
+      <c r="K45" s="3"/>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A46" s="1">
         <v>10</v>
       </c>
-      <c r="B42" s="2">
+      <c r="B46" s="2">
         <v>10</v>
       </c>
-      <c r="F42" s="2">
+      <c r="F46" s="2">
         <v>9265</v>
       </c>
-      <c r="G42" s="2">
+      <c r="G46" s="2">
         <f>100*20*70+10*30*45</f>
         <v>153500</v>
       </c>
-      <c r="H42" s="2">
+      <c r="H46" s="2">
         <f>100*160^3/12-90*120^3/12</f>
         <v>21173333.333333336</v>
       </c>
-      <c r="I42" s="2">
-        <f t="shared" si="16"/>
+      <c r="I46" s="2">
+        <f t="shared" si="18"/>
         <v>6.7168332808564228</v>
       </c>
-      <c r="J42" s="5"/>
-      <c r="K42" s="3"/>
-    </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A43" s="1">
+      <c r="J46" s="5"/>
+      <c r="K46" s="3"/>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A47" s="1">
         <v>11</v>
       </c>
-      <c r="B43" s="2">
+      <c r="B47" s="2">
         <v>200</v>
       </c>
-      <c r="C43" s="2">
+      <c r="C47" s="2">
         <v>360</v>
       </c>
-      <c r="D43" s="2">
-        <v>0</v>
-      </c>
-      <c r="E43" s="2">
-        <f t="shared" ref="E43" si="19">C43/2-D43</f>
+      <c r="D47" s="2">
+        <v>0</v>
+      </c>
+      <c r="E47" s="2">
+        <f t="shared" ref="E47" si="21">C47/2-D47</f>
         <v>180</v>
       </c>
-      <c r="G43" s="2">
-        <f t="shared" ref="G43:G48" si="20">B43*D43*(E43+D43/2)</f>
-        <v>0</v>
-      </c>
-      <c r="H43" s="2">
-        <f t="shared" ref="H43" si="21">B43*C43^3/12</f>
+      <c r="G47" s="2">
+        <f t="shared" ref="G47:G52" si="22">B47*D47*(E47+D47/2)</f>
+        <v>0</v>
+      </c>
+      <c r="H47" s="2">
+        <f t="shared" ref="H47" si="23">B47*C47^3/12</f>
         <v>777600000</v>
       </c>
-      <c r="I43" s="2">
-        <f t="shared" si="16"/>
-        <v>0</v>
-      </c>
-      <c r="J43" s="5">
+      <c r="I47" s="2">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="J47" s="5">
         <f>350*1000000</f>
         <v>350000000</v>
       </c>
-      <c r="K43" s="3">
-        <f t="shared" ref="K43" si="22">J43/H43*E43</f>
+      <c r="K47" s="3">
+        <f t="shared" ref="K47" si="24">J47/H47*E47</f>
         <v>81.018518518518519</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A44" s="1">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A48" s="1">
         <v>11</v>
       </c>
-      <c r="B44" s="2">
+      <c r="B48" s="2">
         <v>200</v>
       </c>
-      <c r="C44" s="2">
+      <c r="C48" s="2">
         <v>360</v>
       </c>
-      <c r="D44" s="2">
-        <f>C44/2</f>
+      <c r="D48" s="2">
+        <f>C48/2</f>
         <v>180</v>
       </c>
-      <c r="E44" s="2">
-        <f t="shared" ref="E44:E45" si="23">C44/2-D44</f>
-        <v>0</v>
-      </c>
-      <c r="G44" s="2">
-        <f t="shared" si="20"/>
+      <c r="E48" s="2">
+        <f t="shared" ref="E48:E49" si="25">C48/2-D48</f>
+        <v>0</v>
+      </c>
+      <c r="G48" s="2">
+        <f t="shared" si="22"/>
         <v>3240000</v>
       </c>
-      <c r="H44" s="2">
-        <f t="shared" ref="H44:H45" si="24">B44*C44^3/12</f>
+      <c r="H48" s="2">
+        <f t="shared" ref="H48:H49" si="26">B48*C48^3/12</f>
         <v>777600000</v>
       </c>
-      <c r="I44" s="2">
-        <f t="shared" si="16"/>
-        <v>0</v>
-      </c>
-      <c r="J44" s="5">
+      <c r="I48" s="2">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="J48" s="5">
         <f>350*1000000</f>
         <v>350000000</v>
       </c>
-      <c r="K44" s="3">
-        <f t="shared" ref="K44:K45" si="25">J44/H44*E44</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A45" s="1">
+      <c r="K48" s="3">
+        <f t="shared" ref="K48:K49" si="27">J48/H48*E48</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A49" s="1">
         <v>12</v>
       </c>
-      <c r="B45" s="2">
+      <c r="B49" s="2">
         <v>100</v>
       </c>
-      <c r="C45" s="2">
+      <c r="C49" s="2">
         <v>220</v>
       </c>
-      <c r="D45" s="2">
-        <v>0</v>
-      </c>
-      <c r="E45" s="2">
-        <f t="shared" si="23"/>
+      <c r="D49" s="2">
+        <v>0</v>
+      </c>
+      <c r="E49" s="2">
+        <f t="shared" si="25"/>
         <v>110</v>
       </c>
-      <c r="G45" s="2">
-        <f t="shared" si="20"/>
-        <v>0</v>
-      </c>
-      <c r="H45" s="2">
-        <f t="shared" si="24"/>
+      <c r="G49" s="2">
+        <f t="shared" si="22"/>
+        <v>0</v>
+      </c>
+      <c r="H49" s="2">
+        <f t="shared" si="26"/>
         <v>88733333.333333328</v>
       </c>
-      <c r="I45" s="2">
-        <f t="shared" si="16"/>
-        <v>0</v>
-      </c>
-      <c r="J45" s="5">
+      <c r="I49" s="2">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="J49" s="5">
         <f>76.3*1000000</f>
         <v>76300000</v>
       </c>
-      <c r="K45" s="3">
-        <f t="shared" si="25"/>
+      <c r="K49" s="3">
+        <f t="shared" si="27"/>
         <v>94.586776859504141</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A46" s="1">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A50" s="1">
         <v>12</v>
       </c>
-      <c r="B46" s="2">
+      <c r="B50" s="2">
         <v>100</v>
       </c>
-      <c r="C46" s="2">
+      <c r="C50" s="2">
         <v>220</v>
       </c>
-      <c r="D46" s="2">
+      <c r="D50" s="2">
         <v>35</v>
       </c>
-      <c r="E46" s="2">
-        <f t="shared" ref="E46:E47" si="26">C46/2-D46</f>
+      <c r="E50" s="2">
+        <f t="shared" ref="E50:E51" si="28">C50/2-D50</f>
         <v>75</v>
       </c>
-      <c r="G46" s="2">
-        <f t="shared" si="20"/>
+      <c r="G50" s="2">
+        <f t="shared" si="22"/>
         <v>323750</v>
       </c>
-      <c r="H46" s="2">
-        <f t="shared" ref="H46:H47" si="27">B46*C46^3/12</f>
+      <c r="H50" s="2">
+        <f t="shared" ref="H50:H51" si="29">B50*C50^3/12</f>
         <v>88733333.333333328</v>
       </c>
-      <c r="I46" s="2">
-        <f t="shared" si="16"/>
-        <v>0</v>
-      </c>
-      <c r="J46" s="5">
-        <f t="shared" ref="J46:J48" si="28">76.3*1000000</f>
+      <c r="I50" s="2">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="J50" s="5">
+        <f t="shared" ref="J50:J52" si="30">76.3*1000000</f>
         <v>76300000</v>
       </c>
-      <c r="K46" s="3">
-        <f t="shared" ref="K46:K47" si="29">J46/H46*E46</f>
+      <c r="K50" s="3">
+        <f t="shared" ref="K50:K51" si="31">J50/H50*E50</f>
         <v>64.490984222389187</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A47" s="1">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A51" s="1">
         <v>12</v>
       </c>
-      <c r="B47" s="2">
+      <c r="B51" s="2">
         <v>100</v>
       </c>
-      <c r="C47" s="2">
+      <c r="C51" s="2">
         <v>220</v>
       </c>
-      <c r="D47" s="2">
+      <c r="D51" s="2">
         <v>60</v>
       </c>
-      <c r="E47" s="2">
-        <f t="shared" si="26"/>
+      <c r="E51" s="2">
+        <f t="shared" si="28"/>
         <v>50</v>
       </c>
-      <c r="G47" s="2">
-        <f t="shared" si="20"/>
+      <c r="G51" s="2">
+        <f t="shared" si="22"/>
         <v>480000</v>
       </c>
-      <c r="H47" s="2">
-        <f t="shared" si="27"/>
+      <c r="H51" s="2">
+        <f t="shared" si="29"/>
         <v>88733333.333333328</v>
       </c>
-      <c r="I47" s="2">
-        <f t="shared" si="16"/>
-        <v>0</v>
-      </c>
-      <c r="J47" s="5">
-        <f t="shared" si="28"/>
+      <c r="I51" s="2">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="J51" s="5">
+        <f t="shared" si="30"/>
         <v>76300000</v>
       </c>
-      <c r="K47" s="3">
-        <f t="shared" si="29"/>
+      <c r="K51" s="3">
+        <f t="shared" si="31"/>
         <v>42.993989481592791</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A48" s="1">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A52" s="1">
         <v>12</v>
       </c>
-      <c r="B48" s="2">
+      <c r="B52" s="2">
         <v>100</v>
       </c>
-      <c r="C48" s="2">
+      <c r="C52" s="2">
         <v>220</v>
       </c>
-      <c r="D48" s="2">
+      <c r="D52" s="2">
         <v>85</v>
       </c>
-      <c r="E48" s="2">
-        <f t="shared" ref="E48" si="30">C48/2-D48</f>
+      <c r="E52" s="2">
+        <f t="shared" ref="E52" si="32">C52/2-D52</f>
         <v>25</v>
       </c>
-      <c r="G48" s="2">
-        <f t="shared" si="20"/>
+      <c r="G52" s="2">
+        <f t="shared" si="22"/>
         <v>573750</v>
       </c>
-      <c r="H48" s="2">
-        <f t="shared" ref="H48" si="31">B48*C48^3/12</f>
+      <c r="H52" s="2">
+        <f t="shared" ref="H52" si="33">B52*C52^3/12</f>
         <v>88733333.333333328</v>
       </c>
-      <c r="I48" s="2">
-        <f t="shared" si="16"/>
-        <v>0</v>
-      </c>
-      <c r="J48" s="5">
-        <f t="shared" si="28"/>
+      <c r="I52" s="2">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="J52" s="5">
+        <f t="shared" si="30"/>
         <v>76300000</v>
       </c>
-      <c r="K48" s="3">
-        <f t="shared" ref="K48" si="32">J48/H48*E48</f>
+      <c r="K52" s="3">
+        <f t="shared" ref="K52" si="34">J52/H52*E52</f>
         <v>21.496994740796396</v>
       </c>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A49" s="1">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A53" s="1">
         <v>13</v>
       </c>
-      <c r="B49" s="2">
+      <c r="B53" s="2">
         <v>10</v>
       </c>
-      <c r="E49" s="2">
-        <v>0</v>
-      </c>
-      <c r="H49" s="2">
+      <c r="E53" s="2">
+        <v>0</v>
+      </c>
+      <c r="H53" s="2">
         <f>100*160^3/12-90*120^3/12</f>
         <v>21173333.333333336</v>
       </c>
-      <c r="J49" s="5">
+      <c r="J53" s="5">
         <f>73*1000000</f>
         <v>73000000</v>
       </c>
-      <c r="K49" s="3">
-        <f t="shared" ref="K49:K50" si="33">J49/H49*E49</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A50" s="1">
+      <c r="K53" s="3">
+        <f t="shared" ref="K53:K54" si="35">J53/H53*E53</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A54" s="1">
         <v>13</v>
       </c>
-      <c r="B50" s="2">
+      <c r="B54" s="2">
         <v>10</v>
       </c>
-      <c r="E50" s="2">
+      <c r="E54" s="2">
         <v>30</v>
       </c>
-      <c r="H50" s="2">
+      <c r="H54" s="2">
         <f>100*160^3/12-90*120^3/12</f>
         <v>21173333.333333336</v>
       </c>
-      <c r="J50" s="5">
+      <c r="J54" s="5">
         <f>73*1000000</f>
         <v>73000000</v>
       </c>
-      <c r="K50" s="3">
-        <f t="shared" si="33"/>
+      <c r="K54" s="3">
+        <f t="shared" si="35"/>
         <v>103.43198992443322</v>
       </c>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A51" s="1">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A55" s="1">
         <v>13</v>
       </c>
-      <c r="B51" s="2">
+      <c r="B55" s="2">
         <v>10</v>
       </c>
-      <c r="E51" s="2">
+      <c r="E55" s="2">
         <v>60</v>
       </c>
-      <c r="H51" s="2">
+      <c r="H55" s="2">
         <f>100*160^3/12-90*120^3/12</f>
         <v>21173333.333333336</v>
       </c>
-      <c r="J51" s="5">
+      <c r="J55" s="5">
         <f>73*1000000</f>
         <v>73000000</v>
       </c>
-      <c r="K51" s="3">
-        <f t="shared" ref="K51:K55" si="34">J51/H51*E51</f>
+      <c r="K55" s="3">
+        <f t="shared" ref="K55:K59" si="36">J55/H55*E55</f>
         <v>206.86397984886645</v>
       </c>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A52" s="1">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A56" s="1">
         <v>13</v>
       </c>
-      <c r="B52" s="2">
+      <c r="B56" s="2">
         <v>10</v>
       </c>
-      <c r="E52" s="2">
+      <c r="E56" s="2">
         <v>80</v>
       </c>
-      <c r="H52" s="2">
+      <c r="H56" s="2">
         <f>100*160^3/12-90*120^3/12</f>
         <v>21173333.333333336</v>
       </c>
-      <c r="J52" s="5">
+      <c r="J56" s="5">
         <f>73*1000000</f>
         <v>73000000</v>
       </c>
-      <c r="K52" s="3">
-        <f t="shared" si="34"/>
+      <c r="K56" s="3">
+        <f t="shared" si="36"/>
         <v>275.81863979848862</v>
       </c>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A53" s="1">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A57" s="1">
         <v>14</v>
       </c>
-      <c r="B53" s="2">
+      <c r="B57" s="2">
         <v>200</v>
       </c>
-      <c r="C53" s="2">
+      <c r="C57" s="2">
         <v>360</v>
       </c>
-      <c r="D53" s="2">
-        <v>0</v>
-      </c>
-      <c r="E53" s="2">
-        <f t="shared" ref="E53:E54" si="35">C53/2-D53</f>
+      <c r="D57" s="2">
+        <v>0</v>
+      </c>
+      <c r="E57" s="2">
+        <f t="shared" ref="E57:E58" si="37">C57/2-D57</f>
         <v>180</v>
       </c>
-      <c r="F53" s="2">
+      <c r="F57" s="2">
         <f>80*4/2*1000</f>
         <v>160000</v>
       </c>
-      <c r="G53" s="2">
-        <f>B53*D53*(E53+D53/2)</f>
-        <v>0</v>
-      </c>
-      <c r="H53" s="2">
-        <f t="shared" ref="H53" si="36">B53*C53^3/12</f>
+      <c r="G57" s="2">
+        <f>B57*D57*(E57+D57/2)</f>
+        <v>0</v>
+      </c>
+      <c r="H57" s="2">
+        <f t="shared" ref="H57" si="38">B57*C57^3/12</f>
         <v>777600000</v>
       </c>
-      <c r="I53" s="2">
-        <f>F53*G53/H53/B53</f>
-        <v>0</v>
-      </c>
-      <c r="J53" s="5">
+      <c r="I57" s="3">
+        <f>F57*G57/H57/B57</f>
+        <v>0</v>
+      </c>
+      <c r="J57" s="5">
         <f>80*4^2/8*1000000</f>
         <v>160000000</v>
       </c>
-      <c r="K53" s="3">
-        <f t="shared" ref="K53" si="37">J53/H53*E53</f>
+      <c r="K57" s="3">
+        <f t="shared" ref="K57" si="39">J57/H57*E57</f>
         <v>37.037037037037038</v>
       </c>
     </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A54" s="1">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A58" s="1">
         <v>14</v>
       </c>
-      <c r="B54" s="2">
+      <c r="B58" s="2">
         <v>200</v>
       </c>
-      <c r="C54" s="2">
+      <c r="C58" s="2">
         <v>360</v>
       </c>
-      <c r="D54" s="2">
-        <f>C54/2</f>
+      <c r="D58" s="2">
+        <f>C58/2</f>
         <v>180</v>
       </c>
-      <c r="E54" s="2">
-        <f t="shared" si="35"/>
-        <v>0</v>
-      </c>
-      <c r="F54" s="2">
+      <c r="E58" s="2">
+        <f t="shared" si="37"/>
+        <v>0</v>
+      </c>
+      <c r="F58" s="2">
         <f>80*4/2*1000</f>
         <v>160000</v>
       </c>
-      <c r="G54" s="2">
-        <f>B54*D54*(E54+D54/2)</f>
+      <c r="G58" s="2">
+        <f>B58*D58*(E58+D58/2)</f>
         <v>3240000</v>
       </c>
-      <c r="H54" s="2">
-        <f t="shared" ref="H54:H55" si="38">B54*C54^3/12</f>
+      <c r="H58" s="2">
+        <f t="shared" ref="H58:H59" si="40">B58*C58^3/12</f>
         <v>777600000</v>
       </c>
-      <c r="I54" s="2">
-        <f>F54*G54/H54/B54</f>
+      <c r="I58" s="3">
+        <f>F58*G58/H58/B58</f>
         <v>3.333333333333333</v>
       </c>
-      <c r="J54" s="5">
+      <c r="J58" s="5">
         <f>80*4^2/8*1000000</f>
         <v>160000000</v>
       </c>
-      <c r="K54" s="3">
-        <f t="shared" si="34"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A55" s="1">
+      <c r="K58" s="3">
+        <f t="shared" si="36"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A59" s="1">
         <v>15</v>
       </c>
-      <c r="B55" s="2">
+      <c r="B59" s="2">
         <v>360</v>
       </c>
-      <c r="C55" s="2">
+      <c r="C59" s="2">
         <v>600</v>
       </c>
-      <c r="D55" s="2">
-        <f>C55/2-50</f>
+      <c r="D59" s="2">
+        <f>C59/2-50</f>
         <v>250</v>
       </c>
-      <c r="E55" s="2">
-        <f t="shared" ref="E55" si="39">C55/2-D55</f>
+      <c r="E59" s="2">
+        <f t="shared" ref="E59" si="41">C59/2-D59</f>
         <v>50</v>
       </c>
-      <c r="F55" s="2">
+      <c r="F59" s="2">
         <f>350*6*1000</f>
         <v>2100000</v>
       </c>
-      <c r="G55" s="2">
-        <f>B55*D55*(E55+D55/2)</f>
+      <c r="G59" s="2">
+        <f>B59*D59*(E59+D59/2)</f>
         <v>15750000</v>
       </c>
-      <c r="H55" s="2">
-        <f t="shared" si="38"/>
+      <c r="H59" s="5">
+        <f t="shared" si="40"/>
         <v>6480000000</v>
       </c>
-      <c r="I55" s="2">
-        <f>F55*G55/H55/B55</f>
+      <c r="I59" s="3">
+        <f>F59*G59/H59/B59</f>
         <v>14.178240740740742</v>
       </c>
-      <c r="J55" s="5">
+      <c r="J59" s="5">
         <f>350*6*3*1000000</f>
         <v>6300000000</v>
       </c>
-      <c r="K55" s="3">
-        <f t="shared" si="34"/>
+      <c r="K59" s="3">
+        <f t="shared" si="36"/>
         <v>48.611111111111107</v>
       </c>
     </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="D57" s="2">
-        <f>10000*10/100</f>
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B59" s="2" t="s">
+    <row r="66" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B66" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="C59" s="2" t="s">
+      <c r="C66" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="D59" s="2" t="s">
+      <c r="D66" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="E59" s="2" t="s">
+      <c r="E66" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="F59" s="2" t="s">
+      <c r="F66" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="G59" s="2" t="s">
+      <c r="G66" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="H59" s="2" t="s">
+      <c r="H66" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="I59" s="2" t="s">
+      <c r="I66" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="J59" s="2" t="s">
+      <c r="J66" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="K59" s="2" t="s">
+      <c r="K66" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="L59" s="2" t="s">
+      <c r="L66" s="2" t="s">
         <v>40</v>
-      </c>
-    </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A60" s="1">
-        <v>1</v>
-      </c>
-      <c r="B60" s="2">
-        <v>1000</v>
-      </c>
-      <c r="C60" s="2">
-        <v>500</v>
-      </c>
-      <c r="D60" s="2">
-        <v>-50</v>
-      </c>
-      <c r="E60" s="2">
-        <f t="shared" ref="E60:E66" si="40">ATAN(-2*D60/(B60-C60))/2</f>
-        <v>9.8697779924940388E-2</v>
-      </c>
-      <c r="F60" s="2">
-        <f t="shared" ref="F60:F66" si="41">E60*180/PI()</f>
-        <v>5.6549662370101066</v>
-      </c>
-      <c r="G60" s="2">
-        <f t="shared" ref="G60:G66" si="42">(B60+C60)/2</f>
-        <v>750</v>
-      </c>
-      <c r="H60" s="2">
-        <f t="shared" ref="H60:H66" si="43">SQRT((B60-C60)^2/4+D60^2)</f>
-        <v>254.95097567963924</v>
-      </c>
-      <c r="I60" s="2">
-        <f t="shared" ref="I60:I66" si="44">G60+H60</f>
-        <v>1004.9509756796392</v>
-      </c>
-      <c r="J60" s="2">
-        <f t="shared" ref="J60:J66" si="45">G60-H60</f>
-        <v>495.04902432036079</v>
-      </c>
-      <c r="K60" s="2">
-        <f t="shared" ref="K60:K64" si="46">F60+45</f>
-        <v>50.654966237010107</v>
-      </c>
-      <c r="L60" s="2">
-        <f t="shared" ref="L60:L64" si="47">K60-90</f>
-        <v>-39.345033762989893</v>
-      </c>
-    </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A61" s="1">
-        <v>2</v>
-      </c>
-      <c r="B61" s="2">
-        <v>5333333.3333333302</v>
-      </c>
-      <c r="C61" s="2">
-        <v>3333333.3333333302</v>
-      </c>
-      <c r="D61" s="2">
-        <v>-2400000</v>
-      </c>
-      <c r="E61" s="2">
-        <f t="shared" si="40"/>
-        <v>0.5880026035475675</v>
-      </c>
-      <c r="F61" s="2">
-        <f t="shared" si="41"/>
-        <v>33.690067525979785</v>
-      </c>
-      <c r="G61" s="2">
-        <f t="shared" si="42"/>
-        <v>4333333.3333333302</v>
-      </c>
-      <c r="H61" s="2">
-        <f t="shared" si="43"/>
-        <v>2600000</v>
-      </c>
-      <c r="I61" s="2">
-        <f t="shared" si="44"/>
-        <v>6933333.3333333302</v>
-      </c>
-      <c r="J61" s="2">
-        <f t="shared" si="45"/>
-        <v>1733333.3333333302</v>
-      </c>
-      <c r="K61" s="2">
-        <f t="shared" si="46"/>
-        <v>78.690067525979785</v>
-      </c>
-      <c r="L61" s="2">
-        <f t="shared" si="47"/>
-        <v>-11.309932474020215</v>
-      </c>
-    </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A62" s="1">
-        <v>3</v>
-      </c>
-      <c r="B62" s="2">
-        <v>532</v>
-      </c>
-      <c r="C62" s="2">
-        <v>740</v>
-      </c>
-      <c r="D62" s="2">
-        <v>345</v>
-      </c>
-      <c r="E62" s="2">
-        <f t="shared" si="40"/>
-        <v>0.6390052264115833</v>
-      </c>
-      <c r="F62" s="2">
-        <f t="shared" si="41"/>
-        <v>36.612302560185327</v>
-      </c>
-      <c r="G62" s="2">
-        <f t="shared" si="42"/>
-        <v>636</v>
-      </c>
-      <c r="H62" s="2">
-        <f t="shared" si="43"/>
-        <v>360.33456675706259</v>
-      </c>
-      <c r="I62" s="2">
-        <f t="shared" si="44"/>
-        <v>996.33456675706259</v>
-      </c>
-      <c r="J62" s="2">
-        <f t="shared" si="45"/>
-        <v>275.66543324293741</v>
-      </c>
-      <c r="K62" s="2">
-        <f t="shared" si="46"/>
-        <v>81.612302560185327</v>
-      </c>
-      <c r="L62" s="2">
-        <f t="shared" si="47"/>
-        <v>-8.3876974398146729</v>
-      </c>
-    </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A63" s="1">
-        <v>4</v>
-      </c>
-      <c r="B63" s="2">
-        <v>300</v>
-      </c>
-      <c r="C63" s="2">
-        <v>150</v>
-      </c>
-      <c r="D63" s="2">
-        <v>200</v>
-      </c>
-      <c r="E63" s="2">
-        <f t="shared" si="40"/>
-        <v>-0.60601282826216218</v>
-      </c>
-      <c r="F63" s="2">
-        <f t="shared" si="41"/>
-        <v>-34.721977390208266</v>
-      </c>
-      <c r="G63" s="2">
-        <f t="shared" si="42"/>
-        <v>225</v>
-      </c>
-      <c r="H63" s="2">
-        <f t="shared" si="43"/>
-        <v>213.60009363293827</v>
-      </c>
-      <c r="I63" s="2">
-        <f t="shared" si="44"/>
-        <v>438.6000936329383</v>
-      </c>
-      <c r="J63" s="2">
-        <f t="shared" si="45"/>
-        <v>11.399906367061732</v>
-      </c>
-      <c r="K63" s="2">
-        <f t="shared" si="46"/>
-        <v>10.278022609791734</v>
-      </c>
-      <c r="L63" s="2">
-        <f t="shared" si="47"/>
-        <v>-79.721977390208266</v>
-      </c>
-    </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A64" s="1">
-        <v>5</v>
-      </c>
-      <c r="B64" s="2">
-        <v>50</v>
-      </c>
-      <c r="C64" s="2">
-        <v>-10</v>
-      </c>
-      <c r="D64" s="2">
-        <v>40</v>
-      </c>
-      <c r="E64" s="2">
-        <f t="shared" si="40"/>
-        <v>-0.46364760900080609</v>
-      </c>
-      <c r="F64" s="2">
-        <f t="shared" si="41"/>
-        <v>-26.56505117707799</v>
-      </c>
-      <c r="G64" s="2">
-        <f t="shared" si="42"/>
-        <v>20</v>
-      </c>
-      <c r="H64" s="2">
-        <f t="shared" si="43"/>
-        <v>50</v>
-      </c>
-      <c r="I64" s="2">
-        <f t="shared" si="44"/>
-        <v>70</v>
-      </c>
-      <c r="J64" s="2">
-        <f t="shared" si="45"/>
-        <v>-30</v>
-      </c>
-      <c r="K64" s="2">
-        <f t="shared" si="46"/>
-        <v>18.43494882292201</v>
-      </c>
-      <c r="L64" s="2">
-        <f t="shared" si="47"/>
-        <v>-71.56505117707799</v>
-      </c>
-    </row>
-    <row r="65" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A65" s="1">
-        <v>6</v>
-      </c>
-      <c r="B65" s="2">
-        <v>800</v>
-      </c>
-      <c r="C65" s="2">
-        <v>400</v>
-      </c>
-      <c r="D65" s="2">
-        <v>-550</v>
-      </c>
-      <c r="E65" s="2">
-        <f t="shared" si="40"/>
-        <v>0.61101266160549483</v>
-      </c>
-      <c r="F65" s="2">
-        <f t="shared" si="41"/>
-        <v>35.008446739050015</v>
-      </c>
-      <c r="G65" s="2">
-        <f t="shared" si="42"/>
-        <v>600</v>
-      </c>
-      <c r="H65" s="2">
-        <f t="shared" si="43"/>
-        <v>585.23499553598128</v>
-      </c>
-      <c r="I65" s="2">
-        <f t="shared" si="44"/>
-        <v>1185.2349955359814</v>
-      </c>
-      <c r="J65" s="2">
-        <f t="shared" si="45"/>
-        <v>14.765004464018716</v>
-      </c>
-      <c r="K65" s="2">
-        <f t="shared" ref="K65:K72" si="48">F65+45</f>
-        <v>80.008446739050015</v>
-      </c>
-      <c r="L65" s="2">
-        <f t="shared" ref="L65:L72" si="49">K65-90</f>
-        <v>-9.9915532609499849</v>
-      </c>
-    </row>
-    <row r="66" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A66" s="1">
-        <v>7</v>
-      </c>
-      <c r="B66" s="2">
-        <f>K39</f>
-        <v>30.864197530864196</v>
-      </c>
-      <c r="C66" s="2">
-        <v>0</v>
-      </c>
-      <c r="D66" s="2">
-        <f>I39</f>
-        <v>3.9609053497942388</v>
-      </c>
-      <c r="E66" s="2">
-        <f t="shared" si="40"/>
-        <v>-0.12562163201205953</v>
-      </c>
-      <c r="F66" s="2">
-        <f t="shared" si="41"/>
-        <v>-7.1975893298365268</v>
-      </c>
-      <c r="G66" s="2">
-        <f t="shared" si="42"/>
-        <v>15.432098765432098</v>
-      </c>
-      <c r="H66" s="2">
-        <f t="shared" si="43"/>
-        <v>15.932308165990248</v>
-      </c>
-      <c r="I66" s="2">
-        <f t="shared" si="44"/>
-        <v>31.364406931422344</v>
-      </c>
-      <c r="J66" s="2">
-        <f t="shared" si="45"/>
-        <v>-0.50020940055815011</v>
-      </c>
-      <c r="K66" s="2">
-        <f t="shared" si="48"/>
-        <v>37.802410670163475</v>
-      </c>
-      <c r="L66" s="2">
-        <f t="shared" si="49"/>
-        <v>-52.197589329836525</v>
-      </c>
-      <c r="M66" s="2">
-        <f>L66*2</f>
-        <v>-104.39517865967305</v>
       </c>
     </row>
     <row r="67" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A67" s="1">
-        <v>8</v>
-      </c>
-      <c r="B67" s="2">
-        <v>-150</v>
-      </c>
-      <c r="C67" s="2">
-        <v>352</v>
-      </c>
-      <c r="D67" s="2">
-        <v>-24</v>
-      </c>
-      <c r="E67" s="2">
-        <f t="shared" ref="E67:E71" si="50">ATAN(-2*D67/(B67-C67))/2</f>
-        <v>-4.7663858426665248E-2</v>
-      </c>
-      <c r="F67" s="2">
-        <f t="shared" ref="F67:F71" si="51">E67*180/PI()</f>
-        <v>-2.7309379231569828</v>
-      </c>
-      <c r="G67" s="2">
-        <f t="shared" ref="G67:G71" si="52">(B67+C67)/2</f>
-        <v>101</v>
-      </c>
-      <c r="H67" s="2">
-        <f t="shared" ref="H67:H71" si="53">SQRT((B67-C67)^2/4+D67^2)</f>
-        <v>252.14479966876175</v>
-      </c>
-      <c r="I67" s="2">
-        <f t="shared" ref="I67:I71" si="54">G67+H67</f>
-        <v>353.14479966876172</v>
-      </c>
-      <c r="J67" s="2">
-        <f t="shared" ref="J67:J71" si="55">G67-H67</f>
-        <v>-151.14479966876175</v>
-      </c>
-      <c r="K67" s="2">
-        <f t="shared" si="48"/>
-        <v>42.269062076843014</v>
-      </c>
-      <c r="L67" s="2">
-        <f t="shared" si="49"/>
-        <v>-47.730937923156986</v>
-      </c>
-      <c r="M67" s="2">
-        <f>L67*2</f>
-        <v>-95.461875846313973</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="B67" s="3">
+        <v>1000</v>
+      </c>
+      <c r="C67" s="3">
+        <v>500</v>
+      </c>
+      <c r="D67" s="3">
+        <v>-50</v>
+      </c>
+      <c r="E67" s="3">
+        <f t="shared" ref="E67:E73" si="42">ATAN(-2*D67/(B67-C67))/2</f>
+        <v>9.8697779924940388E-2</v>
+      </c>
+      <c r="F67" s="3">
+        <f t="shared" ref="F67:F73" si="43">E67*180/PI()</f>
+        <v>5.6549662370101066</v>
+      </c>
+      <c r="G67" s="3">
+        <f t="shared" ref="G67:G73" si="44">(B67+C67)/2</f>
+        <v>750</v>
+      </c>
+      <c r="H67" s="3">
+        <f t="shared" ref="H67:H73" si="45">SQRT((B67-C67)^2/4+D67^2)</f>
+        <v>254.95097567963924</v>
+      </c>
+      <c r="I67" s="3">
+        <f t="shared" ref="I67:I73" si="46">G67+H67</f>
+        <v>1004.9509756796392</v>
+      </c>
+      <c r="J67" s="3">
+        <f t="shared" ref="J67:J73" si="47">G67-H67</f>
+        <v>495.04902432036079</v>
+      </c>
+      <c r="K67" s="3">
+        <f t="shared" ref="K67:K71" si="48">F67+45</f>
+        <v>50.654966237010107</v>
+      </c>
+      <c r="L67" s="3">
+        <f t="shared" ref="L67:L71" si="49">K67-90</f>
+        <v>-39.345033762989893</v>
+      </c>
+      <c r="M67" s="3"/>
     </row>
     <row r="68" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A68" s="1">
-        <v>9</v>
-      </c>
-      <c r="B68" s="2">
-        <v>-400</v>
-      </c>
-      <c r="C68" s="2">
-        <v>-300</v>
-      </c>
-      <c r="D68" s="2">
-        <v>120</v>
-      </c>
-      <c r="E68" s="2">
-        <f t="shared" si="50"/>
+        <v>2</v>
+      </c>
+      <c r="B68" s="3">
+        <v>5333333.3333333302</v>
+      </c>
+      <c r="C68" s="3">
+        <v>3333333.3333333302</v>
+      </c>
+      <c r="D68" s="3">
+        <v>-2400000</v>
+      </c>
+      <c r="E68" s="3">
+        <f t="shared" si="42"/>
         <v>0.5880026035475675</v>
       </c>
-      <c r="F68" s="2">
-        <f t="shared" si="51"/>
+      <c r="F68" s="3">
+        <f t="shared" si="43"/>
         <v>33.690067525979785</v>
       </c>
-      <c r="G68" s="2">
-        <f t="shared" si="52"/>
-        <v>-350</v>
-      </c>
-      <c r="H68" s="2">
-        <f t="shared" si="53"/>
-        <v>130</v>
-      </c>
-      <c r="I68" s="2">
-        <f t="shared" si="54"/>
-        <v>-220</v>
-      </c>
-      <c r="J68" s="2">
-        <f t="shared" si="55"/>
-        <v>-480</v>
-      </c>
-      <c r="K68" s="2">
+      <c r="G68" s="3">
+        <f t="shared" si="44"/>
+        <v>4333333.3333333302</v>
+      </c>
+      <c r="H68" s="3">
+        <f t="shared" si="45"/>
+        <v>2600000</v>
+      </c>
+      <c r="I68" s="3">
+        <f t="shared" si="46"/>
+        <v>6933333.3333333302</v>
+      </c>
+      <c r="J68" s="3">
+        <f t="shared" si="47"/>
+        <v>1733333.3333333302</v>
+      </c>
+      <c r="K68" s="3">
         <f t="shared" si="48"/>
         <v>78.690067525979785</v>
       </c>
-      <c r="L68" s="2">
+      <c r="L68" s="3">
         <f t="shared" si="49"/>
         <v>-11.309932474020215</v>
       </c>
+      <c r="M68" s="3"/>
     </row>
     <row r="69" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A69" s="1">
-        <v>10</v>
-      </c>
-      <c r="B69" s="2">
-        <v>-150</v>
-      </c>
-      <c r="C69" s="2">
-        <v>120</v>
-      </c>
-      <c r="D69" s="2">
-        <v>80</v>
-      </c>
-      <c r="E69" s="2">
-        <f t="shared" si="50"/>
-        <v>0.26747753689304821</v>
-      </c>
-      <c r="F69" s="2">
-        <f t="shared" si="51"/>
-        <v>15.325333978526434</v>
-      </c>
-      <c r="G69" s="2">
-        <f t="shared" si="52"/>
-        <v>-15</v>
-      </c>
-      <c r="H69" s="2">
-        <f t="shared" si="53"/>
-        <v>156.92354826475216</v>
-      </c>
-      <c r="I69" s="2">
-        <f t="shared" si="54"/>
-        <v>141.92354826475216</v>
-      </c>
-      <c r="J69" s="2">
-        <f t="shared" si="55"/>
-        <v>-171.92354826475216</v>
-      </c>
-      <c r="K69" s="2">
+        <v>3</v>
+      </c>
+      <c r="B69" s="3">
+        <v>532</v>
+      </c>
+      <c r="C69" s="3">
+        <v>740</v>
+      </c>
+      <c r="D69" s="3">
+        <v>345</v>
+      </c>
+      <c r="E69" s="3">
+        <f t="shared" si="42"/>
+        <v>0.6390052264115833</v>
+      </c>
+      <c r="F69" s="3">
+        <f t="shared" si="43"/>
+        <v>36.612302560185327</v>
+      </c>
+      <c r="G69" s="3">
+        <f t="shared" si="44"/>
+        <v>636</v>
+      </c>
+      <c r="H69" s="3">
+        <f t="shared" si="45"/>
+        <v>360.33456675706259</v>
+      </c>
+      <c r="I69" s="3">
+        <f t="shared" si="46"/>
+        <v>996.33456675706259</v>
+      </c>
+      <c r="J69" s="3">
+        <f t="shared" si="47"/>
+        <v>275.66543324293741</v>
+      </c>
+      <c r="K69" s="3">
         <f t="shared" si="48"/>
-        <v>60.32533397852643</v>
-      </c>
-      <c r="L69" s="2">
+        <v>81.612302560185327</v>
+      </c>
+      <c r="L69" s="3">
         <f t="shared" si="49"/>
-        <v>-29.67466602147357</v>
-      </c>
+        <v>-8.3876974398146729</v>
+      </c>
+      <c r="M69" s="3"/>
     </row>
     <row r="70" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A70" s="1">
-        <v>11</v>
-      </c>
-      <c r="B70" s="2">
-        <v>265</v>
-      </c>
-      <c r="C70" s="2">
-        <v>128</v>
-      </c>
-      <c r="D70" s="2">
-        <v>95</v>
-      </c>
-      <c r="E70" s="2">
-        <f t="shared" si="50"/>
-        <v>-0.47304018463635611</v>
-      </c>
-      <c r="F70" s="2">
-        <f t="shared" si="51"/>
-        <v>-27.103206119752414</v>
-      </c>
-      <c r="G70" s="2">
-        <f t="shared" si="52"/>
-        <v>196.5</v>
-      </c>
-      <c r="H70" s="2">
-        <f t="shared" si="53"/>
-        <v>117.1206642740725</v>
-      </c>
-      <c r="I70" s="2">
-        <f t="shared" si="54"/>
-        <v>313.62066427407251</v>
-      </c>
-      <c r="J70" s="2">
-        <f t="shared" si="55"/>
-        <v>79.379335725927504</v>
-      </c>
-      <c r="K70" s="2">
+        <v>4</v>
+      </c>
+      <c r="B70" s="3">
+        <v>300</v>
+      </c>
+      <c r="C70" s="3">
+        <v>150</v>
+      </c>
+      <c r="D70" s="3">
+        <v>200</v>
+      </c>
+      <c r="E70" s="3">
+        <f t="shared" si="42"/>
+        <v>-0.60601282826216218</v>
+      </c>
+      <c r="F70" s="3">
+        <f t="shared" si="43"/>
+        <v>-34.721977390208266</v>
+      </c>
+      <c r="G70" s="3">
+        <f t="shared" si="44"/>
+        <v>225</v>
+      </c>
+      <c r="H70" s="3">
+        <f t="shared" si="45"/>
+        <v>213.60009363293827</v>
+      </c>
+      <c r="I70" s="3">
+        <f t="shared" si="46"/>
+        <v>438.6000936329383</v>
+      </c>
+      <c r="J70" s="3">
+        <f t="shared" si="47"/>
+        <v>11.399906367061732</v>
+      </c>
+      <c r="K70" s="3">
         <f t="shared" si="48"/>
-        <v>17.896793880247586</v>
-      </c>
-      <c r="L70" s="2">
+        <v>10.278022609791734</v>
+      </c>
+      <c r="L70" s="3">
         <f t="shared" si="49"/>
-        <v>-72.103206119752414</v>
-      </c>
+        <v>-79.721977390208266</v>
+      </c>
+      <c r="M70" s="3"/>
     </row>
     <row r="71" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A71" s="1">
-        <v>12</v>
-      </c>
-      <c r="B71" s="2">
-        <v>132</v>
-      </c>
-      <c r="C71" s="2">
-        <v>-387</v>
-      </c>
-      <c r="D71" s="2">
-        <v>-765</v>
-      </c>
-      <c r="E71" s="2">
-        <f t="shared" si="50"/>
-        <v>0.62188051502639119</v>
-      </c>
-      <c r="F71" s="2">
-        <f t="shared" si="51"/>
-        <v>35.631128872434189</v>
-      </c>
-      <c r="G71" s="2">
-        <f t="shared" si="52"/>
-        <v>-127.5</v>
-      </c>
-      <c r="H71" s="2">
-        <f t="shared" si="53"/>
-        <v>807.81510879656116</v>
-      </c>
-      <c r="I71" s="2">
-        <f t="shared" si="54"/>
-        <v>680.31510879656116</v>
-      </c>
-      <c r="J71" s="2">
-        <f t="shared" si="55"/>
-        <v>-935.31510879656116</v>
-      </c>
-      <c r="K71" s="2">
+        <v>5</v>
+      </c>
+      <c r="B71" s="3">
+        <v>50</v>
+      </c>
+      <c r="C71" s="3">
+        <v>-10</v>
+      </c>
+      <c r="D71" s="3">
+        <v>40</v>
+      </c>
+      <c r="E71" s="3">
+        <f t="shared" si="42"/>
+        <v>-0.46364760900080609</v>
+      </c>
+      <c r="F71" s="3">
+        <f t="shared" si="43"/>
+        <v>-26.56505117707799</v>
+      </c>
+      <c r="G71" s="3">
+        <f t="shared" si="44"/>
+        <v>20</v>
+      </c>
+      <c r="H71" s="3">
+        <f t="shared" si="45"/>
+        <v>50</v>
+      </c>
+      <c r="I71" s="3">
+        <f t="shared" si="46"/>
+        <v>70</v>
+      </c>
+      <c r="J71" s="3">
+        <f t="shared" si="47"/>
+        <v>-30</v>
+      </c>
+      <c r="K71" s="3">
         <f t="shared" si="48"/>
-        <v>80.631128872434189</v>
-      </c>
-      <c r="L71" s="2">
+        <v>18.43494882292201</v>
+      </c>
+      <c r="L71" s="3">
         <f t="shared" si="49"/>
-        <v>-9.3688711275658108</v>
-      </c>
+        <v>-71.56505117707799</v>
+      </c>
+      <c r="M71" s="3"/>
     </row>
     <row r="72" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A72" s="1">
+        <v>6</v>
+      </c>
+      <c r="B72" s="3">
+        <v>800</v>
+      </c>
+      <c r="C72" s="3">
+        <v>400</v>
+      </c>
+      <c r="D72" s="3">
+        <v>-550</v>
+      </c>
+      <c r="E72" s="3">
+        <f t="shared" si="42"/>
+        <v>0.61101266160549483</v>
+      </c>
+      <c r="F72" s="3">
+        <f t="shared" si="43"/>
+        <v>35.008446739050015</v>
+      </c>
+      <c r="G72" s="3">
+        <f t="shared" si="44"/>
+        <v>600</v>
+      </c>
+      <c r="H72" s="3">
+        <f t="shared" si="45"/>
+        <v>585.23499553598128</v>
+      </c>
+      <c r="I72" s="3">
+        <f t="shared" si="46"/>
+        <v>1185.2349955359814</v>
+      </c>
+      <c r="J72" s="3">
+        <f t="shared" si="47"/>
+        <v>14.765004464018716</v>
+      </c>
+      <c r="K72" s="3">
+        <f t="shared" ref="K72:K79" si="50">F72+45</f>
+        <v>80.008446739050015</v>
+      </c>
+      <c r="L72" s="3">
+        <f t="shared" ref="L72:L79" si="51">K72-90</f>
+        <v>-9.9915532609499849</v>
+      </c>
+      <c r="M72" s="3"/>
+    </row>
+    <row r="73" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A73" s="1">
+        <v>7</v>
+      </c>
+      <c r="B73" s="3">
+        <f>K43</f>
+        <v>30.864197530864196</v>
+      </c>
+      <c r="C73" s="3">
+        <v>0</v>
+      </c>
+      <c r="D73" s="3">
+        <f>I43</f>
+        <v>3.9609053497942388</v>
+      </c>
+      <c r="E73" s="3">
+        <f t="shared" si="42"/>
+        <v>-0.12562163201205953</v>
+      </c>
+      <c r="F73" s="3">
+        <f t="shared" si="43"/>
+        <v>-7.1975893298365268</v>
+      </c>
+      <c r="G73" s="3">
+        <f t="shared" si="44"/>
+        <v>15.432098765432098</v>
+      </c>
+      <c r="H73" s="3">
+        <f t="shared" si="45"/>
+        <v>15.932308165990248</v>
+      </c>
+      <c r="I73" s="3">
+        <f t="shared" si="46"/>
+        <v>31.364406931422344</v>
+      </c>
+      <c r="J73" s="3">
+        <f t="shared" si="47"/>
+        <v>-0.50020940055815011</v>
+      </c>
+      <c r="K73" s="3">
+        <f t="shared" si="50"/>
+        <v>37.802410670163475</v>
+      </c>
+      <c r="L73" s="3">
+        <f t="shared" si="51"/>
+        <v>-52.197589329836525</v>
+      </c>
+      <c r="M73" s="3">
+        <f>L73*2</f>
+        <v>-104.39517865967305</v>
+      </c>
+    </row>
+    <row r="74" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A74" s="1">
+        <v>8</v>
+      </c>
+      <c r="B74" s="3">
+        <v>-150</v>
+      </c>
+      <c r="C74" s="3">
+        <v>352</v>
+      </c>
+      <c r="D74" s="3">
+        <v>-24</v>
+      </c>
+      <c r="E74" s="3">
+        <f t="shared" ref="E74:E78" si="52">ATAN(-2*D74/(B74-C74))/2</f>
+        <v>-4.7663858426665248E-2</v>
+      </c>
+      <c r="F74" s="3">
+        <f t="shared" ref="F74:F78" si="53">E74*180/PI()</f>
+        <v>-2.7309379231569828</v>
+      </c>
+      <c r="G74" s="3">
+        <f t="shared" ref="G74:G78" si="54">(B74+C74)/2</f>
+        <v>101</v>
+      </c>
+      <c r="H74" s="3">
+        <f t="shared" ref="H74:H78" si="55">SQRT((B74-C74)^2/4+D74^2)</f>
+        <v>252.14479966876175</v>
+      </c>
+      <c r="I74" s="3">
+        <f t="shared" ref="I74:I78" si="56">G74+H74</f>
+        <v>353.14479966876172</v>
+      </c>
+      <c r="J74" s="3">
+        <f t="shared" ref="J74:J78" si="57">G74-H74</f>
+        <v>-151.14479966876175</v>
+      </c>
+      <c r="K74" s="3">
+        <f t="shared" si="50"/>
+        <v>42.269062076843014</v>
+      </c>
+      <c r="L74" s="3">
+        <f t="shared" si="51"/>
+        <v>-47.730937923156986</v>
+      </c>
+      <c r="M74" s="3">
+        <f>L74*2</f>
+        <v>-95.461875846313973</v>
+      </c>
+    </row>
+    <row r="75" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A75" s="1">
+        <v>9</v>
+      </c>
+      <c r="B75" s="3">
+        <v>-400</v>
+      </c>
+      <c r="C75" s="3">
+        <v>-300</v>
+      </c>
+      <c r="D75" s="3">
+        <v>120</v>
+      </c>
+      <c r="E75" s="3">
+        <f t="shared" si="52"/>
+        <v>0.5880026035475675</v>
+      </c>
+      <c r="F75" s="3">
+        <f t="shared" si="53"/>
+        <v>33.690067525979785</v>
+      </c>
+      <c r="G75" s="3">
+        <f t="shared" si="54"/>
+        <v>-350</v>
+      </c>
+      <c r="H75" s="3">
+        <f t="shared" si="55"/>
+        <v>130</v>
+      </c>
+      <c r="I75" s="3">
+        <f t="shared" si="56"/>
+        <v>-220</v>
+      </c>
+      <c r="J75" s="3">
+        <f t="shared" si="57"/>
+        <v>-480</v>
+      </c>
+      <c r="K75" s="3">
+        <f t="shared" si="50"/>
+        <v>78.690067525979785</v>
+      </c>
+      <c r="L75" s="3">
+        <f t="shared" si="51"/>
+        <v>-11.309932474020215</v>
+      </c>
+      <c r="M75" s="3"/>
+    </row>
+    <row r="76" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A76" s="1">
+        <v>10</v>
+      </c>
+      <c r="B76" s="3">
+        <v>-150</v>
+      </c>
+      <c r="C76" s="3">
+        <v>120</v>
+      </c>
+      <c r="D76" s="3">
+        <v>80</v>
+      </c>
+      <c r="E76" s="3">
+        <f t="shared" si="52"/>
+        <v>0.26747753689304821</v>
+      </c>
+      <c r="F76" s="3">
+        <f t="shared" si="53"/>
+        <v>15.325333978526434</v>
+      </c>
+      <c r="G76" s="3">
+        <f t="shared" si="54"/>
+        <v>-15</v>
+      </c>
+      <c r="H76" s="3">
+        <f t="shared" si="55"/>
+        <v>156.92354826475216</v>
+      </c>
+      <c r="I76" s="3">
+        <f t="shared" si="56"/>
+        <v>141.92354826475216</v>
+      </c>
+      <c r="J76" s="3">
+        <f t="shared" si="57"/>
+        <v>-171.92354826475216</v>
+      </c>
+      <c r="K76" s="3">
+        <f t="shared" si="50"/>
+        <v>60.32533397852643</v>
+      </c>
+      <c r="L76" s="3">
+        <f t="shared" si="51"/>
+        <v>-29.67466602147357</v>
+      </c>
+      <c r="M76" s="3"/>
+    </row>
+    <row r="77" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A77" s="1">
+        <v>11</v>
+      </c>
+      <c r="B77" s="3">
+        <v>265</v>
+      </c>
+      <c r="C77" s="3">
+        <v>128</v>
+      </c>
+      <c r="D77" s="3">
+        <v>95</v>
+      </c>
+      <c r="E77" s="3">
+        <f t="shared" si="52"/>
+        <v>-0.47304018463635611</v>
+      </c>
+      <c r="F77" s="3">
+        <f t="shared" si="53"/>
+        <v>-27.103206119752414</v>
+      </c>
+      <c r="G77" s="3">
+        <f t="shared" si="54"/>
+        <v>196.5</v>
+      </c>
+      <c r="H77" s="3">
+        <f t="shared" si="55"/>
+        <v>117.1206642740725</v>
+      </c>
+      <c r="I77" s="3">
+        <f t="shared" si="56"/>
+        <v>313.62066427407251</v>
+      </c>
+      <c r="J77" s="3">
+        <f t="shared" si="57"/>
+        <v>79.379335725927504</v>
+      </c>
+      <c r="K77" s="3">
+        <f t="shared" si="50"/>
+        <v>17.896793880247586</v>
+      </c>
+      <c r="L77" s="3">
+        <f t="shared" si="51"/>
+        <v>-72.103206119752414</v>
+      </c>
+      <c r="M77" s="3"/>
+    </row>
+    <row r="78" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A78" s="1">
+        <v>12</v>
+      </c>
+      <c r="B78" s="3">
+        <v>132</v>
+      </c>
+      <c r="C78" s="3">
+        <v>-387</v>
+      </c>
+      <c r="D78" s="3">
+        <v>-765</v>
+      </c>
+      <c r="E78" s="3">
+        <f t="shared" si="52"/>
+        <v>0.62188051502639119</v>
+      </c>
+      <c r="F78" s="3">
+        <f t="shared" si="53"/>
+        <v>35.631128872434189</v>
+      </c>
+      <c r="G78" s="3">
+        <f t="shared" si="54"/>
+        <v>-127.5</v>
+      </c>
+      <c r="H78" s="3">
+        <f t="shared" si="55"/>
+        <v>807.81510879656116</v>
+      </c>
+      <c r="I78" s="3">
+        <f t="shared" si="56"/>
+        <v>680.31510879656116</v>
+      </c>
+      <c r="J78" s="3">
+        <f t="shared" si="57"/>
+        <v>-935.31510879656116</v>
+      </c>
+      <c r="K78" s="3">
+        <f t="shared" si="50"/>
+        <v>80.631128872434189</v>
+      </c>
+      <c r="L78" s="3">
+        <f t="shared" si="51"/>
+        <v>-9.3688711275658108</v>
+      </c>
+      <c r="M78" s="3"/>
+    </row>
+    <row r="79" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A79" s="1">
         <v>13</v>
       </c>
-      <c r="B72" s="2">
-        <f>K55</f>
+      <c r="B79" s="3">
+        <f>K59</f>
         <v>48.611111111111107</v>
       </c>
-      <c r="C72" s="2">
-        <v>0</v>
-      </c>
-      <c r="D72" s="2">
-        <f>I55</f>
+      <c r="C79" s="3">
+        <v>0</v>
+      </c>
+      <c r="D79" s="3">
+        <f>I59</f>
         <v>14.178240740740742</v>
       </c>
-      <c r="E72" s="2">
-        <f t="shared" ref="E72" si="56">ATAN(-2*D72/(B72-C72))/2</f>
+      <c r="E79" s="3">
+        <f t="shared" ref="E79" si="58">ATAN(-2*D79/(B79-C79))/2</f>
         <v>-0.26403722421317988</v>
       </c>
-      <c r="F72" s="2">
-        <f t="shared" ref="F72" si="57">E72*180/PI()</f>
+      <c r="F79" s="3">
+        <f t="shared" ref="F79" si="59">E79*180/PI()</f>
         <v>-15.128218581764637</v>
       </c>
-      <c r="G72" s="2">
-        <f t="shared" ref="G72" si="58">(B72+C72)/2</f>
+      <c r="G79" s="3">
+        <f t="shared" ref="G79" si="60">(B79+C79)/2</f>
         <v>24.305555555555554</v>
       </c>
-      <c r="H72" s="2">
-        <f t="shared" ref="H72" si="59">SQRT((B72-C72)^2/4+D72^2)</f>
+      <c r="H79" s="3">
+        <f t="shared" ref="H79" si="61">SQRT((B79-C79)^2/4+D79^2)</f>
         <v>28.138630765668005</v>
       </c>
-      <c r="I72" s="2">
-        <f t="shared" ref="I72" si="60">G72+H72</f>
+      <c r="I79" s="3">
+        <f t="shared" ref="I79" si="62">G79+H79</f>
         <v>52.444186321223555</v>
       </c>
-      <c r="J72" s="2">
-        <f t="shared" ref="J72" si="61">G72-H72</f>
+      <c r="J79" s="3">
+        <f t="shared" ref="J79" si="63">G79-H79</f>
         <v>-3.833075210112451</v>
       </c>
-      <c r="K72" s="2">
-        <f t="shared" si="48"/>
+      <c r="K79" s="3">
+        <f t="shared" si="50"/>
         <v>29.871781418235365</v>
       </c>
-      <c r="L72" s="2">
-        <f t="shared" si="49"/>
+      <c r="L79" s="3">
+        <f t="shared" si="51"/>
         <v>-60.128218581764635</v>
       </c>
-    </row>
-    <row r="75" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="B75" s="2" t="s">
+      <c r="M79" s="3"/>
+    </row>
+    <row r="80" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B80" s="3"/>
+      <c r="C80" s="3"/>
+      <c r="D80" s="3"/>
+      <c r="E80" s="3"/>
+      <c r="F80" s="3"/>
+      <c r="G80" s="3"/>
+      <c r="H80" s="3"/>
+      <c r="I80" s="3"/>
+      <c r="J80" s="3"/>
+      <c r="K80" s="3"/>
+      <c r="L80" s="3"/>
+      <c r="M80" s="3"/>
+    </row>
+    <row r="82" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B82" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="C75" s="2" t="s">
+      <c r="C82" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="D75" s="2" t="s">
+      <c r="D82" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="E75" s="2" t="s">
+      <c r="E82" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="F75" s="2" t="s">
+      <c r="F82" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="G75" s="2" t="s">
+      <c r="G82" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="H75" s="2" t="s">
+      <c r="H82" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="I75" s="2" t="s">
+      <c r="I82" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="J75" s="2" t="s">
+      <c r="J82" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="K75" s="2" t="s">
+      <c r="K82" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="L75" s="2" t="s">
+      <c r="L82" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="M75" s="2" t="s">
+      <c r="M82" s="2" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="76" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A76" s="1" t="s">
+    <row r="83" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A83" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="B76" s="2">
+      <c r="B83" s="2">
         <v>2000</v>
       </c>
-      <c r="C76" s="2">
+      <c r="C83" s="2">
         <v>50</v>
       </c>
-      <c r="D76" s="2">
+      <c r="D83" s="2">
         <v>30</v>
       </c>
-      <c r="E76" s="2">
+      <c r="E83" s="2">
         <v>0.3</v>
       </c>
-      <c r="F76" s="2">
-        <f>PI()*(D76/2)^2</f>
+      <c r="F83" s="2">
+        <f>PI()*(D83/2)^2</f>
         <v>706.85834705770344</v>
       </c>
-      <c r="G76" s="2">
+      <c r="G83" s="2">
         <f>3600*1000</f>
         <v>3600000</v>
       </c>
-      <c r="H76" s="2">
-        <f>G76/F76</f>
+      <c r="H83" s="2">
+        <f>G83/F83</f>
         <v>5092.9581789406511</v>
       </c>
-      <c r="I76" s="2">
-        <f>C76/B76</f>
+      <c r="I83" s="2">
+        <f>C83/B83</f>
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="J76" s="2">
-        <f>H76/I76</f>
+      <c r="J83" s="2">
+        <f>H83/I83</f>
         <v>203718.32715762604</v>
       </c>
-      <c r="K76" s="2">
-        <f>E76/D76</f>
+      <c r="K83" s="2">
+        <f>E83/D83</f>
         <v>0.01</v>
       </c>
-      <c r="L76" s="2">
-        <f>K76/I76</f>
+      <c r="L83" s="2">
+        <f>K83/I83</f>
         <v>0.39999999999999997</v>
       </c>
-      <c r="M76" s="2">
-        <f>J76/(2*(1+L76))</f>
+      <c r="M83" s="2">
+        <f>J83/(2*(1+L83))</f>
         <v>72756.545413437882</v>
       </c>
     </row>
-    <row r="79" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="B79" s="2" t="s">
+    <row r="86" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B86" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="C79" s="2" t="s">
+      <c r="C86" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="D79" s="2" t="s">
+      <c r="D86" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="E79" s="2" t="s">
+      <c r="E86" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="F79" s="2" t="s">
+      <c r="F86" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="G79" s="2" t="s">
+      <c r="G86" s="2" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="80" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A80" s="1" t="s">
+    <row r="87" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A87" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="B80" s="2">
+      <c r="B87" s="2">
         <v>50</v>
       </c>
-      <c r="C80" s="2">
-        <f>PI()*(B80/2)^2</f>
+      <c r="C87" s="2">
+        <f>PI()*(B87/2)^2</f>
         <v>1963.4954084936207</v>
       </c>
-      <c r="D80" s="2">
+      <c r="D87" s="2">
         <v>205000</v>
       </c>
-      <c r="E80" s="2">
+      <c r="E87" s="2">
         <f>390*1000</f>
         <v>390000</v>
       </c>
-      <c r="F80" s="2">
+      <c r="F87" s="2">
         <v>1300</v>
       </c>
-      <c r="G80" s="2">
-        <f>E80*F80/C80/D80</f>
+      <c r="G87" s="2">
+        <f>E87*F87/C87/D87</f>
         <v>1.2595755105965414</v>
       </c>
     </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A81" s="1" t="s">
+    <row r="88" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A88" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="C81" s="2">
+      <c r="C88" s="2">
         <v>1000</v>
       </c>
-      <c r="D81" s="2">
+      <c r="D88" s="2">
         <v>200000</v>
       </c>
-      <c r="E81" s="2">
+      <c r="E88" s="2">
         <f>200*1000</f>
         <v>200000</v>
       </c>
-      <c r="F81" s="2">
+      <c r="F88" s="2">
         <v>1000</v>
       </c>
-      <c r="G81" s="2">
-        <f>E81*F81/C81/D81</f>
+      <c r="G88" s="2">
+        <f>E88*F88/C88/D88</f>
         <v>1</v>
       </c>
     </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="C82" s="2">
+    <row r="89" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="C89" s="2">
         <v>2000</v>
       </c>
-      <c r="D82" s="2">
+      <c r="D89" s="2">
         <v>27000</v>
       </c>
-      <c r="E82" s="2">
+      <c r="E89" s="2">
         <f>250*1000</f>
         <v>250000</v>
       </c>
-      <c r="F82" s="2">
+      <c r="F89" s="2">
         <v>2000</v>
       </c>
-      <c r="G82" s="2">
-        <f>E82*F82/C82/D82</f>
+      <c r="G89" s="2">
+        <f>E89*F89/C89/D89</f>
         <v>9.2592592592592595</v>
       </c>
     </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B83" s="2">
+    <row r="90" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B90" s="2">
         <v>500</v>
       </c>
-      <c r="C83" s="2">
-        <f>B83^2</f>
+      <c r="C90" s="2">
+        <f>B90^2</f>
         <v>250000</v>
       </c>
-      <c r="D83" s="2">
+      <c r="D90" s="2">
         <v>28500</v>
       </c>
-      <c r="E83" s="2">
+      <c r="E90" s="2">
         <f>7800*1000</f>
         <v>7800000</v>
       </c>
-      <c r="F83" s="2">
+      <c r="F90" s="2">
         <v>2400</v>
       </c>
-      <c r="G83" s="2">
-        <f>E83*F83/C83/D83</f>
+      <c r="G90" s="2">
+        <f>E90*F90/C90/D90</f>
         <v>2.6273684210526316</v>
       </c>
-      <c r="I83" s="2">
+      <c r="I90" s="2">
         <f>ATAN(0.2)*180/PI()/2</f>
         <v>5.6549662370101066</v>
       </c>
     </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B84" s="2">
+    <row r="91" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B91" s="2">
         <v>550</v>
       </c>
-      <c r="C84" s="2">
-        <f>B84^2</f>
+      <c r="C91" s="2">
+        <f>B91^2</f>
         <v>302500</v>
       </c>
-      <c r="D84" s="2">
+      <c r="D91" s="2">
         <v>28500</v>
       </c>
-      <c r="E84" s="2">
+      <c r="E91" s="2">
         <f>7800*1000</f>
         <v>7800000</v>
       </c>
-      <c r="F84" s="2">
+      <c r="F91" s="2">
         <v>2400</v>
       </c>
-      <c r="G84" s="2">
-        <f>E84*F84/C84/D84</f>
+      <c r="G91" s="2">
+        <f>E91*F91/C91/D91</f>
         <v>2.1713788603740758</v>
       </c>
     </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B85" s="2">
-        <f>SQRT(C85)</f>
+    <row r="92" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B92" s="2">
+        <f>SQRT(C92)</f>
         <v>452.0224821005304</v>
       </c>
-      <c r="C85" s="2">
-        <f>E85*F85/D85/G85</f>
+      <c r="C92" s="2">
+        <f>E92*F92/D92/G92</f>
         <v>204324.32432432432</v>
       </c>
-      <c r="D85" s="2">
+      <c r="D92" s="2">
         <v>37000</v>
       </c>
-      <c r="E85" s="2">
+      <c r="E92" s="2">
         <f>3600*1000</f>
         <v>3600000</v>
       </c>
-      <c r="F85" s="2">
+      <c r="F92" s="2">
         <v>2100</v>
       </c>
-      <c r="G85" s="2">
+      <c r="G92" s="2">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
2018.03.29 error of stress and strain
</commit_message>
<xml_diff>
--- a/quiz_calc.xlsx
+++ b/quiz_calc.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17830"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive - 경남대학교\GitHub\structural_mechanics_II\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F4B71AA-B9C7-445E-A20F-AF02A5F0D751}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="11610"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="11610" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="171027" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -285,7 +286,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="6">
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="176" formatCode="0_ ;[Red]\-0\ "/>
@@ -677,11 +678,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P92"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L79" sqref="L79"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H44" sqref="H44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1429,11 +1430,11 @@
         <v>240000</v>
       </c>
       <c r="E16" s="2">
-        <f>B16/2</f>
+        <f t="shared" ref="E16:F19" si="8">B16/2</f>
         <v>200</v>
       </c>
       <c r="F16" s="2">
-        <f>C16/2</f>
+        <f t="shared" si="8"/>
         <v>300</v>
       </c>
       <c r="G16" s="2">
@@ -1459,7 +1460,7 @@
         <v>3200000000</v>
       </c>
       <c r="M16" s="2">
-        <f t="shared" ref="M16" si="8">SUM(K16:L16)</f>
+        <f t="shared" ref="M16" si="9">SUM(K16:L16)</f>
         <v>10400000000</v>
       </c>
       <c r="N16" s="4">
@@ -1483,11 +1484,11 @@
         <v>300</v>
       </c>
       <c r="E17" s="2">
-        <f>B17/2</f>
+        <f t="shared" si="8"/>
         <v>7.5</v>
       </c>
       <c r="F17" s="2">
-        <f>C17/2</f>
+        <f t="shared" si="8"/>
         <v>10</v>
       </c>
       <c r="G17" s="2">
@@ -1513,7 +1514,7 @@
         <v>5625</v>
       </c>
       <c r="M17" s="2">
-        <f t="shared" ref="M17" si="9">SUM(K17:L17)</f>
+        <f t="shared" ref="M17" si="10">SUM(K17:L17)</f>
         <v>135625</v>
       </c>
       <c r="N17" s="4">
@@ -1537,11 +1538,11 @@
         <v>2000</v>
       </c>
       <c r="E18" s="2">
-        <f>B18/2</f>
+        <f t="shared" si="8"/>
         <v>50</v>
       </c>
       <c r="F18" s="2">
-        <f>C18/2</f>
+        <f t="shared" si="8"/>
         <v>10</v>
       </c>
       <c r="G18" s="2">
@@ -1568,7 +1569,7 @@
         <v>1666666.6666666667</v>
       </c>
       <c r="M18" s="2">
-        <f t="shared" ref="M18" si="10">SUM(K18:L18)</f>
+        <f t="shared" ref="M18" si="11">SUM(K18:L18)</f>
         <v>3111458.3333333335</v>
       </c>
       <c r="N18" s="4">
@@ -1592,11 +1593,11 @@
         <v>1200</v>
       </c>
       <c r="E19" s="2">
-        <f>B19/2</f>
+        <f t="shared" si="8"/>
         <v>5</v>
       </c>
       <c r="F19" s="2">
-        <f>C19/2</f>
+        <f t="shared" si="8"/>
         <v>60</v>
       </c>
       <c r="G19" s="2">
@@ -1623,7 +1624,7 @@
         <v>10000</v>
       </c>
       <c r="M19" s="2">
-        <f t="shared" ref="M19:M20" si="11">SUM(K19:L19)</f>
+        <f t="shared" ref="M19" si="12">SUM(K19:L19)</f>
         <v>3746875</v>
       </c>
       <c r="N19" s="4">
@@ -1900,7 +1901,7 @@
         <v>25</v>
       </c>
       <c r="E35" s="2">
-        <f t="shared" ref="E35:E43" si="12">C35/2-D35</f>
+        <f t="shared" ref="E35:E43" si="13">C35/2-D35</f>
         <v>100</v>
       </c>
       <c r="F35" s="2">
@@ -1912,7 +1913,7 @@
         <v>351562.5</v>
       </c>
       <c r="H35" s="2">
-        <f t="shared" ref="H35:H43" si="13">B35*C35^3/12</f>
+        <f t="shared" ref="H35:H43" si="14">B35*C35^3/12</f>
         <v>162760416.66666666</v>
       </c>
       <c r="I35" s="2">
@@ -1945,7 +1946,7 @@
         <v>125</v>
       </c>
       <c r="E36" s="2">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="F36" s="2">
@@ -1957,7 +1958,7 @@
         <v>976562.5</v>
       </c>
       <c r="H36" s="2">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>162760416.66666666</v>
       </c>
       <c r="I36" s="2">
@@ -1965,11 +1966,11 @@
         <v>57.6</v>
       </c>
       <c r="J36" s="5">
-        <f t="shared" ref="J36:J37" si="14">250000000</f>
+        <f t="shared" ref="J36:J37" si="15">250000000</f>
         <v>250000000</v>
       </c>
       <c r="K36" s="3">
-        <f t="shared" ref="K36:K37" si="15">J36/H36*E36</f>
+        <f t="shared" ref="K36:K37" si="16">J36/H36*E36</f>
         <v>0</v>
       </c>
     </row>
@@ -1989,7 +1990,7 @@
         <v>0</v>
       </c>
       <c r="E37" s="2">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>125</v>
       </c>
       <c r="F37" s="2">
@@ -2001,7 +2002,7 @@
         <v>0</v>
       </c>
       <c r="H37" s="2">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>162760416.66666666</v>
       </c>
       <c r="I37" s="2">
@@ -2009,11 +2010,11 @@
         <v>0</v>
       </c>
       <c r="J37" s="5">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>250000000</v>
       </c>
       <c r="K37" s="3">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>192</v>
       </c>
     </row>
@@ -2032,7 +2033,7 @@
         <v>60</v>
       </c>
       <c r="E38" s="2">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="F38" s="2">
@@ -2044,7 +2045,7 @@
         <v>90000</v>
       </c>
       <c r="H38" s="2">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>7200000</v>
       </c>
       <c r="I38" s="2">
@@ -2068,7 +2069,7 @@
         <v>300</v>
       </c>
       <c r="E39" s="2">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="F39" s="2">
@@ -2079,7 +2080,7 @@
         <v>18000000</v>
       </c>
       <c r="H39" s="2">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>7200000000</v>
       </c>
       <c r="I39" s="2">
@@ -2103,11 +2104,11 @@
         <v>0</v>
       </c>
       <c r="E40" s="2">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>300</v>
       </c>
       <c r="H40" s="2">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>7200000000</v>
       </c>
       <c r="J40" s="5">
@@ -2115,7 +2116,7 @@
         <v>750000000</v>
       </c>
       <c r="K40" s="3">
-        <f t="shared" ref="K40" si="16">J40/H40*E40</f>
+        <f t="shared" ref="K40" si="17">J40/H40*E40</f>
         <v>31.25</v>
       </c>
     </row>
@@ -2133,7 +2134,7 @@
         <v>250</v>
       </c>
       <c r="E41" s="2">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="F41" s="2">
@@ -2144,7 +2145,7 @@
         <v>9375000</v>
       </c>
       <c r="H41" s="2">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>3125000000</v>
       </c>
       <c r="I41" s="2">
@@ -2168,11 +2169,11 @@
         <v>0</v>
       </c>
       <c r="E42" s="2">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>250</v>
       </c>
       <c r="H42" s="2">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>3125000000</v>
       </c>
       <c r="J42" s="5">
@@ -2180,7 +2181,7 @@
         <v>6000000000</v>
       </c>
       <c r="K42" s="3">
-        <f t="shared" ref="K42:K43" si="17">J42/H42*E42</f>
+        <f t="shared" ref="K42:K43" si="18">J42/H42*E42</f>
         <v>480</v>
       </c>
     </row>
@@ -2199,7 +2200,7 @@
         <v>140</v>
       </c>
       <c r="E43" s="2">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>40</v>
       </c>
       <c r="F43" s="2">
@@ -2211,18 +2212,18 @@
         <v>3696000</v>
       </c>
       <c r="H43" s="2">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>933120000</v>
       </c>
       <c r="I43" s="2">
-        <f t="shared" ref="I43:I52" si="18">F43*G43/H43/B43</f>
+        <f t="shared" ref="I43:I52" si="19">F43*G43/H43/B43</f>
         <v>3.9609053497942388</v>
       </c>
       <c r="J43" s="5">
         <v>720000000</v>
       </c>
       <c r="K43" s="3">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>30.864197530864196</v>
       </c>
     </row>
@@ -2240,7 +2241,7 @@
         <v>250</v>
       </c>
       <c r="E44" s="2">
-        <f t="shared" ref="E44" si="19">C44/2-D44</f>
+        <f t="shared" ref="E44" si="20">C44/2-D44</f>
         <v>0</v>
       </c>
       <c r="F44" s="2">
@@ -2251,11 +2252,11 @@
         <v>9375000</v>
       </c>
       <c r="H44" s="2">
-        <f t="shared" ref="H44" si="20">B44*C44^3/12</f>
+        <f t="shared" ref="H44" si="21">B44*C44^3/12</f>
         <v>3125000000</v>
       </c>
       <c r="I44" s="2">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>7.53</v>
       </c>
       <c r="J44" s="5"/>
@@ -2269,7 +2270,7 @@
         <v>10</v>
       </c>
       <c r="F45" s="2">
-        <v>9265</v>
+        <v>92650</v>
       </c>
       <c r="G45" s="2">
         <f>100*20*70+10*60*30</f>
@@ -2279,9 +2280,9 @@
         <f>100*160^3/12-90*120^3/12</f>
         <v>21173333.333333336</v>
       </c>
-      <c r="I45" s="2">
-        <f t="shared" si="18"/>
-        <v>6.9137437027707804</v>
+      <c r="I45" s="3">
+        <f t="shared" si="19"/>
+        <v>69.137437027707804</v>
       </c>
       <c r="J45" s="5"/>
       <c r="K45" s="3"/>
@@ -2294,7 +2295,7 @@
         <v>10</v>
       </c>
       <c r="F46" s="2">
-        <v>9265</v>
+        <v>92650</v>
       </c>
       <c r="G46" s="2">
         <f>100*20*70+10*30*45</f>
@@ -2304,9 +2305,9 @@
         <f>100*160^3/12-90*120^3/12</f>
         <v>21173333.333333336</v>
       </c>
-      <c r="I46" s="2">
-        <f t="shared" si="18"/>
-        <v>6.7168332808564228</v>
+      <c r="I46" s="3">
+        <f t="shared" si="19"/>
+        <v>67.168332808564216</v>
       </c>
       <c r="J46" s="5"/>
       <c r="K46" s="3"/>
@@ -2325,19 +2326,19 @@
         <v>0</v>
       </c>
       <c r="E47" s="2">
-        <f t="shared" ref="E47" si="21">C47/2-D47</f>
+        <f t="shared" ref="E47" si="22">C47/2-D47</f>
         <v>180</v>
       </c>
       <c r="G47" s="2">
-        <f t="shared" ref="G47:G52" si="22">B47*D47*(E47+D47/2)</f>
+        <f t="shared" ref="G47:G52" si="23">B47*D47*(E47+D47/2)</f>
         <v>0</v>
       </c>
       <c r="H47" s="2">
-        <f t="shared" ref="H47" si="23">B47*C47^3/12</f>
+        <f t="shared" ref="H47" si="24">B47*C47^3/12</f>
         <v>777600000</v>
       </c>
       <c r="I47" s="2">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="J47" s="5">
@@ -2345,7 +2346,7 @@
         <v>350000000</v>
       </c>
       <c r="K47" s="3">
-        <f t="shared" ref="K47" si="24">J47/H47*E47</f>
+        <f t="shared" ref="K47" si="25">J47/H47*E47</f>
         <v>81.018518518518519</v>
       </c>
     </row>
@@ -2364,19 +2365,19 @@
         <v>180</v>
       </c>
       <c r="E48" s="2">
-        <f t="shared" ref="E48:E49" si="25">C48/2-D48</f>
+        <f t="shared" ref="E48:E49" si="26">C48/2-D48</f>
         <v>0</v>
       </c>
       <c r="G48" s="2">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>3240000</v>
       </c>
       <c r="H48" s="2">
-        <f t="shared" ref="H48:H49" si="26">B48*C48^3/12</f>
+        <f t="shared" ref="H48:H49" si="27">B48*C48^3/12</f>
         <v>777600000</v>
       </c>
       <c r="I48" s="2">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="J48" s="5">
@@ -2384,7 +2385,7 @@
         <v>350000000</v>
       </c>
       <c r="K48" s="3">
-        <f t="shared" ref="K48:K49" si="27">J48/H48*E48</f>
+        <f t="shared" ref="K48:K49" si="28">J48/H48*E48</f>
         <v>0</v>
       </c>
     </row>
@@ -2402,19 +2403,19 @@
         <v>0</v>
       </c>
       <c r="E49" s="2">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>110</v>
       </c>
       <c r="G49" s="2">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
       <c r="H49" s="2">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>88733333.333333328</v>
       </c>
       <c r="I49" s="2">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="J49" s="5">
@@ -2422,7 +2423,7 @@
         <v>76300000</v>
       </c>
       <c r="K49" s="3">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>94.586776859504141</v>
       </c>
     </row>
@@ -2440,27 +2441,27 @@
         <v>35</v>
       </c>
       <c r="E50" s="2">
-        <f t="shared" ref="E50:E51" si="28">C50/2-D50</f>
+        <f t="shared" ref="E50:E51" si="29">C50/2-D50</f>
         <v>75</v>
       </c>
       <c r="G50" s="2">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>323750</v>
       </c>
       <c r="H50" s="2">
-        <f t="shared" ref="H50:H51" si="29">B50*C50^3/12</f>
+        <f t="shared" ref="H50:H51" si="30">B50*C50^3/12</f>
         <v>88733333.333333328</v>
       </c>
       <c r="I50" s="2">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="J50" s="5">
-        <f t="shared" ref="J50:J52" si="30">76.3*1000000</f>
+        <f t="shared" ref="J50:J52" si="31">76.3*1000000</f>
         <v>76300000</v>
       </c>
       <c r="K50" s="3">
-        <f t="shared" ref="K50:K51" si="31">J50/H50*E50</f>
+        <f t="shared" ref="K50:K51" si="32">J50/H50*E50</f>
         <v>64.490984222389187</v>
       </c>
     </row>
@@ -2478,27 +2479,27 @@
         <v>60</v>
       </c>
       <c r="E51" s="2">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>50</v>
       </c>
       <c r="G51" s="2">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>480000</v>
       </c>
       <c r="H51" s="2">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>88733333.333333328</v>
       </c>
       <c r="I51" s="2">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="J51" s="5">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v>76300000</v>
       </c>
       <c r="K51" s="3">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>42.993989481592791</v>
       </c>
     </row>
@@ -2516,27 +2517,27 @@
         <v>85</v>
       </c>
       <c r="E52" s="2">
-        <f t="shared" ref="E52" si="32">C52/2-D52</f>
+        <f t="shared" ref="E52" si="33">C52/2-D52</f>
         <v>25</v>
       </c>
       <c r="G52" s="2">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>573750</v>
       </c>
       <c r="H52" s="2">
-        <f t="shared" ref="H52" si="33">B52*C52^3/12</f>
+        <f t="shared" ref="H52" si="34">B52*C52^3/12</f>
         <v>88733333.333333328</v>
       </c>
       <c r="I52" s="2">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="J52" s="5">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v>76300000</v>
       </c>
       <c r="K52" s="3">
-        <f t="shared" ref="K52" si="34">J52/H52*E52</f>
+        <f t="shared" ref="K52" si="35">J52/H52*E52</f>
         <v>21.496994740796396</v>
       </c>
     </row>
@@ -2559,7 +2560,7 @@
         <v>73000000</v>
       </c>
       <c r="K53" s="3">
-        <f t="shared" ref="K53:K54" si="35">J53/H53*E53</f>
+        <f t="shared" ref="K53:K54" si="36">J53/H53*E53</f>
         <v>0</v>
       </c>
     </row>
@@ -2582,7 +2583,7 @@
         <v>73000000</v>
       </c>
       <c r="K54" s="3">
-        <f t="shared" si="35"/>
+        <f t="shared" si="36"/>
         <v>103.43198992443322</v>
       </c>
     </row>
@@ -2605,7 +2606,7 @@
         <v>73000000</v>
       </c>
       <c r="K55" s="3">
-        <f t="shared" ref="K55:K59" si="36">J55/H55*E55</f>
+        <f t="shared" ref="K55:K59" si="37">J55/H55*E55</f>
         <v>206.86397984886645</v>
       </c>
     </row>
@@ -2628,7 +2629,7 @@
         <v>73000000</v>
       </c>
       <c r="K56" s="3">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>275.81863979848862</v>
       </c>
     </row>
@@ -2646,7 +2647,7 @@
         <v>0</v>
       </c>
       <c r="E57" s="2">
-        <f t="shared" ref="E57:E58" si="37">C57/2-D57</f>
+        <f t="shared" ref="E57:E58" si="38">C57/2-D57</f>
         <v>180</v>
       </c>
       <c r="F57" s="2">
@@ -2658,7 +2659,7 @@
         <v>0</v>
       </c>
       <c r="H57" s="2">
-        <f t="shared" ref="H57" si="38">B57*C57^3/12</f>
+        <f t="shared" ref="H57" si="39">B57*C57^3/12</f>
         <v>777600000</v>
       </c>
       <c r="I57" s="3">
@@ -2670,7 +2671,7 @@
         <v>160000000</v>
       </c>
       <c r="K57" s="3">
-        <f t="shared" ref="K57" si="39">J57/H57*E57</f>
+        <f t="shared" ref="K57" si="40">J57/H57*E57</f>
         <v>37.037037037037038</v>
       </c>
     </row>
@@ -2689,7 +2690,7 @@
         <v>180</v>
       </c>
       <c r="E58" s="2">
-        <f t="shared" si="37"/>
+        <f t="shared" si="38"/>
         <v>0</v>
       </c>
       <c r="F58" s="2">
@@ -2701,7 +2702,7 @@
         <v>3240000</v>
       </c>
       <c r="H58" s="2">
-        <f t="shared" ref="H58:H59" si="40">B58*C58^3/12</f>
+        <f t="shared" ref="H58:H59" si="41">B58*C58^3/12</f>
         <v>777600000</v>
       </c>
       <c r="I58" s="3">
@@ -2713,7 +2714,7 @@
         <v>160000000</v>
       </c>
       <c r="K58" s="3">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>0</v>
       </c>
     </row>
@@ -2732,7 +2733,7 @@
         <v>250</v>
       </c>
       <c r="E59" s="2">
-        <f t="shared" ref="E59" si="41">C59/2-D59</f>
+        <f t="shared" ref="E59" si="42">C59/2-D59</f>
         <v>50</v>
       </c>
       <c r="F59" s="2">
@@ -2744,7 +2745,7 @@
         <v>15750000</v>
       </c>
       <c r="H59" s="5">
-        <f t="shared" si="40"/>
+        <f t="shared" si="41"/>
         <v>6480000000</v>
       </c>
       <c r="I59" s="3">
@@ -2756,7 +2757,7 @@
         <v>6300000000</v>
       </c>
       <c r="K59" s="3">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>48.611111111111107</v>
       </c>
     </row>
@@ -2809,35 +2810,35 @@
         <v>-50</v>
       </c>
       <c r="E67" s="3">
-        <f t="shared" ref="E67:E73" si="42">ATAN(-2*D67/(B67-C67))/2</f>
+        <f t="shared" ref="E67:E73" si="43">ATAN(-2*D67/(B67-C67))/2</f>
         <v>9.8697779924940388E-2</v>
       </c>
       <c r="F67" s="3">
-        <f t="shared" ref="F67:F73" si="43">E67*180/PI()</f>
+        <f t="shared" ref="F67:F73" si="44">E67*180/PI()</f>
         <v>5.6549662370101066</v>
       </c>
       <c r="G67" s="3">
-        <f t="shared" ref="G67:G73" si="44">(B67+C67)/2</f>
+        <f t="shared" ref="G67:G73" si="45">(B67+C67)/2</f>
         <v>750</v>
       </c>
       <c r="H67" s="3">
-        <f t="shared" ref="H67:H73" si="45">SQRT((B67-C67)^2/4+D67^2)</f>
+        <f t="shared" ref="H67:H73" si="46">SQRT((B67-C67)^2/4+D67^2)</f>
         <v>254.95097567963924</v>
       </c>
       <c r="I67" s="3">
-        <f t="shared" ref="I67:I73" si="46">G67+H67</f>
+        <f t="shared" ref="I67:I73" si="47">G67+H67</f>
         <v>1004.9509756796392</v>
       </c>
       <c r="J67" s="3">
-        <f t="shared" ref="J67:J73" si="47">G67-H67</f>
+        <f t="shared" ref="J67:J73" si="48">G67-H67</f>
         <v>495.04902432036079</v>
       </c>
       <c r="K67" s="3">
-        <f t="shared" ref="K67:K71" si="48">F67+45</f>
+        <f t="shared" ref="K67:K71" si="49">F67+45</f>
         <v>50.654966237010107</v>
       </c>
       <c r="L67" s="3">
-        <f t="shared" ref="L67:L71" si="49">K67-90</f>
+        <f t="shared" ref="L67:L71" si="50">K67-90</f>
         <v>-39.345033762989893</v>
       </c>
       <c r="M67" s="3"/>
@@ -2856,35 +2857,35 @@
         <v>-2400000</v>
       </c>
       <c r="E68" s="3">
-        <f t="shared" si="42"/>
+        <f t="shared" si="43"/>
         <v>0.5880026035475675</v>
       </c>
       <c r="F68" s="3">
-        <f t="shared" si="43"/>
+        <f t="shared" si="44"/>
         <v>33.690067525979785</v>
       </c>
       <c r="G68" s="3">
-        <f t="shared" si="44"/>
+        <f t="shared" si="45"/>
         <v>4333333.3333333302</v>
       </c>
       <c r="H68" s="3">
-        <f t="shared" si="45"/>
+        <f t="shared" si="46"/>
         <v>2600000</v>
       </c>
       <c r="I68" s="3">
-        <f t="shared" si="46"/>
+        <f t="shared" si="47"/>
         <v>6933333.3333333302</v>
       </c>
       <c r="J68" s="3">
-        <f t="shared" si="47"/>
+        <f t="shared" si="48"/>
         <v>1733333.3333333302</v>
       </c>
       <c r="K68" s="3">
-        <f t="shared" si="48"/>
+        <f t="shared" si="49"/>
         <v>78.690067525979785</v>
       </c>
       <c r="L68" s="3">
-        <f t="shared" si="49"/>
+        <f t="shared" si="50"/>
         <v>-11.309932474020215</v>
       </c>
       <c r="M68" s="3"/>
@@ -2903,35 +2904,35 @@
         <v>345</v>
       </c>
       <c r="E69" s="3">
-        <f t="shared" si="42"/>
+        <f t="shared" si="43"/>
         <v>0.6390052264115833</v>
       </c>
       <c r="F69" s="3">
-        <f t="shared" si="43"/>
+        <f t="shared" si="44"/>
         <v>36.612302560185327</v>
       </c>
       <c r="G69" s="3">
-        <f t="shared" si="44"/>
+        <f t="shared" si="45"/>
         <v>636</v>
       </c>
       <c r="H69" s="3">
-        <f t="shared" si="45"/>
+        <f t="shared" si="46"/>
         <v>360.33456675706259</v>
       </c>
       <c r="I69" s="3">
-        <f t="shared" si="46"/>
+        <f t="shared" si="47"/>
         <v>996.33456675706259</v>
       </c>
       <c r="J69" s="3">
-        <f t="shared" si="47"/>
+        <f t="shared" si="48"/>
         <v>275.66543324293741</v>
       </c>
       <c r="K69" s="3">
-        <f t="shared" si="48"/>
+        <f t="shared" si="49"/>
         <v>81.612302560185327</v>
       </c>
       <c r="L69" s="3">
-        <f t="shared" si="49"/>
+        <f t="shared" si="50"/>
         <v>-8.3876974398146729</v>
       </c>
       <c r="M69" s="3"/>
@@ -2950,35 +2951,35 @@
         <v>200</v>
       </c>
       <c r="E70" s="3">
-        <f t="shared" si="42"/>
+        <f t="shared" si="43"/>
         <v>-0.60601282826216218</v>
       </c>
       <c r="F70" s="3">
-        <f t="shared" si="43"/>
+        <f t="shared" si="44"/>
         <v>-34.721977390208266</v>
       </c>
       <c r="G70" s="3">
-        <f t="shared" si="44"/>
+        <f t="shared" si="45"/>
         <v>225</v>
       </c>
       <c r="H70" s="3">
-        <f t="shared" si="45"/>
+        <f t="shared" si="46"/>
         <v>213.60009363293827</v>
       </c>
       <c r="I70" s="3">
-        <f t="shared" si="46"/>
+        <f t="shared" si="47"/>
         <v>438.6000936329383</v>
       </c>
       <c r="J70" s="3">
-        <f t="shared" si="47"/>
+        <f t="shared" si="48"/>
         <v>11.399906367061732</v>
       </c>
       <c r="K70" s="3">
-        <f t="shared" si="48"/>
+        <f t="shared" si="49"/>
         <v>10.278022609791734</v>
       </c>
       <c r="L70" s="3">
-        <f t="shared" si="49"/>
+        <f t="shared" si="50"/>
         <v>-79.721977390208266</v>
       </c>
       <c r="M70" s="3"/>
@@ -2997,35 +2998,35 @@
         <v>40</v>
       </c>
       <c r="E71" s="3">
-        <f t="shared" si="42"/>
+        <f t="shared" si="43"/>
         <v>-0.46364760900080609</v>
       </c>
       <c r="F71" s="3">
-        <f t="shared" si="43"/>
+        <f t="shared" si="44"/>
         <v>-26.56505117707799</v>
       </c>
       <c r="G71" s="3">
-        <f t="shared" si="44"/>
+        <f t="shared" si="45"/>
         <v>20</v>
       </c>
       <c r="H71" s="3">
-        <f t="shared" si="45"/>
+        <f t="shared" si="46"/>
         <v>50</v>
       </c>
       <c r="I71" s="3">
-        <f t="shared" si="46"/>
+        <f t="shared" si="47"/>
         <v>70</v>
       </c>
       <c r="J71" s="3">
-        <f t="shared" si="47"/>
+        <f t="shared" si="48"/>
         <v>-30</v>
       </c>
       <c r="K71" s="3">
-        <f t="shared" si="48"/>
+        <f t="shared" si="49"/>
         <v>18.43494882292201</v>
       </c>
       <c r="L71" s="3">
-        <f t="shared" si="49"/>
+        <f t="shared" si="50"/>
         <v>-71.56505117707799</v>
       </c>
       <c r="M71" s="3"/>
@@ -3044,35 +3045,35 @@
         <v>-550</v>
       </c>
       <c r="E72" s="3">
-        <f t="shared" si="42"/>
+        <f t="shared" si="43"/>
         <v>0.61101266160549483</v>
       </c>
       <c r="F72" s="3">
-        <f t="shared" si="43"/>
+        <f t="shared" si="44"/>
         <v>35.008446739050015</v>
       </c>
       <c r="G72" s="3">
-        <f t="shared" si="44"/>
+        <f t="shared" si="45"/>
         <v>600</v>
       </c>
       <c r="H72" s="3">
-        <f t="shared" si="45"/>
+        <f t="shared" si="46"/>
         <v>585.23499553598128</v>
       </c>
       <c r="I72" s="3">
-        <f t="shared" si="46"/>
+        <f t="shared" si="47"/>
         <v>1185.2349955359814</v>
       </c>
       <c r="J72" s="3">
-        <f t="shared" si="47"/>
+        <f t="shared" si="48"/>
         <v>14.765004464018716</v>
       </c>
       <c r="K72" s="3">
-        <f t="shared" ref="K72:K79" si="50">F72+45</f>
+        <f t="shared" ref="K72:K79" si="51">F72+45</f>
         <v>80.008446739050015</v>
       </c>
       <c r="L72" s="3">
-        <f t="shared" ref="L72:L79" si="51">K72-90</f>
+        <f t="shared" ref="L72:L79" si="52">K72-90</f>
         <v>-9.9915532609499849</v>
       </c>
       <c r="M72" s="3"/>
@@ -3093,35 +3094,35 @@
         <v>3.9609053497942388</v>
       </c>
       <c r="E73" s="3">
-        <f t="shared" si="42"/>
+        <f t="shared" si="43"/>
         <v>-0.12562163201205953</v>
       </c>
       <c r="F73" s="3">
-        <f t="shared" si="43"/>
+        <f t="shared" si="44"/>
         <v>-7.1975893298365268</v>
       </c>
       <c r="G73" s="3">
-        <f t="shared" si="44"/>
+        <f t="shared" si="45"/>
         <v>15.432098765432098</v>
       </c>
       <c r="H73" s="3">
-        <f t="shared" si="45"/>
+        <f t="shared" si="46"/>
         <v>15.932308165990248</v>
       </c>
       <c r="I73" s="3">
-        <f t="shared" si="46"/>
+        <f t="shared" si="47"/>
         <v>31.364406931422344</v>
       </c>
       <c r="J73" s="3">
-        <f t="shared" si="47"/>
+        <f t="shared" si="48"/>
         <v>-0.50020940055815011</v>
       </c>
       <c r="K73" s="3">
-        <f t="shared" si="50"/>
+        <f t="shared" si="51"/>
         <v>37.802410670163475</v>
       </c>
       <c r="L73" s="3">
-        <f t="shared" si="51"/>
+        <f t="shared" si="52"/>
         <v>-52.197589329836525</v>
       </c>
       <c r="M73" s="3">
@@ -3143,35 +3144,35 @@
         <v>-24</v>
       </c>
       <c r="E74" s="3">
-        <f t="shared" ref="E74:E78" si="52">ATAN(-2*D74/(B74-C74))/2</f>
+        <f t="shared" ref="E74:E78" si="53">ATAN(-2*D74/(B74-C74))/2</f>
         <v>-4.7663858426665248E-2</v>
       </c>
       <c r="F74" s="3">
-        <f t="shared" ref="F74:F78" si="53">E74*180/PI()</f>
+        <f t="shared" ref="F74:F78" si="54">E74*180/PI()</f>
         <v>-2.7309379231569828</v>
       </c>
       <c r="G74" s="3">
-        <f t="shared" ref="G74:G78" si="54">(B74+C74)/2</f>
+        <f t="shared" ref="G74:G78" si="55">(B74+C74)/2</f>
         <v>101</v>
       </c>
       <c r="H74" s="3">
-        <f t="shared" ref="H74:H78" si="55">SQRT((B74-C74)^2/4+D74^2)</f>
+        <f t="shared" ref="H74:H78" si="56">SQRT((B74-C74)^2/4+D74^2)</f>
         <v>252.14479966876175</v>
       </c>
       <c r="I74" s="3">
-        <f t="shared" ref="I74:I78" si="56">G74+H74</f>
+        <f t="shared" ref="I74:I78" si="57">G74+H74</f>
         <v>353.14479966876172</v>
       </c>
       <c r="J74" s="3">
-        <f t="shared" ref="J74:J78" si="57">G74-H74</f>
+        <f t="shared" ref="J74:J78" si="58">G74-H74</f>
         <v>-151.14479966876175</v>
       </c>
       <c r="K74" s="3">
-        <f t="shared" si="50"/>
+        <f t="shared" si="51"/>
         <v>42.269062076843014</v>
       </c>
       <c r="L74" s="3">
-        <f t="shared" si="51"/>
+        <f t="shared" si="52"/>
         <v>-47.730937923156986</v>
       </c>
       <c r="M74" s="3">
@@ -3193,35 +3194,35 @@
         <v>120</v>
       </c>
       <c r="E75" s="3">
+        <f t="shared" si="53"/>
+        <v>0.5880026035475675</v>
+      </c>
+      <c r="F75" s="3">
+        <f t="shared" si="54"/>
+        <v>33.690067525979785</v>
+      </c>
+      <c r="G75" s="3">
+        <f t="shared" si="55"/>
+        <v>-350</v>
+      </c>
+      <c r="H75" s="3">
+        <f t="shared" si="56"/>
+        <v>130</v>
+      </c>
+      <c r="I75" s="3">
+        <f t="shared" si="57"/>
+        <v>-220</v>
+      </c>
+      <c r="J75" s="3">
+        <f t="shared" si="58"/>
+        <v>-480</v>
+      </c>
+      <c r="K75" s="3">
+        <f t="shared" si="51"/>
+        <v>78.690067525979785</v>
+      </c>
+      <c r="L75" s="3">
         <f t="shared" si="52"/>
-        <v>0.5880026035475675</v>
-      </c>
-      <c r="F75" s="3">
-        <f t="shared" si="53"/>
-        <v>33.690067525979785</v>
-      </c>
-      <c r="G75" s="3">
-        <f t="shared" si="54"/>
-        <v>-350</v>
-      </c>
-      <c r="H75" s="3">
-        <f t="shared" si="55"/>
-        <v>130</v>
-      </c>
-      <c r="I75" s="3">
-        <f t="shared" si="56"/>
-        <v>-220</v>
-      </c>
-      <c r="J75" s="3">
-        <f t="shared" si="57"/>
-        <v>-480</v>
-      </c>
-      <c r="K75" s="3">
-        <f t="shared" si="50"/>
-        <v>78.690067525979785</v>
-      </c>
-      <c r="L75" s="3">
-        <f t="shared" si="51"/>
         <v>-11.309932474020215</v>
       </c>
       <c r="M75" s="3"/>
@@ -3240,35 +3241,35 @@
         <v>80</v>
       </c>
       <c r="E76" s="3">
+        <f t="shared" si="53"/>
+        <v>0.26747753689304821</v>
+      </c>
+      <c r="F76" s="3">
+        <f t="shared" si="54"/>
+        <v>15.325333978526434</v>
+      </c>
+      <c r="G76" s="3">
+        <f t="shared" si="55"/>
+        <v>-15</v>
+      </c>
+      <c r="H76" s="3">
+        <f t="shared" si="56"/>
+        <v>156.92354826475216</v>
+      </c>
+      <c r="I76" s="3">
+        <f t="shared" si="57"/>
+        <v>141.92354826475216</v>
+      </c>
+      <c r="J76" s="3">
+        <f t="shared" si="58"/>
+        <v>-171.92354826475216</v>
+      </c>
+      <c r="K76" s="3">
+        <f t="shared" si="51"/>
+        <v>60.32533397852643</v>
+      </c>
+      <c r="L76" s="3">
         <f t="shared" si="52"/>
-        <v>0.26747753689304821</v>
-      </c>
-      <c r="F76" s="3">
-        <f t="shared" si="53"/>
-        <v>15.325333978526434</v>
-      </c>
-      <c r="G76" s="3">
-        <f t="shared" si="54"/>
-        <v>-15</v>
-      </c>
-      <c r="H76" s="3">
-        <f t="shared" si="55"/>
-        <v>156.92354826475216</v>
-      </c>
-      <c r="I76" s="3">
-        <f t="shared" si="56"/>
-        <v>141.92354826475216</v>
-      </c>
-      <c r="J76" s="3">
-        <f t="shared" si="57"/>
-        <v>-171.92354826475216</v>
-      </c>
-      <c r="K76" s="3">
-        <f t="shared" si="50"/>
-        <v>60.32533397852643</v>
-      </c>
-      <c r="L76" s="3">
-        <f t="shared" si="51"/>
         <v>-29.67466602147357</v>
       </c>
       <c r="M76" s="3"/>
@@ -3287,35 +3288,35 @@
         <v>95</v>
       </c>
       <c r="E77" s="3">
+        <f t="shared" si="53"/>
+        <v>-0.47304018463635611</v>
+      </c>
+      <c r="F77" s="3">
+        <f t="shared" si="54"/>
+        <v>-27.103206119752414</v>
+      </c>
+      <c r="G77" s="3">
+        <f t="shared" si="55"/>
+        <v>196.5</v>
+      </c>
+      <c r="H77" s="3">
+        <f t="shared" si="56"/>
+        <v>117.1206642740725</v>
+      </c>
+      <c r="I77" s="3">
+        <f t="shared" si="57"/>
+        <v>313.62066427407251</v>
+      </c>
+      <c r="J77" s="3">
+        <f t="shared" si="58"/>
+        <v>79.379335725927504</v>
+      </c>
+      <c r="K77" s="3">
+        <f t="shared" si="51"/>
+        <v>17.896793880247586</v>
+      </c>
+      <c r="L77" s="3">
         <f t="shared" si="52"/>
-        <v>-0.47304018463635611</v>
-      </c>
-      <c r="F77" s="3">
-        <f t="shared" si="53"/>
-        <v>-27.103206119752414</v>
-      </c>
-      <c r="G77" s="3">
-        <f t="shared" si="54"/>
-        <v>196.5</v>
-      </c>
-      <c r="H77" s="3">
-        <f t="shared" si="55"/>
-        <v>117.1206642740725</v>
-      </c>
-      <c r="I77" s="3">
-        <f t="shared" si="56"/>
-        <v>313.62066427407251</v>
-      </c>
-      <c r="J77" s="3">
-        <f t="shared" si="57"/>
-        <v>79.379335725927504</v>
-      </c>
-      <c r="K77" s="3">
-        <f t="shared" si="50"/>
-        <v>17.896793880247586</v>
-      </c>
-      <c r="L77" s="3">
-        <f t="shared" si="51"/>
         <v>-72.103206119752414</v>
       </c>
       <c r="M77" s="3"/>
@@ -3334,35 +3335,35 @@
         <v>-765</v>
       </c>
       <c r="E78" s="3">
+        <f t="shared" si="53"/>
+        <v>0.62188051502639119</v>
+      </c>
+      <c r="F78" s="3">
+        <f t="shared" si="54"/>
+        <v>35.631128872434189</v>
+      </c>
+      <c r="G78" s="3">
+        <f t="shared" si="55"/>
+        <v>-127.5</v>
+      </c>
+      <c r="H78" s="3">
+        <f t="shared" si="56"/>
+        <v>807.81510879656116</v>
+      </c>
+      <c r="I78" s="3">
+        <f t="shared" si="57"/>
+        <v>680.31510879656116</v>
+      </c>
+      <c r="J78" s="3">
+        <f t="shared" si="58"/>
+        <v>-935.31510879656116</v>
+      </c>
+      <c r="K78" s="3">
+        <f t="shared" si="51"/>
+        <v>80.631128872434189</v>
+      </c>
+      <c r="L78" s="3">
         <f t="shared" si="52"/>
-        <v>0.62188051502639119</v>
-      </c>
-      <c r="F78" s="3">
-        <f t="shared" si="53"/>
-        <v>35.631128872434189</v>
-      </c>
-      <c r="G78" s="3">
-        <f t="shared" si="54"/>
-        <v>-127.5</v>
-      </c>
-      <c r="H78" s="3">
-        <f t="shared" si="55"/>
-        <v>807.81510879656116</v>
-      </c>
-      <c r="I78" s="3">
-        <f t="shared" si="56"/>
-        <v>680.31510879656116</v>
-      </c>
-      <c r="J78" s="3">
-        <f t="shared" si="57"/>
-        <v>-935.31510879656116</v>
-      </c>
-      <c r="K78" s="3">
-        <f t="shared" si="50"/>
-        <v>80.631128872434189</v>
-      </c>
-      <c r="L78" s="3">
-        <f t="shared" si="51"/>
         <v>-9.3688711275658108</v>
       </c>
       <c r="M78" s="3"/>
@@ -3383,35 +3384,35 @@
         <v>14.178240740740742</v>
       </c>
       <c r="E79" s="3">
-        <f t="shared" ref="E79" si="58">ATAN(-2*D79/(B79-C79))/2</f>
+        <f t="shared" ref="E79" si="59">ATAN(-2*D79/(B79-C79))/2</f>
         <v>-0.26403722421317988</v>
       </c>
       <c r="F79" s="3">
-        <f t="shared" ref="F79" si="59">E79*180/PI()</f>
+        <f t="shared" ref="F79" si="60">E79*180/PI()</f>
         <v>-15.128218581764637</v>
       </c>
       <c r="G79" s="3">
-        <f t="shared" ref="G79" si="60">(B79+C79)/2</f>
+        <f t="shared" ref="G79" si="61">(B79+C79)/2</f>
         <v>24.305555555555554</v>
       </c>
       <c r="H79" s="3">
-        <f t="shared" ref="H79" si="61">SQRT((B79-C79)^2/4+D79^2)</f>
+        <f t="shared" ref="H79" si="62">SQRT((B79-C79)^2/4+D79^2)</f>
         <v>28.138630765668005</v>
       </c>
       <c r="I79" s="3">
-        <f t="shared" ref="I79" si="62">G79+H79</f>
+        <f t="shared" ref="I79" si="63">G79+H79</f>
         <v>52.444186321223555</v>
       </c>
       <c r="J79" s="3">
-        <f t="shared" ref="J79" si="63">G79-H79</f>
+        <f t="shared" ref="J79" si="64">G79-H79</f>
         <v>-3.833075210112451</v>
       </c>
       <c r="K79" s="3">
-        <f t="shared" si="50"/>
+        <f t="shared" si="51"/>
         <v>29.871781418235365</v>
       </c>
       <c r="L79" s="3">
-        <f t="shared" si="51"/>
+        <f t="shared" si="52"/>
         <v>-60.128218581764635</v>
       </c>
       <c r="M79" s="3"/>

</xml_diff>

<commit_message>
2019.03.13 error of properties of section, and so on.
</commit_message>
<xml_diff>
--- a/quiz_calc.xlsx
+++ b/quiz_calc.xlsx
@@ -1,31 +1,36 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive - 경남대학교\GitHub\structural_mechanics_II\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F4B71AA-B9C7-445E-A20F-AF02A5F0D751}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DCF7BBB-9A17-4D45-B9C1-F1B80A68ECE0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="11610" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027" iterateDelta="1E-4"/>
+  <calcPr calcId="179021" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="78">
   <si>
     <t>Ix</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -280,6 +285,62 @@
   </si>
   <si>
     <t>y to btm of this area</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>F1x</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>F1y</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>F2x</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>F2y</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>F1_mag</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>F2_mag</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Rx</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Ry</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>R</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>theta (degree)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>F1_ang (degree)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>F2_ang (degree)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>x</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>y</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -679,10 +740,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P92"/>
+  <dimension ref="A1:P97"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H44" sqref="H44"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J4" sqref="J4:M4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -706,642 +767,603 @@
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B1" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="N1" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="O1" s="4" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="B2" s="2">
+        <v>4</v>
+      </c>
+      <c r="C2" s="2">
+        <v>300</v>
+      </c>
+      <c r="D2" s="2">
+        <v>1</v>
+      </c>
+      <c r="E2" s="2">
+        <v>210</v>
+      </c>
+      <c r="F2" s="2">
+        <f>B2*COS(C2/180*PI())</f>
+        <v>2.0000000000000004</v>
+      </c>
+      <c r="G2" s="2">
+        <f>B2*SIN(C2/180*PI())</f>
+        <v>-3.4641016151377544</v>
+      </c>
+      <c r="H2" s="2">
+        <f>D2*COS(E2/180*PI())</f>
+        <v>-0.8660254037844386</v>
+      </c>
+      <c r="I2" s="2">
+        <f>D2*SIN(E2/180*PI())</f>
+        <v>-0.50000000000000011</v>
+      </c>
+      <c r="J2" s="3">
+        <f>SUM(F2,H2)</f>
+        <v>1.1339745962155618</v>
+      </c>
+      <c r="K2" s="3">
+        <f>SUM(G2+I2)</f>
+        <v>-3.9641016151377544</v>
+      </c>
+      <c r="L2" s="3">
+        <f>SQRT(J2^2+K2^2)</f>
+        <v>4.1231056256176606</v>
+      </c>
+      <c r="M2" s="3">
+        <f>IF(J2&gt;0,ATAN(K2/J2)/PI()*180,180+ATAN(K2/J2)/PI()*180)</f>
+        <v>-74.036243467926482</v>
+      </c>
+      <c r="N2" s="4">
+        <f>(-G2*2+I2*1)/-K2</f>
+        <v>1.6216040491313504</v>
+      </c>
+      <c r="O2" s="4">
+        <f>(F2*1-H2*1)/J2</f>
+        <v>2.527415881580847</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="B3" s="2">
+        <v>8</v>
+      </c>
+      <c r="C3" s="2">
+        <v>-45</v>
+      </c>
+      <c r="D3" s="2">
+        <v>4</v>
+      </c>
+      <c r="E3" s="2">
+        <v>110</v>
+      </c>
+      <c r="F3" s="2">
+        <f>B3*COS(C3/180*PI())</f>
+        <v>5.6568542494923806</v>
+      </c>
+      <c r="G3" s="2">
+        <f>B3*SIN(C3/180*PI())</f>
+        <v>-5.6568542494923797</v>
+      </c>
+      <c r="H3" s="2">
+        <f>D3*COS(E3/180*PI())</f>
+        <v>-1.3680805733026749</v>
+      </c>
+      <c r="I3" s="2">
+        <f>D3*SIN(E3/180*PI())</f>
+        <v>3.7587704831436337</v>
+      </c>
+      <c r="J3" s="3">
+        <f>SUM(F3,H3)</f>
+        <v>4.288773676189706</v>
+      </c>
+      <c r="K3" s="3">
+        <f>SUM(G3+I3)</f>
+        <v>-1.898083766348746</v>
+      </c>
+      <c r="L3" s="3">
+        <f>SQRT(J3^2+K3^2)</f>
+        <v>4.6900214956495034</v>
+      </c>
+      <c r="M3" s="3">
+        <f>IF(J3&gt;0,ATAN(K3/J3)/PI()*180,180+ATAN(K3/J3)/PI()*180)</f>
+        <v>-23.872757364070893</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="F4" s="2">
+        <v>1</v>
+      </c>
+      <c r="G4" s="2">
+        <v>2</v>
+      </c>
+      <c r="H4" s="2">
+        <v>2</v>
+      </c>
+      <c r="I4" s="2">
+        <v>-2</v>
+      </c>
+      <c r="J4" s="3">
+        <f>SUM(F4,H4)</f>
+        <v>3</v>
+      </c>
+      <c r="K4" s="3">
+        <f>SUM(G4+I4)</f>
+        <v>0</v>
+      </c>
+      <c r="L4" s="3">
+        <f>SQRT(J4^2+K4^2)</f>
+        <v>3</v>
+      </c>
+      <c r="M4" s="3">
+        <f>IF(J4&gt;0,ATAN(K4/J4)/PI()*180,180+ATAN(K4/J4)/PI()*180)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="B6" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C6" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D6" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E6" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F6" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G6" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H6" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I6" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="J6" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="K6" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="L6" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="M6" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="N1" s="4" t="s">
+      <c r="N6" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="O1" s="4" t="s">
+      <c r="O6" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="P1" s="4" t="s">
+      <c r="P6" s="4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A2" s="1">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A7" s="1">
         <v>1</v>
       </c>
-      <c r="B2" s="2">
+      <c r="B7" s="2">
         <v>70</v>
       </c>
-      <c r="C2" s="2">
+      <c r="C7" s="2">
         <v>120</v>
       </c>
-      <c r="D2" s="2">
-        <f>B2*C2</f>
+      <c r="D7" s="2">
+        <f>B7*C7</f>
         <v>8400</v>
       </c>
-      <c r="E2" s="2">
-        <f t="shared" ref="E2:F5" si="0">B2/2</f>
+      <c r="E7" s="2">
+        <f t="shared" ref="E7:F10" si="0">B7/2</f>
         <v>35</v>
       </c>
-      <c r="F2" s="2">
+      <c r="F7" s="2">
         <f t="shared" si="0"/>
         <v>60</v>
       </c>
-      <c r="G2" s="2">
-        <v>0</v>
-      </c>
-      <c r="H2" s="2">
-        <v>0</v>
-      </c>
-      <c r="I2" s="2">
-        <f>D2*G2/D2</f>
-        <v>0</v>
-      </c>
-      <c r="J2" s="2">
-        <f>D2*H2/D2</f>
-        <v>0</v>
-      </c>
-      <c r="K2" s="2">
-        <f t="shared" ref="K2:K8" si="1">B2*C2^3/12+H2^2*D2</f>
+      <c r="G7" s="2">
+        <v>0</v>
+      </c>
+      <c r="H7" s="2">
+        <v>0</v>
+      </c>
+      <c r="I7" s="2">
+        <f>D7*G7/D7</f>
+        <v>0</v>
+      </c>
+      <c r="J7" s="2">
+        <f>D7*H7/D7</f>
+        <v>0</v>
+      </c>
+      <c r="K7" s="2">
+        <f t="shared" ref="K7:K13" si="1">B7*C7^3/12+H7^2*D7</f>
         <v>10080000</v>
       </c>
-      <c r="L2" s="2">
-        <f t="shared" ref="L2:L8" si="2">C2*B2^3/12+G2^2*D2</f>
+      <c r="L7" s="2">
+        <f t="shared" ref="L7:L13" si="2">C7*B7^3/12+G7^2*D7</f>
         <v>3430000</v>
       </c>
-      <c r="M2" s="2">
-        <f>SUM(K2:L2)</f>
+      <c r="M7" s="2">
+        <f>SUM(K7:L7)</f>
         <v>13510000</v>
       </c>
-      <c r="N2" s="4">
-        <f t="shared" ref="N2:N8" si="3">D2*G2*H2</f>
-        <v>0</v>
-      </c>
-      <c r="O2" s="4">
-        <f>SQRT(L2/D2)</f>
+      <c r="N7" s="4">
+        <f t="shared" ref="N7:N13" si="3">D7*G7*H7</f>
+        <v>0</v>
+      </c>
+      <c r="O7" s="4">
+        <f>SQRT(L7/D7)</f>
         <v>20.207259421636902</v>
       </c>
-      <c r="P2" s="4">
-        <f>SQRT(K2/D2)</f>
+      <c r="P7" s="4">
+        <f>SQRT(K7/D7)</f>
         <v>34.641016151377549</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A3" s="1">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A8" s="1">
         <v>2</v>
       </c>
-      <c r="B3" s="2">
+      <c r="B8" s="2">
         <v>40</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C8" s="2">
         <v>70</v>
       </c>
-      <c r="D3" s="2">
-        <f>B3*C3</f>
+      <c r="D8" s="2">
+        <f>B8*C8</f>
         <v>2800</v>
       </c>
-      <c r="E3" s="2">
+      <c r="E8" s="2">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="F3" s="2">
+      <c r="F8" s="2">
         <f t="shared" si="0"/>
         <v>35</v>
       </c>
-      <c r="G3" s="2">
-        <v>0</v>
-      </c>
-      <c r="H3" s="2">
-        <v>0</v>
-      </c>
-      <c r="I3" s="2">
-        <f>D3*G3/D3</f>
-        <v>0</v>
-      </c>
-      <c r="J3" s="2">
-        <f>D3*H3/D3</f>
-        <v>0</v>
-      </c>
-      <c r="K3" s="2">
+      <c r="G8" s="2">
+        <v>0</v>
+      </c>
+      <c r="H8" s="2">
+        <v>0</v>
+      </c>
+      <c r="I8" s="2">
+        <f>D8*G8/D8</f>
+        <v>0</v>
+      </c>
+      <c r="J8" s="2">
+        <f>D8*H8/D8</f>
+        <v>0</v>
+      </c>
+      <c r="K8" s="2">
         <f t="shared" si="1"/>
         <v>1143333.3333333333</v>
       </c>
-      <c r="L3" s="2">
+      <c r="L8" s="2">
         <f t="shared" si="2"/>
         <v>373333.33333333331</v>
       </c>
-      <c r="M3" s="2">
-        <f t="shared" ref="M3:M8" si="4">SUM(K3:L3)</f>
+      <c r="M8" s="2">
+        <f t="shared" ref="M8:M13" si="4">SUM(K8:L8)</f>
         <v>1516666.6666666665</v>
       </c>
-      <c r="N3" s="4">
+      <c r="N8" s="4">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="O3" s="4">
-        <f>SQRT(L3/D3)</f>
+      <c r="O8" s="4">
+        <f>SQRT(L8/D8)</f>
         <v>11.547005383792515</v>
       </c>
-      <c r="P3" s="4">
-        <f>SQRT(K3/D3)</f>
+      <c r="P8" s="4">
+        <f>SQRT(K8/D8)</f>
         <v>20.207259421636902</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A4" s="1">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A9" s="1">
         <v>3</v>
       </c>
-      <c r="B4" s="2">
+      <c r="B9" s="2">
         <v>40</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C9" s="2">
         <v>16</v>
       </c>
-      <c r="D4" s="2">
-        <f>B4*C4</f>
+      <c r="D9" s="2">
+        <f>B9*C9</f>
         <v>640</v>
       </c>
-      <c r="E4" s="2">
+      <c r="E9" s="2">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="F4" s="2">
+      <c r="F9" s="2">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="G4" s="2">
+      <c r="G9" s="2">
         <v>-23</v>
       </c>
-      <c r="H4" s="2">
+      <c r="H9" s="2">
         <v>18</v>
       </c>
-      <c r="I4" s="2">
-        <f>D4*G4/D4</f>
+      <c r="I9" s="2">
+        <f>D9*G9/D9</f>
         <v>-23</v>
       </c>
-      <c r="J4" s="2">
-        <f>D4*H4/D4</f>
+      <c r="J9" s="2">
+        <f>D9*H9/D9</f>
         <v>18</v>
       </c>
-      <c r="K4" s="2">
+      <c r="K9" s="2">
         <f t="shared" si="1"/>
         <v>221013.33333333334</v>
       </c>
-      <c r="L4" s="2">
+      <c r="L9" s="2">
         <f t="shared" si="2"/>
         <v>423893.33333333331</v>
       </c>
-      <c r="M4" s="2">
+      <c r="M9" s="2">
         <f t="shared" si="4"/>
         <v>644906.66666666663</v>
       </c>
-      <c r="N4" s="4">
+      <c r="N9" s="4">
         <f t="shared" si="3"/>
         <v>-264960</v>
       </c>
-      <c r="O4" s="4">
-        <f>SQRT(L4/D4)</f>
+      <c r="O9" s="4">
+        <f>SQRT(L9/D9)</f>
         <v>25.735837529276822</v>
       </c>
-      <c r="P4" s="4">
-        <f>SQRT(K4/D4)</f>
+      <c r="P9" s="4">
+        <f>SQRT(K9/D9)</f>
         <v>18.58314648635514</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A5" s="1">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A10" s="1">
         <v>4</v>
       </c>
-      <c r="B5" s="2">
+      <c r="B10" s="2">
         <v>30</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C10" s="2">
         <v>40</v>
       </c>
-      <c r="D5" s="2">
-        <f>B5*C5</f>
+      <c r="D10" s="2">
+        <f>B10*C10</f>
         <v>1200</v>
       </c>
-      <c r="E5" s="2">
+      <c r="E10" s="2">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="F5" s="2">
+      <c r="F10" s="2">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="G5" s="2">
-        <v>0</v>
-      </c>
-      <c r="H5" s="2">
-        <v>0</v>
-      </c>
-      <c r="I5" s="2">
-        <f>D5*G5/D5</f>
-        <v>0</v>
-      </c>
-      <c r="J5" s="2">
-        <f>D5*H5/D5</f>
-        <v>0</v>
-      </c>
-      <c r="K5" s="2">
+      <c r="G10" s="2">
+        <v>0</v>
+      </c>
+      <c r="H10" s="2">
+        <v>0</v>
+      </c>
+      <c r="I10" s="2">
+        <f>D10*G10/D10</f>
+        <v>0</v>
+      </c>
+      <c r="J10" s="2">
+        <f>D10*H10/D10</f>
+        <v>0</v>
+      </c>
+      <c r="K10" s="2">
         <f t="shared" si="1"/>
         <v>160000</v>
       </c>
-      <c r="L5" s="2">
+      <c r="L10" s="2">
         <f t="shared" si="2"/>
         <v>90000</v>
       </c>
-      <c r="M5" s="2">
+      <c r="M10" s="2">
         <f t="shared" si="4"/>
         <v>250000</v>
       </c>
-      <c r="N5" s="4">
+      <c r="N10" s="4">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="O5" s="4">
-        <f>SQRT(L5/D5)</f>
+      <c r="O10" s="4">
+        <f>SQRT(L10/D10)</f>
         <v>8.6602540378443873</v>
       </c>
-      <c r="P5" s="4">
-        <f>SQRT(K5/D5)</f>
+      <c r="P10" s="4">
+        <f>SQRT(K10/D10)</f>
         <v>11.547005383792516</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="K6" s="2">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="K11" s="2">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="L6" s="2">
+      <c r="L11" s="2">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="M6" s="2">
+      <c r="M11" s="2">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="N6" s="4">
+      <c r="N11" s="4">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A7" s="1">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A12" s="1">
         <v>5</v>
       </c>
-      <c r="B7" s="2">
+      <c r="B12" s="2">
         <v>25</v>
       </c>
-      <c r="C7" s="2">
+      <c r="C12" s="2">
         <v>100</v>
       </c>
-      <c r="D7" s="2">
-        <f>B7*C7</f>
+      <c r="D12" s="2">
+        <f>B12*C12</f>
         <v>2500</v>
       </c>
-      <c r="E7" s="2">
-        <f>B7/2</f>
+      <c r="E12" s="2">
+        <f>B12/2</f>
         <v>12.5</v>
       </c>
-      <c r="F7" s="2">
-        <f>C7/2</f>
+      <c r="F12" s="2">
+        <f>C12/2</f>
         <v>50</v>
       </c>
-      <c r="G7" s="2">
+      <c r="G12" s="2">
         <v>12.5</v>
       </c>
-      <c r="H7" s="2">
+      <c r="H12" s="2">
         <v>75</v>
       </c>
-      <c r="I7" s="2">
-        <f>D7*H7</f>
+      <c r="I12" s="2">
+        <f>D12*H12</f>
         <v>187500</v>
       </c>
-      <c r="J7" s="2">
-        <f>D7*G7</f>
+      <c r="J12" s="2">
+        <f>D12*G12</f>
         <v>31250</v>
       </c>
-      <c r="K7" s="2">
+      <c r="K12" s="2">
         <f t="shared" si="1"/>
         <v>16145833.333333334</v>
       </c>
-      <c r="L7" s="2">
+      <c r="L12" s="2">
         <f t="shared" si="2"/>
         <v>520833.33333333331</v>
       </c>
-      <c r="M7" s="2">
+      <c r="M12" s="2">
         <f t="shared" si="4"/>
         <v>16666666.666666668</v>
       </c>
-      <c r="N7" s="4">
+      <c r="N12" s="4">
         <f t="shared" si="3"/>
         <v>2343750</v>
       </c>
-      <c r="O7" s="4">
-        <f>SQRT(L7/D7)</f>
+      <c r="O12" s="4">
+        <f>SQRT(L12/D12)</f>
         <v>14.433756729740644</v>
       </c>
-      <c r="P7" s="4">
-        <f>SQRT(K7/D7)</f>
+      <c r="P12" s="4">
+        <f>SQRT(K12/D12)</f>
         <v>80.363756341607967</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A8" s="1">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A13" s="1">
         <v>6</v>
       </c>
-      <c r="B8" s="2">
+      <c r="B13" s="2">
         <v>100</v>
       </c>
-      <c r="C8" s="2">
+      <c r="C13" s="2">
         <v>25</v>
       </c>
-      <c r="D8" s="2">
-        <f>B8*C8</f>
+      <c r="D13" s="2">
+        <f>B13*C13</f>
         <v>2500</v>
       </c>
-      <c r="E8" s="2">
-        <f>B8/2</f>
+      <c r="E13" s="2">
+        <f>B13/2</f>
         <v>50</v>
       </c>
-      <c r="F8" s="2">
-        <f>C8/2</f>
+      <c r="F13" s="2">
+        <f>C13/2</f>
         <v>12.5</v>
       </c>
-      <c r="G8" s="2">
+      <c r="G13" s="2">
         <v>50</v>
       </c>
-      <c r="H8" s="2">
+      <c r="H13" s="2">
         <v>12.5</v>
       </c>
-      <c r="I8" s="2">
-        <f>D8*H8</f>
+      <c r="I13" s="2">
+        <f>D13*H13</f>
         <v>31250</v>
       </c>
-      <c r="J8" s="2">
-        <f>D8*G8</f>
+      <c r="J13" s="2">
+        <f>D13*G13</f>
         <v>125000</v>
       </c>
-      <c r="K8" s="2">
+      <c r="K13" s="2">
         <f t="shared" si="1"/>
         <v>520833.33333333331</v>
       </c>
-      <c r="L8" s="2">
+      <c r="L13" s="2">
         <f t="shared" si="2"/>
         <v>8333333.333333333</v>
       </c>
-      <c r="M8" s="2">
+      <c r="M13" s="2">
         <f t="shared" si="4"/>
         <v>8854166.666666666</v>
       </c>
-      <c r="N8" s="4">
+      <c r="N13" s="4">
         <f t="shared" si="3"/>
         <v>1562500</v>
       </c>
-      <c r="O8" s="4">
-        <f>SQRT(L8/D8)</f>
-        <v>57.735026918962575</v>
-      </c>
-      <c r="P8" s="4">
-        <f>SQRT(K8/D8)</f>
-        <v>14.433756729740644</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A9" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D9" s="2">
-        <f>SUM(D7:D8)</f>
-        <v>5000</v>
-      </c>
-      <c r="E9" s="2">
-        <f>SUM(J7:J8)/D9</f>
-        <v>31.25</v>
-      </c>
-      <c r="F9" s="2">
-        <f>SUM(I7:I8)/D9</f>
-        <v>43.75</v>
-      </c>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A10" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B10" s="2">
-        <v>25</v>
-      </c>
-      <c r="C10" s="2">
-        <v>100</v>
-      </c>
-      <c r="D10" s="2">
-        <f>B10*C10</f>
-        <v>2500</v>
-      </c>
-      <c r="E10" s="2">
-        <f>B10/2</f>
-        <v>12.5</v>
-      </c>
-      <c r="F10" s="2">
-        <f>C10/2</f>
-        <v>50</v>
-      </c>
-      <c r="G10" s="2">
-        <f>B10/2-E9</f>
-        <v>-18.75</v>
-      </c>
-      <c r="H10" s="2">
-        <f>C11+C10/2-F9</f>
-        <v>31.25</v>
-      </c>
-      <c r="K10" s="2">
-        <f>B10*C10^3/12+H10^2*D10</f>
-        <v>4524739.583333333</v>
-      </c>
-      <c r="L10" s="2">
-        <f>C10*B10^3/12+G10^2*D10</f>
-        <v>1009114.5833333334</v>
-      </c>
-      <c r="N10" s="4">
-        <f>D10*G10*H10</f>
-        <v>-1464843.75</v>
-      </c>
-      <c r="O10" s="4">
-        <f>SQRT(L10/D10)</f>
-        <v>20.090939085401992</v>
-      </c>
-      <c r="P10" s="4">
-        <f>SQRT(K10/D10)</f>
-        <v>42.542870534712783</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A11" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B11" s="2">
-        <v>100</v>
-      </c>
-      <c r="C11" s="2">
-        <v>25</v>
-      </c>
-      <c r="D11" s="2">
-        <f>B11*C11</f>
-        <v>2500</v>
-      </c>
-      <c r="E11" s="2">
-        <f>B11/2</f>
-        <v>50</v>
-      </c>
-      <c r="F11" s="2">
-        <f>C11/2</f>
-        <v>12.5</v>
-      </c>
-      <c r="G11" s="2">
-        <f>B11/2-E9</f>
-        <v>18.75</v>
-      </c>
-      <c r="H11" s="2">
-        <f>C11/2-F9</f>
-        <v>-31.25</v>
-      </c>
-      <c r="K11" s="2">
-        <f>B11*C11^3/12+H11^2*D11</f>
-        <v>2571614.5833333335</v>
-      </c>
-      <c r="L11" s="2">
-        <f>C11*B11^3/12+G11^2*D11</f>
-        <v>2962239.583333333</v>
-      </c>
-      <c r="N11" s="4">
-        <f>D11*G11*H11</f>
-        <v>-1464843.75</v>
-      </c>
-      <c r="O11" s="4">
-        <f>SQRT(L11/D11)</f>
-        <v>34.422315920538139</v>
-      </c>
-      <c r="P11" s="4">
-        <f>SQRT(K11/D11)</f>
-        <v>32.072508996543029</v>
-      </c>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A12" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D12" s="2">
-        <f>SUM(D10:D11)</f>
-        <v>5000</v>
-      </c>
-      <c r="K12" s="3">
-        <f t="shared" ref="K12:N12" si="5">SUM(K10:K11)</f>
-        <v>7096354.166666666</v>
-      </c>
-      <c r="L12" s="3">
-        <f t="shared" si="5"/>
-        <v>3971354.1666666665</v>
-      </c>
-      <c r="M12" s="3">
-        <f>SUM(K12:L12)</f>
-        <v>11067708.333333332</v>
-      </c>
-      <c r="N12" s="4">
-        <f t="shared" si="5"/>
-        <v>-2929687.5</v>
-      </c>
-      <c r="O12" s="4">
-        <f>SQRT(L12/D12)</f>
-        <v>28.182810955143086</v>
-      </c>
-      <c r="P12" s="4">
-        <f>SQRT(K12/D12)</f>
-        <v>37.673211083385674</v>
-      </c>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A13" s="1">
-        <v>7</v>
-      </c>
-      <c r="B13" s="2">
-        <v>30</v>
-      </c>
-      <c r="C13" s="2">
-        <v>50</v>
-      </c>
-      <c r="D13" s="2">
-        <f>B13*C13</f>
-        <v>1500</v>
-      </c>
-      <c r="E13" s="2">
-        <f>B13/2</f>
-        <v>15</v>
-      </c>
-      <c r="F13" s="2">
-        <f>C13/2</f>
-        <v>25</v>
-      </c>
-      <c r="G13" s="2">
-        <v>0</v>
-      </c>
-      <c r="H13" s="2">
-        <v>0</v>
-      </c>
-      <c r="I13" s="2">
-        <f>D13*G13/D13</f>
-        <v>0</v>
-      </c>
-      <c r="J13" s="2">
-        <f>D13*H13/D13</f>
-        <v>0</v>
-      </c>
-      <c r="K13" s="2">
-        <f>B13*C13^3/12+H13^2*D13</f>
-        <v>312500</v>
-      </c>
-      <c r="L13" s="2">
-        <f>C13*B13^3/12+G13^2*D13</f>
-        <v>112500</v>
-      </c>
-      <c r="M13" s="2">
-        <f t="shared" ref="M13" si="6">SUM(K13:L13)</f>
-        <v>425000</v>
-      </c>
-      <c r="N13" s="4">
-        <f>D13*G13*H13</f>
-        <v>0</v>
-      </c>
       <c r="O13" s="4">
         <f>SQRT(L13/D13)</f>
-        <v>8.6602540378443873</v>
+        <v>57.735026918962575</v>
       </c>
       <c r="P13" s="4">
         <f>SQRT(K13/D13)</f>
@@ -1349,2332 +1371,2545 @@
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A14" s="1">
+      <c r="A14" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D14" s="2">
+        <f>SUM(D12:D13)</f>
+        <v>5000</v>
+      </c>
+      <c r="E14" s="2">
+        <f>SUM(J12:J13)/D14</f>
+        <v>31.25</v>
+      </c>
+      <c r="F14" s="2">
+        <f>SUM(I12:I13)/D14</f>
+        <v>43.75</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A15" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B15" s="2">
+        <v>25</v>
+      </c>
+      <c r="C15" s="2">
+        <v>100</v>
+      </c>
+      <c r="D15" s="2">
+        <f>B15*C15</f>
+        <v>2500</v>
+      </c>
+      <c r="E15" s="2">
+        <f>B15/2</f>
+        <v>12.5</v>
+      </c>
+      <c r="F15" s="2">
+        <f>C15/2</f>
+        <v>50</v>
+      </c>
+      <c r="G15" s="2">
+        <f>B15/2-E14</f>
+        <v>-18.75</v>
+      </c>
+      <c r="H15" s="2">
+        <f>C16+C15/2-F14</f>
+        <v>31.25</v>
+      </c>
+      <c r="K15" s="2">
+        <f>B15*C15^3/12+H15^2*D15</f>
+        <v>4524739.583333333</v>
+      </c>
+      <c r="L15" s="2">
+        <f>C15*B15^3/12+G15^2*D15</f>
+        <v>1009114.5833333334</v>
+      </c>
+      <c r="N15" s="4">
+        <f>D15*G15*H15</f>
+        <v>-1464843.75</v>
+      </c>
+      <c r="O15" s="4">
+        <f>SQRT(L15/D15)</f>
+        <v>20.090939085401992</v>
+      </c>
+      <c r="P15" s="4">
+        <f>SQRT(K15/D15)</f>
+        <v>42.542870534712783</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A16" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B16" s="2">
+        <v>100</v>
+      </c>
+      <c r="C16" s="2">
+        <v>25</v>
+      </c>
+      <c r="D16" s="2">
+        <f>B16*C16</f>
+        <v>2500</v>
+      </c>
+      <c r="E16" s="2">
+        <f>B16/2</f>
+        <v>50</v>
+      </c>
+      <c r="F16" s="2">
+        <f>C16/2</f>
+        <v>12.5</v>
+      </c>
+      <c r="G16" s="2">
+        <f>B16/2-E14</f>
+        <v>18.75</v>
+      </c>
+      <c r="H16" s="2">
+        <f>C16/2-F14</f>
+        <v>-31.25</v>
+      </c>
+      <c r="K16" s="2">
+        <f>B16*C16^3/12+H16^2*D16</f>
+        <v>2571614.5833333335</v>
+      </c>
+      <c r="L16" s="2">
+        <f>C16*B16^3/12+G16^2*D16</f>
+        <v>2962239.583333333</v>
+      </c>
+      <c r="N16" s="4">
+        <f>D16*G16*H16</f>
+        <v>-1464843.75</v>
+      </c>
+      <c r="O16" s="4">
+        <f>SQRT(L16/D16)</f>
+        <v>34.422315920538139</v>
+      </c>
+      <c r="P16" s="4">
+        <f>SQRT(K16/D16)</f>
+        <v>32.072508996543029</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A17" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D17" s="2">
+        <f>SUM(D15:D16)</f>
+        <v>5000</v>
+      </c>
+      <c r="K17" s="3">
+        <f t="shared" ref="K17:N17" si="5">SUM(K15:K16)</f>
+        <v>7096354.166666666</v>
+      </c>
+      <c r="L17" s="3">
+        <f t="shared" si="5"/>
+        <v>3971354.1666666665</v>
+      </c>
+      <c r="M17" s="3">
+        <f>SUM(K17:L17)</f>
+        <v>11067708.333333332</v>
+      </c>
+      <c r="N17" s="4">
+        <f t="shared" si="5"/>
+        <v>-2929687.5</v>
+      </c>
+      <c r="O17" s="4">
+        <f>SQRT(L17/D17)</f>
+        <v>28.182810955143086</v>
+      </c>
+      <c r="P17" s="4">
+        <f>SQRT(K17/D17)</f>
+        <v>37.673211083385674</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A18" s="1">
+        <v>7</v>
+      </c>
+      <c r="B18" s="2">
+        <v>30</v>
+      </c>
+      <c r="C18" s="2">
+        <v>50</v>
+      </c>
+      <c r="D18" s="2">
+        <f>B18*C18</f>
+        <v>1500</v>
+      </c>
+      <c r="E18" s="2">
+        <f>B18/2</f>
+        <v>15</v>
+      </c>
+      <c r="F18" s="2">
+        <f>C18/2</f>
+        <v>25</v>
+      </c>
+      <c r="G18" s="2">
+        <v>0</v>
+      </c>
+      <c r="H18" s="2">
+        <v>0</v>
+      </c>
+      <c r="I18" s="2">
+        <f>D18*G18/D18</f>
+        <v>0</v>
+      </c>
+      <c r="J18" s="2">
+        <f>D18*H18/D18</f>
+        <v>0</v>
+      </c>
+      <c r="K18" s="2">
+        <f>B18*C18^3/12+H18^2*D18</f>
+        <v>312500</v>
+      </c>
+      <c r="L18" s="2">
+        <f>C18*B18^3/12+G18^2*D18</f>
+        <v>112500</v>
+      </c>
+      <c r="M18" s="2">
+        <f t="shared" ref="M18" si="6">SUM(K18:L18)</f>
+        <v>425000</v>
+      </c>
+      <c r="N18" s="4">
+        <f>D18*G18*H18</f>
+        <v>0</v>
+      </c>
+      <c r="O18" s="4">
+        <f>SQRT(L18/D18)</f>
+        <v>8.6602540378443873</v>
+      </c>
+      <c r="P18" s="4">
+        <f>SQRT(K18/D18)</f>
+        <v>14.433756729740644</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A19" s="1">
         <v>8</v>
       </c>
-      <c r="B14" s="2">
+      <c r="B19" s="2">
         <v>250</v>
       </c>
-      <c r="C14" s="2">
+      <c r="C19" s="2">
         <v>500</v>
       </c>
-      <c r="D14" s="2">
-        <f>B14*C14</f>
+      <c r="D19" s="2">
+        <f>B19*C19</f>
         <v>125000</v>
       </c>
-      <c r="E14" s="2">
-        <f>B14/2</f>
+      <c r="E19" s="2">
+        <f>B19/2</f>
         <v>125</v>
       </c>
-      <c r="F14" s="2">
-        <f>C14/2</f>
+      <c r="F19" s="2">
+        <f>C19/2</f>
         <v>250</v>
       </c>
-      <c r="G14" s="2">
-        <v>0</v>
-      </c>
-      <c r="H14" s="2">
-        <v>0</v>
-      </c>
-      <c r="I14" s="2">
-        <f>D14*G14/D14</f>
-        <v>0</v>
-      </c>
-      <c r="J14" s="2">
-        <f>D14*H14/D14</f>
-        <v>0</v>
-      </c>
-      <c r="K14" s="2">
-        <f>B14*C14^3/12+H14^2*D14</f>
+      <c r="G19" s="2">
+        <v>0</v>
+      </c>
+      <c r="H19" s="2">
+        <v>0</v>
+      </c>
+      <c r="I19" s="2">
+        <f>D19*G19/D19</f>
+        <v>0</v>
+      </c>
+      <c r="J19" s="2">
+        <f>D19*H19/D19</f>
+        <v>0</v>
+      </c>
+      <c r="K19" s="2">
+        <f>B19*C19^3/12+H19^2*D19</f>
         <v>2604166666.6666665</v>
       </c>
-      <c r="L14" s="2">
-        <f>C14*B14^3/12+G14^2*D14</f>
+      <c r="L19" s="2">
+        <f>C19*B19^3/12+G19^2*D19</f>
         <v>651041666.66666663</v>
       </c>
-      <c r="M14" s="2">
-        <f t="shared" ref="M14" si="7">SUM(K14:L14)</f>
+      <c r="M19" s="2">
+        <f t="shared" ref="M19" si="7">SUM(K19:L19)</f>
         <v>3255208333.333333</v>
       </c>
-      <c r="N14" s="4">
-        <f>D14*G14*H14</f>
-        <v>0</v>
-      </c>
-      <c r="O14" s="4">
-        <f>SQRT(L14/D14)</f>
+      <c r="N19" s="4">
+        <f>D19*G19*H19</f>
+        <v>0</v>
+      </c>
+      <c r="O19" s="4">
+        <f>SQRT(L19/D19)</f>
         <v>72.168783648703211</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="E15" s="2">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="E20" s="2">
         <f>250*50*(200+50/2)</f>
         <v>2812500</v>
       </c>
-      <c r="G15" s="2">
+      <c r="G20" s="2">
         <f>250*250*(250/2)</f>
         <v>7812500</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A16" s="1">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A21" s="1">
         <v>9</v>
       </c>
-      <c r="B16" s="2">
+      <c r="B21" s="2">
         <v>400</v>
       </c>
-      <c r="C16" s="2">
+      <c r="C21" s="2">
         <v>600</v>
       </c>
-      <c r="D16" s="2">
-        <f>B16*C16</f>
+      <c r="D21" s="2">
+        <f>B21*C21</f>
         <v>240000</v>
       </c>
-      <c r="E16" s="2">
-        <f t="shared" ref="E16:F19" si="8">B16/2</f>
+      <c r="E21" s="2">
+        <f t="shared" ref="E21:F24" si="8">B21/2</f>
         <v>200</v>
       </c>
-      <c r="F16" s="2">
+      <c r="F21" s="2">
         <f t="shared" si="8"/>
         <v>300</v>
       </c>
-      <c r="G16" s="2">
-        <v>0</v>
-      </c>
-      <c r="H16" s="2">
-        <v>0</v>
-      </c>
-      <c r="I16" s="2">
-        <f>D16*G16/D16</f>
-        <v>0</v>
-      </c>
-      <c r="J16" s="2">
-        <f>D16*H16/D16</f>
-        <v>0</v>
-      </c>
-      <c r="K16" s="2">
-        <f>B16*C16^3/12+H16^2*D16</f>
+      <c r="G21" s="2">
+        <v>0</v>
+      </c>
+      <c r="H21" s="2">
+        <v>0</v>
+      </c>
+      <c r="I21" s="2">
+        <f>D21*G21/D21</f>
+        <v>0</v>
+      </c>
+      <c r="J21" s="2">
+        <f>D21*H21/D21</f>
+        <v>0</v>
+      </c>
+      <c r="K21" s="2">
+        <f>B21*C21^3/12+H21^2*D21</f>
         <v>7200000000</v>
       </c>
-      <c r="L16" s="2">
-        <f>C16*B16^3/12+G16^2*D16</f>
+      <c r="L21" s="2">
+        <f>C21*B21^3/12+G21^2*D21</f>
         <v>3200000000</v>
       </c>
-      <c r="M16" s="2">
-        <f t="shared" ref="M16" si="9">SUM(K16:L16)</f>
+      <c r="M21" s="2">
+        <f t="shared" ref="M21" si="9">SUM(K21:L21)</f>
         <v>10400000000</v>
       </c>
-      <c r="N16" s="4">
-        <f>D16*G16*H16</f>
-        <v>0</v>
-      </c>
-      <c r="O16" s="4">
-        <f>SQRT(L16/D16)</f>
+      <c r="N21" s="4">
+        <f>D21*G21*H21</f>
+        <v>0</v>
+      </c>
+      <c r="O21" s="4">
+        <f>SQRT(L21/D21)</f>
         <v>115.47005383792515</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="B17" s="2">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="B22" s="2">
         <v>15</v>
       </c>
-      <c r="C17" s="2">
+      <c r="C22" s="2">
         <v>20</v>
       </c>
-      <c r="D17" s="2">
-        <f>B17*C17</f>
+      <c r="D22" s="2">
+        <f>B22*C22</f>
         <v>300</v>
       </c>
-      <c r="E17" s="2">
+      <c r="E22" s="2">
         <f t="shared" si="8"/>
         <v>7.5</v>
       </c>
-      <c r="F17" s="2">
+      <c r="F22" s="2">
         <f t="shared" si="8"/>
         <v>10</v>
       </c>
-      <c r="G17" s="2">
-        <v>0</v>
-      </c>
-      <c r="H17" s="2">
+      <c r="G22" s="2">
+        <v>0</v>
+      </c>
+      <c r="H22" s="2">
         <v>20</v>
       </c>
-      <c r="I17" s="2">
-        <f>D17*G17/D17</f>
-        <v>0</v>
-      </c>
-      <c r="J17" s="2">
-        <f>D17*H17/D17</f>
+      <c r="I22" s="2">
+        <f>D22*G22/D22</f>
+        <v>0</v>
+      </c>
+      <c r="J22" s="2">
+        <f>D22*H22/D22</f>
         <v>20</v>
       </c>
-      <c r="K17" s="2">
-        <f>B17*C17^3/12+H17^2*D17</f>
+      <c r="K22" s="2">
+        <f>B22*C22^3/12+H22^2*D22</f>
         <v>130000</v>
       </c>
-      <c r="L17" s="2">
-        <f>C17*B17^3/12+G17^2*D17</f>
+      <c r="L22" s="2">
+        <f>C22*B22^3/12+G22^2*D22</f>
         <v>5625</v>
       </c>
-      <c r="M17" s="2">
-        <f t="shared" ref="M17" si="10">SUM(K17:L17)</f>
+      <c r="M22" s="2">
+        <f t="shared" ref="M22" si="10">SUM(K22:L22)</f>
         <v>135625</v>
       </c>
-      <c r="N17" s="4">
-        <f>D17*G17*H17</f>
-        <v>0</v>
-      </c>
-      <c r="O17" s="4">
-        <f>SQRT(L17/D17)</f>
+      <c r="N22" s="4">
+        <f>D22*G22*H22</f>
+        <v>0</v>
+      </c>
+      <c r="O22" s="4">
+        <f>SQRT(L22/D22)</f>
         <v>4.3301270189221936</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="B18" s="2">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="B23" s="2">
         <v>100</v>
       </c>
-      <c r="C18" s="2">
+      <c r="C23" s="2">
         <v>20</v>
       </c>
-      <c r="D18" s="2">
-        <f>B18*C18</f>
+      <c r="D23" s="2">
+        <f>B23*C23</f>
         <v>2000</v>
       </c>
-      <c r="E18" s="2">
+      <c r="E23" s="2">
         <f t="shared" si="8"/>
         <v>50</v>
       </c>
-      <c r="F18" s="2">
+      <c r="F23" s="2">
         <f t="shared" si="8"/>
         <v>10</v>
       </c>
-      <c r="G18" s="2">
-        <v>0</v>
-      </c>
-      <c r="H18" s="2">
+      <c r="G23" s="2">
+        <v>0</v>
+      </c>
+      <c r="H23" s="2">
         <f>130-103.75</f>
         <v>26.25</v>
       </c>
-      <c r="I18" s="2">
-        <f>D18*G18/D18</f>
-        <v>0</v>
-      </c>
-      <c r="J18" s="2">
-        <f>D18*H18/D18</f>
+      <c r="I23" s="2">
+        <f>D23*G23/D23</f>
+        <v>0</v>
+      </c>
+      <c r="J23" s="2">
+        <f>D23*H23/D23</f>
         <v>26.25</v>
       </c>
-      <c r="K18" s="3">
-        <f>B18*C18^3/12+H18^2*D18</f>
+      <c r="K23" s="3">
+        <f>B23*C23^3/12+H23^2*D23</f>
         <v>1444791.6666666667</v>
       </c>
-      <c r="L18" s="2">
-        <f>C18*B18^3/12+G18^2*D18</f>
+      <c r="L23" s="2">
+        <f>C23*B23^3/12+G23^2*D23</f>
         <v>1666666.6666666667</v>
       </c>
-      <c r="M18" s="2">
-        <f t="shared" ref="M18" si="11">SUM(K18:L18)</f>
+      <c r="M23" s="2">
+        <f t="shared" ref="M23" si="11">SUM(K23:L23)</f>
         <v>3111458.3333333335</v>
       </c>
-      <c r="N18" s="4">
-        <f>D18*G18*H18</f>
-        <v>0</v>
-      </c>
-      <c r="O18" s="4">
-        <f>SQRT(L18/D18)</f>
+      <c r="N23" s="4">
+        <f>D23*G23*H23</f>
+        <v>0</v>
+      </c>
+      <c r="O23" s="4">
+        <f>SQRT(L23/D23)</f>
         <v>28.867513459481287</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="B19" s="2">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="B24" s="2">
         <v>10</v>
       </c>
-      <c r="C19" s="2">
+      <c r="C24" s="2">
         <v>120</v>
       </c>
-      <c r="D19" s="2">
-        <f>B19*C19</f>
+      <c r="D24" s="2">
+        <f>B24*C24</f>
         <v>1200</v>
       </c>
-      <c r="E19" s="2">
+      <c r="E24" s="2">
         <f t="shared" si="8"/>
         <v>5</v>
       </c>
-      <c r="F19" s="2">
+      <c r="F24" s="2">
         <f t="shared" si="8"/>
         <v>60</v>
       </c>
-      <c r="G19" s="2">
-        <v>0</v>
-      </c>
-      <c r="H19" s="2">
+      <c r="G24" s="2">
+        <v>0</v>
+      </c>
+      <c r="H24" s="2">
         <f>103.75-60</f>
         <v>43.75</v>
       </c>
-      <c r="I19" s="2">
-        <f>D19*G19/D19</f>
-        <v>0</v>
-      </c>
-      <c r="J19" s="2">
-        <f>D19*H19/D19</f>
+      <c r="I24" s="2">
+        <f>D24*G24/D24</f>
+        <v>0</v>
+      </c>
+      <c r="J24" s="2">
+        <f>D24*H24/D24</f>
         <v>43.75</v>
       </c>
-      <c r="K19" s="3">
-        <f>B19*C19^3/12+H19^2*D19</f>
+      <c r="K24" s="3">
+        <f>B24*C24^3/12+H24^2*D24</f>
         <v>3736875</v>
       </c>
-      <c r="L19" s="2">
-        <f>C19*B19^3/12+G19^2*D19</f>
+      <c r="L24" s="2">
+        <f>C24*B24^3/12+G24^2*D24</f>
         <v>10000</v>
       </c>
-      <c r="M19" s="2">
-        <f t="shared" ref="M19" si="12">SUM(K19:L19)</f>
+      <c r="M24" s="2">
+        <f t="shared" ref="M24" si="12">SUM(K24:L24)</f>
         <v>3746875</v>
       </c>
-      <c r="N19" s="4">
-        <f>D19*G19*H19</f>
-        <v>0</v>
-      </c>
-      <c r="O19" s="4">
-        <f>SQRT(L19/D19)</f>
+      <c r="N24" s="4">
+        <f>D24*G24*H24</f>
+        <v>0</v>
+      </c>
+      <c r="O24" s="4">
+        <f>SQRT(L24/D24)</f>
         <v>2.8867513459481291</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="K20" s="3">
-        <f>SUM(K18:K19)</f>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="K25" s="3">
+        <f>SUM(K23:K24)</f>
         <v>5181666.666666667</v>
       </c>
-      <c r="L20" s="3">
-        <f>K20/103.75</f>
+      <c r="L25" s="3">
+        <f>K25/103.75</f>
         <v>49943.77510040161</v>
       </c>
-      <c r="M20" s="3">
-        <f>K20/(140-103.75)</f>
+      <c r="M25" s="3">
+        <f>K25/(140-103.75)</f>
         <v>142942.52873563219</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="B21" s="3">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="B26" s="3">
         <f>700*(120^2+70^2)</f>
         <v>13510000</v>
       </c>
-      <c r="G21" s="3"/>
-      <c r="H21" s="3"/>
-      <c r="K21" s="3"/>
-    </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="K22" s="3"/>
-    </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="B25" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C25" s="2" t="s">
+      <c r="G26" s="3"/>
+      <c r="H26" s="3"/>
+      <c r="K26" s="3"/>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="K27" s="3"/>
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="B30" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C30" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D25" s="2" t="s">
+      <c r="D30" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="E25" s="2" t="s">
+      <c r="E30" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="F25" s="2" t="s">
+      <c r="F30" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="G25" s="2" t="s">
+      <c r="G30" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="H25" s="2" t="s">
+      <c r="H30" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="I25" s="2" t="s">
+      <c r="I30" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="J25" s="2" t="s">
+      <c r="J30" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A26" s="1">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A31" s="1">
         <v>1</v>
       </c>
-      <c r="B26" s="2">
+      <c r="B31" s="2">
         <v>1000</v>
       </c>
-      <c r="C26" s="2">
+      <c r="C31" s="2">
         <v>500</v>
       </c>
-      <c r="D26" s="2">
+      <c r="D31" s="2">
         <v>-50</v>
       </c>
-      <c r="E26" s="2">
-        <f>ATAN(-2*D26/(B26-C26))/2</f>
+      <c r="E31" s="2">
+        <f>ATAN(-2*D31/(B31-C31))/2</f>
         <v>9.8697779924940388E-2</v>
       </c>
-      <c r="F26" s="3">
-        <f>E26*180/PI()</f>
+      <c r="F31" s="3">
+        <f>E31*180/PI()</f>
         <v>5.6549662370101066</v>
       </c>
-      <c r="G26" s="3">
-        <f>(B26+C26)/2</f>
+      <c r="G31" s="3">
+        <f>(B31+C31)/2</f>
         <v>750</v>
       </c>
-      <c r="H26" s="3">
-        <f>SQRT((B26-C26)^2/4+D26^2)</f>
+      <c r="H31" s="3">
+        <f>SQRT((B31-C31)^2/4+D31^2)</f>
         <v>254.95097567963924</v>
       </c>
-      <c r="I26" s="3">
-        <f>G26+H26</f>
+      <c r="I31" s="3">
+        <f>G31+H31</f>
         <v>1004.9509756796392</v>
       </c>
-      <c r="J26" s="3">
-        <f>G26-H26</f>
+      <c r="J31" s="3">
+        <f>G31-H31</f>
         <v>495.04902432036079</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A27" s="1">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A32" s="1">
         <v>2</v>
       </c>
-      <c r="B27" s="2">
+      <c r="B32" s="2">
         <v>5333333.3333333302</v>
       </c>
-      <c r="C27" s="2">
+      <c r="C32" s="2">
         <v>3333333.3333333302</v>
       </c>
-      <c r="D27" s="2">
+      <c r="D32" s="2">
         <v>-2400000</v>
       </c>
-      <c r="E27" s="2">
-        <f>ATAN(-2*D27/(B27-C27))/2</f>
+      <c r="E32" s="2">
+        <f>ATAN(-2*D32/(B32-C32))/2</f>
         <v>0.5880026035475675</v>
       </c>
-      <c r="F27" s="3">
-        <f>E27*180/PI()</f>
+      <c r="F32" s="3">
+        <f>E32*180/PI()</f>
         <v>33.690067525979785</v>
       </c>
-      <c r="G27" s="3">
-        <f>(B27+C27)/2</f>
+      <c r="G32" s="3">
+        <f>(B32+C32)/2</f>
         <v>4333333.3333333302</v>
       </c>
-      <c r="H27" s="3">
-        <f>SQRT((B27-C27)^2/4+D27^2)</f>
+      <c r="H32" s="3">
+        <f>SQRT((B32-C32)^2/4+D32^2)</f>
         <v>2600000</v>
       </c>
-      <c r="I27" s="3">
-        <f>G27+H27</f>
+      <c r="I32" s="3">
+        <f>G32+H32</f>
         <v>6933333.3333333302</v>
       </c>
-      <c r="J27" s="3">
-        <f>G27-H27</f>
+      <c r="J32" s="3">
+        <f>G32-H32</f>
         <v>1733333.3333333302</v>
       </c>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A28" s="1">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A33" s="1">
         <v>3</v>
       </c>
-      <c r="B28" s="2">
+      <c r="B33" s="2">
         <v>532</v>
       </c>
-      <c r="C28" s="2">
+      <c r="C33" s="2">
         <v>740</v>
       </c>
-      <c r="D28" s="2">
+      <c r="D33" s="2">
         <v>345</v>
       </c>
-      <c r="E28" s="2">
-        <f>ATAN(-2*D28/(B28-C28))/2</f>
+      <c r="E33" s="2">
+        <f>ATAN(-2*D33/(B33-C33))/2</f>
         <v>0.6390052264115833</v>
       </c>
-      <c r="F28" s="3">
-        <f>E28*180/PI()</f>
+      <c r="F33" s="3">
+        <f>E33*180/PI()</f>
         <v>36.612302560185327</v>
       </c>
-      <c r="G28" s="3">
-        <f>(B28+C28)/2</f>
+      <c r="G33" s="3">
+        <f>(B33+C33)/2</f>
         <v>636</v>
       </c>
-      <c r="H28" s="3">
-        <f>SQRT((B28-C28)^2/4+D28^2)</f>
+      <c r="H33" s="3">
+        <f>SQRT((B33-C33)^2/4+D33^2)</f>
         <v>360.33456675706259</v>
       </c>
-      <c r="I28" s="3">
-        <f>G28+H28</f>
+      <c r="I33" s="3">
+        <f>G33+H33</f>
         <v>996.33456675706259</v>
       </c>
-      <c r="J28" s="3">
-        <f>G28-H28</f>
+      <c r="J33" s="3">
+        <f>G33-H33</f>
         <v>275.66543324293741</v>
       </c>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A29" s="1">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A34" s="1">
         <v>4</v>
       </c>
-      <c r="B29" s="2">
-        <f>K13</f>
+      <c r="B34" s="2">
+        <f>K18</f>
         <v>312500</v>
       </c>
-      <c r="C29" s="2">
-        <f>L13</f>
+      <c r="C34" s="2">
+        <f>L18</f>
         <v>112500</v>
       </c>
-      <c r="D29" s="2">
-        <f>N13</f>
-        <v>0</v>
-      </c>
-      <c r="E29" s="2">
-        <f>ATAN(-2*D29/(B29-C29))/2</f>
-        <v>0</v>
-      </c>
-      <c r="F29" s="3">
-        <f>E29*180/PI()</f>
-        <v>0</v>
-      </c>
-      <c r="G29" s="3">
-        <f>(B29+C29)/2</f>
+      <c r="D34" s="2">
+        <f>N18</f>
+        <v>0</v>
+      </c>
+      <c r="E34" s="2">
+        <f>ATAN(-2*D34/(B34-C34))/2</f>
+        <v>0</v>
+      </c>
+      <c r="F34" s="3">
+        <f>E34*180/PI()</f>
+        <v>0</v>
+      </c>
+      <c r="G34" s="3">
+        <f>(B34+C34)/2</f>
         <v>212500</v>
       </c>
-      <c r="H29" s="3">
-        <f>SQRT((B29-C29)^2/4+D29^2)</f>
+      <c r="H34" s="3">
+        <f>SQRT((B34-C34)^2/4+D34^2)</f>
         <v>100000</v>
       </c>
-      <c r="I29" s="3">
-        <f>G29+H29</f>
+      <c r="I34" s="3">
+        <f>G34+H34</f>
         <v>312500</v>
       </c>
-      <c r="J29" s="3">
-        <f>G29-H29</f>
+      <c r="J34" s="3">
+        <f>G34-H34</f>
         <v>112500</v>
       </c>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="C31" s="2">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="C36" s="2">
         <f>7530000/300/500</f>
         <v>50.2</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B34" s="2" t="s">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B39" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C34" s="2" t="s">
+      <c r="C39" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D34" s="2" t="s">
+      <c r="D39" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="E34" s="2" t="s">
+      <c r="E39" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="F34" s="2" t="s">
+      <c r="F39" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="G34" s="2" t="s">
+      <c r="G39" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="H34" s="2" t="s">
+      <c r="H39" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="I34" s="2" t="s">
+      <c r="I39" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="J34" s="2" t="s">
+      <c r="J39" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="K34" s="2" t="s">
+      <c r="K39" s="2" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A35" s="1">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A40" s="1">
         <v>1</v>
       </c>
-      <c r="B35" s="2">
+      <c r="B40" s="2">
         <f>250/2</f>
         <v>125</v>
       </c>
-      <c r="C35" s="2">
+      <c r="C40" s="2">
         <f>500/2</f>
         <v>250</v>
       </c>
-      <c r="D35" s="2">
+      <c r="D40" s="2">
         <f>50/2</f>
         <v>25</v>
       </c>
-      <c r="E35" s="2">
-        <f t="shared" ref="E35:E43" si="13">C35/2-D35</f>
+      <c r="E40" s="2">
+        <f t="shared" ref="E40:E48" si="13">C40/2-D40</f>
         <v>100</v>
       </c>
-      <c r="F35" s="2">
+      <c r="F40" s="2">
         <f>1200*1000</f>
         <v>1200000</v>
       </c>
-      <c r="G35" s="2">
-        <f>B35*D35*(E35+D35/2)</f>
+      <c r="G40" s="2">
+        <f>B40*D40*(E40+D40/2)</f>
         <v>351562.5</v>
       </c>
-      <c r="H35" s="2">
-        <f t="shared" ref="H35:H43" si="14">B35*C35^3/12</f>
+      <c r="H40" s="2">
+        <f t="shared" ref="H40:H48" si="14">B40*C40^3/12</f>
         <v>162760416.66666666</v>
       </c>
-      <c r="I35" s="2">
-        <f>F35*G35/H35/B35</f>
+      <c r="I40" s="2">
+        <f>F40*G40/H40/B40</f>
         <v>20.736000000000001</v>
       </c>
-      <c r="J35" s="5">
+      <c r="J40" s="5">
         <f>250000000</f>
         <v>250000000</v>
       </c>
-      <c r="K35" s="3">
-        <f>J35/H35*E35</f>
+      <c r="K40" s="3">
+        <f>J40/H40*E40</f>
         <v>153.6</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A36" s="1">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A41" s="1">
         <v>2</v>
       </c>
-      <c r="B36" s="2">
+      <c r="B41" s="2">
         <f>250/2</f>
         <v>125</v>
       </c>
-      <c r="C36" s="2">
+      <c r="C41" s="2">
         <f>500/2</f>
         <v>250</v>
       </c>
-      <c r="D36" s="2">
-        <f>C36/2</f>
+      <c r="D41" s="2">
+        <f>C41/2</f>
         <v>125</v>
       </c>
-      <c r="E36" s="2">
+      <c r="E41" s="2">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
-      <c r="F36" s="2">
+      <c r="F41" s="2">
         <f>1200*1000</f>
         <v>1200000</v>
       </c>
-      <c r="G36" s="2">
-        <f>B36*D36*(E36+D36/2)</f>
+      <c r="G41" s="2">
+        <f>B41*D41*(E41+D41/2)</f>
         <v>976562.5</v>
       </c>
-      <c r="H36" s="2">
+      <c r="H41" s="2">
         <f t="shared" si="14"/>
         <v>162760416.66666666</v>
       </c>
-      <c r="I36" s="2">
-        <f>F36*G36/H36/B36</f>
+      <c r="I41" s="2">
+        <f>F41*G41/H41/B41</f>
         <v>57.6</v>
       </c>
-      <c r="J36" s="5">
-        <f t="shared" ref="J36:J37" si="15">250000000</f>
+      <c r="J41" s="5">
+        <f t="shared" ref="J41:J42" si="15">250000000</f>
         <v>250000000</v>
       </c>
-      <c r="K36" s="3">
-        <f t="shared" ref="K36:K37" si="16">J36/H36*E36</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A37" s="1">
+      <c r="K41" s="3">
+        <f t="shared" ref="K41:K42" si="16">J41/H41*E41</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A42" s="1">
         <v>3</v>
       </c>
-      <c r="B37" s="2">
+      <c r="B42" s="2">
         <f>250/2</f>
         <v>125</v>
       </c>
-      <c r="C37" s="2">
+      <c r="C42" s="2">
         <f>500/2</f>
         <v>250</v>
       </c>
-      <c r="D37" s="2">
-        <v>0</v>
-      </c>
-      <c r="E37" s="2">
+      <c r="D42" s="2">
+        <v>0</v>
+      </c>
+      <c r="E42" s="2">
         <f t="shared" si="13"/>
         <v>125</v>
       </c>
-      <c r="F37" s="2">
+      <c r="F42" s="2">
         <f>1200*1000</f>
         <v>1200000</v>
       </c>
-      <c r="G37" s="2">
-        <f>B37*D37*(E37+D37/2)</f>
-        <v>0</v>
-      </c>
-      <c r="H37" s="2">
+      <c r="G42" s="2">
+        <f>B42*D42*(E42+D42/2)</f>
+        <v>0</v>
+      </c>
+      <c r="H42" s="2">
         <f t="shared" si="14"/>
         <v>162760416.66666666</v>
       </c>
-      <c r="I37" s="2">
-        <f>F37*G37/H37/B37</f>
-        <v>0</v>
-      </c>
-      <c r="J37" s="5">
+      <c r="I42" s="2">
+        <f>F42*G42/H42/B42</f>
+        <v>0</v>
+      </c>
+      <c r="J42" s="5">
         <f t="shared" si="15"/>
         <v>250000000</v>
       </c>
-      <c r="K37" s="3">
+      <c r="K42" s="3">
         <f t="shared" si="16"/>
         <v>192</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A38" s="1">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A43" s="1">
         <v>4</v>
       </c>
-      <c r="B38" s="2">
+      <c r="B43" s="2">
         <v>50</v>
       </c>
-      <c r="C38" s="2">
+      <c r="C43" s="2">
         <v>120</v>
       </c>
-      <c r="D38" s="2">
-        <f>C38/2</f>
+      <c r="D43" s="2">
+        <f>C43/2</f>
         <v>60</v>
       </c>
-      <c r="E38" s="2">
+      <c r="E43" s="2">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
-      <c r="F38" s="2">
+      <c r="F43" s="2">
         <f>75*1000</f>
         <v>75000</v>
       </c>
-      <c r="G38" s="2">
-        <f>B38*D38*(E38+D38/2)</f>
+      <c r="G43" s="2">
+        <f>B43*D43*(E43+D43/2)</f>
         <v>90000</v>
       </c>
-      <c r="H38" s="2">
+      <c r="H43" s="2">
         <f t="shared" si="14"/>
         <v>7200000</v>
       </c>
-      <c r="I38" s="2">
-        <f>F38*G38/H38/B38</f>
+      <c r="I43" s="2">
+        <f>F43*G43/H43/B43</f>
         <v>18.75</v>
       </c>
-      <c r="J38" s="5"/>
-      <c r="K38" s="3"/>
-    </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A39" s="1">
+      <c r="J43" s="5"/>
+      <c r="K43" s="3"/>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A44" s="1">
         <v>5</v>
       </c>
-      <c r="B39" s="2">
+      <c r="B44" s="2">
         <v>400</v>
       </c>
-      <c r="C39" s="2">
+      <c r="C44" s="2">
         <v>600</v>
       </c>
-      <c r="D39" s="2">
+      <c r="D44" s="2">
         <v>300</v>
       </c>
-      <c r="E39" s="2">
+      <c r="E44" s="2">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
-      <c r="F39" s="2">
+      <c r="F44" s="2">
         <v>500000</v>
       </c>
-      <c r="G39" s="2">
-        <f>B39*D39*(E39+D39/2)</f>
+      <c r="G44" s="2">
+        <f>B44*D44*(E44+D44/2)</f>
         <v>18000000</v>
       </c>
-      <c r="H39" s="2">
+      <c r="H44" s="2">
         <f t="shared" si="14"/>
         <v>7200000000</v>
       </c>
-      <c r="I39" s="2">
-        <f>F39*G39/H39/B39</f>
+      <c r="I44" s="2">
+        <f>F44*G44/H44/B44</f>
         <v>3.125</v>
       </c>
-      <c r="J39" s="5"/>
-      <c r="K39" s="3"/>
-    </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A40" s="1">
+      <c r="J44" s="5"/>
+      <c r="K44" s="3"/>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A45" s="1">
         <v>5</v>
       </c>
-      <c r="B40" s="2">
+      <c r="B45" s="2">
         <v>400</v>
       </c>
-      <c r="C40" s="2">
+      <c r="C45" s="2">
         <v>600</v>
       </c>
-      <c r="D40" s="2">
-        <v>0</v>
-      </c>
-      <c r="E40" s="2">
+      <c r="D45" s="2">
+        <v>0</v>
+      </c>
+      <c r="E45" s="2">
         <f t="shared" si="13"/>
         <v>300</v>
       </c>
-      <c r="H40" s="2">
+      <c r="H45" s="2">
         <f t="shared" si="14"/>
         <v>7200000000</v>
       </c>
-      <c r="J40" s="5">
+      <c r="J45" s="5">
         <f>750000000</f>
         <v>750000000</v>
       </c>
-      <c r="K40" s="3">
-        <f t="shared" ref="K40" si="17">J40/H40*E40</f>
+      <c r="K45" s="3">
+        <f t="shared" ref="K45" si="17">J45/H45*E45</f>
         <v>31.25</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A41" s="1">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A46" s="1">
         <v>6</v>
       </c>
-      <c r="B41" s="2">
+      <c r="B46" s="2">
         <v>300</v>
       </c>
-      <c r="C41" s="2">
+      <c r="C46" s="2">
         <v>500</v>
       </c>
-      <c r="D41" s="2">
+      <c r="D46" s="2">
         <v>250</v>
       </c>
-      <c r="E41" s="2">
+      <c r="E46" s="2">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
-      <c r="F41" s="2">
+      <c r="F46" s="2">
         <v>2000000</v>
       </c>
-      <c r="G41" s="2">
-        <f>B41*D41*(E41+D41/2)</f>
+      <c r="G46" s="2">
+        <f>B46*D46*(E46+D46/2)</f>
         <v>9375000</v>
       </c>
-      <c r="H41" s="2">
+      <c r="H46" s="2">
         <f t="shared" si="14"/>
         <v>3125000000</v>
       </c>
-      <c r="I41" s="2">
-        <f>F41*G41/H41/B41</f>
+      <c r="I46" s="2">
+        <f>F46*G46/H46/B46</f>
         <v>20</v>
       </c>
-      <c r="J41" s="5"/>
-      <c r="K41" s="3"/>
-    </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A42" s="1">
+      <c r="J46" s="5"/>
+      <c r="K46" s="3"/>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A47" s="1">
         <v>6</v>
       </c>
-      <c r="B42" s="2">
+      <c r="B47" s="2">
         <v>300</v>
       </c>
-      <c r="C42" s="2">
+      <c r="C47" s="2">
         <v>500</v>
       </c>
-      <c r="D42" s="2">
-        <v>0</v>
-      </c>
-      <c r="E42" s="2">
+      <c r="D47" s="2">
+        <v>0</v>
+      </c>
+      <c r="E47" s="2">
         <f t="shared" si="13"/>
         <v>250</v>
       </c>
-      <c r="H42" s="2">
+      <c r="H47" s="2">
         <f t="shared" si="14"/>
         <v>3125000000</v>
       </c>
-      <c r="J42" s="5">
+      <c r="J47" s="5">
         <f>6000000000</f>
         <v>6000000000</v>
       </c>
-      <c r="K42" s="3">
-        <f t="shared" ref="K42:K43" si="18">J42/H42*E42</f>
+      <c r="K47" s="3">
+        <f t="shared" ref="K47:K48" si="18">J47/H47*E47</f>
         <v>480</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A43" s="1">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A48" s="1">
         <v>7</v>
       </c>
-      <c r="B43" s="2">
+      <c r="B48" s="2">
         <v>240</v>
       </c>
-      <c r="C43" s="2">
+      <c r="C48" s="2">
         <v>360</v>
       </c>
-      <c r="D43" s="2">
-        <f>C43/2-40</f>
+      <c r="D48" s="2">
+        <f>C48/2-40</f>
         <v>140</v>
       </c>
-      <c r="E43" s="2">
+      <c r="E48" s="2">
         <f t="shared" si="13"/>
         <v>40</v>
       </c>
-      <c r="F43" s="2">
+      <c r="F48" s="2">
         <f>240*1000</f>
         <v>240000</v>
       </c>
-      <c r="G43" s="2">
-        <f>B43*D43*(E43+D43/2)</f>
+      <c r="G48" s="2">
+        <f>B48*D48*(E48+D48/2)</f>
         <v>3696000</v>
       </c>
-      <c r="H43" s="2">
+      <c r="H48" s="2">
         <f t="shared" si="14"/>
         <v>933120000</v>
       </c>
-      <c r="I43" s="2">
-        <f t="shared" ref="I43:I52" si="19">F43*G43/H43/B43</f>
+      <c r="I48" s="2">
+        <f t="shared" ref="I48:I57" si="19">F48*G48/H48/B48</f>
         <v>3.9609053497942388</v>
       </c>
-      <c r="J43" s="5">
+      <c r="J48" s="5">
         <v>720000000</v>
       </c>
-      <c r="K43" s="3">
+      <c r="K48" s="3">
         <f t="shared" si="18"/>
         <v>30.864197530864196</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A44" s="1">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A49" s="1">
         <v>8</v>
       </c>
-      <c r="B44" s="2">
+      <c r="B49" s="2">
         <v>300</v>
       </c>
-      <c r="C44" s="2">
+      <c r="C49" s="2">
         <v>500</v>
       </c>
-      <c r="D44" s="2">
+      <c r="D49" s="2">
         <v>250</v>
       </c>
-      <c r="E44" s="2">
-        <f t="shared" ref="E44" si="20">C44/2-D44</f>
-        <v>0</v>
-      </c>
-      <c r="F44" s="2">
+      <c r="E49" s="2">
+        <f t="shared" ref="E49" si="20">C49/2-D49</f>
+        <v>0</v>
+      </c>
+      <c r="F49" s="2">
         <v>753000</v>
       </c>
-      <c r="G44" s="2">
-        <f>B44*D44*(E44+D44/2)</f>
+      <c r="G49" s="2">
+        <f>B49*D49*(E49+D49/2)</f>
         <v>9375000</v>
       </c>
-      <c r="H44" s="2">
-        <f t="shared" ref="H44" si="21">B44*C44^3/12</f>
+      <c r="H49" s="2">
+        <f t="shared" ref="H49" si="21">B49*C49^3/12</f>
         <v>3125000000</v>
       </c>
-      <c r="I44" s="2">
+      <c r="I49" s="2">
         <f t="shared" si="19"/>
         <v>7.53</v>
       </c>
-      <c r="J44" s="5"/>
-      <c r="K44" s="3"/>
-    </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A45" s="1">
+      <c r="J49" s="5"/>
+      <c r="K49" s="3"/>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A50" s="1">
         <v>9</v>
       </c>
-      <c r="B45" s="2">
+      <c r="B50" s="2">
         <v>10</v>
       </c>
-      <c r="F45" s="2">
+      <c r="F50" s="2">
         <v>92650</v>
       </c>
-      <c r="G45" s="2">
+      <c r="G50" s="2">
         <f>100*20*70+10*60*30</f>
         <v>158000</v>
       </c>
-      <c r="H45" s="2">
+      <c r="H50" s="2">
         <f>100*160^3/12-90*120^3/12</f>
         <v>21173333.333333336</v>
       </c>
-      <c r="I45" s="3">
+      <c r="I50" s="3">
         <f t="shared" si="19"/>
         <v>69.137437027707804</v>
       </c>
-      <c r="J45" s="5"/>
-      <c r="K45" s="3"/>
-    </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A46" s="1">
+      <c r="J50" s="5"/>
+      <c r="K50" s="3"/>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A51" s="1">
         <v>10</v>
       </c>
-      <c r="B46" s="2">
+      <c r="B51" s="2">
         <v>10</v>
       </c>
-      <c r="F46" s="2">
+      <c r="F51" s="2">
         <v>92650</v>
       </c>
-      <c r="G46" s="2">
+      <c r="G51" s="2">
         <f>100*20*70+10*30*45</f>
         <v>153500</v>
       </c>
-      <c r="H46" s="2">
+      <c r="H51" s="2">
         <f>100*160^3/12-90*120^3/12</f>
         <v>21173333.333333336</v>
       </c>
-      <c r="I46" s="3">
+      <c r="I51" s="3">
         <f t="shared" si="19"/>
         <v>67.168332808564216</v>
       </c>
-      <c r="J46" s="5"/>
-      <c r="K46" s="3"/>
-    </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A47" s="1">
+      <c r="J51" s="5"/>
+      <c r="K51" s="3"/>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A52" s="1">
         <v>11</v>
       </c>
-      <c r="B47" s="2">
+      <c r="B52" s="2">
         <v>200</v>
       </c>
-      <c r="C47" s="2">
+      <c r="C52" s="2">
         <v>360</v>
       </c>
-      <c r="D47" s="2">
-        <v>0</v>
-      </c>
-      <c r="E47" s="2">
-        <f t="shared" ref="E47" si="22">C47/2-D47</f>
+      <c r="D52" s="2">
+        <v>0</v>
+      </c>
+      <c r="E52" s="2">
+        <f t="shared" ref="E52" si="22">C52/2-D52</f>
         <v>180</v>
       </c>
-      <c r="G47" s="2">
-        <f t="shared" ref="G47:G52" si="23">B47*D47*(E47+D47/2)</f>
-        <v>0</v>
-      </c>
-      <c r="H47" s="2">
-        <f t="shared" ref="H47" si="24">B47*C47^3/12</f>
+      <c r="G52" s="2">
+        <f t="shared" ref="G52:G57" si="23">B52*D52*(E52+D52/2)</f>
+        <v>0</v>
+      </c>
+      <c r="H52" s="2">
+        <f t="shared" ref="H52" si="24">B52*C52^3/12</f>
         <v>777600000</v>
       </c>
-      <c r="I47" s="2">
+      <c r="I52" s="2">
         <f t="shared" si="19"/>
         <v>0</v>
       </c>
-      <c r="J47" s="5">
+      <c r="J52" s="5">
         <f>350*1000000</f>
         <v>350000000</v>
       </c>
-      <c r="K47" s="3">
-        <f t="shared" ref="K47" si="25">J47/H47*E47</f>
+      <c r="K52" s="3">
+        <f t="shared" ref="K52" si="25">J52/H52*E52</f>
         <v>81.018518518518519</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A48" s="1">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A53" s="1">
         <v>11</v>
       </c>
-      <c r="B48" s="2">
+      <c r="B53" s="2">
         <v>200</v>
       </c>
-      <c r="C48" s="2">
+      <c r="C53" s="2">
         <v>360</v>
       </c>
-      <c r="D48" s="2">
-        <f>C48/2</f>
+      <c r="D53" s="2">
+        <f>C53/2</f>
         <v>180</v>
       </c>
-      <c r="E48" s="2">
-        <f t="shared" ref="E48:E49" si="26">C48/2-D48</f>
-        <v>0</v>
-      </c>
-      <c r="G48" s="2">
+      <c r="E53" s="2">
+        <f t="shared" ref="E53:E54" si="26">C53/2-D53</f>
+        <v>0</v>
+      </c>
+      <c r="G53" s="2">
         <f t="shared" si="23"/>
         <v>3240000</v>
       </c>
-      <c r="H48" s="2">
-        <f t="shared" ref="H48:H49" si="27">B48*C48^3/12</f>
+      <c r="H53" s="2">
+        <f t="shared" ref="H53:H54" si="27">B53*C53^3/12</f>
         <v>777600000</v>
       </c>
-      <c r="I48" s="2">
+      <c r="I53" s="2">
         <f t="shared" si="19"/>
         <v>0</v>
       </c>
-      <c r="J48" s="5">
+      <c r="J53" s="5">
         <f>350*1000000</f>
         <v>350000000</v>
       </c>
-      <c r="K48" s="3">
-        <f t="shared" ref="K48:K49" si="28">J48/H48*E48</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A49" s="1">
+      <c r="K53" s="3">
+        <f t="shared" ref="K53:K54" si="28">J53/H53*E53</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A54" s="1">
         <v>12</v>
       </c>
-      <c r="B49" s="2">
+      <c r="B54" s="2">
         <v>100</v>
       </c>
-      <c r="C49" s="2">
+      <c r="C54" s="2">
         <v>220</v>
       </c>
-      <c r="D49" s="2">
-        <v>0</v>
-      </c>
-      <c r="E49" s="2">
+      <c r="D54" s="2">
+        <v>0</v>
+      </c>
+      <c r="E54" s="2">
         <f t="shared" si="26"/>
         <v>110</v>
       </c>
-      <c r="G49" s="2">
+      <c r="G54" s="2">
         <f t="shared" si="23"/>
         <v>0</v>
       </c>
-      <c r="H49" s="2">
+      <c r="H54" s="2">
         <f t="shared" si="27"/>
         <v>88733333.333333328</v>
       </c>
-      <c r="I49" s="2">
+      <c r="I54" s="2">
         <f t="shared" si="19"/>
         <v>0</v>
       </c>
-      <c r="J49" s="5">
+      <c r="J54" s="5">
         <f>76.3*1000000</f>
         <v>76300000</v>
       </c>
-      <c r="K49" s="3">
+      <c r="K54" s="3">
         <f t="shared" si="28"/>
         <v>94.586776859504141</v>
       </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A50" s="1">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A55" s="1">
         <v>12</v>
       </c>
-      <c r="B50" s="2">
+      <c r="B55" s="2">
         <v>100</v>
       </c>
-      <c r="C50" s="2">
+      <c r="C55" s="2">
         <v>220</v>
       </c>
-      <c r="D50" s="2">
+      <c r="D55" s="2">
         <v>35</v>
       </c>
-      <c r="E50" s="2">
-        <f t="shared" ref="E50:E51" si="29">C50/2-D50</f>
+      <c r="E55" s="2">
+        <f t="shared" ref="E55:E56" si="29">C55/2-D55</f>
         <v>75</v>
       </c>
-      <c r="G50" s="2">
+      <c r="G55" s="2">
         <f t="shared" si="23"/>
         <v>323750</v>
       </c>
-      <c r="H50" s="2">
-        <f t="shared" ref="H50:H51" si="30">B50*C50^3/12</f>
+      <c r="H55" s="2">
+        <f t="shared" ref="H55:H56" si="30">B55*C55^3/12</f>
         <v>88733333.333333328</v>
       </c>
-      <c r="I50" s="2">
+      <c r="I55" s="2">
         <f t="shared" si="19"/>
         <v>0</v>
       </c>
-      <c r="J50" s="5">
-        <f t="shared" ref="J50:J52" si="31">76.3*1000000</f>
+      <c r="J55" s="5">
+        <f t="shared" ref="J55:J57" si="31">76.3*1000000</f>
         <v>76300000</v>
       </c>
-      <c r="K50" s="3">
-        <f t="shared" ref="K50:K51" si="32">J50/H50*E50</f>
+      <c r="K55" s="3">
+        <f t="shared" ref="K55:K56" si="32">J55/H55*E55</f>
         <v>64.490984222389187</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A51" s="1">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A56" s="1">
         <v>12</v>
       </c>
-      <c r="B51" s="2">
+      <c r="B56" s="2">
         <v>100</v>
       </c>
-      <c r="C51" s="2">
+      <c r="C56" s="2">
         <v>220</v>
       </c>
-      <c r="D51" s="2">
+      <c r="D56" s="2">
         <v>60</v>
       </c>
-      <c r="E51" s="2">
+      <c r="E56" s="2">
         <f t="shared" si="29"/>
         <v>50</v>
       </c>
-      <c r="G51" s="2">
+      <c r="G56" s="2">
         <f t="shared" si="23"/>
         <v>480000</v>
       </c>
-      <c r="H51" s="2">
+      <c r="H56" s="2">
         <f t="shared" si="30"/>
         <v>88733333.333333328</v>
       </c>
-      <c r="I51" s="2">
+      <c r="I56" s="2">
         <f t="shared" si="19"/>
         <v>0</v>
       </c>
-      <c r="J51" s="5">
+      <c r="J56" s="5">
         <f t="shared" si="31"/>
         <v>76300000</v>
       </c>
-      <c r="K51" s="3">
+      <c r="K56" s="3">
         <f t="shared" si="32"/>
         <v>42.993989481592791</v>
       </c>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A52" s="1">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A57" s="1">
         <v>12</v>
       </c>
-      <c r="B52" s="2">
+      <c r="B57" s="2">
         <v>100</v>
       </c>
-      <c r="C52" s="2">
+      <c r="C57" s="2">
         <v>220</v>
       </c>
-      <c r="D52" s="2">
+      <c r="D57" s="2">
         <v>85</v>
       </c>
-      <c r="E52" s="2">
-        <f t="shared" ref="E52" si="33">C52/2-D52</f>
+      <c r="E57" s="2">
+        <f t="shared" ref="E57" si="33">C57/2-D57</f>
         <v>25</v>
       </c>
-      <c r="G52" s="2">
+      <c r="G57" s="2">
         <f t="shared" si="23"/>
         <v>573750</v>
       </c>
-      <c r="H52" s="2">
-        <f t="shared" ref="H52" si="34">B52*C52^3/12</f>
+      <c r="H57" s="2">
+        <f t="shared" ref="H57" si="34">B57*C57^3/12</f>
         <v>88733333.333333328</v>
       </c>
-      <c r="I52" s="2">
+      <c r="I57" s="2">
         <f t="shared" si="19"/>
         <v>0</v>
       </c>
-      <c r="J52" s="5">
+      <c r="J57" s="5">
         <f t="shared" si="31"/>
         <v>76300000</v>
       </c>
-      <c r="K52" s="3">
-        <f t="shared" ref="K52" si="35">J52/H52*E52</f>
+      <c r="K57" s="3">
+        <f t="shared" ref="K57" si="35">J57/H57*E57</f>
         <v>21.496994740796396</v>
       </c>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A53" s="1">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A58" s="1">
         <v>13</v>
       </c>
-      <c r="B53" s="2">
+      <c r="B58" s="2">
         <v>10</v>
       </c>
-      <c r="E53" s="2">
-        <v>0</v>
-      </c>
-      <c r="H53" s="2">
+      <c r="E58" s="2">
+        <v>0</v>
+      </c>
+      <c r="H58" s="2">
         <f>100*160^3/12-90*120^3/12</f>
         <v>21173333.333333336</v>
       </c>
-      <c r="J53" s="5">
+      <c r="J58" s="5">
         <f>73*1000000</f>
         <v>73000000</v>
       </c>
-      <c r="K53" s="3">
-        <f t="shared" ref="K53:K54" si="36">J53/H53*E53</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A54" s="1">
+      <c r="K58" s="3">
+        <f t="shared" ref="K58:K59" si="36">J58/H58*E58</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A59" s="1">
         <v>13</v>
       </c>
-      <c r="B54" s="2">
+      <c r="B59" s="2">
         <v>10</v>
       </c>
-      <c r="E54" s="2">
+      <c r="E59" s="2">
         <v>30</v>
       </c>
-      <c r="H54" s="2">
+      <c r="H59" s="2">
         <f>100*160^3/12-90*120^3/12</f>
         <v>21173333.333333336</v>
       </c>
-      <c r="J54" s="5">
+      <c r="J59" s="5">
         <f>73*1000000</f>
         <v>73000000</v>
       </c>
-      <c r="K54" s="3">
+      <c r="K59" s="3">
         <f t="shared" si="36"/>
         <v>103.43198992443322</v>
       </c>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A55" s="1">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A60" s="1">
         <v>13</v>
       </c>
-      <c r="B55" s="2">
+      <c r="B60" s="2">
         <v>10</v>
       </c>
-      <c r="E55" s="2">
+      <c r="E60" s="2">
         <v>60</v>
       </c>
-      <c r="H55" s="2">
+      <c r="H60" s="2">
         <f>100*160^3/12-90*120^3/12</f>
         <v>21173333.333333336</v>
       </c>
-      <c r="J55" s="5">
+      <c r="J60" s="5">
         <f>73*1000000</f>
         <v>73000000</v>
       </c>
-      <c r="K55" s="3">
-        <f t="shared" ref="K55:K59" si="37">J55/H55*E55</f>
+      <c r="K60" s="3">
+        <f t="shared" ref="K60:K64" si="37">J60/H60*E60</f>
         <v>206.86397984886645</v>
       </c>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A56" s="1">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A61" s="1">
         <v>13</v>
       </c>
-      <c r="B56" s="2">
+      <c r="B61" s="2">
         <v>10</v>
       </c>
-      <c r="E56" s="2">
+      <c r="E61" s="2">
         <v>80</v>
       </c>
-      <c r="H56" s="2">
+      <c r="H61" s="2">
         <f>100*160^3/12-90*120^3/12</f>
         <v>21173333.333333336</v>
       </c>
-      <c r="J56" s="5">
+      <c r="J61" s="5">
         <f>73*1000000</f>
         <v>73000000</v>
       </c>
-      <c r="K56" s="3">
+      <c r="K61" s="3">
         <f t="shared" si="37"/>
         <v>275.81863979848862</v>
       </c>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A57" s="1">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A62" s="1">
         <v>14</v>
       </c>
-      <c r="B57" s="2">
+      <c r="B62" s="2">
         <v>200</v>
       </c>
-      <c r="C57" s="2">
+      <c r="C62" s="2">
         <v>360</v>
       </c>
-      <c r="D57" s="2">
-        <v>0</v>
-      </c>
-      <c r="E57" s="2">
-        <f t="shared" ref="E57:E58" si="38">C57/2-D57</f>
+      <c r="D62" s="2">
+        <v>0</v>
+      </c>
+      <c r="E62" s="2">
+        <f t="shared" ref="E62:E63" si="38">C62/2-D62</f>
         <v>180</v>
       </c>
-      <c r="F57" s="2">
+      <c r="F62" s="2">
         <f>80*4/2*1000</f>
         <v>160000</v>
       </c>
-      <c r="G57" s="2">
-        <f>B57*D57*(E57+D57/2)</f>
-        <v>0</v>
-      </c>
-      <c r="H57" s="2">
-        <f t="shared" ref="H57" si="39">B57*C57^3/12</f>
+      <c r="G62" s="2">
+        <f>B62*D62*(E62+D62/2)</f>
+        <v>0</v>
+      </c>
+      <c r="H62" s="2">
+        <f t="shared" ref="H62" si="39">B62*C62^3/12</f>
         <v>777600000</v>
       </c>
-      <c r="I57" s="3">
-        <f>F57*G57/H57/B57</f>
-        <v>0</v>
-      </c>
-      <c r="J57" s="5">
+      <c r="I62" s="3">
+        <f>F62*G62/H62/B62</f>
+        <v>0</v>
+      </c>
+      <c r="J62" s="5">
         <f>80*4^2/8*1000000</f>
         <v>160000000</v>
       </c>
-      <c r="K57" s="3">
-        <f t="shared" ref="K57" si="40">J57/H57*E57</f>
+      <c r="K62" s="3">
+        <f t="shared" ref="K62" si="40">J62/H62*E62</f>
         <v>37.037037037037038</v>
       </c>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A58" s="1">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A63" s="1">
         <v>14</v>
       </c>
-      <c r="B58" s="2">
+      <c r="B63" s="2">
         <v>200</v>
       </c>
-      <c r="C58" s="2">
+      <c r="C63" s="2">
         <v>360</v>
       </c>
-      <c r="D58" s="2">
-        <f>C58/2</f>
+      <c r="D63" s="2">
+        <f>C63/2</f>
         <v>180</v>
       </c>
-      <c r="E58" s="2">
+      <c r="E63" s="2">
         <f t="shared" si="38"/>
         <v>0</v>
       </c>
-      <c r="F58" s="2">
+      <c r="F63" s="2">
         <f>80*4/2*1000</f>
         <v>160000</v>
       </c>
-      <c r="G58" s="2">
-        <f>B58*D58*(E58+D58/2)</f>
+      <c r="G63" s="2">
+        <f>B63*D63*(E63+D63/2)</f>
         <v>3240000</v>
       </c>
-      <c r="H58" s="2">
-        <f t="shared" ref="H58:H59" si="41">B58*C58^3/12</f>
+      <c r="H63" s="2">
+        <f t="shared" ref="H63:H64" si="41">B63*C63^3/12</f>
         <v>777600000</v>
       </c>
-      <c r="I58" s="3">
-        <f>F58*G58/H58/B58</f>
+      <c r="I63" s="3">
+        <f>F63*G63/H63/B63</f>
         <v>3.333333333333333</v>
       </c>
-      <c r="J58" s="5">
+      <c r="J63" s="5">
         <f>80*4^2/8*1000000</f>
         <v>160000000</v>
       </c>
-      <c r="K58" s="3">
+      <c r="K63" s="3">
         <f t="shared" si="37"/>
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A59" s="1">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A64" s="1">
         <v>15</v>
       </c>
-      <c r="B59" s="2">
+      <c r="B64" s="2">
         <v>360</v>
       </c>
-      <c r="C59" s="2">
+      <c r="C64" s="2">
         <v>600</v>
       </c>
-      <c r="D59" s="2">
-        <f>C59/2-50</f>
+      <c r="D64" s="2">
+        <f>C64/2-50</f>
         <v>250</v>
       </c>
-      <c r="E59" s="2">
-        <f t="shared" ref="E59" si="42">C59/2-D59</f>
+      <c r="E64" s="2">
+        <f t="shared" ref="E64" si="42">C64/2-D64</f>
         <v>50</v>
       </c>
-      <c r="F59" s="2">
+      <c r="F64" s="2">
         <f>350*6*1000</f>
         <v>2100000</v>
       </c>
-      <c r="G59" s="2">
-        <f>B59*D59*(E59+D59/2)</f>
+      <c r="G64" s="2">
+        <f>B64*D64*(E64+D64/2)</f>
         <v>15750000</v>
       </c>
-      <c r="H59" s="5">
+      <c r="H64" s="5">
         <f t="shared" si="41"/>
         <v>6480000000</v>
       </c>
-      <c r="I59" s="3">
-        <f>F59*G59/H59/B59</f>
+      <c r="I64" s="3">
+        <f>F64*G64/H64/B64</f>
         <v>14.178240740740742</v>
       </c>
-      <c r="J59" s="5">
+      <c r="J64" s="5">
         <f>350*6*3*1000000</f>
         <v>6300000000</v>
       </c>
-      <c r="K59" s="3">
+      <c r="K64" s="3">
         <f t="shared" si="37"/>
         <v>48.611111111111107</v>
       </c>
     </row>
-    <row r="66" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="B66" s="2" t="s">
+    <row r="71" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B71" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="C66" s="2" t="s">
+      <c r="C71" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="D66" s="2" t="s">
+      <c r="D71" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="E66" s="2" t="s">
+      <c r="E71" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="F66" s="2" t="s">
+      <c r="F71" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="G66" s="2" t="s">
+      <c r="G71" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="H66" s="2" t="s">
+      <c r="H71" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="I66" s="2" t="s">
+      <c r="I71" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="J66" s="2" t="s">
+      <c r="J71" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="K66" s="2" t="s">
+      <c r="K71" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="L66" s="2" t="s">
+      <c r="L71" s="2" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="67" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A67" s="1">
+    <row r="72" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A72" s="1">
         <v>1</v>
       </c>
-      <c r="B67" s="3">
+      <c r="B72" s="3">
         <v>1000</v>
       </c>
-      <c r="C67" s="3">
+      <c r="C72" s="3">
         <v>500</v>
       </c>
-      <c r="D67" s="3">
+      <c r="D72" s="3">
         <v>-50</v>
       </c>
-      <c r="E67" s="3">
-        <f t="shared" ref="E67:E73" si="43">ATAN(-2*D67/(B67-C67))/2</f>
+      <c r="E72" s="3">
+        <f t="shared" ref="E72:E78" si="43">ATAN(-2*D72/(B72-C72))/2</f>
         <v>9.8697779924940388E-2</v>
       </c>
-      <c r="F67" s="3">
-        <f t="shared" ref="F67:F73" si="44">E67*180/PI()</f>
+      <c r="F72" s="3">
+        <f t="shared" ref="F72:F78" si="44">E72*180/PI()</f>
         <v>5.6549662370101066</v>
       </c>
-      <c r="G67" s="3">
-        <f t="shared" ref="G67:G73" si="45">(B67+C67)/2</f>
+      <c r="G72" s="3">
+        <f t="shared" ref="G72:G78" si="45">(B72+C72)/2</f>
         <v>750</v>
       </c>
-      <c r="H67" s="3">
-        <f t="shared" ref="H67:H73" si="46">SQRT((B67-C67)^2/4+D67^2)</f>
+      <c r="H72" s="3">
+        <f t="shared" ref="H72:H78" si="46">SQRT((B72-C72)^2/4+D72^2)</f>
         <v>254.95097567963924</v>
       </c>
-      <c r="I67" s="3">
-        <f t="shared" ref="I67:I73" si="47">G67+H67</f>
+      <c r="I72" s="3">
+        <f t="shared" ref="I72:I78" si="47">G72+H72</f>
         <v>1004.9509756796392</v>
       </c>
-      <c r="J67" s="3">
-        <f t="shared" ref="J67:J73" si="48">G67-H67</f>
+      <c r="J72" s="3">
+        <f t="shared" ref="J72:J78" si="48">G72-H72</f>
         <v>495.04902432036079</v>
       </c>
-      <c r="K67" s="3">
-        <f t="shared" ref="K67:K71" si="49">F67+45</f>
+      <c r="K72" s="3">
+        <f t="shared" ref="K72:K76" si="49">F72+45</f>
         <v>50.654966237010107</v>
       </c>
-      <c r="L67" s="3">
-        <f t="shared" ref="L67:L71" si="50">K67-90</f>
+      <c r="L72" s="3">
+        <f t="shared" ref="L72:L76" si="50">K72-90</f>
         <v>-39.345033762989893</v>
       </c>
-      <c r="M67" s="3"/>
-    </row>
-    <row r="68" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A68" s="1">
+      <c r="M72" s="3"/>
+    </row>
+    <row r="73" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A73" s="1">
         <v>2</v>
       </c>
-      <c r="B68" s="3">
+      <c r="B73" s="3">
         <v>5333333.3333333302</v>
       </c>
-      <c r="C68" s="3">
+      <c r="C73" s="3">
         <v>3333333.3333333302</v>
       </c>
-      <c r="D68" s="3">
+      <c r="D73" s="3">
         <v>-2400000</v>
       </c>
-      <c r="E68" s="3">
+      <c r="E73" s="3">
         <f t="shared" si="43"/>
         <v>0.5880026035475675</v>
       </c>
-      <c r="F68" s="3">
+      <c r="F73" s="3">
         <f t="shared" si="44"/>
         <v>33.690067525979785</v>
       </c>
-      <c r="G68" s="3">
+      <c r="G73" s="3">
         <f t="shared" si="45"/>
         <v>4333333.3333333302</v>
       </c>
-      <c r="H68" s="3">
+      <c r="H73" s="3">
         <f t="shared" si="46"/>
         <v>2600000</v>
       </c>
-      <c r="I68" s="3">
+      <c r="I73" s="3">
         <f t="shared" si="47"/>
         <v>6933333.3333333302</v>
       </c>
-      <c r="J68" s="3">
+      <c r="J73" s="3">
         <f t="shared" si="48"/>
         <v>1733333.3333333302</v>
       </c>
-      <c r="K68" s="3">
+      <c r="K73" s="3">
         <f t="shared" si="49"/>
         <v>78.690067525979785</v>
       </c>
-      <c r="L68" s="3">
+      <c r="L73" s="3">
         <f t="shared" si="50"/>
         <v>-11.309932474020215</v>
       </c>
-      <c r="M68" s="3"/>
-    </row>
-    <row r="69" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A69" s="1">
+      <c r="M73" s="3"/>
+    </row>
+    <row r="74" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A74" s="1">
         <v>3</v>
       </c>
-      <c r="B69" s="3">
+      <c r="B74" s="3">
         <v>532</v>
       </c>
-      <c r="C69" s="3">
+      <c r="C74" s="3">
         <v>740</v>
       </c>
-      <c r="D69" s="3">
+      <c r="D74" s="3">
         <v>345</v>
       </c>
-      <c r="E69" s="3">
+      <c r="E74" s="3">
         <f t="shared" si="43"/>
         <v>0.6390052264115833</v>
       </c>
-      <c r="F69" s="3">
+      <c r="F74" s="3">
         <f t="shared" si="44"/>
         <v>36.612302560185327</v>
       </c>
-      <c r="G69" s="3">
+      <c r="G74" s="3">
         <f t="shared" si="45"/>
         <v>636</v>
       </c>
-      <c r="H69" s="3">
+      <c r="H74" s="3">
         <f t="shared" si="46"/>
         <v>360.33456675706259</v>
       </c>
-      <c r="I69" s="3">
+      <c r="I74" s="3">
         <f t="shared" si="47"/>
         <v>996.33456675706259</v>
       </c>
-      <c r="J69" s="3">
+      <c r="J74" s="3">
         <f t="shared" si="48"/>
         <v>275.66543324293741</v>
       </c>
-      <c r="K69" s="3">
+      <c r="K74" s="3">
         <f t="shared" si="49"/>
         <v>81.612302560185327</v>
       </c>
-      <c r="L69" s="3">
+      <c r="L74" s="3">
         <f t="shared" si="50"/>
         <v>-8.3876974398146729</v>
       </c>
-      <c r="M69" s="3"/>
-    </row>
-    <row r="70" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A70" s="1">
+      <c r="M74" s="3"/>
+    </row>
+    <row r="75" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A75" s="1">
         <v>4</v>
       </c>
-      <c r="B70" s="3">
+      <c r="B75" s="3">
         <v>300</v>
       </c>
-      <c r="C70" s="3">
+      <c r="C75" s="3">
         <v>150</v>
       </c>
-      <c r="D70" s="3">
+      <c r="D75" s="3">
         <v>200</v>
       </c>
-      <c r="E70" s="3">
+      <c r="E75" s="3">
         <f t="shared" si="43"/>
         <v>-0.60601282826216218</v>
       </c>
-      <c r="F70" s="3">
+      <c r="F75" s="3">
         <f t="shared" si="44"/>
         <v>-34.721977390208266</v>
       </c>
-      <c r="G70" s="3">
+      <c r="G75" s="3">
         <f t="shared" si="45"/>
         <v>225</v>
       </c>
-      <c r="H70" s="3">
+      <c r="H75" s="3">
         <f t="shared" si="46"/>
         <v>213.60009363293827</v>
       </c>
-      <c r="I70" s="3">
+      <c r="I75" s="3">
         <f t="shared" si="47"/>
         <v>438.6000936329383</v>
       </c>
-      <c r="J70" s="3">
+      <c r="J75" s="3">
         <f t="shared" si="48"/>
         <v>11.399906367061732</v>
       </c>
-      <c r="K70" s="3">
+      <c r="K75" s="3">
         <f t="shared" si="49"/>
         <v>10.278022609791734</v>
       </c>
-      <c r="L70" s="3">
+      <c r="L75" s="3">
         <f t="shared" si="50"/>
         <v>-79.721977390208266</v>
       </c>
-      <c r="M70" s="3"/>
-    </row>
-    <row r="71" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A71" s="1">
+      <c r="M75" s="3"/>
+    </row>
+    <row r="76" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A76" s="1">
         <v>5</v>
       </c>
-      <c r="B71" s="3">
+      <c r="B76" s="3">
         <v>50</v>
       </c>
-      <c r="C71" s="3">
+      <c r="C76" s="3">
         <v>-10</v>
       </c>
-      <c r="D71" s="3">
+      <c r="D76" s="3">
         <v>40</v>
       </c>
-      <c r="E71" s="3">
+      <c r="E76" s="3">
         <f t="shared" si="43"/>
         <v>-0.46364760900080609</v>
       </c>
-      <c r="F71" s="3">
+      <c r="F76" s="3">
         <f t="shared" si="44"/>
         <v>-26.56505117707799</v>
       </c>
-      <c r="G71" s="3">
+      <c r="G76" s="3">
         <f t="shared" si="45"/>
         <v>20</v>
       </c>
-      <c r="H71" s="3">
+      <c r="H76" s="3">
         <f t="shared" si="46"/>
         <v>50</v>
       </c>
-      <c r="I71" s="3">
+      <c r="I76" s="3">
         <f t="shared" si="47"/>
         <v>70</v>
       </c>
-      <c r="J71" s="3">
+      <c r="J76" s="3">
         <f t="shared" si="48"/>
         <v>-30</v>
       </c>
-      <c r="K71" s="3">
+      <c r="K76" s="3">
         <f t="shared" si="49"/>
         <v>18.43494882292201</v>
       </c>
-      <c r="L71" s="3">
+      <c r="L76" s="3">
         <f t="shared" si="50"/>
         <v>-71.56505117707799</v>
       </c>
-      <c r="M71" s="3"/>
-    </row>
-    <row r="72" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A72" s="1">
+      <c r="M76" s="3"/>
+    </row>
+    <row r="77" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A77" s="1">
         <v>6</v>
       </c>
-      <c r="B72" s="3">
+      <c r="B77" s="3">
         <v>800</v>
       </c>
-      <c r="C72" s="3">
+      <c r="C77" s="3">
         <v>400</v>
       </c>
-      <c r="D72" s="3">
+      <c r="D77" s="3">
         <v>-550</v>
       </c>
-      <c r="E72" s="3">
+      <c r="E77" s="3">
         <f t="shared" si="43"/>
         <v>0.61101266160549483</v>
       </c>
-      <c r="F72" s="3">
+      <c r="F77" s="3">
         <f t="shared" si="44"/>
         <v>35.008446739050015</v>
       </c>
-      <c r="G72" s="3">
+      <c r="G77" s="3">
         <f t="shared" si="45"/>
         <v>600</v>
       </c>
-      <c r="H72" s="3">
+      <c r="H77" s="3">
         <f t="shared" si="46"/>
         <v>585.23499553598128</v>
       </c>
-      <c r="I72" s="3">
+      <c r="I77" s="3">
         <f t="shared" si="47"/>
         <v>1185.2349955359814</v>
       </c>
-      <c r="J72" s="3">
+      <c r="J77" s="3">
         <f t="shared" si="48"/>
         <v>14.765004464018716</v>
       </c>
-      <c r="K72" s="3">
-        <f t="shared" ref="K72:K79" si="51">F72+45</f>
+      <c r="K77" s="3">
+        <f t="shared" ref="K77:K84" si="51">F77+45</f>
         <v>80.008446739050015</v>
       </c>
-      <c r="L72" s="3">
-        <f t="shared" ref="L72:L79" si="52">K72-90</f>
+      <c r="L77" s="3">
+        <f t="shared" ref="L77:L84" si="52">K77-90</f>
         <v>-9.9915532609499849</v>
       </c>
-      <c r="M72" s="3"/>
-    </row>
-    <row r="73" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A73" s="1">
+      <c r="M77" s="3"/>
+    </row>
+    <row r="78" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A78" s="1">
         <v>7</v>
       </c>
-      <c r="B73" s="3">
-        <f>K43</f>
+      <c r="B78" s="3">
+        <f>K48</f>
         <v>30.864197530864196</v>
       </c>
-      <c r="C73" s="3">
-        <v>0</v>
-      </c>
-      <c r="D73" s="3">
-        <f>I43</f>
+      <c r="C78" s="3">
+        <v>0</v>
+      </c>
+      <c r="D78" s="3">
+        <f>I48</f>
         <v>3.9609053497942388</v>
       </c>
-      <c r="E73" s="3">
+      <c r="E78" s="3">
         <f t="shared" si="43"/>
         <v>-0.12562163201205953</v>
       </c>
-      <c r="F73" s="3">
+      <c r="F78" s="3">
         <f t="shared" si="44"/>
         <v>-7.1975893298365268</v>
       </c>
-      <c r="G73" s="3">
+      <c r="G78" s="3">
         <f t="shared" si="45"/>
         <v>15.432098765432098</v>
       </c>
-      <c r="H73" s="3">
+      <c r="H78" s="3">
         <f t="shared" si="46"/>
         <v>15.932308165990248</v>
       </c>
-      <c r="I73" s="3">
+      <c r="I78" s="3">
         <f t="shared" si="47"/>
         <v>31.364406931422344</v>
       </c>
-      <c r="J73" s="3">
+      <c r="J78" s="3">
         <f t="shared" si="48"/>
         <v>-0.50020940055815011</v>
       </c>
-      <c r="K73" s="3">
+      <c r="K78" s="3">
         <f t="shared" si="51"/>
         <v>37.802410670163475</v>
       </c>
-      <c r="L73" s="3">
+      <c r="L78" s="3">
         <f t="shared" si="52"/>
         <v>-52.197589329836525</v>
       </c>
-      <c r="M73" s="3">
-        <f>L73*2</f>
+      <c r="M78" s="3">
+        <f>L78*2</f>
         <v>-104.39517865967305</v>
       </c>
     </row>
-    <row r="74" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A74" s="1">
+    <row r="79" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A79" s="1">
         <v>8</v>
       </c>
-      <c r="B74" s="3">
+      <c r="B79" s="3">
         <v>-150</v>
       </c>
-      <c r="C74" s="3">
+      <c r="C79" s="3">
         <v>352</v>
       </c>
-      <c r="D74" s="3">
+      <c r="D79" s="3">
         <v>-24</v>
       </c>
-      <c r="E74" s="3">
-        <f t="shared" ref="E74:E78" si="53">ATAN(-2*D74/(B74-C74))/2</f>
+      <c r="E79" s="3">
+        <f t="shared" ref="E79:E83" si="53">ATAN(-2*D79/(B79-C79))/2</f>
         <v>-4.7663858426665248E-2</v>
       </c>
-      <c r="F74" s="3">
-        <f t="shared" ref="F74:F78" si="54">E74*180/PI()</f>
+      <c r="F79" s="3">
+        <f t="shared" ref="F79:F83" si="54">E79*180/PI()</f>
         <v>-2.7309379231569828</v>
       </c>
-      <c r="G74" s="3">
-        <f t="shared" ref="G74:G78" si="55">(B74+C74)/2</f>
+      <c r="G79" s="3">
+        <f t="shared" ref="G79:G83" si="55">(B79+C79)/2</f>
         <v>101</v>
       </c>
-      <c r="H74" s="3">
-        <f t="shared" ref="H74:H78" si="56">SQRT((B74-C74)^2/4+D74^2)</f>
+      <c r="H79" s="3">
+        <f t="shared" ref="H79:H83" si="56">SQRT((B79-C79)^2/4+D79^2)</f>
         <v>252.14479966876175</v>
       </c>
-      <c r="I74" s="3">
-        <f t="shared" ref="I74:I78" si="57">G74+H74</f>
+      <c r="I79" s="3">
+        <f t="shared" ref="I79:I83" si="57">G79+H79</f>
         <v>353.14479966876172</v>
       </c>
-      <c r="J74" s="3">
-        <f t="shared" ref="J74:J78" si="58">G74-H74</f>
+      <c r="J79" s="3">
+        <f t="shared" ref="J79:J83" si="58">G79-H79</f>
         <v>-151.14479966876175</v>
       </c>
-      <c r="K74" s="3">
+      <c r="K79" s="3">
         <f t="shared" si="51"/>
         <v>42.269062076843014</v>
       </c>
-      <c r="L74" s="3">
+      <c r="L79" s="3">
         <f t="shared" si="52"/>
         <v>-47.730937923156986</v>
       </c>
-      <c r="M74" s="3">
-        <f>L74*2</f>
+      <c r="M79" s="3">
+        <f>L79*2</f>
         <v>-95.461875846313973</v>
       </c>
     </row>
-    <row r="75" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A75" s="1">
+    <row r="80" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A80" s="1">
         <v>9</v>
       </c>
-      <c r="B75" s="3">
+      <c r="B80" s="3">
         <v>-400</v>
       </c>
-      <c r="C75" s="3">
+      <c r="C80" s="3">
         <v>-300</v>
       </c>
-      <c r="D75" s="3">
+      <c r="D80" s="3">
         <v>120</v>
       </c>
-      <c r="E75" s="3">
+      <c r="E80" s="3">
         <f t="shared" si="53"/>
         <v>0.5880026035475675</v>
       </c>
-      <c r="F75" s="3">
+      <c r="F80" s="3">
         <f t="shared" si="54"/>
         <v>33.690067525979785</v>
       </c>
-      <c r="G75" s="3">
+      <c r="G80" s="3">
         <f t="shared" si="55"/>
         <v>-350</v>
       </c>
-      <c r="H75" s="3">
+      <c r="H80" s="3">
         <f t="shared" si="56"/>
         <v>130</v>
       </c>
-      <c r="I75" s="3">
+      <c r="I80" s="3">
         <f t="shared" si="57"/>
         <v>-220</v>
       </c>
-      <c r="J75" s="3">
+      <c r="J80" s="3">
         <f t="shared" si="58"/>
         <v>-480</v>
       </c>
-      <c r="K75" s="3">
+      <c r="K80" s="3">
         <f t="shared" si="51"/>
         <v>78.690067525979785</v>
       </c>
-      <c r="L75" s="3">
+      <c r="L80" s="3">
         <f t="shared" si="52"/>
         <v>-11.309932474020215</v>
       </c>
-      <c r="M75" s="3"/>
-    </row>
-    <row r="76" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A76" s="1">
+      <c r="M80" s="3"/>
+    </row>
+    <row r="81" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A81" s="1">
         <v>10</v>
       </c>
-      <c r="B76" s="3">
+      <c r="B81" s="3">
         <v>-150</v>
       </c>
-      <c r="C76" s="3">
+      <c r="C81" s="3">
         <v>120</v>
       </c>
-      <c r="D76" s="3">
+      <c r="D81" s="3">
         <v>80</v>
       </c>
-      <c r="E76" s="3">
+      <c r="E81" s="3">
         <f t="shared" si="53"/>
         <v>0.26747753689304821</v>
       </c>
-      <c r="F76" s="3">
+      <c r="F81" s="3">
         <f t="shared" si="54"/>
         <v>15.325333978526434</v>
       </c>
-      <c r="G76" s="3">
+      <c r="G81" s="3">
         <f t="shared" si="55"/>
         <v>-15</v>
       </c>
-      <c r="H76" s="3">
+      <c r="H81" s="3">
         <f t="shared" si="56"/>
         <v>156.92354826475216</v>
       </c>
-      <c r="I76" s="3">
+      <c r="I81" s="3">
         <f t="shared" si="57"/>
         <v>141.92354826475216</v>
       </c>
-      <c r="J76" s="3">
+      <c r="J81" s="3">
         <f t="shared" si="58"/>
         <v>-171.92354826475216</v>
       </c>
-      <c r="K76" s="3">
+      <c r="K81" s="3">
         <f t="shared" si="51"/>
         <v>60.32533397852643</v>
       </c>
-      <c r="L76" s="3">
+      <c r="L81" s="3">
         <f t="shared" si="52"/>
         <v>-29.67466602147357</v>
       </c>
-      <c r="M76" s="3"/>
-    </row>
-    <row r="77" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A77" s="1">
+      <c r="M81" s="3"/>
+    </row>
+    <row r="82" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A82" s="1">
         <v>11</v>
       </c>
-      <c r="B77" s="3">
+      <c r="B82" s="3">
         <v>265</v>
       </c>
-      <c r="C77" s="3">
+      <c r="C82" s="3">
         <v>128</v>
       </c>
-      <c r="D77" s="3">
+      <c r="D82" s="3">
         <v>95</v>
       </c>
-      <c r="E77" s="3">
+      <c r="E82" s="3">
         <f t="shared" si="53"/>
         <v>-0.47304018463635611</v>
       </c>
-      <c r="F77" s="3">
+      <c r="F82" s="3">
         <f t="shared" si="54"/>
         <v>-27.103206119752414</v>
       </c>
-      <c r="G77" s="3">
+      <c r="G82" s="3">
         <f t="shared" si="55"/>
         <v>196.5</v>
       </c>
-      <c r="H77" s="3">
+      <c r="H82" s="3">
         <f t="shared" si="56"/>
         <v>117.1206642740725</v>
       </c>
-      <c r="I77" s="3">
+      <c r="I82" s="3">
         <f t="shared" si="57"/>
         <v>313.62066427407251</v>
       </c>
-      <c r="J77" s="3">
+      <c r="J82" s="3">
         <f t="shared" si="58"/>
         <v>79.379335725927504</v>
       </c>
-      <c r="K77" s="3">
+      <c r="K82" s="3">
         <f t="shared" si="51"/>
         <v>17.896793880247586</v>
       </c>
-      <c r="L77" s="3">
+      <c r="L82" s="3">
         <f t="shared" si="52"/>
         <v>-72.103206119752414</v>
       </c>
-      <c r="M77" s="3"/>
-    </row>
-    <row r="78" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A78" s="1">
+      <c r="M82" s="3"/>
+    </row>
+    <row r="83" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A83" s="1">
         <v>12</v>
       </c>
-      <c r="B78" s="3">
+      <c r="B83" s="3">
         <v>132</v>
       </c>
-      <c r="C78" s="3">
+      <c r="C83" s="3">
         <v>-387</v>
       </c>
-      <c r="D78" s="3">
+      <c r="D83" s="3">
         <v>-765</v>
       </c>
-      <c r="E78" s="3">
+      <c r="E83" s="3">
         <f t="shared" si="53"/>
         <v>0.62188051502639119</v>
       </c>
-      <c r="F78" s="3">
+      <c r="F83" s="3">
         <f t="shared" si="54"/>
         <v>35.631128872434189</v>
       </c>
-      <c r="G78" s="3">
+      <c r="G83" s="3">
         <f t="shared" si="55"/>
         <v>-127.5</v>
       </c>
-      <c r="H78" s="3">
+      <c r="H83" s="3">
         <f t="shared" si="56"/>
         <v>807.81510879656116</v>
       </c>
-      <c r="I78" s="3">
+      <c r="I83" s="3">
         <f t="shared" si="57"/>
         <v>680.31510879656116</v>
       </c>
-      <c r="J78" s="3">
+      <c r="J83" s="3">
         <f t="shared" si="58"/>
         <v>-935.31510879656116</v>
       </c>
-      <c r="K78" s="3">
+      <c r="K83" s="3">
         <f t="shared" si="51"/>
         <v>80.631128872434189</v>
       </c>
-      <c r="L78" s="3">
+      <c r="L83" s="3">
         <f t="shared" si="52"/>
         <v>-9.3688711275658108</v>
       </c>
-      <c r="M78" s="3"/>
-    </row>
-    <row r="79" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A79" s="1">
+      <c r="M83" s="3"/>
+    </row>
+    <row r="84" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A84" s="1">
         <v>13</v>
       </c>
-      <c r="B79" s="3">
-        <f>K59</f>
+      <c r="B84" s="3">
+        <f>K64</f>
         <v>48.611111111111107</v>
       </c>
-      <c r="C79" s="3">
-        <v>0</v>
-      </c>
-      <c r="D79" s="3">
-        <f>I59</f>
+      <c r="C84" s="3">
+        <v>0</v>
+      </c>
+      <c r="D84" s="3">
+        <f>I64</f>
         <v>14.178240740740742</v>
       </c>
-      <c r="E79" s="3">
-        <f t="shared" ref="E79" si="59">ATAN(-2*D79/(B79-C79))/2</f>
+      <c r="E84" s="3">
+        <f t="shared" ref="E84" si="59">ATAN(-2*D84/(B84-C84))/2</f>
         <v>-0.26403722421317988</v>
       </c>
-      <c r="F79" s="3">
-        <f t="shared" ref="F79" si="60">E79*180/PI()</f>
+      <c r="F84" s="3">
+        <f t="shared" ref="F84" si="60">E84*180/PI()</f>
         <v>-15.128218581764637</v>
       </c>
-      <c r="G79" s="3">
-        <f t="shared" ref="G79" si="61">(B79+C79)/2</f>
+      <c r="G84" s="3">
+        <f t="shared" ref="G84" si="61">(B84+C84)/2</f>
         <v>24.305555555555554</v>
       </c>
-      <c r="H79" s="3">
-        <f t="shared" ref="H79" si="62">SQRT((B79-C79)^2/4+D79^2)</f>
+      <c r="H84" s="3">
+        <f t="shared" ref="H84" si="62">SQRT((B84-C84)^2/4+D84^2)</f>
         <v>28.138630765668005</v>
       </c>
-      <c r="I79" s="3">
-        <f t="shared" ref="I79" si="63">G79+H79</f>
+      <c r="I84" s="3">
+        <f t="shared" ref="I84" si="63">G84+H84</f>
         <v>52.444186321223555</v>
       </c>
-      <c r="J79" s="3">
-        <f t="shared" ref="J79" si="64">G79-H79</f>
+      <c r="J84" s="3">
+        <f t="shared" ref="J84" si="64">G84-H84</f>
         <v>-3.833075210112451</v>
       </c>
-      <c r="K79" s="3">
+      <c r="K84" s="3">
         <f t="shared" si="51"/>
         <v>29.871781418235365</v>
       </c>
-      <c r="L79" s="3">
+      <c r="L84" s="3">
         <f t="shared" si="52"/>
         <v>-60.128218581764635</v>
       </c>
-      <c r="M79" s="3"/>
-    </row>
-    <row r="80" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="B80" s="3"/>
-      <c r="C80" s="3"/>
-      <c r="D80" s="3"/>
-      <c r="E80" s="3"/>
-      <c r="F80" s="3"/>
-      <c r="G80" s="3"/>
-      <c r="H80" s="3"/>
-      <c r="I80" s="3"/>
-      <c r="J80" s="3"/>
-      <c r="K80" s="3"/>
-      <c r="L80" s="3"/>
-      <c r="M80" s="3"/>
-    </row>
-    <row r="82" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="B82" s="2" t="s">
+      <c r="M84" s="3"/>
+    </row>
+    <row r="85" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B85" s="3"/>
+      <c r="C85" s="3"/>
+      <c r="D85" s="3"/>
+      <c r="E85" s="3"/>
+      <c r="F85" s="3"/>
+      <c r="G85" s="3"/>
+      <c r="H85" s="3"/>
+      <c r="I85" s="3"/>
+      <c r="J85" s="3"/>
+      <c r="K85" s="3"/>
+      <c r="L85" s="3"/>
+      <c r="M85" s="3"/>
+    </row>
+    <row r="87" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B87" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="C82" s="2" t="s">
+      <c r="C87" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="D82" s="2" t="s">
+      <c r="D87" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="E82" s="2" t="s">
+      <c r="E87" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="F82" s="2" t="s">
+      <c r="F87" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="G82" s="2" t="s">
+      <c r="G87" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="H82" s="2" t="s">
+      <c r="H87" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="I82" s="2" t="s">
+      <c r="I87" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="J82" s="2" t="s">
+      <c r="J87" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="K82" s="2" t="s">
+      <c r="K87" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="L82" s="2" t="s">
+      <c r="L87" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="M82" s="2" t="s">
+      <c r="M87" s="2" t="s">
         <v>52</v>
-      </c>
-    </row>
-    <row r="83" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A83" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="B83" s="2">
-        <v>2000</v>
-      </c>
-      <c r="C83" s="2">
-        <v>50</v>
-      </c>
-      <c r="D83" s="2">
-        <v>30</v>
-      </c>
-      <c r="E83" s="2">
-        <v>0.3</v>
-      </c>
-      <c r="F83" s="2">
-        <f>PI()*(D83/2)^2</f>
-        <v>706.85834705770344</v>
-      </c>
-      <c r="G83" s="2">
-        <f>3600*1000</f>
-        <v>3600000</v>
-      </c>
-      <c r="H83" s="2">
-        <f>G83/F83</f>
-        <v>5092.9581789406511</v>
-      </c>
-      <c r="I83" s="2">
-        <f>C83/B83</f>
-        <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="J83" s="2">
-        <f>H83/I83</f>
-        <v>203718.32715762604</v>
-      </c>
-      <c r="K83" s="2">
-        <f>E83/D83</f>
-        <v>0.01</v>
-      </c>
-      <c r="L83" s="2">
-        <f>K83/I83</f>
-        <v>0.39999999999999997</v>
-      </c>
-      <c r="M83" s="2">
-        <f>J83/(2*(1+L83))</f>
-        <v>72756.545413437882</v>
-      </c>
-    </row>
-    <row r="86" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="B86" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="C86" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="D86" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="E86" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="F86" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="G86" s="2" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="87" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A87" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="B87" s="2">
-        <v>50</v>
-      </c>
-      <c r="C87" s="2">
-        <f>PI()*(B87/2)^2</f>
-        <v>1963.4954084936207</v>
-      </c>
-      <c r="D87" s="2">
-        <v>205000</v>
-      </c>
-      <c r="E87" s="2">
-        <f>390*1000</f>
-        <v>390000</v>
-      </c>
-      <c r="F87" s="2">
-        <v>1300</v>
-      </c>
-      <c r="G87" s="2">
-        <f>E87*F87/C87/D87</f>
-        <v>1.2595755105965414</v>
       </c>
     </row>
     <row r="88" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A88" s="1" t="s">
         <v>55</v>
       </c>
+      <c r="B88" s="2">
+        <v>2000</v>
+      </c>
       <c r="C88" s="2">
+        <v>50</v>
+      </c>
+      <c r="D88" s="2">
+        <v>30</v>
+      </c>
+      <c r="E88" s="2">
+        <v>0.3</v>
+      </c>
+      <c r="F88" s="2">
+        <f>PI()*(D88/2)^2</f>
+        <v>706.85834705770344</v>
+      </c>
+      <c r="G88" s="2">
+        <f>3600*1000</f>
+        <v>3600000</v>
+      </c>
+      <c r="H88" s="2">
+        <f>G88/F88</f>
+        <v>5092.9581789406511</v>
+      </c>
+      <c r="I88" s="2">
+        <f>C88/B88</f>
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="J88" s="2">
+        <f>H88/I88</f>
+        <v>203718.32715762604</v>
+      </c>
+      <c r="K88" s="2">
+        <f>E88/D88</f>
+        <v>0.01</v>
+      </c>
+      <c r="L88" s="2">
+        <f>K88/I88</f>
+        <v>0.39999999999999997</v>
+      </c>
+      <c r="M88" s="2">
+        <f>J88/(2*(1+L88))</f>
+        <v>72756.545413437882</v>
+      </c>
+    </row>
+    <row r="91" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B91" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C91" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D91" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="E91" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="F91" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="G91" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="92" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A92" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B92" s="2">
+        <v>50</v>
+      </c>
+      <c r="C92" s="2">
+        <f>PI()*(B92/2)^2</f>
+        <v>1963.4954084936207</v>
+      </c>
+      <c r="D92" s="2">
+        <v>205000</v>
+      </c>
+      <c r="E92" s="2">
+        <f>390*1000</f>
+        <v>390000</v>
+      </c>
+      <c r="F92" s="2">
+        <v>1300</v>
+      </c>
+      <c r="G92" s="2">
+        <f>E92*F92/C92/D92</f>
+        <v>1.2595755105965414</v>
+      </c>
+    </row>
+    <row r="93" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A93" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C93" s="2">
         <v>1000</v>
       </c>
-      <c r="D88" s="2">
+      <c r="D93" s="2">
         <v>200000</v>
       </c>
-      <c r="E88" s="2">
+      <c r="E93" s="2">
         <f>200*1000</f>
         <v>200000</v>
       </c>
-      <c r="F88" s="2">
+      <c r="F93" s="2">
         <v>1000</v>
       </c>
-      <c r="G88" s="2">
-        <f>E88*F88/C88/D88</f>
+      <c r="G93" s="2">
+        <f>E93*F93/C93/D93</f>
         <v>1</v>
       </c>
     </row>
-    <row r="89" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="C89" s="2">
+    <row r="94" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="C94" s="2">
         <v>2000</v>
       </c>
-      <c r="D89" s="2">
+      <c r="D94" s="2">
         <v>27000</v>
       </c>
-      <c r="E89" s="2">
+      <c r="E94" s="2">
         <f>250*1000</f>
         <v>250000</v>
       </c>
-      <c r="F89" s="2">
+      <c r="F94" s="2">
         <v>2000</v>
       </c>
-      <c r="G89" s="2">
-        <f>E89*F89/C89/D89</f>
+      <c r="G94" s="2">
+        <f>E94*F94/C94/D94</f>
         <v>9.2592592592592595</v>
       </c>
     </row>
-    <row r="90" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="B90" s="2">
+    <row r="95" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B95" s="2">
         <v>500</v>
       </c>
-      <c r="C90" s="2">
-        <f>B90^2</f>
+      <c r="C95" s="2">
+        <f>B95^2</f>
         <v>250000</v>
       </c>
-      <c r="D90" s="2">
+      <c r="D95" s="2">
         <v>28500</v>
       </c>
-      <c r="E90" s="2">
+      <c r="E95" s="2">
         <f>7800*1000</f>
         <v>7800000</v>
       </c>
-      <c r="F90" s="2">
+      <c r="F95" s="2">
         <v>2400</v>
       </c>
-      <c r="G90" s="2">
-        <f>E90*F90/C90/D90</f>
+      <c r="G95" s="2">
+        <f>E95*F95/C95/D95</f>
         <v>2.6273684210526316</v>
       </c>
-      <c r="I90" s="2">
+      <c r="I95" s="2">
         <f>ATAN(0.2)*180/PI()/2</f>
         <v>5.6549662370101066</v>
       </c>
     </row>
-    <row r="91" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="B91" s="2">
+    <row r="96" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B96" s="2">
         <v>550</v>
       </c>
-      <c r="C91" s="2">
-        <f>B91^2</f>
+      <c r="C96" s="2">
+        <f>B96^2</f>
         <v>302500</v>
       </c>
-      <c r="D91" s="2">
+      <c r="D96" s="2">
         <v>28500</v>
       </c>
-      <c r="E91" s="2">
+      <c r="E96" s="2">
         <f>7800*1000</f>
         <v>7800000</v>
       </c>
-      <c r="F91" s="2">
+      <c r="F96" s="2">
         <v>2400</v>
       </c>
-      <c r="G91" s="2">
-        <f>E91*F91/C91/D91</f>
+      <c r="G96" s="2">
+        <f>E96*F96/C96/D96</f>
         <v>2.1713788603740758</v>
       </c>
     </row>
-    <row r="92" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="B92" s="2">
-        <f>SQRT(C92)</f>
+    <row r="97" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B97" s="2">
+        <f>SQRT(C97)</f>
         <v>452.0224821005304</v>
       </c>
-      <c r="C92" s="2">
-        <f>E92*F92/D92/G92</f>
+      <c r="C97" s="2">
+        <f>E97*F97/D97/G97</f>
         <v>204324.32432432432</v>
       </c>
-      <c r="D92" s="2">
+      <c r="D97" s="2">
         <v>37000</v>
       </c>
-      <c r="E92" s="2">
+      <c r="E97" s="2">
         <f>3600*1000</f>
         <v>3600000</v>
       </c>
-      <c r="F92" s="2">
+      <c r="F97" s="2">
         <v>2100</v>
       </c>
-      <c r="G92" s="2">
+      <c r="G97" s="2">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
2019.04.17 addition of review quizzes of Part IV. stress of column
</commit_message>
<xml_diff>
--- a/quiz_calc.xlsx
+++ b/quiz_calc.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive - 경남대학교\GitHub\structural_mechanics_II\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DCF7BBB-9A17-4D45-B9C1-F1B80A68ECE0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="11610" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="11610"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="179021" iterateDelta="1E-4"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -30,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="89">
   <si>
     <t>Ix</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -341,20 +340,67 @@
   </si>
   <si>
     <t>y</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>b</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>h</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>e_cr</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>e</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>sigma_a</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>sigma_b</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>sigma_t</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>sigma_c</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>I_y</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>S_y</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>M=Pe</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="6">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="9">
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="176" formatCode="0_ ;[Red]\-0\ "/>
     <numFmt numFmtId="177" formatCode="0.000_ ;[Red]\-0.000\ "/>
     <numFmt numFmtId="178" formatCode="0.0000_ ;[Red]\-0.0000\ "/>
     <numFmt numFmtId="179" formatCode="0.00000_ ;[Red]\-0.00000\ "/>
     <numFmt numFmtId="180" formatCode="0.0000E+00"/>
+    <numFmt numFmtId="181" formatCode="_-* #,##0.0000_-;\-* #,##0.0000_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="182" formatCode="_-* #,##0.000_-;\-* #,##0.000_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="183" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;_-;_-@_-"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -406,7 +452,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -423,6 +469,21 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="180" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="181" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="182" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="183" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="183" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -739,11 +800,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P97"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:P113"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4:M4"/>
+    <sheetView tabSelected="1" topLeftCell="A79" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A89" sqref="A89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -3462,7 +3523,7 @@
       </c>
       <c r="M80" s="3"/>
     </row>
-    <row r="81" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A81" s="1">
         <v>10</v>
       </c>
@@ -3509,7 +3570,7 @@
       </c>
       <c r="M81" s="3"/>
     </row>
-    <row r="82" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A82" s="1">
         <v>11</v>
       </c>
@@ -3556,7 +3617,7 @@
       </c>
       <c r="M82" s="3"/>
     </row>
-    <row r="83" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A83" s="1">
         <v>12</v>
       </c>
@@ -3603,7 +3664,7 @@
       </c>
       <c r="M83" s="3"/>
     </row>
-    <row r="84" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A84" s="1">
         <v>13</v>
       </c>
@@ -3652,7 +3713,7 @@
       </c>
       <c r="M84" s="3"/>
     </row>
-    <row r="85" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B85" s="3"/>
       <c r="C85" s="3"/>
       <c r="D85" s="3"/>
@@ -3666,250 +3727,813 @@
       <c r="L85" s="3"/>
       <c r="M85" s="3"/>
     </row>
-    <row r="87" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="B87" s="2" t="s">
+    <row r="86" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B86" s="3"/>
+      <c r="C86" s="3"/>
+      <c r="D86" s="3"/>
+      <c r="E86" s="3"/>
+      <c r="F86" s="3"/>
+      <c r="G86" s="3"/>
+      <c r="H86" s="3"/>
+      <c r="I86" s="3"/>
+      <c r="J86" s="3"/>
+      <c r="K86" s="3"/>
+      <c r="L86" s="3"/>
+      <c r="M86" s="3"/>
+    </row>
+    <row r="87" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B87" s="3"/>
+      <c r="C87" s="3"/>
+      <c r="D87" s="3"/>
+      <c r="E87" s="3"/>
+      <c r="F87" s="3"/>
+      <c r="G87" s="3"/>
+      <c r="H87" s="3"/>
+      <c r="I87" s="3"/>
+      <c r="J87" s="3"/>
+      <c r="K87" s="3"/>
+      <c r="L87" s="3"/>
+      <c r="M87" s="3"/>
+    </row>
+    <row r="88" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B88" s="3"/>
+      <c r="C88" s="3"/>
+      <c r="D88" s="3"/>
+      <c r="E88" s="3"/>
+      <c r="F88" s="3"/>
+      <c r="G88" s="3"/>
+      <c r="H88" s="3"/>
+      <c r="I88" s="3"/>
+      <c r="J88" s="3"/>
+      <c r="K88" s="3"/>
+      <c r="L88" s="3"/>
+      <c r="M88" s="3"/>
+    </row>
+    <row r="89" spans="1:14" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A89" t="s">
+        <v>78</v>
+      </c>
+      <c r="B89" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="C89" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="D89" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="E89" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="F89" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="G89" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="H89" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="I89" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="K89" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="L89" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="M89" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="N89" s="6" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="90" spans="1:14" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A90">
+        <v>300</v>
+      </c>
+      <c r="B90" s="10">
+        <v>200</v>
+      </c>
+      <c r="C90" s="7">
+        <f>A90/6</f>
+        <v>50</v>
+      </c>
+      <c r="D90" s="8">
+        <f>A90*B90</f>
+        <v>60000</v>
+      </c>
+      <c r="E90" s="10">
+        <f>A90^3*B90/12</f>
+        <v>450000000</v>
+      </c>
+      <c r="F90" s="10">
+        <f>A90^2*B90/6</f>
+        <v>3000000</v>
+      </c>
+      <c r="G90" s="9">
+        <v>300000</v>
+      </c>
+      <c r="H90" s="9">
+        <v>100</v>
+      </c>
+      <c r="I90" s="9">
+        <f>G90*H90</f>
+        <v>30000000</v>
+      </c>
+      <c r="K90" s="6">
+        <f>-G90/D90</f>
+        <v>-5</v>
+      </c>
+      <c r="L90" s="6">
+        <f>I90/F90</f>
+        <v>10</v>
+      </c>
+      <c r="M90" s="6">
+        <f>K90+L90</f>
+        <v>5</v>
+      </c>
+      <c r="N90" s="6">
+        <f>K90-L90</f>
+        <v>-15</v>
+      </c>
+    </row>
+    <row r="91" spans="1:14" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A91">
+        <v>500</v>
+      </c>
+      <c r="B91" s="10">
+        <v>300</v>
+      </c>
+      <c r="C91" s="7">
+        <f>A91/6</f>
+        <v>83.333333333333329</v>
+      </c>
+      <c r="D91" s="8">
+        <f>A91*B91</f>
+        <v>150000</v>
+      </c>
+      <c r="E91" s="10">
+        <f>A91^3*B91/12</f>
+        <v>3125000000</v>
+      </c>
+      <c r="F91" s="10">
+        <f>A91^2*B91/6</f>
+        <v>12500000</v>
+      </c>
+      <c r="G91" s="9">
+        <v>3253600</v>
+      </c>
+      <c r="H91" s="9">
+        <v>47</v>
+      </c>
+      <c r="I91" s="9">
+        <f>G91*H91</f>
+        <v>152919200</v>
+      </c>
+      <c r="K91" s="6">
+        <f>-G91/D91</f>
+        <v>-21.690666666666665</v>
+      </c>
+      <c r="L91" s="6">
+        <f>I91/F91</f>
+        <v>12.233536000000001</v>
+      </c>
+      <c r="M91" s="6">
+        <f>K91+L91</f>
+        <v>-9.4571306666666644</v>
+      </c>
+      <c r="N91" s="6">
+        <f>K91-L91</f>
+        <v>-33.924202666666666</v>
+      </c>
+    </row>
+    <row r="92" spans="1:14" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B92" s="6"/>
+      <c r="C92" s="7"/>
+      <c r="D92" s="8">
+        <v>4678</v>
+      </c>
+      <c r="E92" s="8"/>
+      <c r="F92" s="8">
+        <v>481000</v>
+      </c>
+      <c r="G92" s="8">
+        <f>53.3*1000</f>
+        <v>53300</v>
+      </c>
+      <c r="H92" s="8">
+        <v>750.5</v>
+      </c>
+      <c r="I92" s="8">
+        <f>G92*H92</f>
+        <v>40001650</v>
+      </c>
+      <c r="K92" s="6">
+        <f>-G92/D92</f>
+        <v>-11.39375801624626</v>
+      </c>
+      <c r="L92" s="6">
+        <f>I92/F92</f>
+        <v>83.163513513513507</v>
+      </c>
+      <c r="M92" s="6">
+        <f>K92+L92</f>
+        <v>71.769755497267255</v>
+      </c>
+      <c r="N92" s="6">
+        <f>K92-L92</f>
+        <v>-94.55727152975976</v>
+      </c>
+    </row>
+    <row r="93" spans="1:14" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A93">
+        <v>300</v>
+      </c>
+      <c r="B93" s="10">
+        <v>250</v>
+      </c>
+      <c r="C93" s="7">
+        <f>A93/6</f>
+        <v>50</v>
+      </c>
+      <c r="D93" s="8">
+        <f>A93*B93</f>
+        <v>75000</v>
+      </c>
+      <c r="E93" s="10">
+        <f>A93^3*B93/12</f>
+        <v>562500000</v>
+      </c>
+      <c r="F93" s="10">
+        <f>A93^2*B93/6</f>
+        <v>3750000</v>
+      </c>
+      <c r="G93" s="9">
+        <v>925600</v>
+      </c>
+      <c r="H93" s="9">
+        <v>40</v>
+      </c>
+      <c r="I93" s="9">
+        <f>G93*H93</f>
+        <v>37024000</v>
+      </c>
+      <c r="K93" s="6">
+        <f>-G93/D93</f>
+        <v>-12.341333333333333</v>
+      </c>
+      <c r="L93" s="6">
+        <f>I93/F93</f>
+        <v>9.8730666666666664</v>
+      </c>
+      <c r="M93" s="6">
+        <f>K93+L93</f>
+        <v>-2.4682666666666666</v>
+      </c>
+      <c r="N93" s="6">
+        <f>K93-L93</f>
+        <v>-22.214399999999998</v>
+      </c>
+    </row>
+    <row r="94" spans="1:14" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A94">
+        <v>488</v>
+      </c>
+      <c r="B94" s="10">
+        <v>320</v>
+      </c>
+      <c r="C94" s="7">
+        <f>A94/6</f>
+        <v>81.333333333333329</v>
+      </c>
+      <c r="D94" s="8">
+        <f>A94*B94</f>
+        <v>156160</v>
+      </c>
+      <c r="E94" s="10">
+        <f>A94^3*B94/12</f>
+        <v>3099047253.3333335</v>
+      </c>
+      <c r="F94" s="10">
+        <f>A94^2*B94/6</f>
+        <v>12701013.333333334</v>
+      </c>
+      <c r="G94" s="9">
+        <v>5213400</v>
+      </c>
+      <c r="H94" s="9">
+        <v>180</v>
+      </c>
+      <c r="I94" s="9">
+        <f>G94*H94</f>
+        <v>938412000</v>
+      </c>
+      <c r="K94" s="6">
+        <f>-G94/D94</f>
+        <v>-33.384989754098363</v>
+      </c>
+      <c r="L94" s="6">
+        <f>I94/F94</f>
+        <v>73.884813390217687</v>
+      </c>
+      <c r="M94" s="6">
+        <f>K94+L94</f>
+        <v>40.499823636119324</v>
+      </c>
+      <c r="N94" s="6">
+        <f>K94-L94</f>
+        <v>-107.26980314431606</v>
+      </c>
+    </row>
+    <row r="95" spans="1:14" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A95">
+        <v>480</v>
+      </c>
+      <c r="B95" s="10">
+        <v>300</v>
+      </c>
+      <c r="C95" s="7">
+        <f>A95/6</f>
+        <v>80</v>
+      </c>
+      <c r="D95" s="8">
+        <f>A95*B95</f>
+        <v>144000</v>
+      </c>
+      <c r="E95" s="10">
+        <f>A95^3*B95/12</f>
+        <v>2764800000</v>
+      </c>
+      <c r="F95" s="10">
+        <f>A95^2*B95/6</f>
+        <v>11520000</v>
+      </c>
+      <c r="G95" s="9">
+        <v>5000000</v>
+      </c>
+      <c r="H95" s="9">
+        <v>0</v>
+      </c>
+      <c r="I95" s="9">
+        <f>G95*H95</f>
+        <v>0</v>
+      </c>
+      <c r="K95" s="6">
+        <f>-G95/D95</f>
+        <v>-34.722222222222221</v>
+      </c>
+      <c r="L95" s="6">
+        <f>I95/F95</f>
+        <v>0</v>
+      </c>
+      <c r="M95" s="6">
+        <f>K95+L95</f>
+        <v>-34.722222222222221</v>
+      </c>
+      <c r="N95" s="6">
+        <f>K95-L95</f>
+        <v>-34.722222222222221</v>
+      </c>
+    </row>
+    <row r="96" spans="1:14" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A96">
+        <v>480</v>
+      </c>
+      <c r="B96" s="10">
+        <v>300</v>
+      </c>
+      <c r="C96" s="7">
+        <f>A96/6</f>
+        <v>80</v>
+      </c>
+      <c r="D96" s="8">
+        <f>A96*B96</f>
+        <v>144000</v>
+      </c>
+      <c r="E96" s="10">
+        <f>A96^3*B96/12</f>
+        <v>2764800000</v>
+      </c>
+      <c r="F96" s="10">
+        <f>A96^2*B96/6</f>
+        <v>11520000</v>
+      </c>
+      <c r="G96" s="9">
+        <v>5000000</v>
+      </c>
+      <c r="H96" s="9">
+        <v>40</v>
+      </c>
+      <c r="I96" s="9">
+        <f>G96*H96</f>
+        <v>200000000</v>
+      </c>
+      <c r="K96" s="6">
+        <f>-G96/D96</f>
+        <v>-34.722222222222221</v>
+      </c>
+      <c r="L96" s="6">
+        <f>I96/F96</f>
+        <v>17.361111111111111</v>
+      </c>
+      <c r="M96" s="6">
+        <f>K96+L96</f>
+        <v>-17.361111111111111</v>
+      </c>
+      <c r="N96" s="6">
+        <f>K96-L96</f>
+        <v>-52.083333333333329</v>
+      </c>
+    </row>
+    <row r="97" spans="1:14" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A97">
+        <v>480</v>
+      </c>
+      <c r="B97" s="10">
+        <v>300</v>
+      </c>
+      <c r="C97" s="7">
+        <f>A97/6</f>
+        <v>80</v>
+      </c>
+      <c r="D97" s="8">
+        <f>A97*B97</f>
+        <v>144000</v>
+      </c>
+      <c r="E97" s="10">
+        <f>A97^3*B97/12</f>
+        <v>2764800000</v>
+      </c>
+      <c r="F97" s="10">
+        <f>A97^2*B97/6</f>
+        <v>11520000</v>
+      </c>
+      <c r="G97" s="9">
+        <v>5000000</v>
+      </c>
+      <c r="H97" s="9">
+        <v>80</v>
+      </c>
+      <c r="I97" s="9">
+        <f>G97*H97</f>
+        <v>400000000</v>
+      </c>
+      <c r="K97" s="6">
+        <f>-G97/D97</f>
+        <v>-34.722222222222221</v>
+      </c>
+      <c r="L97" s="6">
+        <f>I97/F97</f>
+        <v>34.722222222222221</v>
+      </c>
+      <c r="M97" s="6">
+        <f>K97+L97</f>
+        <v>0</v>
+      </c>
+      <c r="N97" s="6">
+        <f>K97-L97</f>
+        <v>-69.444444444444443</v>
+      </c>
+    </row>
+    <row r="98" spans="1:14" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A98">
+        <v>480</v>
+      </c>
+      <c r="B98" s="10">
+        <v>300</v>
+      </c>
+      <c r="C98" s="7">
+        <f>A98/6</f>
+        <v>80</v>
+      </c>
+      <c r="D98" s="8">
+        <f>A98*B98</f>
+        <v>144000</v>
+      </c>
+      <c r="E98" s="10">
+        <f>A98^3*B98/12</f>
+        <v>2764800000</v>
+      </c>
+      <c r="F98" s="10">
+        <f>A98^2*B98/6</f>
+        <v>11520000</v>
+      </c>
+      <c r="G98" s="9">
+        <v>5000000</v>
+      </c>
+      <c r="H98" s="9">
+        <v>120</v>
+      </c>
+      <c r="I98" s="9">
+        <f>G98*H98</f>
+        <v>600000000</v>
+      </c>
+      <c r="K98" s="6">
+        <f>-G98/D98</f>
+        <v>-34.722222222222221</v>
+      </c>
+      <c r="L98" s="6">
+        <f>I98/F98</f>
+        <v>52.083333333333336</v>
+      </c>
+      <c r="M98" s="6">
+        <f>K98+L98</f>
+        <v>17.361111111111114</v>
+      </c>
+      <c r="N98" s="6">
+        <f>K98-L98</f>
+        <v>-86.805555555555557</v>
+      </c>
+    </row>
+    <row r="99" spans="1:14" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B99" s="10"/>
+      <c r="C99" s="7"/>
+      <c r="D99" s="8"/>
+      <c r="E99" s="10"/>
+      <c r="F99" s="10"/>
+      <c r="G99" s="9"/>
+      <c r="H99" s="9"/>
+      <c r="I99" s="9"/>
+      <c r="K99" s="6"/>
+      <c r="L99" s="6"/>
+      <c r="M99" s="6"/>
+      <c r="N99" s="6"/>
+    </row>
+    <row r="100" spans="1:14" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B100" s="10"/>
+      <c r="C100" s="7"/>
+      <c r="D100" s="8"/>
+      <c r="E100" s="10"/>
+      <c r="F100" s="10"/>
+      <c r="G100" s="9"/>
+      <c r="H100" s="9"/>
+      <c r="I100" s="9"/>
+      <c r="K100" s="6"/>
+      <c r="L100" s="6"/>
+      <c r="M100" s="6"/>
+      <c r="N100" s="6"/>
+    </row>
+    <row r="101" spans="1:14" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B101" s="10"/>
+      <c r="C101" s="7"/>
+      <c r="D101" s="8"/>
+      <c r="E101" s="10"/>
+      <c r="F101" s="10"/>
+      <c r="G101" s="9"/>
+      <c r="H101" s="9"/>
+      <c r="I101" s="9"/>
+      <c r="K101" s="6"/>
+      <c r="L101" s="6"/>
+      <c r="M101" s="6"/>
+      <c r="N101" s="6"/>
+    </row>
+    <row r="103" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B103" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="C87" s="2" t="s">
+      <c r="C103" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="D87" s="2" t="s">
+      <c r="D103" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="E87" s="2" t="s">
+      <c r="E103" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="F87" s="2" t="s">
+      <c r="F103" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="G87" s="2" t="s">
+      <c r="G103" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="H87" s="2" t="s">
+      <c r="H103" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="I87" s="2" t="s">
+      <c r="I103" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="J87" s="2" t="s">
+      <c r="J103" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="K87" s="2" t="s">
+      <c r="K103" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="L87" s="2" t="s">
+      <c r="L103" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="M87" s="2" t="s">
+      <c r="M103" s="2" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="88" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A88" s="1" t="s">
+    <row r="104" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A104" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="B88" s="2">
+      <c r="B104" s="2">
         <v>2000</v>
       </c>
-      <c r="C88" s="2">
+      <c r="C104" s="2">
         <v>50</v>
       </c>
-      <c r="D88" s="2">
+      <c r="D104" s="2">
         <v>30</v>
       </c>
-      <c r="E88" s="2">
+      <c r="E104" s="2">
         <v>0.3</v>
       </c>
-      <c r="F88" s="2">
-        <f>PI()*(D88/2)^2</f>
+      <c r="F104" s="2">
+        <f>PI()*(D104/2)^2</f>
         <v>706.85834705770344</v>
       </c>
-      <c r="G88" s="2">
+      <c r="G104" s="2">
         <f>3600*1000</f>
         <v>3600000</v>
       </c>
-      <c r="H88" s="2">
-        <f>G88/F88</f>
+      <c r="H104" s="2">
+        <f>G104/F104</f>
         <v>5092.9581789406511</v>
       </c>
-      <c r="I88" s="2">
-        <f>C88/B88</f>
+      <c r="I104" s="2">
+        <f>C104/B104</f>
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="J88" s="2">
-        <f>H88/I88</f>
+      <c r="J104" s="2">
+        <f>H104/I104</f>
         <v>203718.32715762604</v>
       </c>
-      <c r="K88" s="2">
-        <f>E88/D88</f>
+      <c r="K104" s="2">
+        <f>E104/D104</f>
         <v>0.01</v>
       </c>
-      <c r="L88" s="2">
-        <f>K88/I88</f>
+      <c r="L104" s="2">
+        <f>K104/I104</f>
         <v>0.39999999999999997</v>
       </c>
-      <c r="M88" s="2">
-        <f>J88/(2*(1+L88))</f>
+      <c r="M104" s="2">
+        <f>J104/(2*(1+L104))</f>
         <v>72756.545413437882</v>
       </c>
     </row>
-    <row r="91" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="B91" s="2" t="s">
+    <row r="107" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B107" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="C91" s="2" t="s">
+      <c r="C107" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="D91" s="2" t="s">
+      <c r="D107" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="E91" s="2" t="s">
+      <c r="E107" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="F91" s="2" t="s">
+      <c r="F107" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="G91" s="2" t="s">
+      <c r="G107" s="2" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="92" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A92" s="1" t="s">
+    <row r="108" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A108" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="B92" s="2">
+      <c r="B108" s="2">
         <v>50</v>
       </c>
-      <c r="C92" s="2">
-        <f>PI()*(B92/2)^2</f>
+      <c r="C108" s="2">
+        <f>PI()*(B108/2)^2</f>
         <v>1963.4954084936207</v>
       </c>
-      <c r="D92" s="2">
+      <c r="D108" s="2">
         <v>205000</v>
       </c>
-      <c r="E92" s="2">
+      <c r="E108" s="2">
         <f>390*1000</f>
         <v>390000</v>
       </c>
-      <c r="F92" s="2">
+      <c r="F108" s="2">
         <v>1300</v>
       </c>
-      <c r="G92" s="2">
-        <f>E92*F92/C92/D92</f>
+      <c r="G108" s="2">
+        <f>E108*F108/C108/D108</f>
         <v>1.2595755105965414</v>
       </c>
     </row>
-    <row r="93" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A93" s="1" t="s">
+    <row r="109" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A109" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="C93" s="2">
+      <c r="C109" s="2">
         <v>1000</v>
       </c>
-      <c r="D93" s="2">
+      <c r="D109" s="2">
         <v>200000</v>
       </c>
-      <c r="E93" s="2">
+      <c r="E109" s="2">
         <f>200*1000</f>
         <v>200000</v>
       </c>
-      <c r="F93" s="2">
+      <c r="F109" s="2">
         <v>1000</v>
       </c>
-      <c r="G93" s="2">
-        <f>E93*F93/C93/D93</f>
+      <c r="G109" s="2">
+        <f>E109*F109/C109/D109</f>
         <v>1</v>
       </c>
     </row>
-    <row r="94" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="C94" s="2">
+    <row r="110" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="C110" s="2">
         <v>2000</v>
       </c>
-      <c r="D94" s="2">
+      <c r="D110" s="2">
         <v>27000</v>
       </c>
-      <c r="E94" s="2">
+      <c r="E110" s="2">
         <f>250*1000</f>
         <v>250000</v>
       </c>
-      <c r="F94" s="2">
+      <c r="F110" s="2">
         <v>2000</v>
       </c>
-      <c r="G94" s="2">
-        <f>E94*F94/C94/D94</f>
+      <c r="G110" s="2">
+        <f>E110*F110/C110/D110</f>
         <v>9.2592592592592595</v>
       </c>
     </row>
-    <row r="95" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="B95" s="2">
+    <row r="111" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B111" s="2">
         <v>500</v>
       </c>
-      <c r="C95" s="2">
-        <f>B95^2</f>
+      <c r="C111" s="2">
+        <f>B111^2</f>
         <v>250000</v>
       </c>
-      <c r="D95" s="2">
+      <c r="D111" s="2">
         <v>28500</v>
       </c>
-      <c r="E95" s="2">
+      <c r="E111" s="2">
         <f>7800*1000</f>
         <v>7800000</v>
       </c>
-      <c r="F95" s="2">
+      <c r="F111" s="2">
         <v>2400</v>
       </c>
-      <c r="G95" s="2">
-        <f>E95*F95/C95/D95</f>
+      <c r="G111" s="2">
+        <f>E111*F111/C111/D111</f>
         <v>2.6273684210526316</v>
       </c>
-      <c r="I95" s="2">
+      <c r="I111" s="2">
         <f>ATAN(0.2)*180/PI()/2</f>
         <v>5.6549662370101066</v>
       </c>
     </row>
-    <row r="96" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="B96" s="2">
+    <row r="112" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B112" s="2">
         <v>550</v>
       </c>
-      <c r="C96" s="2">
-        <f>B96^2</f>
+      <c r="C112" s="2">
+        <f>B112^2</f>
         <v>302500</v>
       </c>
-      <c r="D96" s="2">
+      <c r="D112" s="2">
         <v>28500</v>
       </c>
-      <c r="E96" s="2">
+      <c r="E112" s="2">
         <f>7800*1000</f>
         <v>7800000</v>
       </c>
-      <c r="F96" s="2">
+      <c r="F112" s="2">
         <v>2400</v>
       </c>
-      <c r="G96" s="2">
-        <f>E96*F96/C96/D96</f>
+      <c r="G112" s="2">
+        <f>E112*F112/C112/D112</f>
         <v>2.1713788603740758</v>
       </c>
     </row>
-    <row r="97" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B97" s="2">
-        <f>SQRT(C97)</f>
+    <row r="113" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B113" s="2">
+        <f>SQRT(C113)</f>
         <v>452.0224821005304</v>
       </c>
-      <c r="C97" s="2">
-        <f>E97*F97/D97/G97</f>
+      <c r="C113" s="2">
+        <f>E113*F113/D113/G113</f>
         <v>204324.32432432432</v>
       </c>
-      <c r="D97" s="2">
+      <c r="D113" s="2">
         <v>37000</v>
       </c>
-      <c r="E97" s="2">
+      <c r="E113" s="2">
         <f>3600*1000</f>
         <v>3600000</v>
       </c>
-      <c r="F97" s="2">
+      <c r="F113" s="2">
         <v>2100</v>
       </c>
-      <c r="G97" s="2">
+      <c r="G113" s="2">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
2020.09.11 update and correction for various trivial stuff
</commit_message>
<xml_diff>
--- a/quiz_calc.xlsx
+++ b/quiz_calc.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive - 경남대학교\GitHub\structural_mechanics_II\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{333B46F5-1811-42ED-8251-657DA896AF1F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="11610"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -22,6 +23,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -29,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="91">
   <si>
     <t>Ix</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -384,20 +388,27 @@
   </si>
   <si>
     <t>M=Pe</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>S</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>sigma</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="9">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="8">
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="176" formatCode="0_ ;[Red]\-0\ "/>
     <numFmt numFmtId="177" formatCode="0.000_ ;[Red]\-0.000\ "/>
     <numFmt numFmtId="178" formatCode="0.0000_ ;[Red]\-0.0000\ "/>
     <numFmt numFmtId="179" formatCode="0.00000_ ;[Red]\-0.00000\ "/>
-    <numFmt numFmtId="180" formatCode="0.0000E+00"/>
     <numFmt numFmtId="181" formatCode="_-* #,##0.0000_-;\-* #,##0.0000_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="182" formatCode="_-* #,##0.000_-;\-* #,##0.000_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="183" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;_-;_-@_-"/>
@@ -452,7 +463,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -466,9 +477,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="179" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="181" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1">
@@ -800,11 +808,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P113"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A79" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A89" sqref="A89"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="L61" sqref="L61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -2063,7 +2071,7 @@
         <v>1733333.3333333302</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A33" s="1">
         <v>3</v>
       </c>
@@ -2101,7 +2109,7 @@
         <v>275.66543324293741</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A34" s="1">
         <v>4</v>
       </c>
@@ -2142,13 +2150,13 @@
         <v>112500</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.3">
       <c r="C36" s="2">
         <f>7530000/300/500</f>
         <v>50.2</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B39" s="2" t="s">
         <v>28</v>
       </c>
@@ -2179,882 +2187,1036 @@
       <c r="K39" s="2" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L39" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="M39" s="2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A40" s="1">
         <v>1</v>
       </c>
-      <c r="B40" s="2">
+      <c r="B40" s="7">
         <f>250/2</f>
         <v>125</v>
       </c>
-      <c r="C40" s="2">
+      <c r="C40" s="7">
         <f>500/2</f>
         <v>250</v>
       </c>
-      <c r="D40" s="2">
+      <c r="D40" s="7">
         <f>50/2</f>
         <v>25</v>
       </c>
-      <c r="E40" s="2">
+      <c r="E40" s="7">
         <f t="shared" ref="E40:E48" si="13">C40/2-D40</f>
         <v>100</v>
       </c>
-      <c r="F40" s="2">
+      <c r="F40" s="7">
         <f>1200*1000</f>
         <v>1200000</v>
       </c>
-      <c r="G40" s="2">
+      <c r="G40" s="7">
         <f>B40*D40*(E40+D40/2)</f>
         <v>351562.5</v>
       </c>
-      <c r="H40" s="2">
+      <c r="H40" s="7">
         <f t="shared" ref="H40:H48" si="14">B40*C40^3/12</f>
         <v>162760416.66666666</v>
       </c>
-      <c r="I40" s="2">
+      <c r="I40" s="7">
         <f>F40*G40/H40/B40</f>
         <v>20.736000000000001</v>
       </c>
-      <c r="J40" s="5">
+      <c r="J40" s="7">
         <f>250000000</f>
         <v>250000000</v>
       </c>
-      <c r="K40" s="3">
+      <c r="K40" s="7">
         <f>J40/H40*E40</f>
         <v>153.6</v>
       </c>
-    </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L40" s="5">
+        <f t="shared" ref="L40:L51" si="15">H40/E40</f>
+        <v>1627604.1666666665</v>
+      </c>
+      <c r="M40" s="5">
+        <f t="shared" ref="M40:M51" si="16">J40/L40</f>
+        <v>153.60000000000002</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A41" s="1">
         <v>2</v>
       </c>
-      <c r="B41" s="2">
+      <c r="B41" s="7">
         <f>250/2</f>
         <v>125</v>
       </c>
-      <c r="C41" s="2">
+      <c r="C41" s="7">
         <f>500/2</f>
         <v>250</v>
       </c>
-      <c r="D41" s="2">
+      <c r="D41" s="7">
         <f>C41/2</f>
         <v>125</v>
       </c>
-      <c r="E41" s="2">
+      <c r="E41" s="7">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
-      <c r="F41" s="2">
+      <c r="F41" s="7">
         <f>1200*1000</f>
         <v>1200000</v>
       </c>
-      <c r="G41" s="2">
+      <c r="G41" s="7">
         <f>B41*D41*(E41+D41/2)</f>
         <v>976562.5</v>
       </c>
-      <c r="H41" s="2">
+      <c r="H41" s="7">
         <f t="shared" si="14"/>
         <v>162760416.66666666</v>
       </c>
-      <c r="I41" s="2">
+      <c r="I41" s="7">
         <f>F41*G41/H41/B41</f>
         <v>57.6</v>
       </c>
-      <c r="J41" s="5">
-        <f t="shared" ref="J41:J42" si="15">250000000</f>
+      <c r="J41" s="7">
+        <f t="shared" ref="J41:J42" si="17">250000000</f>
         <v>250000000</v>
       </c>
-      <c r="K41" s="3">
-        <f t="shared" ref="K41:K42" si="16">J41/H41*E41</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="K41" s="7">
+        <f t="shared" ref="K41:K42" si="18">J41/H41*E41</f>
+        <v>0</v>
+      </c>
+      <c r="L41" s="5"/>
+      <c r="M41" s="5"/>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A42" s="1">
         <v>3</v>
       </c>
-      <c r="B42" s="2">
+      <c r="B42" s="7">
         <f>250/2</f>
         <v>125</v>
       </c>
-      <c r="C42" s="2">
+      <c r="C42" s="7">
         <f>500/2</f>
         <v>250</v>
       </c>
-      <c r="D42" s="2">
-        <v>0</v>
-      </c>
-      <c r="E42" s="2">
+      <c r="D42" s="7">
+        <v>0</v>
+      </c>
+      <c r="E42" s="7">
         <f t="shared" si="13"/>
         <v>125</v>
       </c>
-      <c r="F42" s="2">
+      <c r="F42" s="7">
         <f>1200*1000</f>
         <v>1200000</v>
       </c>
-      <c r="G42" s="2">
+      <c r="G42" s="7">
         <f>B42*D42*(E42+D42/2)</f>
         <v>0</v>
       </c>
-      <c r="H42" s="2">
+      <c r="H42" s="7">
         <f t="shared" si="14"/>
         <v>162760416.66666666</v>
       </c>
-      <c r="I42" s="2">
+      <c r="I42" s="7">
         <f>F42*G42/H42/B42</f>
         <v>0</v>
       </c>
-      <c r="J42" s="5">
+      <c r="J42" s="7">
+        <f t="shared" si="17"/>
+        <v>250000000</v>
+      </c>
+      <c r="K42" s="7">
+        <f t="shared" si="18"/>
+        <v>192</v>
+      </c>
+      <c r="L42" s="5">
         <f t="shared" si="15"/>
-        <v>250000000</v>
-      </c>
-      <c r="K42" s="3">
+        <v>1302083.3333333333</v>
+      </c>
+      <c r="M42" s="5">
         <f t="shared" si="16"/>
         <v>192</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A43" s="1">
         <v>4</v>
       </c>
-      <c r="B43" s="2">
+      <c r="B43" s="7">
         <v>50</v>
       </c>
-      <c r="C43" s="2">
+      <c r="C43" s="7">
         <v>120</v>
       </c>
-      <c r="D43" s="2">
+      <c r="D43" s="7">
         <f>C43/2</f>
         <v>60</v>
       </c>
-      <c r="E43" s="2">
+      <c r="E43" s="7">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
-      <c r="F43" s="2">
+      <c r="F43" s="7">
         <f>75*1000</f>
         <v>75000</v>
       </c>
-      <c r="G43" s="2">
+      <c r="G43" s="7">
         <f>B43*D43*(E43+D43/2)</f>
         <v>90000</v>
       </c>
-      <c r="H43" s="2">
+      <c r="H43" s="7">
         <f t="shared" si="14"/>
         <v>7200000</v>
       </c>
-      <c r="I43" s="2">
+      <c r="I43" s="7">
         <f>F43*G43/H43/B43</f>
         <v>18.75</v>
       </c>
-      <c r="J43" s="5"/>
-      <c r="K43" s="3"/>
-    </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J43" s="7"/>
+      <c r="K43" s="7"/>
+      <c r="L43" s="5"/>
+      <c r="M43" s="5"/>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A44" s="1">
         <v>5</v>
       </c>
-      <c r="B44" s="2">
+      <c r="B44" s="7">
         <v>400</v>
       </c>
-      <c r="C44" s="2">
+      <c r="C44" s="7">
         <v>600</v>
       </c>
-      <c r="D44" s="2">
+      <c r="D44" s="7">
         <v>300</v>
       </c>
-      <c r="E44" s="2">
+      <c r="E44" s="7">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
-      <c r="F44" s="2">
+      <c r="F44" s="7">
         <v>500000</v>
       </c>
-      <c r="G44" s="2">
+      <c r="G44" s="7">
         <f>B44*D44*(E44+D44/2)</f>
         <v>18000000</v>
       </c>
-      <c r="H44" s="2">
+      <c r="H44" s="7">
         <f t="shared" si="14"/>
         <v>7200000000</v>
       </c>
-      <c r="I44" s="2">
+      <c r="I44" s="7">
         <f>F44*G44/H44/B44</f>
         <v>3.125</v>
       </c>
-      <c r="J44" s="5"/>
-      <c r="K44" s="3"/>
-    </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J44" s="7"/>
+      <c r="K44" s="7"/>
+      <c r="L44" s="5"/>
+      <c r="M44" s="5"/>
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A45" s="1">
         <v>5</v>
       </c>
-      <c r="B45" s="2">
+      <c r="B45" s="7">
         <v>400</v>
       </c>
-      <c r="C45" s="2">
+      <c r="C45" s="7">
         <v>600</v>
       </c>
-      <c r="D45" s="2">
-        <v>0</v>
-      </c>
-      <c r="E45" s="2">
+      <c r="D45" s="7">
+        <v>0</v>
+      </c>
+      <c r="E45" s="7">
         <f t="shared" si="13"/>
         <v>300</v>
       </c>
-      <c r="H45" s="2">
+      <c r="F45" s="7"/>
+      <c r="G45" s="7"/>
+      <c r="H45" s="7">
         <f t="shared" si="14"/>
         <v>7200000000</v>
       </c>
-      <c r="J45" s="5">
+      <c r="I45" s="7"/>
+      <c r="J45" s="7">
         <f>750000000</f>
         <v>750000000</v>
       </c>
-      <c r="K45" s="3">
-        <f t="shared" ref="K45" si="17">J45/H45*E45</f>
+      <c r="K45" s="7">
+        <f t="shared" ref="K45" si="19">J45/H45*E45</f>
         <v>31.25</v>
       </c>
-    </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L45" s="5">
+        <f t="shared" si="15"/>
+        <v>24000000</v>
+      </c>
+      <c r="M45" s="5">
+        <f t="shared" si="16"/>
+        <v>31.25</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A46" s="1">
         <v>6</v>
       </c>
-      <c r="B46" s="2">
+      <c r="B46" s="7">
         <v>300</v>
       </c>
-      <c r="C46" s="2">
+      <c r="C46" s="7">
         <v>500</v>
       </c>
-      <c r="D46" s="2">
+      <c r="D46" s="7">
         <v>250</v>
       </c>
-      <c r="E46" s="2">
+      <c r="E46" s="7">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
-      <c r="F46" s="2">
+      <c r="F46" s="7">
         <v>2000000</v>
       </c>
-      <c r="G46" s="2">
+      <c r="G46" s="7">
         <f>B46*D46*(E46+D46/2)</f>
         <v>9375000</v>
       </c>
-      <c r="H46" s="2">
+      <c r="H46" s="7">
         <f t="shared" si="14"/>
         <v>3125000000</v>
       </c>
-      <c r="I46" s="2">
+      <c r="I46" s="7">
         <f>F46*G46/H46/B46</f>
         <v>20</v>
       </c>
-      <c r="J46" s="5"/>
-      <c r="K46" s="3"/>
-    </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J46" s="7"/>
+      <c r="K46" s="7"/>
+      <c r="L46" s="5"/>
+      <c r="M46" s="5"/>
+    </row>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A47" s="1">
         <v>6</v>
       </c>
-      <c r="B47" s="2">
+      <c r="B47" s="7">
         <v>300</v>
       </c>
-      <c r="C47" s="2">
+      <c r="C47" s="7">
         <v>500</v>
       </c>
-      <c r="D47" s="2">
-        <v>0</v>
-      </c>
-      <c r="E47" s="2">
+      <c r="D47" s="7">
+        <v>0</v>
+      </c>
+      <c r="E47" s="7">
         <f t="shared" si="13"/>
         <v>250</v>
       </c>
-      <c r="H47" s="2">
+      <c r="F47" s="7"/>
+      <c r="G47" s="7"/>
+      <c r="H47" s="7">
         <f t="shared" si="14"/>
         <v>3125000000</v>
       </c>
-      <c r="J47" s="5">
+      <c r="I47" s="7"/>
+      <c r="J47" s="7">
         <f>6000000000</f>
         <v>6000000000</v>
       </c>
-      <c r="K47" s="3">
-        <f t="shared" ref="K47:K48" si="18">J47/H47*E47</f>
+      <c r="K47" s="7">
+        <f t="shared" ref="K47:K48" si="20">J47/H47*E47</f>
         <v>480</v>
       </c>
-    </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L47" s="5">
+        <f t="shared" si="15"/>
+        <v>12500000</v>
+      </c>
+      <c r="M47" s="5">
+        <f t="shared" si="16"/>
+        <v>480</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A48" s="1">
         <v>7</v>
       </c>
-      <c r="B48" s="2">
+      <c r="B48" s="7">
         <v>240</v>
       </c>
-      <c r="C48" s="2">
+      <c r="C48" s="7">
         <v>360</v>
       </c>
-      <c r="D48" s="2">
+      <c r="D48" s="7">
         <f>C48/2-40</f>
         <v>140</v>
       </c>
-      <c r="E48" s="2">
+      <c r="E48" s="7">
         <f t="shared" si="13"/>
         <v>40</v>
       </c>
-      <c r="F48" s="2">
+      <c r="F48" s="7">
         <f>240*1000</f>
         <v>240000</v>
       </c>
-      <c r="G48" s="2">
+      <c r="G48" s="7">
         <f>B48*D48*(E48+D48/2)</f>
         <v>3696000</v>
       </c>
-      <c r="H48" s="2">
+      <c r="H48" s="7">
         <f t="shared" si="14"/>
         <v>933120000</v>
       </c>
-      <c r="I48" s="2">
-        <f t="shared" ref="I48:I57" si="19">F48*G48/H48/B48</f>
+      <c r="I48" s="7">
+        <f t="shared" ref="I48:I57" si="21">F48*G48/H48/B48</f>
         <v>3.9609053497942388</v>
       </c>
-      <c r="J48" s="5">
+      <c r="J48" s="7">
         <v>720000000</v>
       </c>
-      <c r="K48" s="3">
-        <f t="shared" si="18"/>
+      <c r="K48" s="7">
+        <f t="shared" si="20"/>
         <v>30.864197530864196</v>
       </c>
-    </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L48" s="5">
+        <f t="shared" si="15"/>
+        <v>23328000</v>
+      </c>
+      <c r="M48" s="5">
+        <f t="shared" si="16"/>
+        <v>30.864197530864196</v>
+      </c>
+    </row>
+    <row r="49" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A49" s="1">
         <v>8</v>
       </c>
-      <c r="B49" s="2">
+      <c r="B49" s="7">
         <v>300</v>
       </c>
-      <c r="C49" s="2">
+      <c r="C49" s="7">
         <v>500</v>
       </c>
-      <c r="D49" s="2">
+      <c r="D49" s="7">
         <v>250</v>
       </c>
-      <c r="E49" s="2">
-        <f t="shared" ref="E49" si="20">C49/2-D49</f>
-        <v>0</v>
-      </c>
-      <c r="F49" s="2">
+      <c r="E49" s="7">
+        <f t="shared" ref="E49" si="22">C49/2-D49</f>
+        <v>0</v>
+      </c>
+      <c r="F49" s="7">
         <v>753000</v>
       </c>
-      <c r="G49" s="2">
+      <c r="G49" s="7">
         <f>B49*D49*(E49+D49/2)</f>
         <v>9375000</v>
       </c>
-      <c r="H49" s="2">
-        <f t="shared" ref="H49" si="21">B49*C49^3/12</f>
+      <c r="H49" s="7">
+        <f t="shared" ref="H49" si="23">B49*C49^3/12</f>
         <v>3125000000</v>
       </c>
-      <c r="I49" s="2">
-        <f t="shared" si="19"/>
+      <c r="I49" s="7">
+        <f t="shared" si="21"/>
         <v>7.53</v>
       </c>
-      <c r="J49" s="5"/>
-      <c r="K49" s="3"/>
-    </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J49" s="7"/>
+      <c r="K49" s="7"/>
+      <c r="L49" s="5"/>
+      <c r="M49" s="5"/>
+    </row>
+    <row r="50" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A50" s="1">
         <v>9</v>
       </c>
-      <c r="B50" s="2">
+      <c r="B50" s="7">
         <v>10</v>
       </c>
-      <c r="F50" s="2">
+      <c r="C50" s="7"/>
+      <c r="D50" s="7"/>
+      <c r="E50" s="7"/>
+      <c r="F50" s="7">
         <v>92650</v>
       </c>
-      <c r="G50" s="2">
+      <c r="G50" s="7">
         <f>100*20*70+10*60*30</f>
         <v>158000</v>
       </c>
-      <c r="H50" s="2">
+      <c r="H50" s="7">
         <f>100*160^3/12-90*120^3/12</f>
         <v>21173333.333333336</v>
       </c>
-      <c r="I50" s="3">
-        <f t="shared" si="19"/>
+      <c r="I50" s="7">
+        <f t="shared" si="21"/>
         <v>69.137437027707804</v>
       </c>
-      <c r="J50" s="5"/>
-      <c r="K50" s="3"/>
-    </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J50" s="7"/>
+      <c r="K50" s="7"/>
+      <c r="L50" s="5"/>
+      <c r="M50" s="5"/>
+    </row>
+    <row r="51" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A51" s="1">
         <v>10</v>
       </c>
-      <c r="B51" s="2">
+      <c r="B51" s="7">
         <v>10</v>
       </c>
-      <c r="F51" s="2">
+      <c r="C51" s="7"/>
+      <c r="D51" s="7"/>
+      <c r="E51" s="7"/>
+      <c r="F51" s="7">
         <v>92650</v>
       </c>
-      <c r="G51" s="2">
+      <c r="G51" s="7">
         <f>100*20*70+10*30*45</f>
         <v>153500</v>
       </c>
-      <c r="H51" s="2">
+      <c r="H51" s="7">
         <f>100*160^3/12-90*120^3/12</f>
         <v>21173333.333333336</v>
       </c>
-      <c r="I51" s="3">
-        <f t="shared" si="19"/>
+      <c r="I51" s="7">
+        <f t="shared" si="21"/>
         <v>67.168332808564216</v>
       </c>
-      <c r="J51" s="5"/>
-      <c r="K51" s="3"/>
-    </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J51" s="7"/>
+      <c r="K51" s="7"/>
+      <c r="L51" s="5"/>
+      <c r="M51" s="5"/>
+    </row>
+    <row r="52" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A52" s="1">
         <v>11</v>
       </c>
-      <c r="B52" s="2">
+      <c r="B52" s="7">
         <v>200</v>
       </c>
-      <c r="C52" s="2">
+      <c r="C52" s="7">
         <v>360</v>
       </c>
-      <c r="D52" s="2">
-        <v>0</v>
-      </c>
-      <c r="E52" s="2">
-        <f t="shared" ref="E52" si="22">C52/2-D52</f>
+      <c r="D52" s="7">
+        <v>0</v>
+      </c>
+      <c r="E52" s="7">
+        <f t="shared" ref="E52" si="24">C52/2-D52</f>
         <v>180</v>
       </c>
-      <c r="G52" s="2">
-        <f t="shared" ref="G52:G57" si="23">B52*D52*(E52+D52/2)</f>
-        <v>0</v>
-      </c>
-      <c r="H52" s="2">
-        <f t="shared" ref="H52" si="24">B52*C52^3/12</f>
+      <c r="F52" s="7"/>
+      <c r="G52" s="7">
+        <f t="shared" ref="G52:G57" si="25">B52*D52*(E52+D52/2)</f>
+        <v>0</v>
+      </c>
+      <c r="H52" s="7">
+        <f t="shared" ref="H52" si="26">B52*C52^3/12</f>
         <v>777600000</v>
       </c>
-      <c r="I52" s="2">
-        <f t="shared" si="19"/>
-        <v>0</v>
-      </c>
-      <c r="J52" s="5">
+      <c r="I52" s="7">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="J52" s="7">
         <f>350*1000000</f>
         <v>350000000</v>
       </c>
-      <c r="K52" s="3">
-        <f t="shared" ref="K52" si="25">J52/H52*E52</f>
+      <c r="K52" s="5">
+        <f t="shared" ref="K52" si="27">J52/H52*E52</f>
         <v>81.018518518518519</v>
       </c>
-    </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L52" s="5">
+        <f>H52/E52</f>
+        <v>4320000</v>
+      </c>
+      <c r="M52" s="5">
+        <f>J52/L52</f>
+        <v>81.018518518518519</v>
+      </c>
+    </row>
+    <row r="53" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A53" s="1">
         <v>11</v>
       </c>
-      <c r="B53" s="2">
+      <c r="B53" s="7">
         <v>200</v>
       </c>
-      <c r="C53" s="2">
+      <c r="C53" s="7">
         <v>360</v>
       </c>
-      <c r="D53" s="2">
+      <c r="D53" s="7">
         <f>C53/2</f>
         <v>180</v>
       </c>
-      <c r="E53" s="2">
-        <f t="shared" ref="E53:E54" si="26">C53/2-D53</f>
-        <v>0</v>
-      </c>
-      <c r="G53" s="2">
-        <f t="shared" si="23"/>
+      <c r="E53" s="7">
+        <f t="shared" ref="E53:E54" si="28">C53/2-D53</f>
+        <v>0</v>
+      </c>
+      <c r="F53" s="7"/>
+      <c r="G53" s="7">
+        <f t="shared" si="25"/>
         <v>3240000</v>
       </c>
-      <c r="H53" s="2">
-        <f t="shared" ref="H53:H54" si="27">B53*C53^3/12</f>
+      <c r="H53" s="7">
+        <f t="shared" ref="H53:H54" si="29">B53*C53^3/12</f>
         <v>777600000</v>
       </c>
-      <c r="I53" s="2">
-        <f t="shared" si="19"/>
-        <v>0</v>
-      </c>
-      <c r="J53" s="5">
+      <c r="I53" s="7">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="J53" s="7">
         <f>350*1000000</f>
         <v>350000000</v>
       </c>
-      <c r="K53" s="3">
-        <f t="shared" ref="K53:K54" si="28">J53/H53*E53</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="K53" s="5">
+        <f t="shared" ref="K53:K54" si="30">J53/H53*E53</f>
+        <v>0</v>
+      </c>
+      <c r="L53" s="5"/>
+      <c r="M53" s="5"/>
+    </row>
+    <row r="54" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A54" s="1">
         <v>12</v>
       </c>
-      <c r="B54" s="2">
+      <c r="B54" s="7">
         <v>100</v>
       </c>
-      <c r="C54" s="2">
+      <c r="C54" s="7">
         <v>220</v>
       </c>
-      <c r="D54" s="2">
-        <v>0</v>
-      </c>
-      <c r="E54" s="2">
-        <f t="shared" si="26"/>
+      <c r="D54" s="7">
+        <v>0</v>
+      </c>
+      <c r="E54" s="7">
+        <f t="shared" si="28"/>
         <v>110</v>
       </c>
-      <c r="G54" s="2">
-        <f t="shared" si="23"/>
-        <v>0</v>
-      </c>
-      <c r="H54" s="2">
-        <f t="shared" si="27"/>
+      <c r="F54" s="7"/>
+      <c r="G54" s="7">
+        <f t="shared" si="25"/>
+        <v>0</v>
+      </c>
+      <c r="H54" s="7">
+        <f t="shared" si="29"/>
         <v>88733333.333333328</v>
       </c>
-      <c r="I54" s="2">
-        <f t="shared" si="19"/>
-        <v>0</v>
-      </c>
-      <c r="J54" s="5">
+      <c r="I54" s="7">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="J54" s="7">
         <f>76.3*1000000</f>
         <v>76300000</v>
       </c>
-      <c r="K54" s="3">
-        <f t="shared" si="28"/>
+      <c r="K54" s="5">
+        <f t="shared" si="30"/>
         <v>94.586776859504141</v>
       </c>
-    </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L54" s="5">
+        <f t="shared" ref="L53:L64" si="31">H54/E54</f>
+        <v>806666.66666666663</v>
+      </c>
+      <c r="M54" s="5">
+        <f t="shared" ref="M53:M64" si="32">J54/L54</f>
+        <v>94.586776859504141</v>
+      </c>
+    </row>
+    <row r="55" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A55" s="1">
         <v>12</v>
       </c>
-      <c r="B55" s="2">
+      <c r="B55" s="7">
         <v>100</v>
       </c>
-      <c r="C55" s="2">
+      <c r="C55" s="7">
         <v>220</v>
       </c>
-      <c r="D55" s="2">
+      <c r="D55" s="7">
         <v>35</v>
       </c>
-      <c r="E55" s="2">
-        <f t="shared" ref="E55:E56" si="29">C55/2-D55</f>
+      <c r="E55" s="7">
+        <f t="shared" ref="E55:E56" si="33">C55/2-D55</f>
         <v>75</v>
       </c>
-      <c r="G55" s="2">
-        <f t="shared" si="23"/>
+      <c r="F55" s="7"/>
+      <c r="G55" s="7">
+        <f t="shared" si="25"/>
         <v>323750</v>
       </c>
-      <c r="H55" s="2">
-        <f t="shared" ref="H55:H56" si="30">B55*C55^3/12</f>
+      <c r="H55" s="7">
+        <f t="shared" ref="H55:H56" si="34">B55*C55^3/12</f>
         <v>88733333.333333328</v>
       </c>
-      <c r="I55" s="2">
-        <f t="shared" si="19"/>
-        <v>0</v>
-      </c>
-      <c r="J55" s="5">
-        <f t="shared" ref="J55:J57" si="31">76.3*1000000</f>
+      <c r="I55" s="7">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="J55" s="7">
+        <f t="shared" ref="J55:J57" si="35">76.3*1000000</f>
         <v>76300000</v>
       </c>
-      <c r="K55" s="3">
-        <f t="shared" ref="K55:K56" si="32">J55/H55*E55</f>
+      <c r="K55" s="5">
+        <f t="shared" ref="K55:K56" si="36">J55/H55*E55</f>
         <v>64.490984222389187</v>
       </c>
-    </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L55" s="5"/>
+      <c r="M55" s="5"/>
+    </row>
+    <row r="56" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A56" s="1">
         <v>12</v>
       </c>
-      <c r="B56" s="2">
+      <c r="B56" s="7">
         <v>100</v>
       </c>
-      <c r="C56" s="2">
+      <c r="C56" s="7">
         <v>220</v>
       </c>
-      <c r="D56" s="2">
+      <c r="D56" s="7">
         <v>60</v>
       </c>
-      <c r="E56" s="2">
-        <f t="shared" si="29"/>
+      <c r="E56" s="7">
+        <f t="shared" si="33"/>
         <v>50</v>
       </c>
-      <c r="G56" s="2">
-        <f t="shared" si="23"/>
+      <c r="F56" s="7"/>
+      <c r="G56" s="7">
+        <f t="shared" si="25"/>
         <v>480000</v>
       </c>
-      <c r="H56" s="2">
-        <f t="shared" si="30"/>
+      <c r="H56" s="7">
+        <f t="shared" si="34"/>
         <v>88733333.333333328</v>
       </c>
-      <c r="I56" s="2">
-        <f t="shared" si="19"/>
-        <v>0</v>
-      </c>
-      <c r="J56" s="5">
-        <f t="shared" si="31"/>
+      <c r="I56" s="7">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="J56" s="7">
+        <f t="shared" si="35"/>
         <v>76300000</v>
       </c>
-      <c r="K56" s="3">
-        <f t="shared" si="32"/>
+      <c r="K56" s="5">
+        <f t="shared" si="36"/>
         <v>42.993989481592791</v>
       </c>
-    </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L56" s="5"/>
+      <c r="M56" s="5"/>
+    </row>
+    <row r="57" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A57" s="1">
         <v>12</v>
       </c>
-      <c r="B57" s="2">
+      <c r="B57" s="7">
         <v>100</v>
       </c>
-      <c r="C57" s="2">
+      <c r="C57" s="7">
         <v>220</v>
       </c>
-      <c r="D57" s="2">
+      <c r="D57" s="7">
         <v>85</v>
       </c>
-      <c r="E57" s="2">
-        <f t="shared" ref="E57" si="33">C57/2-D57</f>
+      <c r="E57" s="7">
+        <f t="shared" ref="E57" si="37">C57/2-D57</f>
         <v>25</v>
       </c>
-      <c r="G57" s="2">
-        <f t="shared" si="23"/>
+      <c r="F57" s="7"/>
+      <c r="G57" s="7">
+        <f t="shared" si="25"/>
         <v>573750</v>
       </c>
-      <c r="H57" s="2">
-        <f t="shared" ref="H57" si="34">B57*C57^3/12</f>
+      <c r="H57" s="7">
+        <f t="shared" ref="H57" si="38">B57*C57^3/12</f>
         <v>88733333.333333328</v>
       </c>
-      <c r="I57" s="2">
-        <f t="shared" si="19"/>
-        <v>0</v>
-      </c>
-      <c r="J57" s="5">
-        <f t="shared" si="31"/>
+      <c r="I57" s="7">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="J57" s="7">
+        <f t="shared" si="35"/>
         <v>76300000</v>
       </c>
-      <c r="K57" s="3">
-        <f t="shared" ref="K57" si="35">J57/H57*E57</f>
+      <c r="K57" s="5">
+        <f t="shared" ref="K57" si="39">J57/H57*E57</f>
         <v>21.496994740796396</v>
       </c>
-    </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L57" s="5"/>
+      <c r="M57" s="5"/>
+    </row>
+    <row r="58" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A58" s="1">
         <v>13</v>
       </c>
-      <c r="B58" s="2">
+      <c r="B58" s="7">
         <v>10</v>
       </c>
-      <c r="E58" s="2">
-        <v>0</v>
-      </c>
-      <c r="H58" s="2">
+      <c r="C58" s="7"/>
+      <c r="D58" s="7"/>
+      <c r="E58" s="7">
+        <v>0</v>
+      </c>
+      <c r="F58" s="7"/>
+      <c r="G58" s="7"/>
+      <c r="H58" s="7">
         <f>100*160^3/12-90*120^3/12</f>
         <v>21173333.333333336</v>
       </c>
-      <c r="J58" s="5">
+      <c r="I58" s="7"/>
+      <c r="J58" s="7">
         <f>73*1000000</f>
         <v>73000000</v>
       </c>
-      <c r="K58" s="3">
-        <f t="shared" ref="K58:K59" si="36">J58/H58*E58</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="K58" s="5">
+        <f t="shared" ref="K58:K59" si="40">J58/H58*E58</f>
+        <v>0</v>
+      </c>
+      <c r="L58" s="5"/>
+      <c r="M58" s="5"/>
+    </row>
+    <row r="59" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A59" s="1">
         <v>13</v>
       </c>
-      <c r="B59" s="2">
+      <c r="B59" s="7">
         <v>10</v>
       </c>
-      <c r="E59" s="2">
+      <c r="C59" s="7"/>
+      <c r="D59" s="7"/>
+      <c r="E59" s="7">
         <v>30</v>
       </c>
-      <c r="H59" s="2">
+      <c r="F59" s="7"/>
+      <c r="G59" s="7"/>
+      <c r="H59" s="7">
         <f>100*160^3/12-90*120^3/12</f>
         <v>21173333.333333336</v>
       </c>
-      <c r="J59" s="5">
+      <c r="I59" s="7"/>
+      <c r="J59" s="7">
         <f>73*1000000</f>
         <v>73000000</v>
       </c>
-      <c r="K59" s="3">
-        <f t="shared" si="36"/>
+      <c r="K59" s="5">
+        <f t="shared" si="40"/>
         <v>103.43198992443322</v>
       </c>
-    </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L59" s="5"/>
+      <c r="M59" s="5"/>
+    </row>
+    <row r="60" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A60" s="1">
         <v>13</v>
       </c>
-      <c r="B60" s="2">
+      <c r="B60" s="7">
         <v>10</v>
       </c>
-      <c r="E60" s="2">
+      <c r="C60" s="7"/>
+      <c r="D60" s="7"/>
+      <c r="E60" s="7">
         <v>60</v>
       </c>
-      <c r="H60" s="2">
+      <c r="F60" s="7"/>
+      <c r="G60" s="7"/>
+      <c r="H60" s="7">
         <f>100*160^3/12-90*120^3/12</f>
         <v>21173333.333333336</v>
       </c>
-      <c r="J60" s="5">
+      <c r="I60" s="7"/>
+      <c r="J60" s="7">
         <f>73*1000000</f>
         <v>73000000</v>
       </c>
-      <c r="K60" s="3">
-        <f t="shared" ref="K60:K64" si="37">J60/H60*E60</f>
+      <c r="K60" s="5">
+        <f t="shared" ref="K60:K64" si="41">J60/H60*E60</f>
         <v>206.86397984886645</v>
       </c>
-    </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L60" s="5"/>
+      <c r="M60" s="5"/>
+    </row>
+    <row r="61" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A61" s="1">
         <v>13</v>
       </c>
-      <c r="B61" s="2">
+      <c r="B61" s="7">
         <v>10</v>
       </c>
-      <c r="E61" s="2">
+      <c r="C61" s="7"/>
+      <c r="D61" s="7"/>
+      <c r="E61" s="7">
         <v>80</v>
       </c>
-      <c r="H61" s="2">
+      <c r="F61" s="7"/>
+      <c r="G61" s="7"/>
+      <c r="H61" s="7">
         <f>100*160^3/12-90*120^3/12</f>
         <v>21173333.333333336</v>
       </c>
-      <c r="J61" s="5">
+      <c r="I61" s="7"/>
+      <c r="J61" s="7">
         <f>73*1000000</f>
         <v>73000000</v>
       </c>
-      <c r="K61" s="3">
-        <f t="shared" si="37"/>
+      <c r="K61" s="5">
+        <f t="shared" si="41"/>
         <v>275.81863979848862</v>
       </c>
-    </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L61" s="5">
+        <f t="shared" si="31"/>
+        <v>264666.66666666669</v>
+      </c>
+      <c r="M61" s="5">
+        <f t="shared" si="32"/>
+        <v>275.81863979848862</v>
+      </c>
+    </row>
+    <row r="62" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A62" s="1">
         <v>14</v>
       </c>
-      <c r="B62" s="2">
+      <c r="B62" s="7">
         <v>200</v>
       </c>
-      <c r="C62" s="2">
+      <c r="C62" s="7">
         <v>360</v>
       </c>
-      <c r="D62" s="2">
-        <v>0</v>
-      </c>
-      <c r="E62" s="2">
-        <f t="shared" ref="E62:E63" si="38">C62/2-D62</f>
+      <c r="D62" s="7">
+        <v>0</v>
+      </c>
+      <c r="E62" s="7">
+        <f t="shared" ref="E62:E63" si="42">C62/2-D62</f>
         <v>180</v>
       </c>
-      <c r="F62" s="2">
+      <c r="F62" s="7">
         <f>80*4/2*1000</f>
         <v>160000</v>
       </c>
-      <c r="G62" s="2">
+      <c r="G62" s="7">
         <f>B62*D62*(E62+D62/2)</f>
         <v>0</v>
       </c>
-      <c r="H62" s="2">
-        <f t="shared" ref="H62" si="39">B62*C62^3/12</f>
+      <c r="H62" s="7">
+        <f t="shared" ref="H62" si="43">B62*C62^3/12</f>
         <v>777600000</v>
       </c>
-      <c r="I62" s="3">
+      <c r="I62" s="7">
         <f>F62*G62/H62/B62</f>
         <v>0</v>
       </c>
-      <c r="J62" s="5">
+      <c r="J62" s="7">
         <f>80*4^2/8*1000000</f>
         <v>160000000</v>
       </c>
-      <c r="K62" s="3">
-        <f t="shared" ref="K62" si="40">J62/H62*E62</f>
+      <c r="K62" s="5">
+        <f t="shared" ref="K62" si="44">J62/H62*E62</f>
         <v>37.037037037037038</v>
       </c>
-    </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L62" s="5">
+        <f t="shared" si="31"/>
+        <v>4320000</v>
+      </c>
+      <c r="M62" s="5">
+        <f t="shared" si="32"/>
+        <v>37.037037037037038</v>
+      </c>
+    </row>
+    <row r="63" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A63" s="1">
         <v>14</v>
       </c>
-      <c r="B63" s="2">
+      <c r="B63" s="7">
         <v>200</v>
       </c>
-      <c r="C63" s="2">
+      <c r="C63" s="7">
         <v>360</v>
       </c>
-      <c r="D63" s="2">
+      <c r="D63" s="7">
         <f>C63/2</f>
         <v>180</v>
       </c>
-      <c r="E63" s="2">
-        <f t="shared" si="38"/>
-        <v>0</v>
-      </c>
-      <c r="F63" s="2">
+      <c r="E63" s="7">
+        <f t="shared" si="42"/>
+        <v>0</v>
+      </c>
+      <c r="F63" s="7">
         <f>80*4/2*1000</f>
         <v>160000</v>
       </c>
-      <c r="G63" s="2">
+      <c r="G63" s="7">
         <f>B63*D63*(E63+D63/2)</f>
         <v>3240000</v>
       </c>
-      <c r="H63" s="2">
-        <f t="shared" ref="H63:H64" si="41">B63*C63^3/12</f>
+      <c r="H63" s="7">
+        <f t="shared" ref="H63:H64" si="45">B63*C63^3/12</f>
         <v>777600000</v>
       </c>
-      <c r="I63" s="3">
+      <c r="I63" s="7">
         <f>F63*G63/H63/B63</f>
         <v>3.333333333333333</v>
       </c>
-      <c r="J63" s="5">
+      <c r="J63" s="7">
         <f>80*4^2/8*1000000</f>
         <v>160000000</v>
       </c>
-      <c r="K63" s="3">
-        <f t="shared" si="37"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="K63" s="5">
+        <f t="shared" si="41"/>
+        <v>0</v>
+      </c>
+      <c r="L63" s="5"/>
+      <c r="M63" s="5"/>
+    </row>
+    <row r="64" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A64" s="1">
         <v>15</v>
       </c>
-      <c r="B64" s="2">
+      <c r="B64" s="7">
         <v>360</v>
       </c>
-      <c r="C64" s="2">
+      <c r="C64" s="7">
         <v>600</v>
       </c>
-      <c r="D64" s="2">
+      <c r="D64" s="7">
         <f>C64/2-50</f>
         <v>250</v>
       </c>
-      <c r="E64" s="2">
-        <f t="shared" ref="E64" si="42">C64/2-D64</f>
+      <c r="E64" s="7">
+        <f t="shared" ref="E64" si="46">C64/2-D64</f>
         <v>50</v>
       </c>
-      <c r="F64" s="2">
+      <c r="F64" s="7">
         <f>350*6*1000</f>
         <v>2100000</v>
       </c>
-      <c r="G64" s="2">
+      <c r="G64" s="7">
         <f>B64*D64*(E64+D64/2)</f>
         <v>15750000</v>
       </c>
-      <c r="H64" s="5">
-        <f t="shared" si="41"/>
+      <c r="H64" s="7">
+        <f t="shared" si="45"/>
         <v>6480000000</v>
       </c>
-      <c r="I64" s="3">
+      <c r="I64" s="7">
         <f>F64*G64/H64/B64</f>
         <v>14.178240740740742</v>
       </c>
-      <c r="J64" s="5">
+      <c r="J64" s="7">
         <f>350*6*3*1000000</f>
         <v>6300000000</v>
       </c>
-      <c r="K64" s="3">
-        <f t="shared" si="37"/>
+      <c r="K64" s="5">
+        <f t="shared" si="41"/>
         <v>48.611111111111107</v>
+      </c>
+      <c r="L64" s="5">
+        <f t="shared" si="31"/>
+        <v>129600000</v>
+      </c>
+      <c r="M64" s="5">
+        <f t="shared" si="32"/>
+        <v>48.611111111111114</v>
       </c>
     </row>
     <row r="71" spans="1:13" x14ac:dyDescent="0.3">
@@ -3106,35 +3268,35 @@
         <v>-50</v>
       </c>
       <c r="E72" s="3">
-        <f t="shared" ref="E72:E78" si="43">ATAN(-2*D72/(B72-C72))/2</f>
+        <f t="shared" ref="E72:E78" si="47">ATAN(-2*D72/(B72-C72))/2</f>
         <v>9.8697779924940388E-2</v>
       </c>
       <c r="F72" s="3">
-        <f t="shared" ref="F72:F78" si="44">E72*180/PI()</f>
+        <f t="shared" ref="F72:F78" si="48">E72*180/PI()</f>
         <v>5.6549662370101066</v>
       </c>
       <c r="G72" s="3">
-        <f t="shared" ref="G72:G78" si="45">(B72+C72)/2</f>
+        <f t="shared" ref="G72:G78" si="49">(B72+C72)/2</f>
         <v>750</v>
       </c>
       <c r="H72" s="3">
-        <f t="shared" ref="H72:H78" si="46">SQRT((B72-C72)^2/4+D72^2)</f>
+        <f t="shared" ref="H72:H78" si="50">SQRT((B72-C72)^2/4+D72^2)</f>
         <v>254.95097567963924</v>
       </c>
       <c r="I72" s="3">
-        <f t="shared" ref="I72:I78" si="47">G72+H72</f>
+        <f t="shared" ref="I72:I78" si="51">G72+H72</f>
         <v>1004.9509756796392</v>
       </c>
       <c r="J72" s="3">
-        <f t="shared" ref="J72:J78" si="48">G72-H72</f>
+        <f t="shared" ref="J72:J78" si="52">G72-H72</f>
         <v>495.04902432036079</v>
       </c>
       <c r="K72" s="3">
-        <f t="shared" ref="K72:K76" si="49">F72+45</f>
+        <f t="shared" ref="K72:K76" si="53">F72+45</f>
         <v>50.654966237010107</v>
       </c>
       <c r="L72" s="3">
-        <f t="shared" ref="L72:L76" si="50">K72-90</f>
+        <f t="shared" ref="L72:L76" si="54">K72-90</f>
         <v>-39.345033762989893</v>
       </c>
       <c r="M72" s="3"/>
@@ -3153,35 +3315,35 @@
         <v>-2400000</v>
       </c>
       <c r="E73" s="3">
-        <f t="shared" si="43"/>
+        <f t="shared" si="47"/>
         <v>0.5880026035475675</v>
       </c>
       <c r="F73" s="3">
-        <f t="shared" si="44"/>
+        <f t="shared" si="48"/>
         <v>33.690067525979785</v>
       </c>
       <c r="G73" s="3">
-        <f t="shared" si="45"/>
+        <f t="shared" si="49"/>
         <v>4333333.3333333302</v>
       </c>
       <c r="H73" s="3">
-        <f t="shared" si="46"/>
+        <f t="shared" si="50"/>
         <v>2600000</v>
       </c>
       <c r="I73" s="3">
-        <f t="shared" si="47"/>
+        <f t="shared" si="51"/>
         <v>6933333.3333333302</v>
       </c>
       <c r="J73" s="3">
-        <f t="shared" si="48"/>
+        <f t="shared" si="52"/>
         <v>1733333.3333333302</v>
       </c>
       <c r="K73" s="3">
-        <f t="shared" si="49"/>
+        <f t="shared" si="53"/>
         <v>78.690067525979785</v>
       </c>
       <c r="L73" s="3">
-        <f t="shared" si="50"/>
+        <f t="shared" si="54"/>
         <v>-11.309932474020215</v>
       </c>
       <c r="M73" s="3"/>
@@ -3200,35 +3362,35 @@
         <v>345</v>
       </c>
       <c r="E74" s="3">
-        <f t="shared" si="43"/>
+        <f t="shared" si="47"/>
         <v>0.6390052264115833</v>
       </c>
       <c r="F74" s="3">
-        <f t="shared" si="44"/>
+        <f t="shared" si="48"/>
         <v>36.612302560185327</v>
       </c>
       <c r="G74" s="3">
-        <f t="shared" si="45"/>
+        <f t="shared" si="49"/>
         <v>636</v>
       </c>
       <c r="H74" s="3">
-        <f t="shared" si="46"/>
+        <f t="shared" si="50"/>
         <v>360.33456675706259</v>
       </c>
       <c r="I74" s="3">
-        <f t="shared" si="47"/>
+        <f t="shared" si="51"/>
         <v>996.33456675706259</v>
       </c>
       <c r="J74" s="3">
-        <f t="shared" si="48"/>
+        <f t="shared" si="52"/>
         <v>275.66543324293741</v>
       </c>
       <c r="K74" s="3">
-        <f t="shared" si="49"/>
+        <f t="shared" si="53"/>
         <v>81.612302560185327</v>
       </c>
       <c r="L74" s="3">
-        <f t="shared" si="50"/>
+        <f t="shared" si="54"/>
         <v>-8.3876974398146729</v>
       </c>
       <c r="M74" s="3"/>
@@ -3247,35 +3409,35 @@
         <v>200</v>
       </c>
       <c r="E75" s="3">
-        <f t="shared" si="43"/>
+        <f t="shared" si="47"/>
         <v>-0.60601282826216218</v>
       </c>
       <c r="F75" s="3">
-        <f t="shared" si="44"/>
+        <f t="shared" si="48"/>
         <v>-34.721977390208266</v>
       </c>
       <c r="G75" s="3">
-        <f t="shared" si="45"/>
+        <f t="shared" si="49"/>
         <v>225</v>
       </c>
       <c r="H75" s="3">
-        <f t="shared" si="46"/>
+        <f t="shared" si="50"/>
         <v>213.60009363293827</v>
       </c>
       <c r="I75" s="3">
-        <f t="shared" si="47"/>
+        <f t="shared" si="51"/>
         <v>438.6000936329383</v>
       </c>
       <c r="J75" s="3">
-        <f t="shared" si="48"/>
+        <f t="shared" si="52"/>
         <v>11.399906367061732</v>
       </c>
       <c r="K75" s="3">
-        <f t="shared" si="49"/>
+        <f t="shared" si="53"/>
         <v>10.278022609791734</v>
       </c>
       <c r="L75" s="3">
-        <f t="shared" si="50"/>
+        <f t="shared" si="54"/>
         <v>-79.721977390208266</v>
       </c>
       <c r="M75" s="3"/>
@@ -3294,35 +3456,35 @@
         <v>40</v>
       </c>
       <c r="E76" s="3">
-        <f t="shared" si="43"/>
+        <f t="shared" si="47"/>
         <v>-0.46364760900080609</v>
       </c>
       <c r="F76" s="3">
-        <f t="shared" si="44"/>
+        <f t="shared" si="48"/>
         <v>-26.56505117707799</v>
       </c>
       <c r="G76" s="3">
-        <f t="shared" si="45"/>
+        <f t="shared" si="49"/>
         <v>20</v>
       </c>
       <c r="H76" s="3">
-        <f t="shared" si="46"/>
+        <f t="shared" si="50"/>
         <v>50</v>
       </c>
       <c r="I76" s="3">
-        <f t="shared" si="47"/>
+        <f t="shared" si="51"/>
         <v>70</v>
       </c>
       <c r="J76" s="3">
-        <f t="shared" si="48"/>
+        <f t="shared" si="52"/>
         <v>-30</v>
       </c>
       <c r="K76" s="3">
-        <f t="shared" si="49"/>
+        <f t="shared" si="53"/>
         <v>18.43494882292201</v>
       </c>
       <c r="L76" s="3">
-        <f t="shared" si="50"/>
+        <f t="shared" si="54"/>
         <v>-71.56505117707799</v>
       </c>
       <c r="M76" s="3"/>
@@ -3341,35 +3503,35 @@
         <v>-550</v>
       </c>
       <c r="E77" s="3">
-        <f t="shared" si="43"/>
+        <f t="shared" si="47"/>
         <v>0.61101266160549483</v>
       </c>
       <c r="F77" s="3">
-        <f t="shared" si="44"/>
+        <f t="shared" si="48"/>
         <v>35.008446739050015</v>
       </c>
       <c r="G77" s="3">
-        <f t="shared" si="45"/>
+        <f t="shared" si="49"/>
         <v>600</v>
       </c>
       <c r="H77" s="3">
-        <f t="shared" si="46"/>
+        <f t="shared" si="50"/>
         <v>585.23499553598128</v>
       </c>
       <c r="I77" s="3">
-        <f t="shared" si="47"/>
+        <f t="shared" si="51"/>
         <v>1185.2349955359814</v>
       </c>
       <c r="J77" s="3">
-        <f t="shared" si="48"/>
+        <f t="shared" si="52"/>
         <v>14.765004464018716</v>
       </c>
       <c r="K77" s="3">
-        <f t="shared" ref="K77:K84" si="51">F77+45</f>
+        <f t="shared" ref="K77:K84" si="55">F77+45</f>
         <v>80.008446739050015</v>
       </c>
       <c r="L77" s="3">
-        <f t="shared" ref="L77:L84" si="52">K77-90</f>
+        <f t="shared" ref="L77:L84" si="56">K77-90</f>
         <v>-9.9915532609499849</v>
       </c>
       <c r="M77" s="3"/>
@@ -3390,35 +3552,35 @@
         <v>3.9609053497942388</v>
       </c>
       <c r="E78" s="3">
-        <f t="shared" si="43"/>
+        <f t="shared" si="47"/>
         <v>-0.12562163201205953</v>
       </c>
       <c r="F78" s="3">
-        <f t="shared" si="44"/>
+        <f t="shared" si="48"/>
         <v>-7.1975893298365268</v>
       </c>
       <c r="G78" s="3">
-        <f t="shared" si="45"/>
+        <f t="shared" si="49"/>
         <v>15.432098765432098</v>
       </c>
       <c r="H78" s="3">
-        <f t="shared" si="46"/>
+        <f t="shared" si="50"/>
         <v>15.932308165990248</v>
       </c>
       <c r="I78" s="3">
-        <f t="shared" si="47"/>
+        <f t="shared" si="51"/>
         <v>31.364406931422344</v>
       </c>
       <c r="J78" s="3">
-        <f t="shared" si="48"/>
+        <f t="shared" si="52"/>
         <v>-0.50020940055815011</v>
       </c>
       <c r="K78" s="3">
-        <f t="shared" si="51"/>
+        <f t="shared" si="55"/>
         <v>37.802410670163475</v>
       </c>
       <c r="L78" s="3">
-        <f t="shared" si="52"/>
+        <f t="shared" si="56"/>
         <v>-52.197589329836525</v>
       </c>
       <c r="M78" s="3">
@@ -3440,35 +3602,35 @@
         <v>-24</v>
       </c>
       <c r="E79" s="3">
-        <f t="shared" ref="E79:E83" si="53">ATAN(-2*D79/(B79-C79))/2</f>
+        <f t="shared" ref="E79:E83" si="57">ATAN(-2*D79/(B79-C79))/2</f>
         <v>-4.7663858426665248E-2</v>
       </c>
       <c r="F79" s="3">
-        <f t="shared" ref="F79:F83" si="54">E79*180/PI()</f>
+        <f t="shared" ref="F79:F83" si="58">E79*180/PI()</f>
         <v>-2.7309379231569828</v>
       </c>
       <c r="G79" s="3">
-        <f t="shared" ref="G79:G83" si="55">(B79+C79)/2</f>
+        <f t="shared" ref="G79:G83" si="59">(B79+C79)/2</f>
         <v>101</v>
       </c>
       <c r="H79" s="3">
-        <f t="shared" ref="H79:H83" si="56">SQRT((B79-C79)^2/4+D79^2)</f>
+        <f t="shared" ref="H79:H83" si="60">SQRT((B79-C79)^2/4+D79^2)</f>
         <v>252.14479966876175</v>
       </c>
       <c r="I79" s="3">
-        <f t="shared" ref="I79:I83" si="57">G79+H79</f>
+        <f t="shared" ref="I79:I83" si="61">G79+H79</f>
         <v>353.14479966876172</v>
       </c>
       <c r="J79" s="3">
-        <f t="shared" ref="J79:J83" si="58">G79-H79</f>
+        <f t="shared" ref="J79:J83" si="62">G79-H79</f>
         <v>-151.14479966876175</v>
       </c>
       <c r="K79" s="3">
-        <f t="shared" si="51"/>
+        <f t="shared" si="55"/>
         <v>42.269062076843014</v>
       </c>
       <c r="L79" s="3">
-        <f t="shared" si="52"/>
+        <f t="shared" si="56"/>
         <v>-47.730937923156986</v>
       </c>
       <c r="M79" s="3">
@@ -3490,35 +3652,35 @@
         <v>120</v>
       </c>
       <c r="E80" s="3">
-        <f t="shared" si="53"/>
+        <f t="shared" si="57"/>
         <v>0.5880026035475675</v>
       </c>
       <c r="F80" s="3">
-        <f t="shared" si="54"/>
+        <f t="shared" si="58"/>
         <v>33.690067525979785</v>
       </c>
       <c r="G80" s="3">
+        <f t="shared" si="59"/>
+        <v>-350</v>
+      </c>
+      <c r="H80" s="3">
+        <f t="shared" si="60"/>
+        <v>130</v>
+      </c>
+      <c r="I80" s="3">
+        <f t="shared" si="61"/>
+        <v>-220</v>
+      </c>
+      <c r="J80" s="3">
+        <f t="shared" si="62"/>
+        <v>-480</v>
+      </c>
+      <c r="K80" s="3">
         <f t="shared" si="55"/>
-        <v>-350</v>
-      </c>
-      <c r="H80" s="3">
+        <v>78.690067525979785</v>
+      </c>
+      <c r="L80" s="3">
         <f t="shared" si="56"/>
-        <v>130</v>
-      </c>
-      <c r="I80" s="3">
-        <f t="shared" si="57"/>
-        <v>-220</v>
-      </c>
-      <c r="J80" s="3">
-        <f t="shared" si="58"/>
-        <v>-480</v>
-      </c>
-      <c r="K80" s="3">
-        <f t="shared" si="51"/>
-        <v>78.690067525979785</v>
-      </c>
-      <c r="L80" s="3">
-        <f t="shared" si="52"/>
         <v>-11.309932474020215</v>
       </c>
       <c r="M80" s="3"/>
@@ -3537,35 +3699,35 @@
         <v>80</v>
       </c>
       <c r="E81" s="3">
-        <f t="shared" si="53"/>
+        <f t="shared" si="57"/>
         <v>0.26747753689304821</v>
       </c>
       <c r="F81" s="3">
-        <f t="shared" si="54"/>
+        <f t="shared" si="58"/>
         <v>15.325333978526434</v>
       </c>
       <c r="G81" s="3">
+        <f t="shared" si="59"/>
+        <v>-15</v>
+      </c>
+      <c r="H81" s="3">
+        <f t="shared" si="60"/>
+        <v>156.92354826475216</v>
+      </c>
+      <c r="I81" s="3">
+        <f t="shared" si="61"/>
+        <v>141.92354826475216</v>
+      </c>
+      <c r="J81" s="3">
+        <f t="shared" si="62"/>
+        <v>-171.92354826475216</v>
+      </c>
+      <c r="K81" s="3">
         <f t="shared" si="55"/>
-        <v>-15</v>
-      </c>
-      <c r="H81" s="3">
+        <v>60.32533397852643</v>
+      </c>
+      <c r="L81" s="3">
         <f t="shared" si="56"/>
-        <v>156.92354826475216</v>
-      </c>
-      <c r="I81" s="3">
-        <f t="shared" si="57"/>
-        <v>141.92354826475216</v>
-      </c>
-      <c r="J81" s="3">
-        <f t="shared" si="58"/>
-        <v>-171.92354826475216</v>
-      </c>
-      <c r="K81" s="3">
-        <f t="shared" si="51"/>
-        <v>60.32533397852643</v>
-      </c>
-      <c r="L81" s="3">
-        <f t="shared" si="52"/>
         <v>-29.67466602147357</v>
       </c>
       <c r="M81" s="3"/>
@@ -3584,35 +3746,35 @@
         <v>95</v>
       </c>
       <c r="E82" s="3">
-        <f t="shared" si="53"/>
+        <f t="shared" si="57"/>
         <v>-0.47304018463635611</v>
       </c>
       <c r="F82" s="3">
-        <f t="shared" si="54"/>
+        <f t="shared" si="58"/>
         <v>-27.103206119752414</v>
       </c>
       <c r="G82" s="3">
+        <f t="shared" si="59"/>
+        <v>196.5</v>
+      </c>
+      <c r="H82" s="3">
+        <f t="shared" si="60"/>
+        <v>117.1206642740725</v>
+      </c>
+      <c r="I82" s="3">
+        <f t="shared" si="61"/>
+        <v>313.62066427407251</v>
+      </c>
+      <c r="J82" s="3">
+        <f t="shared" si="62"/>
+        <v>79.379335725927504</v>
+      </c>
+      <c r="K82" s="3">
         <f t="shared" si="55"/>
-        <v>196.5</v>
-      </c>
-      <c r="H82" s="3">
+        <v>17.896793880247586</v>
+      </c>
+      <c r="L82" s="3">
         <f t="shared" si="56"/>
-        <v>117.1206642740725</v>
-      </c>
-      <c r="I82" s="3">
-        <f t="shared" si="57"/>
-        <v>313.62066427407251</v>
-      </c>
-      <c r="J82" s="3">
-        <f t="shared" si="58"/>
-        <v>79.379335725927504</v>
-      </c>
-      <c r="K82" s="3">
-        <f t="shared" si="51"/>
-        <v>17.896793880247586</v>
-      </c>
-      <c r="L82" s="3">
-        <f t="shared" si="52"/>
         <v>-72.103206119752414</v>
       </c>
       <c r="M82" s="3"/>
@@ -3631,35 +3793,35 @@
         <v>-765</v>
       </c>
       <c r="E83" s="3">
-        <f t="shared" si="53"/>
+        <f t="shared" si="57"/>
         <v>0.62188051502639119</v>
       </c>
       <c r="F83" s="3">
-        <f t="shared" si="54"/>
+        <f t="shared" si="58"/>
         <v>35.631128872434189</v>
       </c>
       <c r="G83" s="3">
+        <f t="shared" si="59"/>
+        <v>-127.5</v>
+      </c>
+      <c r="H83" s="3">
+        <f t="shared" si="60"/>
+        <v>807.81510879656116</v>
+      </c>
+      <c r="I83" s="3">
+        <f t="shared" si="61"/>
+        <v>680.31510879656116</v>
+      </c>
+      <c r="J83" s="3">
+        <f t="shared" si="62"/>
+        <v>-935.31510879656116</v>
+      </c>
+      <c r="K83" s="3">
         <f t="shared" si="55"/>
-        <v>-127.5</v>
-      </c>
-      <c r="H83" s="3">
+        <v>80.631128872434189</v>
+      </c>
+      <c r="L83" s="3">
         <f t="shared" si="56"/>
-        <v>807.81510879656116</v>
-      </c>
-      <c r="I83" s="3">
-        <f t="shared" si="57"/>
-        <v>680.31510879656116</v>
-      </c>
-      <c r="J83" s="3">
-        <f t="shared" si="58"/>
-        <v>-935.31510879656116</v>
-      </c>
-      <c r="K83" s="3">
-        <f t="shared" si="51"/>
-        <v>80.631128872434189</v>
-      </c>
-      <c r="L83" s="3">
-        <f t="shared" si="52"/>
         <v>-9.3688711275658108</v>
       </c>
       <c r="M83" s="3"/>
@@ -3680,35 +3842,35 @@
         <v>14.178240740740742</v>
       </c>
       <c r="E84" s="3">
-        <f t="shared" ref="E84" si="59">ATAN(-2*D84/(B84-C84))/2</f>
+        <f t="shared" ref="E84" si="63">ATAN(-2*D84/(B84-C84))/2</f>
         <v>-0.26403722421317988</v>
       </c>
       <c r="F84" s="3">
-        <f t="shared" ref="F84" si="60">E84*180/PI()</f>
+        <f t="shared" ref="F84" si="64">E84*180/PI()</f>
         <v>-15.128218581764637</v>
       </c>
       <c r="G84" s="3">
-        <f t="shared" ref="G84" si="61">(B84+C84)/2</f>
+        <f t="shared" ref="G84" si="65">(B84+C84)/2</f>
         <v>24.305555555555554</v>
       </c>
       <c r="H84" s="3">
-        <f t="shared" ref="H84" si="62">SQRT((B84-C84)^2/4+D84^2)</f>
+        <f t="shared" ref="H84" si="66">SQRT((B84-C84)^2/4+D84^2)</f>
         <v>28.138630765668005</v>
       </c>
       <c r="I84" s="3">
-        <f t="shared" ref="I84" si="63">G84+H84</f>
+        <f t="shared" ref="I84" si="67">G84+H84</f>
         <v>52.444186321223555</v>
       </c>
       <c r="J84" s="3">
-        <f t="shared" ref="J84" si="64">G84-H84</f>
+        <f t="shared" ref="J84" si="68">G84-H84</f>
         <v>-3.833075210112451</v>
       </c>
       <c r="K84" s="3">
-        <f t="shared" si="51"/>
+        <f t="shared" si="55"/>
         <v>29.871781418235365</v>
       </c>
       <c r="L84" s="3">
-        <f t="shared" si="52"/>
+        <f t="shared" si="56"/>
         <v>-60.128218581764635</v>
       </c>
       <c r="M84" s="3"/>
@@ -3773,40 +3935,40 @@
       <c r="A89" t="s">
         <v>78</v>
       </c>
-      <c r="B89" s="6" t="s">
+      <c r="B89" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="C89" s="7" t="s">
+      <c r="C89" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="D89" s="8" t="s">
+      <c r="D89" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="E89" s="8" t="s">
+      <c r="E89" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="F89" s="8" t="s">
+      <c r="F89" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="G89" s="9" t="s">
+      <c r="G89" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="H89" s="9" t="s">
+      <c r="H89" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="I89" s="9" t="s">
+      <c r="I89" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="K89" s="6" t="s">
+      <c r="K89" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="L89" s="6" t="s">
+      <c r="L89" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="M89" s="6" t="s">
+      <c r="M89" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="N89" s="6" t="s">
+      <c r="N89" s="5" t="s">
         <v>85</v>
       </c>
     </row>
@@ -3814,49 +3976,49 @@
       <c r="A90">
         <v>300</v>
       </c>
-      <c r="B90" s="10">
+      <c r="B90" s="9">
         <v>200</v>
       </c>
-      <c r="C90" s="7">
+      <c r="C90" s="6">
         <f>A90/6</f>
         <v>50</v>
       </c>
-      <c r="D90" s="8">
+      <c r="D90" s="7">
         <f>A90*B90</f>
         <v>60000</v>
       </c>
-      <c r="E90" s="10">
+      <c r="E90" s="9">
         <f>A90^3*B90/12</f>
         <v>450000000</v>
       </c>
-      <c r="F90" s="10">
+      <c r="F90" s="9">
         <f>A90^2*B90/6</f>
         <v>3000000</v>
       </c>
-      <c r="G90" s="9">
+      <c r="G90" s="8">
         <v>300000</v>
       </c>
-      <c r="H90" s="9">
+      <c r="H90" s="8">
         <v>100</v>
       </c>
-      <c r="I90" s="9">
-        <f>G90*H90</f>
+      <c r="I90" s="8">
+        <f t="shared" ref="I90:I98" si="69">G90*H90</f>
         <v>30000000</v>
       </c>
-      <c r="K90" s="6">
-        <f>-G90/D90</f>
+      <c r="K90" s="5">
+        <f t="shared" ref="K90:K98" si="70">-G90/D90</f>
         <v>-5</v>
       </c>
-      <c r="L90" s="6">
-        <f>I90/F90</f>
+      <c r="L90" s="5">
+        <f t="shared" ref="L90:L98" si="71">I90/F90</f>
         <v>10</v>
       </c>
-      <c r="M90" s="6">
-        <f>K90+L90</f>
+      <c r="M90" s="5">
+        <f t="shared" ref="M90:M98" si="72">K90+L90</f>
         <v>5</v>
       </c>
-      <c r="N90" s="6">
-        <f>K90-L90</f>
+      <c r="N90" s="5">
+        <f t="shared" ref="N90:N98" si="73">K90-L90</f>
         <v>-15</v>
       </c>
     </row>
@@ -3864,87 +4026,87 @@
       <c r="A91">
         <v>500</v>
       </c>
-      <c r="B91" s="10">
+      <c r="B91" s="9">
         <v>300</v>
       </c>
-      <c r="C91" s="7">
+      <c r="C91" s="6">
         <f>A91/6</f>
         <v>83.333333333333329</v>
       </c>
-      <c r="D91" s="8">
+      <c r="D91" s="7">
         <f>A91*B91</f>
         <v>150000</v>
       </c>
-      <c r="E91" s="10">
+      <c r="E91" s="9">
         <f>A91^3*B91/12</f>
         <v>3125000000</v>
       </c>
-      <c r="F91" s="10">
+      <c r="F91" s="9">
         <f>A91^2*B91/6</f>
         <v>12500000</v>
       </c>
-      <c r="G91" s="9">
+      <c r="G91" s="8">
         <v>3253600</v>
       </c>
-      <c r="H91" s="9">
+      <c r="H91" s="8">
         <v>47</v>
       </c>
-      <c r="I91" s="9">
-        <f>G91*H91</f>
+      <c r="I91" s="8">
+        <f t="shared" si="69"/>
         <v>152919200</v>
       </c>
-      <c r="K91" s="6">
-        <f>-G91/D91</f>
+      <c r="K91" s="5">
+        <f t="shared" si="70"/>
         <v>-21.690666666666665</v>
       </c>
-      <c r="L91" s="6">
-        <f>I91/F91</f>
+      <c r="L91" s="5">
+        <f t="shared" si="71"/>
         <v>12.233536000000001</v>
       </c>
-      <c r="M91" s="6">
-        <f>K91+L91</f>
+      <c r="M91" s="5">
+        <f t="shared" si="72"/>
         <v>-9.4571306666666644</v>
       </c>
-      <c r="N91" s="6">
-        <f>K91-L91</f>
+      <c r="N91" s="5">
+        <f t="shared" si="73"/>
         <v>-33.924202666666666</v>
       </c>
     </row>
     <row r="92" spans="1:14" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B92" s="6"/>
-      <c r="C92" s="7"/>
-      <c r="D92" s="8">
+      <c r="B92" s="5"/>
+      <c r="C92" s="6"/>
+      <c r="D92" s="7">
         <v>4678</v>
       </c>
-      <c r="E92" s="8"/>
-      <c r="F92" s="8">
+      <c r="E92" s="7"/>
+      <c r="F92" s="7">
         <v>481000</v>
       </c>
-      <c r="G92" s="8">
+      <c r="G92" s="7">
         <f>53.3*1000</f>
         <v>53300</v>
       </c>
-      <c r="H92" s="8">
+      <c r="H92" s="7">
         <v>750.5</v>
       </c>
-      <c r="I92" s="8">
-        <f>G92*H92</f>
+      <c r="I92" s="7">
+        <f t="shared" si="69"/>
         <v>40001650</v>
       </c>
-      <c r="K92" s="6">
-        <f>-G92/D92</f>
+      <c r="K92" s="5">
+        <f t="shared" si="70"/>
         <v>-11.39375801624626</v>
       </c>
-      <c r="L92" s="6">
-        <f>I92/F92</f>
+      <c r="L92" s="5">
+        <f t="shared" si="71"/>
         <v>83.163513513513507</v>
       </c>
-      <c r="M92" s="6">
-        <f>K92+L92</f>
+      <c r="M92" s="5">
+        <f t="shared" si="72"/>
         <v>71.769755497267255</v>
       </c>
-      <c r="N92" s="6">
-        <f>K92-L92</f>
+      <c r="N92" s="5">
+        <f t="shared" si="73"/>
         <v>-94.55727152975976</v>
       </c>
     </row>
@@ -3952,49 +4114,49 @@
       <c r="A93">
         <v>300</v>
       </c>
-      <c r="B93" s="10">
+      <c r="B93" s="9">
         <v>250</v>
       </c>
-      <c r="C93" s="7">
-        <f>A93/6</f>
+      <c r="C93" s="6">
+        <f t="shared" ref="C93:C98" si="74">A93/6</f>
         <v>50</v>
       </c>
-      <c r="D93" s="8">
-        <f>A93*B93</f>
+      <c r="D93" s="7">
+        <f t="shared" ref="D93:D98" si="75">A93*B93</f>
         <v>75000</v>
       </c>
-      <c r="E93" s="10">
-        <f>A93^3*B93/12</f>
+      <c r="E93" s="9">
+        <f t="shared" ref="E93:E98" si="76">A93^3*B93/12</f>
         <v>562500000</v>
       </c>
-      <c r="F93" s="10">
-        <f>A93^2*B93/6</f>
+      <c r="F93" s="9">
+        <f t="shared" ref="F93:F98" si="77">A93^2*B93/6</f>
         <v>3750000</v>
       </c>
-      <c r="G93" s="9">
+      <c r="G93" s="8">
         <v>925600</v>
       </c>
-      <c r="H93" s="9">
+      <c r="H93" s="8">
         <v>40</v>
       </c>
-      <c r="I93" s="9">
-        <f>G93*H93</f>
+      <c r="I93" s="8">
+        <f t="shared" si="69"/>
         <v>37024000</v>
       </c>
-      <c r="K93" s="6">
-        <f>-G93/D93</f>
+      <c r="K93" s="5">
+        <f t="shared" si="70"/>
         <v>-12.341333333333333</v>
       </c>
-      <c r="L93" s="6">
-        <f>I93/F93</f>
+      <c r="L93" s="5">
+        <f t="shared" si="71"/>
         <v>9.8730666666666664</v>
       </c>
-      <c r="M93" s="6">
-        <f>K93+L93</f>
+      <c r="M93" s="5">
+        <f t="shared" si="72"/>
         <v>-2.4682666666666666</v>
       </c>
-      <c r="N93" s="6">
-        <f>K93-L93</f>
+      <c r="N93" s="5">
+        <f t="shared" si="73"/>
         <v>-22.214399999999998</v>
       </c>
     </row>
@@ -4002,49 +4164,49 @@
       <c r="A94">
         <v>488</v>
       </c>
-      <c r="B94" s="10">
+      <c r="B94" s="9">
         <v>320</v>
       </c>
-      <c r="C94" s="7">
-        <f>A94/6</f>
+      <c r="C94" s="6">
+        <f t="shared" si="74"/>
         <v>81.333333333333329</v>
       </c>
-      <c r="D94" s="8">
-        <f>A94*B94</f>
+      <c r="D94" s="7">
+        <f t="shared" si="75"/>
         <v>156160</v>
       </c>
-      <c r="E94" s="10">
-        <f>A94^3*B94/12</f>
+      <c r="E94" s="9">
+        <f t="shared" si="76"/>
         <v>3099047253.3333335</v>
       </c>
-      <c r="F94" s="10">
-        <f>A94^2*B94/6</f>
+      <c r="F94" s="9">
+        <f t="shared" si="77"/>
         <v>12701013.333333334</v>
       </c>
-      <c r="G94" s="9">
+      <c r="G94" s="8">
         <v>5213400</v>
       </c>
-      <c r="H94" s="9">
+      <c r="H94" s="8">
         <v>180</v>
       </c>
-      <c r="I94" s="9">
-        <f>G94*H94</f>
+      <c r="I94" s="8">
+        <f t="shared" si="69"/>
         <v>938412000</v>
       </c>
-      <c r="K94" s="6">
-        <f>-G94/D94</f>
+      <c r="K94" s="5">
+        <f t="shared" si="70"/>
         <v>-33.384989754098363</v>
       </c>
-      <c r="L94" s="6">
-        <f>I94/F94</f>
+      <c r="L94" s="5">
+        <f t="shared" si="71"/>
         <v>73.884813390217687</v>
       </c>
-      <c r="M94" s="6">
-        <f>K94+L94</f>
+      <c r="M94" s="5">
+        <f t="shared" si="72"/>
         <v>40.499823636119324</v>
       </c>
-      <c r="N94" s="6">
-        <f>K94-L94</f>
+      <c r="N94" s="5">
+        <f t="shared" si="73"/>
         <v>-107.26980314431606</v>
       </c>
     </row>
@@ -4052,49 +4214,49 @@
       <c r="A95">
         <v>480</v>
       </c>
-      <c r="B95" s="10">
+      <c r="B95" s="9">
         <v>300</v>
       </c>
-      <c r="C95" s="7">
-        <f>A95/6</f>
+      <c r="C95" s="6">
+        <f t="shared" si="74"/>
         <v>80</v>
       </c>
-      <c r="D95" s="8">
-        <f>A95*B95</f>
+      <c r="D95" s="7">
+        <f t="shared" si="75"/>
         <v>144000</v>
       </c>
-      <c r="E95" s="10">
-        <f>A95^3*B95/12</f>
+      <c r="E95" s="9">
+        <f t="shared" si="76"/>
         <v>2764800000</v>
       </c>
-      <c r="F95" s="10">
-        <f>A95^2*B95/6</f>
+      <c r="F95" s="9">
+        <f t="shared" si="77"/>
         <v>11520000</v>
       </c>
-      <c r="G95" s="9">
+      <c r="G95" s="8">
         <v>5000000</v>
       </c>
-      <c r="H95" s="9">
-        <v>0</v>
-      </c>
-      <c r="I95" s="9">
-        <f>G95*H95</f>
-        <v>0</v>
-      </c>
-      <c r="K95" s="6">
-        <f>-G95/D95</f>
+      <c r="H95" s="8">
+        <v>0</v>
+      </c>
+      <c r="I95" s="8">
+        <f t="shared" si="69"/>
+        <v>0</v>
+      </c>
+      <c r="K95" s="5">
+        <f t="shared" si="70"/>
         <v>-34.722222222222221</v>
       </c>
-      <c r="L95" s="6">
-        <f>I95/F95</f>
-        <v>0</v>
-      </c>
-      <c r="M95" s="6">
-        <f>K95+L95</f>
+      <c r="L95" s="5">
+        <f t="shared" si="71"/>
+        <v>0</v>
+      </c>
+      <c r="M95" s="5">
+        <f t="shared" si="72"/>
         <v>-34.722222222222221</v>
       </c>
-      <c r="N95" s="6">
-        <f>K95-L95</f>
+      <c r="N95" s="5">
+        <f t="shared" si="73"/>
         <v>-34.722222222222221</v>
       </c>
     </row>
@@ -4102,49 +4264,49 @@
       <c r="A96">
         <v>480</v>
       </c>
-      <c r="B96" s="10">
+      <c r="B96" s="9">
         <v>300</v>
       </c>
-      <c r="C96" s="7">
-        <f>A96/6</f>
+      <c r="C96" s="6">
+        <f t="shared" si="74"/>
         <v>80</v>
       </c>
-      <c r="D96" s="8">
-        <f>A96*B96</f>
+      <c r="D96" s="7">
+        <f t="shared" si="75"/>
         <v>144000</v>
       </c>
-      <c r="E96" s="10">
-        <f>A96^3*B96/12</f>
+      <c r="E96" s="9">
+        <f t="shared" si="76"/>
         <v>2764800000</v>
       </c>
-      <c r="F96" s="10">
-        <f>A96^2*B96/6</f>
+      <c r="F96" s="9">
+        <f t="shared" si="77"/>
         <v>11520000</v>
       </c>
-      <c r="G96" s="9">
+      <c r="G96" s="8">
         <v>5000000</v>
       </c>
-      <c r="H96" s="9">
+      <c r="H96" s="8">
         <v>40</v>
       </c>
-      <c r="I96" s="9">
-        <f>G96*H96</f>
+      <c r="I96" s="8">
+        <f t="shared" si="69"/>
         <v>200000000</v>
       </c>
-      <c r="K96" s="6">
-        <f>-G96/D96</f>
+      <c r="K96" s="5">
+        <f t="shared" si="70"/>
         <v>-34.722222222222221</v>
       </c>
-      <c r="L96" s="6">
-        <f>I96/F96</f>
+      <c r="L96" s="5">
+        <f t="shared" si="71"/>
         <v>17.361111111111111</v>
       </c>
-      <c r="M96" s="6">
-        <f>K96+L96</f>
+      <c r="M96" s="5">
+        <f t="shared" si="72"/>
         <v>-17.361111111111111</v>
       </c>
-      <c r="N96" s="6">
-        <f>K96-L96</f>
+      <c r="N96" s="5">
+        <f t="shared" si="73"/>
         <v>-52.083333333333329</v>
       </c>
     </row>
@@ -4152,49 +4314,49 @@
       <c r="A97">
         <v>480</v>
       </c>
-      <c r="B97" s="10">
+      <c r="B97" s="9">
         <v>300</v>
       </c>
-      <c r="C97" s="7">
-        <f>A97/6</f>
+      <c r="C97" s="6">
+        <f t="shared" si="74"/>
         <v>80</v>
       </c>
-      <c r="D97" s="8">
-        <f>A97*B97</f>
+      <c r="D97" s="7">
+        <f t="shared" si="75"/>
         <v>144000</v>
       </c>
-      <c r="E97" s="10">
-        <f>A97^3*B97/12</f>
+      <c r="E97" s="9">
+        <f t="shared" si="76"/>
         <v>2764800000</v>
       </c>
-      <c r="F97" s="10">
-        <f>A97^2*B97/6</f>
+      <c r="F97" s="9">
+        <f t="shared" si="77"/>
         <v>11520000</v>
       </c>
-      <c r="G97" s="9">
+      <c r="G97" s="8">
         <v>5000000</v>
       </c>
-      <c r="H97" s="9">
+      <c r="H97" s="8">
         <v>80</v>
       </c>
-      <c r="I97" s="9">
-        <f>G97*H97</f>
+      <c r="I97" s="8">
+        <f t="shared" si="69"/>
         <v>400000000</v>
       </c>
-      <c r="K97" s="6">
-        <f>-G97/D97</f>
+      <c r="K97" s="5">
+        <f t="shared" si="70"/>
         <v>-34.722222222222221</v>
       </c>
-      <c r="L97" s="6">
-        <f>I97/F97</f>
+      <c r="L97" s="5">
+        <f t="shared" si="71"/>
         <v>34.722222222222221</v>
       </c>
-      <c r="M97" s="6">
-        <f>K97+L97</f>
-        <v>0</v>
-      </c>
-      <c r="N97" s="6">
-        <f>K97-L97</f>
+      <c r="M97" s="5">
+        <f t="shared" si="72"/>
+        <v>0</v>
+      </c>
+      <c r="N97" s="5">
+        <f t="shared" si="73"/>
         <v>-69.444444444444443</v>
       </c>
     </row>
@@ -4202,93 +4364,93 @@
       <c r="A98">
         <v>480</v>
       </c>
-      <c r="B98" s="10">
+      <c r="B98" s="9">
         <v>300</v>
       </c>
-      <c r="C98" s="7">
-        <f>A98/6</f>
+      <c r="C98" s="6">
+        <f t="shared" si="74"/>
         <v>80</v>
       </c>
-      <c r="D98" s="8">
-        <f>A98*B98</f>
+      <c r="D98" s="7">
+        <f t="shared" si="75"/>
         <v>144000</v>
       </c>
-      <c r="E98" s="10">
-        <f>A98^3*B98/12</f>
+      <c r="E98" s="9">
+        <f t="shared" si="76"/>
         <v>2764800000</v>
       </c>
-      <c r="F98" s="10">
-        <f>A98^2*B98/6</f>
+      <c r="F98" s="9">
+        <f t="shared" si="77"/>
         <v>11520000</v>
       </c>
-      <c r="G98" s="9">
+      <c r="G98" s="8">
         <v>5000000</v>
       </c>
-      <c r="H98" s="9">
+      <c r="H98" s="8">
         <v>120</v>
       </c>
-      <c r="I98" s="9">
-        <f>G98*H98</f>
+      <c r="I98" s="8">
+        <f t="shared" si="69"/>
         <v>600000000</v>
       </c>
-      <c r="K98" s="6">
-        <f>-G98/D98</f>
+      <c r="K98" s="5">
+        <f t="shared" si="70"/>
         <v>-34.722222222222221</v>
       </c>
-      <c r="L98" s="6">
-        <f>I98/F98</f>
+      <c r="L98" s="5">
+        <f t="shared" si="71"/>
         <v>52.083333333333336</v>
       </c>
-      <c r="M98" s="6">
-        <f>K98+L98</f>
+      <c r="M98" s="5">
+        <f t="shared" si="72"/>
         <v>17.361111111111114</v>
       </c>
-      <c r="N98" s="6">
-        <f>K98-L98</f>
+      <c r="N98" s="5">
+        <f t="shared" si="73"/>
         <v>-86.805555555555557</v>
       </c>
     </row>
     <row r="99" spans="1:14" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B99" s="10"/>
-      <c r="C99" s="7"/>
-      <c r="D99" s="8"/>
-      <c r="E99" s="10"/>
-      <c r="F99" s="10"/>
-      <c r="G99" s="9"/>
-      <c r="H99" s="9"/>
-      <c r="I99" s="9"/>
-      <c r="K99" s="6"/>
-      <c r="L99" s="6"/>
-      <c r="M99" s="6"/>
-      <c r="N99" s="6"/>
+      <c r="B99" s="9"/>
+      <c r="C99" s="6"/>
+      <c r="D99" s="7"/>
+      <c r="E99" s="9"/>
+      <c r="F99" s="9"/>
+      <c r="G99" s="8"/>
+      <c r="H99" s="8"/>
+      <c r="I99" s="8"/>
+      <c r="K99" s="5"/>
+      <c r="L99" s="5"/>
+      <c r="M99" s="5"/>
+      <c r="N99" s="5"/>
     </row>
     <row r="100" spans="1:14" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B100" s="10"/>
-      <c r="C100" s="7"/>
-      <c r="D100" s="8"/>
-      <c r="E100" s="10"/>
-      <c r="F100" s="10"/>
-      <c r="G100" s="9"/>
-      <c r="H100" s="9"/>
-      <c r="I100" s="9"/>
-      <c r="K100" s="6"/>
-      <c r="L100" s="6"/>
-      <c r="M100" s="6"/>
-      <c r="N100" s="6"/>
+      <c r="B100" s="9"/>
+      <c r="C100" s="6"/>
+      <c r="D100" s="7"/>
+      <c r="E100" s="9"/>
+      <c r="F100" s="9"/>
+      <c r="G100" s="8"/>
+      <c r="H100" s="8"/>
+      <c r="I100" s="8"/>
+      <c r="K100" s="5"/>
+      <c r="L100" s="5"/>
+      <c r="M100" s="5"/>
+      <c r="N100" s="5"/>
     </row>
     <row r="101" spans="1:14" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B101" s="10"/>
-      <c r="C101" s="7"/>
-      <c r="D101" s="8"/>
-      <c r="E101" s="10"/>
-      <c r="F101" s="10"/>
-      <c r="G101" s="9"/>
-      <c r="H101" s="9"/>
-      <c r="I101" s="9"/>
-      <c r="K101" s="6"/>
-      <c r="L101" s="6"/>
-      <c r="M101" s="6"/>
-      <c r="N101" s="6"/>
+      <c r="B101" s="9"/>
+      <c r="C101" s="6"/>
+      <c r="D101" s="7"/>
+      <c r="E101" s="9"/>
+      <c r="F101" s="9"/>
+      <c r="G101" s="8"/>
+      <c r="H101" s="8"/>
+      <c r="I101" s="8"/>
+      <c r="K101" s="5"/>
+      <c r="L101" s="5"/>
+      <c r="M101" s="5"/>
+      <c r="N101" s="5"/>
     </row>
     <row r="103" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B103" s="2" t="s">

</xml_diff>